<commit_message>
+tsu, heatmap labels added
</commit_message>
<xml_diff>
--- a/RPD_output/dataset_res.xlsx
+++ b/RPD_output/dataset_res.xlsx
@@ -14,11 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="339">
   <si>
     <t>title</t>
   </si>
   <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>oop_name</t>
+  </si>
+  <si>
     <t>Doc</t>
   </si>
   <si>
@@ -163,6 +169,534 @@
     <t>Численное решение инженерных задач</t>
   </si>
   <si>
+    <t>Анализ данных в бизнес-аналитике</t>
+  </si>
+  <si>
+    <t>Анализ заинтересованных сторон _* Stakeholder Analysis</t>
+  </si>
+  <si>
+    <t>Аналитика цепей поставок</t>
+  </si>
+  <si>
+    <t>Архитектура предприятия</t>
+  </si>
+  <si>
+    <t>Аудит</t>
+  </si>
+  <si>
+    <t>Базы данных</t>
+  </si>
+  <si>
+    <t>Бизнес в глобальном контексте _* Business in Global Context</t>
+  </si>
+  <si>
+    <t>Введение в профессиональную деятельность</t>
+  </si>
+  <si>
+    <t>Деловые коммуникации</t>
+  </si>
+  <si>
+    <t>Дополнительные главы анализа данных</t>
+  </si>
+  <si>
+    <t>Дополнительные главы эконометрики</t>
+  </si>
+  <si>
+    <t>Имитационное моделирование</t>
+  </si>
+  <si>
+    <t>Инвестиции</t>
+  </si>
+  <si>
+    <t>Иностранный язык</t>
+  </si>
+  <si>
+    <t>Институциональная экономика</t>
+  </si>
+  <si>
+    <t>Информационные системы моделирования бизнес-процессов</t>
+  </si>
+  <si>
+    <t>Информационные технологии</t>
+  </si>
+  <si>
+    <t>Исследовательский семинар</t>
+  </si>
+  <si>
+    <t>История (история России, всеобщая история)</t>
+  </si>
+  <si>
+    <t>Картины мира: навигация</t>
+  </si>
+  <si>
+    <t>Корпоративная социальная ответственность и этика бизнеса</t>
+  </si>
+  <si>
+    <t>Корпоративные информационные системы</t>
+  </si>
+  <si>
+    <t>Критическое мышление и письмо</t>
+  </si>
+  <si>
+    <t>Линейная алгебра</t>
+  </si>
+  <si>
+    <t>Макроэкономика</t>
+  </si>
+  <si>
+    <t>Маркетинг</t>
+  </si>
+  <si>
+    <t>Математическая статистика</t>
+  </si>
+  <si>
+    <t>Математический анализ</t>
+  </si>
+  <si>
+    <t>Международная экономика</t>
+  </si>
+  <si>
+    <t>Менеджмент</t>
+  </si>
+  <si>
+    <t>Методы принятия оптимальных решений</t>
+  </si>
+  <si>
+    <t>Микроэкономика</t>
+  </si>
+  <si>
+    <t>Микроэкономика 2</t>
+  </si>
+  <si>
+    <t>Моделирование цепей поставок</t>
+  </si>
+  <si>
+    <t>Налоги и налогообложение</t>
+  </si>
+  <si>
+    <t>Операционный менеджмент</t>
+  </si>
+  <si>
+    <t>Оценка бизнеса</t>
+  </si>
+  <si>
+    <t>Пакеты прикладных программ бизнес-планирования и оценки инвестиционных проектов</t>
+  </si>
+  <si>
+    <t>Пакеты прикладных программ оперативного анализа данных</t>
+  </si>
+  <si>
+    <t>Поведенческая экономика и финансы</t>
+  </si>
+  <si>
+    <t>Портфельные инвестиции</t>
+  </si>
+  <si>
+    <t>Право</t>
+  </si>
+  <si>
+    <t>Практикум по картинам мира</t>
+  </si>
+  <si>
+    <t>Предпринимательство</t>
+  </si>
+  <si>
+    <t>Региональная экономика</t>
+  </si>
+  <si>
+    <t>Риск-менеджмент и комплаенс</t>
+  </si>
+  <si>
+    <t>Стратегический менеджмент</t>
+  </si>
+  <si>
+    <t>Теория вероятностей и случайные процессы</t>
+  </si>
+  <si>
+    <t>Теория игр</t>
+  </si>
+  <si>
+    <t>Теория экономических механизмов</t>
+  </si>
+  <si>
+    <t>Управление проектами</t>
+  </si>
+  <si>
+    <t>Финансовая система и институты</t>
+  </si>
+  <si>
+    <t>Финансовые вычисления</t>
+  </si>
+  <si>
+    <t>Финансовый менеджмент</t>
+  </si>
+  <si>
+    <t>Финансовый учет и отчетность</t>
+  </si>
+  <si>
+    <t>Ценообразование</t>
+  </si>
+  <si>
+    <t>Эконометрика</t>
+  </si>
+  <si>
+    <t>Экономика отраслевых рынков</t>
+  </si>
+  <si>
+    <t>Экономическая социология</t>
+  </si>
+  <si>
+    <t>Экономическая статистика</t>
+  </si>
+  <si>
+    <t>Экономический анализ</t>
+  </si>
+  <si>
+    <t>Элективные дисциплины по физической культуре и спорту</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине Раздел 1. Основы тестирования. РД, РД2  Лекции 8 Тестирование и оценка качества Лабораторные занятия 12 ПО. Самостоятельная работа 34 Раздел 2. Формирование и РДЗ Лекции 8 реализация стратегии Лабораторные занятия 12 тестирования ПО Самостоятельная работа 34  Содержание разделов дисциплины:  Раздел 1. Основы тестирования. Тестирование и оценка качества ПО.  В рамках раздела рассматриваются общие теоретические основы процесса тестирования программного обеспечения, в том числе механизмы выявления, формирования и оценка качества,  требований; стратегии и виды тестирования.  Темы лекций: 1. Тестирование ПО. Ретроспектива и основы.  2. Требования. Выявление. Анализ. Документирование. Проверка.  3. Виды и стратегии тестирования.  Темы практических занятий: 1. Отчеты о дефектах.  2. ГОСТР ИСО/МЭК 25041-2014. Требования и оценка качества систем и программного  обеспечения.  3. ГОСТР ИСОЛМЭК 25021-2014. Требования и оценка качества систем и программного  обеспечения. Элементы показателя качества.  4. Управление проектом. Планирование и отчетность.  Названия лабораторных работ:  1. Требования. Выявление, оценка качества и документирование.  Раздел 2. Формирование и реализация стратегии тестирования ПО  Раздел формирует навыки разработки и реализации стратегии тестирования. Рассматриваются такие специализированные виды тестирования как: автоматизированное, регрессионное и тестирование удобства использования.  Темы лекций: 1. Автоматизация тестирования.  2. Регрессионное тестирование. Нефункциональное тестирование.  3. Тестирование удобства использования.  Названия лабораторных работ: 1. Модульное тестирование. 2. Регрессионное тестирование.  Темы практических занятий: 1. Неформальная проверка кода. Оценка качества документированности кода.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины результат Виды учебной деятельности Евы обучения по времени, ч. дисциплине }. Лекции 8 Раздел 1. Основы работы с растровой 2D- ¥ ., РД-1 Лабораторные занятия 16 графикой в дизайне Самостоятельная работа 30 .. Лекции 8 Раздел 2. Основы работы с векторной 2D- ¥ ., РД-1 Лабораторные занятия 16 графикой в дизайне Самостоятельная работа 30  Содержание разделов дисциплины:  Раздел 1. Основы работы с растровой 2)-графикой в дизайне  Введение в изучение растровой графики, цветовых моделей и форматов файлов Темы лекций: 1. Введение. Растровая и векторная графика. Форматы графических файлов.  2  2. Работа с цветом в компьютерной графике: основные определения, параметры цвета 3. Работа с цветом в компьютерной графике: цветовые модели 4. Текст в растровых программах Названия лабораторных работ: Кадрирование, перспектива. Выравнивание горизонта, работа с искажениями Цветокоррекция и перевод в ч/б Работа со слоями, маски слоя, простые коллажи Работа с корректирующими слоями Цветокоррекция с помощью корректирующих слоев Сложные коллажи Кисти, паттерны . Работа с текстом 10. Анимация 11. Создание макета сайта  © чи  \O  Раздел 2. Основы работы с векторной 2)-графикой в дизайне  Введение в изучение векторной графики, верстки документов и подготовка файлов к печати  Темы лекций:  5. Основы разметки и верстки документов  6. Особенности разработки набора печатной продукции  7. Допечатная подготовка файлов  Названия лабораторных работ:  12. Панель инструментов; примитивы, простейшие операции с ними  13. Кривые безье  14. Кривые безье и инструмент форма  15. Узоры из примитивов и кривых безье  16. Работа с текстом (настройки, искривление и т.д.)  17. Работа со слоями  18. Направляющие, сетки, выделение по контуру  19. Заливки  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения 7D Виды учебной деятельности времени, 4. дисциплине Раздел 1. Проектирование и внедрение Лекции 6 дел. тр Ир AP РД2, РД4 Лабораторные занятия 6 информационных систем Самостоятельная работа 30 Лекции 8 Раздел 2. Конфиг ование д фигурир РД1 Лабораторные занятия 8 информационных систем Самостоятельная работа 40 Раздел 3. Интеграция информационных Лекции 8 дел &gt;. трац рмац РДЗ Лабораторные занятия 8 систем Самостоятельная работа 30 Содержание разделов дисциплины: Раздел 1. Проектирование и внедрение информационных систем  Виды обеспечения ИС. Этапы ЖЦ ИС. Организационно-регламентирующие и нормативно-правовые документы (отечественные и международные — стандарты, рекомендации, законы, акты и т.д.). Ключевые категории информационной безопасности. Методы и средства обеспечения информационной безопасности. Понятие требований. Дерево требований. Понятие ИТ-проекта. Участники. Риски. Календарно-сетевое планирование. Работа с системой управления проектами. План-паспорт проекта. Основные направления развития информационных систем и технологий.  Темы лекций:  1. Понятие информационной системы (ИС). Жизненный цикл ИС.  2. Документационное обеспечение вопросов проектирования и внедрения ИС  3. Основные понятия информационной безопасности.  Названия лабораторных работ:  1. Разработка требований к ИС. Планирование ИТ-проекта. Командная работа.  2. Групповая работа в системе управления проектами.  3. Разработка собственных отчетов в системе бизнес-моделирования Business Studio.  Раздел 2. Конфигурирование информационных систем  Понятие конфигурирования ИС. Объекты программной настройки. Модель данных ИС. Объектно-реляционная методология. Пользовательский интерфейс. Политика управления пользователями. Матрица пользовательских авторизаций. Понятие справочника. Разработка объектной модели ИС Business Studio, Directum, 1C, Адванта. Утилиты, редакторы, организационно-регламентирующие документы и другие средства для программной настройки ИС и ее адаптации к области внедрения. Перечень и последовательность мероприятий по программной настройке ИС.  Темы лекций:  4. Управление требованиями. Управление ИТ-проектами.  5. Объекты конфигурирования.  6. Средства конфигурирования.  7. Этапы конфигурирования.  Названия лабораторных работ:  4. Конфигурирование системы бизнес-моделирования Business Studio.  5. Конфигурирование СЭД DIRECTUM.  3  Раздел 3. Интеграция информационных систем Уровни интеграции ИС и БД. Конфликты обмена данными. Импорт/экспорт данных. Понятие пакета импорта/экспорта. Популярные форматы обмена данными. Технологии удаленного вызова процедур и их применение для интеграции ИС. Интеграция ИС Business Studio и Directum, Адванта и MS Excel. Понятие BI, OLAP, BigData.  Темы лекций:  8. Понятие интеграции ИС.  9. Технологии, методы и средства интеграции ИС.  10. Интеллектуальные технологии обработки данных.  11. Современные тенденции развития ИС.  Названия лабораторных работ:  6. Настройка пакетов импорта/экспорта данных в системе бизнес-моделирования Business Studio. 7. Интеграция информационных систем Business Studio и DIRECTUM.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности дн a дисциплине Раздел 1. Теоретические основы и Лекции 8 принципы построения интегрированных РД? Лабораторные занятия 8 корпоративных информационных систем Самостоятельная работа 25 Лекции 8 м Py Лабораторные занятия 8 Самостоятельная работа 25 Лекции 8 Раздел 3. Корпоративные базы данных РДЗ Лабораторные занятия 16 Самостоятельная работа 33  Содержание разделов дисциплины: Раздел 1. Теоретические основы и принципы построения интегрированных корпоративных информационных систем Тенденции развития современных ИТ. Базовые понятия КИС. Главная задача КИС. Классификация КИС. Эволюция КИС: объемно-календарное планирование, статистическое управление запасами, планирование потребности в материалах, планирование потребности в мощностях, планирование производственных ресурсов, системы планирование ресурсов и управления предприятием, управление внутренними ресурсами и внешними связями организации, управление эффективностью бизнеса. Концепция «точно вовремя». Теория ограничений. Темы лекций: 1. Тенденции развития современных IT. 2. Эволюция КИС. Названия лабораторных работ: 1. Создание проекта разработки в Microsoft Dynamics АХ. 2. Создание таблиц. 3. Разработка ЕВ-модели. Раздел 2. Стандартная система управления предприятием Стратегический бизнес-план. План продаж и операций. Основной производственный план. Планирование необходимых материалов и мощностей. Оперативное управление снабжением и производством. Управление финансами. Производство. Темы лекций: 3. Корпорации. Архитектура предприятия. 4. Стандартная система управления предприятием. 5. Состав КИС. Требования, предъявляемые к КИС. 6. Особенности выбора и внедрения КИС. Названия лабораторных работ: 4. Создание пользовательского интерфейса. 5. Безопасность. Создание ролей пользователя. 6. Введение в язык Х+-.  Раздел 3. Корпоративные базы данных  Основные понятия и определения. Организация данных в КИС. Требования, предъявляемые к корпоративным БД. Интеграционные решения корпоративных БД. Технологии доступа к данным в КИС. Хранилища данных. Архитектура хранилищ данных. Темы лекций: 7. Инфраструктура корпоративных информационных систем. 8. Интеграция данных в КИС. 9. Хранилища данных. 10. Безопасность КИС. Названия лабораторных работ: 7. Функциональные возможности языка Х-++. 8. Классы и объекты. 9. Доступ к базе данных. 10. Программная логика процедур обработки хранимой информации.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности Формируемый 06 Разделы дисциплины учения по Виды учебной деятельности промени, a дисциплине .. Лекции 4 Раздел 1. Введение в промышленный PAL. РАФ, к подход к разработке ПО РДЗ, РД4, Лабораторные занятия 2 РД Самостоятельная работа 10 Лекции 2 Раздел 2. Управление проектами по к РД? Лабораторные занятия 4 разработке ПО Самостоятельная работа 10 Лекции 4 Раздел 3. Фаза определения системы РДЗ Лабораторные занятия 4 Самостоятельная работа 12 Лекции 4 Раздел 4. Фаза реализации системы РД4 Лабораторные занятия 4 Самостоятельная работа 10 Лекции 4 Раздел 5. Передача системы РД4 Лабораторные занятия 4 Самостоятельная работа 10 Лекции 4 Раздел 6. Специфика разработки к РД Лабораторные занятия 4 информационных систем Самостоятельная работа 12 Лекции 4 Раздел 7. Общие понятия в области at проектирования ИС РД1 Лабораторные занятия 4 Самостоятельная работа 12 Лекции 2 Раздел 8. Серверные решения РД? Лабораторные занятия 4 Самостоятельная работа 12 Лекции 4 Раздел 9. Клиентские решения РД? Лабораторные занятия 4 Самостоятельная работа 20  Содержание разделов дисциплины:  Раздел 1. Введение в промышленный подход к разработке ПО  Цель и задачи дисциплины, ее роль и место в общей системе подготовки специалиста.  Основные положения: виды обеспечения вычислительной системы; понятия программы, программного комплекса, программной системы, программного обеспечения и программного продукта; определение и задачи программной инженерии.  Особенности промышленного ПО и кризис его разработки: понятие промышленного ПО, основные причины сложности разработки ПО.  Жизненный цикл программного продукта: понятие жизненного цикла, основные процессы жизненного цикла по стандарту ISO/IEC 15288; модели (парадигмы) жизненного цикла.  Методологии разработки ПО. Обзор методологий ЕСПД, MSF, RUP, Agile- методологии. Выбор и адаптация методологии разработки.  Темы лекций:  1. Введение в промышленный подход к разработке ПО  2. Введение в промышленный подход к разработке ПО  Названия лабораторных работ:  1. Инструменты и приемы технического документирования  Раздел 2. Управление проектами по разработке ПО  Основные положения: понятие проекта и управления проектом, цели и содержание проекта.  Введение в планирование: «железный треугольник», структура декомпозиции работ (WBS).  Управление конфигурацией: понятие конфигурации и управления конфигурацией, задачи управления конфигурацией; системы контроля версий; резервное копирование.  Оценка качества процесса разработки: обзор моделей качества; введение в CMMI- Dev.  Темы лекций:  3. Управление проектами по разработке ПО  Названия лабораторных работ:  2. Система управления версиями Git  Раздел 3. Фаза определения системы   Инженерия требований: задачи инженерии требований. Стандарт [ЗО IEC IEEE 29148. Стейкхолдеры.  Анализ потребностей, требования, разработка технического задания, управление изменениями.  Варианты использования (Use Cases): определение и роль в жизненном цикле.  Роль, цель и объекты проектирования. Архитектурное и детальное проектирование. Важность хорошей архитектуры.  Проектирование структуры: алгоритмическая и ОО-декомпозиции, нисходящее и восходящее проектирование. Модули. Многослойная архитектура приложений.  Критерии качества проектирования модулей и классов: зацепление и связность.  Представление проектных решений. UML, ERD, Screen flow.  Проектирование интерфейса пользователя: определение, классификации, основные требования и характеристики. Юзабилити, опыт пользователя. Стандарты и соглашения.  Темы лекций:  4. Фаза определения системы  5. Фаза определения системы  Названия лабораторных работ:  3. Варианты использования. Пользовательские истории  4. Диаграммы UML. Диаграмма вариантов использования  5. Техническое задание  4 Раздел 4. Фаза реализации системы  Методы повышения информативности программ: стили кодирования, системы именования и комментирования. Принципы оптимизации Kona. Безопасное программирование.  Менеджмент качества, обеспечения качества, верификация и валидация, тестирование. Цели, объекты и проблемы тестирования. Понятия тестов, тест-кейсов и тестовых планов.  Критерии качества тестирования: полнота покрытия поведения, операторов, маршрутов и параметров.  Виды тестирования: интеграционное и модульное тестирование; тестирование белого и черного ящика; альфа- и бета-тестирование, приёмочное, регрессионное, дымовое и нагрузочное тестирование и т.д.  Некоторые методы тестирования: инспекция кода, метод многократной разработки, методы эквивалентных разбиений и анализа граничных значений.  Организация тестирования. Средства автоматизации тестирования  Темы лекций:  6. Фаза реализации системы  7. Фаза реализации системы  Названия лабораторных работ:  6. Диаграммы UML. Диаграмма компонентов  7. Диаграмма последовательности  Раздел 5. Передача системы  Цели и задачи документирования. Стандарты.  Программная (системная) документация и пользовательская (эксплуатационная) документация. Принципы работы технического писателя.  Степени (этапы) готовности программных продуктов. Опытная и промышленная эксплуатация.  Общее и детальное планирования испытаний.  Задачи и проблемы внедрения.  Организация сопровождения и поддержки.  Темы лекций:  8. Передача системы  9. Передача системы  Названия лабораторных работ:  8. Эскизный проект. Технический проект  Раздел 6. Специфика разработки информационных систем  Основные группы понятий: система, модель и моделирование, проект и проектирование, данные, информация, информационная система. Задачи и области применение ИС. Уточнение понятий «база данных» и «система управления базами данных».  Модель ANSI/SPARC. Классификации ИС. Файл-серверная и клиент-серверная архитектуры. Многозвенные архитектуры. Микросервисная архитектура.  Темы лекций:  10. Специфика разработки информационных систем  11. Специфика разработки информационных систем  Названия лабораторных работ:  9. Инструменты проектирования БД  Раздел 7. Общие понятия в области проектирования HC  Общий порядок проектирования ИС. Моделирование бизнес-процессов. Выбор СУБД. Валидация требований по документам. САЗЕ-средства, модели и нотации.  Строгое определение понятия «модель данных». Обзор моделей данных. Компоненты реляционной модели данных.  Темы лекций:  12. Общие понятия в области проектирования ИС  13. Общие понятия в области проектирования ИС  Названия лабораторных работ:  10. Проектирование БД. Концептуальная модель  Раздел 8. Серверные решения  Хранимые процедуры. Пользовательские функции. Триггеры. Представления.  Понятия высокой доступности и высокой надёжности.  Индексы: В-деревья, кластерные и некластерные индексы. Обзор тематики оптимизации баз данных.  Резервное копирование и восстановление. Репликация. Зеркалирование. Кластеры.  Транзакции. Свойства ACID. Журнал транзакций. Проблема параллельной обработки. Уровни изоляции. Блокировки и версионирование. Тупики. Длинные и короткие транзакции. Распределенные транзакции.  Темы лекций:  14. Серверные решения  15. Серверные решения  Названия лабораторных работ:  11. Проектирование БД. Физическая модель  Особенности проектирования пользовательского интерфейса информационных систем.  ОКМ. Настольные, веб- и мобильные приложения.  Технологии построения отчетов: встроенные инструменты, компоненты, технологии шаблонов; промышленные средства.  Темы лекций:  16. Клиентские решения  17. Клиентские решения  Названия лабораторных работ:  12. Инструменты проектирования интерфейса пользователя  13. Проектирование интерфейса пользователя  14. Разработка клиент-серверной системы на основе ORM  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности Ан a дисциплине  Раздел 1. Анализ бизнес-процессов Лекции 4 предприятия. Интервалы и гипотезы. РД1, РДЗ Лабораторные занятия 4 Оценка данных предприятия. Самостоятельная работа 25 Раздел 2. Повышение эффективности Лекции 6 деятельности предприятия. АБ- РД Лабораторные занятия 6 тестирование. Дизайн эксперимента. Экспертные методы принятия решений. Самостоятельная работа 25 Раздел 3. Статистические методы, Лекции 6 применяемые для анализа данных Лабораторные занятия 6 предприятия. Параметрические и РД1, РД4 непараметрические критерии. Корреляция Самостоятельная работа 25 и регрессия.  Лекции 6 Раздел 4. Построение выводов по данным PI, Pa Лабораторные занятия 6 с использованием машинного обучения.  Самостоятельная работа 25  Содержание разделов дисциплины:  Раздел 1. Анализ бизнес-процессов предприятия. Интервалы и гипотезы. Оценка данных предприятия.  В разделе рассматриваются виды деятельности в рамках предприятия, требующие проведения аналитики и обработки данных предприятия.  Особое внимание уделяется вопросу оценки параметров деятельности предприятия, показателей качества, показателей эффективности бизнес-процессов при помощи интервальной оценки на основе квантилей, построению доверительных интервалов, оценки плотности распределения параметров производным от нормального, доверительный интервал для показателей представляющих доли (доля кликов по баннеру, например, доля успешных сделок и пр.), доверительные интервалы для бутстрепа, методика проверки гипотез, формулирование гипотез.  Знания и навыки, полученные при изучении материалов раздела, позволят выполнять работы на предпроектном этапе и этапе диагностики деятельности предприятия в ходе выполнения ИТ-проекта.  Темы лекций:  1. Анализ данных предприятия, виды работ, требующих анализ в рамках предприятия.  2. Проблемы построения выводов по данным. Интервальные и доверительные оценки. Проверка гипотез. Критерии согласия.  Названия лабораторных работ:  1. Оценка данных предприятия. Построение доверительных интервалов. Использование критериев согласия.  2. Описание бизнес-процессов предприятия и измерение показателей.  Раздел 2. Повышение эффективности деятельности предприятия. АБ-  тестирование. Дизайн эксперимента. Экспертные методы принятия решений.  В разделе описываются основные подходы, позволяющие выявить какие причины влияют на качество продукта, подходы к повышению качества продукта. Это данные помогают на этапе анализа деятельности выбрать наиболее эффективный вариант ее автоматизации. Эффективность того или иного решения перед внедрением его в рамках предприятия позволяет проверить АБ-тестирование, а также оценить при помощи экспертов.  Знания и навыки, полученные в данном модуле, позволяют при анализе выявить причины неэффективного выполнения процессов (деятельности) и разработать усовершенствованную модель анализируемой системы. На практике отрабатывается применение распространенных методов проведения экспертизы и выбора наиболее эффективной альтернативы автоматизации некоторой деятельности предприятия.  Темы лекций:  3. АБ-тестирование.  4. Методы экспертных оценок.  5. Метод анализа иерархий, метод Дельфи.  Названия лабораторных работ:  3. АБ-тестирование.  4. Использование параметрических и непараметрических критериев в ходе АБ- тестирования.  5. Проведение экспертизы 2 методами (анализа иерархий и Дельфи).  Раздел 3. Статистические методы, применяемые для анализа данных предприятия. Параметрические и непараметрические критерии. Корреляция и  егрессия.  В данном разделе рассматриваются статистические методы применяемые в ходе анализа данных предприятиях. К таким методам относится точёное и интервальное оценивание, корреляционный анализ, в том числе корреляция Пирсона, ранговые методы корреляции Спирмана, Кендала. Рассматривается метод максимального правдоподобия.  Темы лекций:  6. Случайные величины, математическое ожидание, дисперсия, точечное и интервальное оценивание. Оценка плотности распределения.  7. Критерии Пирсона, Колмогорова-Смирнова. Метод максимального правдоподобия. Множественные гипотезы поправка Бонферонни.  8. Корреляционный и регрессионный анализ.  Названия лабораторных работ:  6. Корреляционный анализ.  7. Регрессионный анализ.  8. _Множественная проверка гипотез.  Раздел 4. Построение выводов по данным с использованием машинного обучения.  Введение в машинное обучение. Объекты, признаки объектов. Классификация данных. Линейные методы классификации: логические методы классификации, метод опорных векторов, логистическая регрессия. Качество классификации. Понижение размерности, метод главных компонент. Нейронные сети. Задача классификации и регрессии при помощи нейронных сетей. Кластерный анализ. Оценка качества модели, полученной в ходе машинного обучения.  Темы лекций:  9. Машинное обучение. Классификация. Качества.  10. Нейронные сети, задача регрессии и классификации. Качество моделей.  Названия лабораторных работ:  9. Задача классификации.  10. Понижение размерности.  11. Нейронные сети в задаче регрессии.  4  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения 7 Виды учебной деятельности времени, 4. дисциплине Лекции 22 Раздел 1. Особенности проектирования и д пр Ир РД, РД? Лабораторные занятия 22 разработки информационных систем Самостоятельная работа 100 Содержание разделов дисциплины: Раздел 1. Особенности проектирования и разработки информационных систем  Основные группы понятий: данные, информация, информационная система. Задачи и области применение ИС. Уточнение понятий «база данных» и «система управления базами данных». Классификации ИС. Файл-серверная и клиент-серверная архитектуры. Многозвенные архитектуры. Микросервисная архитектура. Модель ANSI/SPARC.  Темы лекций:  1. Общий порядок проектирования ИС. Анализ предметной области. Проектирование ИС. Выбор архитектуры. Обзор моделей данных.  2. Выбор СУБД. SQL- и №оЗОГ-системы.  3. Программная реализация ИС. Внедрение, развёртывание.  4. Реляционная модель данных. Целостность и достоверность БД. Естественные и суррогатные ключи. Поддержка ссылочной целостности. Аспект манипулирования. Важность алгебры. Достоинства и недостатки SQL.  5. Хранимые процедуры. Пользовательские функции. Триггеры. Представления. Понятия высокой доступности и высокой надёжности. Индексы.  6. Транзакции. Свойства ACID. Журнал транзакций. Проблема параллельной обработки. Уровни изоляции. Блокировки и версионирование. Тупики. Длинные и короткие транзакции. Распределенные транзакции.  7. Технологии построения отчетов: встроенные инструменты, компоненты, технологии шаблонов; промышленные средства.  8. Особенности проектирования пользовательского интерфейса информационных систем.  9. ORM. Настольные, веб- и мобильные приложения.  Названия лабораторных работ:  Проектирование БД  Проектирование БД. Логическая модель Проектирование БД. Физическая модель  Инструменты проектирования интерфейса пользователя Проектирование интерфейса пользователя  Разработка клиент-серверной системы на основе ORM  язь  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности Ан a  дисциплине РД. РД Лекции 12 Раздел 1. Современные \Web-технологии PIG ? Лабораторные занятия 20 Самостоятельная работа 58 Лекции 12 Раздел 2. Язык JavaScript аа Лабораторные занятия 20 Самостоятельная работа 58  Содержание разделов дисциплины: Раздел 1. Современные Web-mexnonoeuu Раздел формирует базовые представления о функционировании WWW, о методах загрузки и обработки страниц браузерами, об устройстве Web-приложений. Темы лекций: 1. Принципы проектирования и реализации Web-приложений. 2. Обзор основных клиентских и серверных технологий. 3. Динамический HTML. 4. Способы обработки данных в локальных хранилищах. Названия лабораторных работ: 1. Структура HTML-кода. 2. Использование AJAX в \е-приложениях. Раздел 2. Язык JavaScript Раздел формирует начальные навыки использования языка программирования JavaScript в контексте HTMLS для применения в Web-приложениях.  Темы лекций:  5. Введение в JavaScript.  6. Функциональное программирование в JavaScript.  7. Объектно-ориентированное программирование в JavaScript.  8. Встроенные объекты JavaScript.  Названия лабораторных работ:  3. Функции в JavaScript.  4. Объекты в JavaScript.  5. Обработка событий в JavaScript.  6. Работа с формами в JavaScript.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения 7 Виды учебной деятельности времени, 4. дисциплине .. Лекции 4 часа Раздел 1. Искусственный интеллект. РД5 Лабораторные занятия 6 часов Введение. Самостоятельная работа 25 часов ‚ Лекции 4 часа Раздел 2. Нейронные сети. Принцип к РДЗ Лабораторные занятия 6 часов работы, алгоритмы обучения Самостоятельная работа 25 часов Лекции 8 часов Раздел 3. Сверточные нейронные сети РД1 Лабораторные занятия 12 часов Самостоятельная работа 25 часов Лекции 4 часа Раздел 4. Нейронные сети-трансформеры. д Ир трансформер РД2 Лабораторные занятия 6 часов Генеративно-состязательные сети. Самостоятельная работа 25 часов Лекции 4 часа Раздел 5. Нейросетевые автоэнкодеры РД4 Лабораторные занятия 6 часов Самостоятельная работа 24 часа Содержание разделов дисциплины: Раздел 1. Искусственный интеллект. Введение.  Определение понятий искусственный интеллект и машинное обучение. История развития искусственного интеллекта. Современные методы, основные тренды и перспективы развития искусственного интеллекта.  Темы лекций:  1. Искусственный интеллект. Введение.  Названия лабораторных работ:  1. Разработка нейронной сети "Однослойный Перцептрон" для классификации числовых последовательностей  Раздел 2. Нейронные сети. Принцип работы, алгоритмы обучения  Введение в искусственные нейронные сети, виды нейронных сетей, области применения, принцип работы. Алгоритмы обучения нейронных сетей, метод обратного распространения ошибки.  Темы лекций:  2. Принцип работы нейронных сетей  3. Алгоритмы обучения нейронных сетей  Названия лабораторных работ:  2. Разработка нейронной сети "Многослойный Перцептрон" с использованием библиотеки Кегаз для распознавания образов на изображениях  Раздел 3. Сверточные нейронные сети  Принцип работы сверточных нейронных сетей, операция свертки, операции MaxPooling, Padding, DropOut, Batch normalization. Различные архитектуры нейронных сетей. Оптимизаторы обучения нейронных сетей: Adam, AdaMax, AdaGrad и т.д.  Темы лекций:  4. Сверточные нейронные сети. Различные архитектуры  5. Обучение сверточных нейронных сетей. Оптимизаторы обучения.  Названия лабораторных работ:  3. Разработка сверточной нейронной сети для сегментации медицинских изображений  Раздел 4. Нейронные сети-трансформеры. Генеративно-состязательные сети.  Принцип работы нейронных сетей-трансформеров. Методы их обучения. Области применения. Принцип работы генеративно-состязательных сетей. Методы их обучения. Области применения.  Темы лекций:  6. Нейронные сети-трансформеры. Генеративно-состязательные сети.  Названия лабораторных работ:  4. Разработка нейронной сети ResNet для классификации объектов на изображениях  Раздел 5. Нейросетевые автоэнкодеры  Принцип работы нейронных сетей автоэнкодеров. Виды автоэнкодеров. Обучение. Применение нейросетевых автоэнкодеров для сегментации изображений.  Темы лекций:  7. Нейросетевые автоэнкодеры  Названия лабораторных работ:  5. Разработка нейронной сети U-Net для сегментации спутниковых снимков  5.</t>
+  </si>
+  <si>
+    <t>(модуля)  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине  Раздел 1. Введение в РД1 Лекции 4 интеллектуальные РД2 Лабораторные занятия 4 системы Самостоятельная работа 24 Раздел 2. Модели РД1 Лекции 4 представления знаний РД2 Лабораторные занятия 4  Самостоятельная работа 24 Раздел 3. Архитектура и РДЗ Лекции 4 технология разработки РД4 Лабораторные занятия 4 экспертных систем Самостоятельная работа 24 Раздел 4. Применение РДЗ Лекции 4 нечеткой логики в РД4 Лабораторные занятия 4 экспертных системах Самостоятельная работа 24 Раздел 5. Генетический РД4 Лекции 4 алгоритм РД5 Лабораторные занятия 4  Самостоятельная работа 24 Раздел 6. РД5 Лекции 4 Искусственные Лабораторные занятия 4 нейронные сети Самостоятельная работа 24  Раздел 1. Введение в интеллектуальные системы  Представление знаний в информационных системах как элемент искусственного интеллекта и новых информационных технологий. Этапы создания искусственного интеллекта. Основные понятия и классификация систем, основанных на знаниях. Принципы приобретения знаний.  Лабораторная работа No]  Разработка экспертной системы на основе продукционных правил.  Раздел 2. Модели представления знаний  Логическая модель представления знаний и правила вывода. Продукционная модель представления знаний и правила их обработки. Выводы, основанные на продукционных правилах. Теория фреймов и фреймовых систем. Объекты с фреймами. Основные атрибуты (слоты) объекта. Процедурные фреймы и слоты. Представление знаний в виде семантической сети. Модель доски объявлений. Модель представления знаний в виде сценария.  Лабораторная работа №2  Разработка экспертной системы на основе применения фреймовой модели представления знаний.  Раздел 3. Архитектура и технология разработки экспертных систем  Введение в экспертные системы. Роли эксперта, инженера знаний и пользователя. Общее описание архитектуры экспертных систем. База знаний, правила, машина вывода, интерфейс пользователя, средства работы с файлами. Технология разработки экспертных систем. Логическое программирование и экспертные системы. Языки искусственного интеллекта. Подсистема анализа и синтеза входных и выходных сообщений. Диалоговая подсистема. Объяснительные способности экспертных систем.  Лабораторная работа №3  Разработка экспертной системы на основе применения модели представления знаний в виде семантической сети.  Раздел 4. Применение нечеткой логики в экспертных системах  Понятие о нечетких множествах и их связь с теорией построения экспертных систем. Коэффициенты уверенности. Взвешивание свидетельств. Отношение правдоподобия гипотез. Функция принадлежности элемента подмножеству. Операции над нечеткими множествами. Дефаззификация нечеткого множества. Нечеткие правила вывода в экспертных системах.  Лабораторная работа №34  Разработка экспертной системы на основе применения нечетких правил вывода.  Раздел 5. Генетический алгоритм  Понятие о генетическом алгоритме. Этапы работы генетического алгоритма. Кодирование информации и формирование популяции. Оценивание популяции. Селекция. Скрещивание и формирование нового поколения. Мутация. Настройка параметров генетического алгоритма. Канонический генетический алгоритм. Пример работы генетического алгоритма. Рекомендации к программной реализации генетического алгоритма. Применение генетического алгоритма для решения задач оптимизации и аппроксимации.  Лабораторная работа №5  Принятие решений на основе применения генетического алгоритма.  Раздел 6. Искусственные нейронные сети  Понятие о нейросетевых системах. Биологические нейронные сети. Формальный нейрон. Искусственные нейронные сети. Обучение нейронной сети. Правило Хебба. Персептрон Розенблатта. Многослойный персептрон. Алгоритм обратного распространения ошибки. Пример работы и обучения нейронной сети. Программная реализация. Нейронные сети на основе радиально-базисных функций. Машина опорных векторов. Сверточные нейронные сети. Нейроэволюционные алгоритмы. Применение нейронных сетей для решения задач аппроксимации, классификации, автоматического управления, распознавания и прогнозирования.  Лабораторная работа №6  Применение искусственных нейронных сетей для обработки информации.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  ИУК (У) - 5.5 И.УК (У)- 5.6  ставлены в  Разделы дисциплины  Формируемы й результат обучения по дисциплине  Виды учебной деятельности Объем  времени, ч.  Раздел 1. Философия и наука: формы и перспективы взаимодействия  Pal  Лекции  Практические занятия Самостоятельная работа  Раздел 2. Становление теоретических конструкций мира  РД1 РД2 РДЗ  Лекции Практические занятия  Самостоятельная работа  Раздел 3. Проблема бытия в философии  РД1  Лекции  Практические занятия  Самостоятельная работа  В RIN IAN] NY  Раздел 4. Лекции 2 Философское учение о ценностях. Практические занятия 2 Философская антропология Самостоятельная работа 6 Раздел 5. Лекции 0 Гносеологические ориентиры в Практические занятия 0 мире постправды Самостоятельная работа 6 Раздел 6. Лекции 0 Я и социальная реальность ХХ Практические занятия  2 века Самостоятельная работа 6 Раздел 7. Лекции 0 Философские проблемы науки и Практические занятия 2  техники Самостоятельная работа  Раздел 8. Лекции 0 Перспективы современного Практические занятия 2 общества Самостоятельная работа 6  Содержание разделов дисциплины:   Раздел 1. Философия и наука: формы и перспективы взаимодействия  Исторические формы мировоззрения: мифологическое, религиозное, философское, научное. Структура мировоззрения. Специфика мировоззрения в ХХ веке  Тема лекции:  1. Специфика философского подхода к пониманию мира.  Тема практического занятия:  1. Смысл и предназначение философии  Раздел 2. Становление теоретических конструкций мира  Специфика мировоззрения в различных культурах (европейской, восточной, российской). Специфические характеристики мировоззренческих и этических проблем различных эпох и различных культур. Формирование основ научного мировоззрения в контексте развития философии эпохи Античности  Тема лекции:  1. Становление теоретических конструкций мира в Европе.  Тема практического занятия:  1. Становление теоретических конструкций мира в России и на Востоке.  Раздел 3. Проблема бытия в философии  Основные принципы формирования научной картины мира. Механистическая, электромагнитная, квантово-релятивистская, синергетическая картины мира. Сложность современной научной картины мира  Tema лекции:  1. Онтологические основания картины мира  Tema практического занятия:  1. Становление теоретических конструкций мира в России и на Востоке   Раздел 4. Философское учение о ценностях. Философская антропология  4 Моральная дилемма как предмет философской этики. Философские подходы к решению моральных дилемм: этика добродетели (Аристотель), этика долга (И.Кант), этика ценностей (прагматизм, утилитаризм), золотое правило нравственности (Конфуций).  Tema лекции:  1.Моральные дилеммы: теория и практика  Tema практического занятия: 1. Этический идеал: принципы и основания  Раздел 5. Гносеологические ориентиры в мире постправды  «Трудная» и «легкая» проблемы сознания в интерпретации Д. Чалмерса. Философский (мысленный) эксперимент. Сознание и физические процессы в мозгу человека. Проблема исследования сознания и проблема исследования объективного мира  Тема практического занятия:  1.Учение о познании и сознании. Гносеологические ориентиры в мире постправды  Раздел 6. Я и социальная реальность ХХ века  Особенности развития современной культуры. Виртуальность как новое измерение культуры. Человек в системе социальных связей. Формирование новых типов социальных связей, новых типов социальных ролей в обществе ХХ] века. Гражданское общество и государство.  Тема практического занятия:  1. Модерн, постмодерн, неопостмодерн - и это все про современность...  Раздел 7. Философские проблемы науки и техники  Отношение «человек-техника», «человек-техника-человек», «техника-человек- техника», «техника-техника» в современном мире: техника, технофобия, техницизм, техносфера, технический прогресс. Антропологические проблемы в период четвертой научно-технической революции  Тема практического занятия: 1. Эпоха 4 научно-технической революции — мир бесконечных перемен.  Раздел 8. Перспективы современного общества  Стратегия устойчивого развития как инструмент регулирования деятельности человека в условиях турбулентности. Трансформация социальных, экономических, политических, культурных, мировоззренческих аспектов реальности в перспективе общественного развития.  Тема практического занятия:  1. Будущее человечества и сценарии будущего.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения м Виды учебной деятельности времени, 4. дисциплине Раздел 1. Конс ование программного Лекции 12 дел. труир прогр РД, РД? Лабораторные занятия 20 обеспечения Самостоятельная работа 40 Лекции 12 Раздел 2. Реализация программного A ция прогр РДЗ Лабораторные занятия 20 обеспечения Самостоятельная работа 40 Содержание разделов дисциплины: Раздел 1. Конструирование программного обеспечения  Раздел формирует навыки построения информационных технологий и систем, достаточные для решения научных и профессиональных задач производства. Рассматриваются современные проблемы и методы прикладной информатики и научно- технического развития информационно-коммуникационных технологий.  Темы лекций:  1. Подготовка к конструированию ПО. Формирование и анализ требований.  2. Качество программного обеспечения.  3. Конструирование программного обеспечения.  4. Правила поставки приложений.  Названия лабораторных работ:  1. Основы алгоритмизации.  2. Линейные алгоритмы. Условные операторы. Циклы.  3. Массивы одномерные и многомерные. Строки.  Раздел 2. Реализация программного обеспечения  Раздел формирует навыки организации работы по моделированию прикладных ИС и реинжинирингу прикладных и информационных процессов предприятия и организации. Рассматриваются вопросы управления проектами по информатизации прикладных задач и созданию ИС предприятий и организаций.  Темы лекций:  5. ООП. Классы  6. Делегаты  7. Документирование кода  Названия лабораторных работ:  4. Проектирование и реализация классов.  5. Наследование. Полиморфизм. Конструкторы.  6. Построение диаграммы классов.  7. Неформальный технический обзор кода.  Тематика курсовых работ (проектов):  1. Проектирование и построение диаграммы классов предметной области «Деканат».  2. Проектирование и построение диаграммы классов предметной области «Автомойка».  3 3. магазин».  4.  5.  Проектирование и построение диаграммы классов предметной области «Интернет-  Проектирование и построение диаграммы классов предметной области «Банк». Проектирование и построение диаграммы классов предметной области «Библиотека».  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения 7 Виды учебной деятельности времени, 4. дисциплине  Лекции 8  Раздел 1. Классификация и основные ss РД-1 Лабораторные занятия 6  понятия операционных систем  Самостоятельная работа 26  Лекции 4 Раздел 2. Процессы и ресурсы ОС РД-2 Лабораторные занятия 6  Самостоятельная работа 20 Раздел 3. Методы и средства Лекции 4 взаимодействия ОС с внешними РД-3 Лабораторные занятия 4 устройствами Самостоятельная работа 20 Раздел 4. Средства организации и Лекции 8 управления параллельными процессами в РД-4 Лабораторные занятия 8 ОС Самостоятельная работа 30  Содержание разделов дисциплины:  Раздел 1. Классификация и основные понятия операционных систем  Основные понятия ОС, основные определения, свойства процесса. Классификация ОС. Клиент/серверные вычисления. Трехуровневая архитектура. Точки зрения пользователя на ОС. Аппаратная архитектура и поддержка ОС. Ядро и процессы. Состояния процесса. Архитектурные концепции операционных систем. Иерархия абстрактных машин. Свойства уровней абстракции. Две концепции виртуальной машины. Концепция микроядра. Объектно- ориентированный подход к проектированию ОС. Организация взаимодействия между модулями. Планирование, как система массового обслуживания. Количественные показатели для оценки эффективности выполнения процессов. Требования к дисциплине планирования. Дисциплины планирования (все о них), характеристики и классификация. Среднесрочное планирование. Долгосрочное планирование  Темы лекций:  1. Введение в ОС. Основные понятия  2. Планирование процессов  3. Управление памятью  Названия лабораторных работ:  1. Автоматизация выполняемых операций с помощью пакетных файлов MS-DOS  2. Взаимодействие с приложениями и службами Windows на VBScript  Раздел 2. Процессы и ресурсы ОС  Порождение программ и процессов. Компиляция. Стадии оптимизации программ. Компоновка и загрузка. Методы связывания. Установка межмодульных связей. Системные вызовы для модульного формирования программ. Цикл жизни процесса. Интерпретации идентификатора процесса. Системные вызовы при работе с процессами. Отличия сегментов контекста процесса. Нити. Собственные ресурсы нити. Системные вызовы для управления нитями. Свойства ресурсов и их представление. Системные вызовы для работы с ресурсами. Состав дескриптора класса ресурса. Отличие манипулятора от дескриптора. Задача обедающих философов. Отличие тупика от бесконечного откладывания. Тупики: предупреждение, обнаружение, развязка. Стратегии предотвращения тупиков. Алгоритм банкира — общие положения. Свойства безопасной ситуации. Алгоритмическая реализация проверки ситуации на безопасность. Алгоритм банкира для одного вида ресурсов. Алгоритм банкира для нескольких видов ресурсов. Назначение матриц С и К, а также векторов Е, P, А. Метод Габермана (графический). Алгоритм Габермана (програмно реализуемый).  Темы лекций:  4. Порождение программ и процессов  3  5. Монопольно используемые ресурсы Названия лабораторных работ: 3. Командный интерфейс и макроязык SHELL ОС FreeBSD 4. _Ошх-процессы на примере ОС Astra Linux Раздел 3. Методы и средства взаимодействия ОС с внешними устройствами Виртуализация устройств и структура драйвера. Метода конструирования виртуальных устройств. Интерфейсы устройств. Способы подключения устройств к ЭВМ. Управление устройствами. Основные уровни драйверов. Дескриптор, таблицы дескрипторов, манипулятор. Примеры драйверов устройств (драйвер системах часов, драйвер клавиатуры, драйверы дисковых запоминающих устройств). Стратегии обслуживания дисковых устройств. Потоки и многоуровневые драйверы. Интерфейс процесса. Буферизация. Иерархическая модель файловой системы. Логическая организация файлов. Интерфейсы. Фундаментальные способы организации файлов. Логическая файловая система. Каталоги. Алиасы и косвенные файлы. Управление доступом. Логическая файловая система. Системные вызовы. Базовая файловая система. Дескриптор файла, расширенный дескриптор файла. Физическая структура файлов. Положения являющиеся общими для любых способов управления дисковой памятью. Смежное и несмежное распределение файлов. Три основных подхода к представлению плана файла. Целостность данных файловой системы. RAID- технология. Загружаемая файловая система. Темы лекций: 6. Управление вводом-выводом 7. Файловые системы Названия лабораторных работ: 5. _ Организация взаимодействия процессов с помощью каналов Критические секции. Задача синхронизации. Общая переменная исключения. Переменная-переключатель. Неальтернативные переключатели (3 решения) Алгоритм Деккера для 2-х процессов. Алгоритм Деккера для М-процессов. Алгоритм Питерсона. Атомарность обращений к памяти. Вариации команд testAndSet. Защита критической секции. Семафоры. Программная реализация семафора. Операции над семафорами. Семафоры множественных ресурсов. Задача «Производители-потребители». Критические секции в языках программирования. Мониторы. Реализация монитора. Расширенная модель монитора. Задача «читатели-писатели». Групповой монитор. Примитивы синхронизации. Секвенсор. Модель рандеву. Асинхронная модель рандеву. Применение скобок. Критических секций. Виртуальные прерывания. Модель виртуальных коммуникационных портов. Именование портов. Общие поля памяти. Выполнение операций над семафорами. Программные каналы. Использование каналов. Очереди сообщений. Правила работы очереди сообщений. Целостность информации. Контроль доступа. Объектно-ориентированная модель доступа и механизмы защиты. Кодирование объектов. Инкапсуляция объектов. Защита объектов. Аутентификация и авторизация. Представление прав доступа. Виды доменов. Процедура авторизации. Темы лекций: 8. Параллельное выполнение процессов 9. Системные средства взаимодействия процессов 10. Защита ресурсов Названия лабораторных работ: 6. Разделяемая память 7. Семафоры  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности Формируемый результат м Объем Разделы дисциплины обучения TD Виды учебной деятельности времени, 4. дисциплине Лекции 4 Раздел 1. Основы информационных систем РД-5 Лабораторные занятия 4 Самостоятельная работа 24 Лекции 6 Раздел 2. Классификация архитект д фикация ар УР РД-1, РД-5 Лабораторные занятия 6 информационных систем Самостоятельная работа 24 Лекции 4 Раздел 3. Распределенные д пред РД-4 Лабораторные занятия 10 информационные системы Самостоятельная работа 24 Раздел 4. Сервис-ориентированная Лекции 6 д “ep р ир РД-2, РД-4 Лабораторные занятия 10 архитектура Самостоятельная работа 24 Раздел 5. Функциональные уровни Лекции 6 дело. кии УР РД-5 Лабораторные занятия 8 информационной системы Самостоятельная работа 24 Раздел 6. Интеграция информационных Лекции 6 дело. тран рмац РД-3 Лабораторные занятия 10 систем Самостоятельная работа 24  Содержание разделов дисциплины:  Раздел 1. Основы информационных систем  Общие понятия информационных систем как класса программно-аппаратного обеспечения. Аппаратные средства создания и поддержки современных информационных  сетей. Темы лекций:  1. Основы информационных систем Названия лабораторных работ:  1. Работа с файлами  Раздел 2. Классификация архитектур информационных систем Централизованная архитектура, архитектура  «файл-сервер», — многозвенная архитектура «клиент-сервер», распределенные архитектура, сервис-ориентированная архитектура. Цели, задачи и функции двух- и трехзвенных информационных систем. Распределение задач системы по звеньям. «Толстый» и «тонкий» клиенты. Сервера приложений. Темы лекций: 2. Классификация архитектур информационных систем Названия лабораторных работ: 2. Клиент-серверверные приложения Раздел 3. Распределенные информационные системы Цели, задачи и функции распределенных информационных систем. Структура распределённых информационных систем. Особенности \/ЕВ-приложений, необходимые компоненты У\ЕВ-ориентированных информационных систем. Темы лекций: 3. Распределенные информационные системы Названия лабораторных работ: 3. Использование ОКМ 4. SOAP сервисы Раздел 4. Функциональные уровни информационной системы Декомпозиция информационных систем на слои и уровни. Выделение подсистем в архитектуре. Темы лекций: 4. Функциональные уровни информационной системы Названия лабораторных работ: 5. Парсинг сайтов 6. Введение в Windows СОМ Эволюция распределенных систем в сервис-ориентированные системы, облачные информационные системы и сервисы. Темы лекций: 5. Сервис-ориентированная архитектура Названия лабораторных работ: 7. REST сервисы 8. Windows Communication Foundation Раздел 6. Интеграция информационных систем Архитектурные и проектные решения для интеграции различных информационных систем между собой. Интерфейсы и протоколы обмена данными. Архитектуры масштабируемых информационных систем. Параллельные информационные системы. Темы лекций: 6. Интеграция информационных систем Названия лабораторных работ: 9. Управление данными в Excel на основе Windows СОМ 10. Управление данными в Word на основе Windows СОМ 11. Автоматизация построения отчетов на основе шаблонов в среде Word Тематика курсовых работ (проектов): Информационная система интернет магазина электроники Информационная система СПА-салонов Информационная система социальной сети пользователей Информационная система маршрутного транспорта города Информационная система образовательного учреждения  иже  4 6. Информационная система спортивного заведения  7. Информационная система доставки продуктов питания  8. Информационная система учета товаров продуктового магазина 9. Информационная система сотрудников предприятия  10. Информационная система компаний доставки воды  11. Информационная система сайтов знакомств  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности ИН a. дисциплине  Раздел 1. Информационные ресурсы и РД-1.РД-5 Лабораторные занятия 10 понятие информационной технологии ° Самостоятельная работа 16 Раздел 2. Информационные системы и РД-3, РД-4,  Лекции 6 базы данных РД-5 Самостоятельная работа 16 Раздел 3. Системы счисления РД-4 Лекции 6  Самостоятельная работа 16 Раздел 4. Алгоритмы и технология их Лекции 4 разработки, основы программирования и РД-2, РД-4 Лабораторные занятия 14 обработки данных Самостоятельная работа 16 Раздел 5. Формы представления и РД-4. РД-5 Лекции 4 преобразования информации ? Самостоятельная работа 16 Раздел 6. Надежность хранения и РД-4. РД-5 Лекции 4 передачи информации ° Самостоятельная работа 16  Содержание разделов дисциплины:  Раздел 1. Информационные ресурсы и понятие информационной технологии  Данные, формирование информации, информационные ресурсы. Виды информационных процессов. Понятие, этапы развития, классификация информационных систем. Информационные технологии: понятие, цель, инструментарий. Соотношение информационной системы и технологии. Геоинформационные системы и технологии. Информационная культура. Информационное моделирование и — формализация. Информационные процессы и информационные системы. Информационные процессы и информационные системы. Информационная технология как система. Информационное управление Темы лекций:  1. Информация, информационные ресурсы, технологии, процессы и системы 2. Информационное моделирование и формализация  Названия лабораторных работ:  1. Основные возможности текстового редактора "MS Word"  Раздел 2. Информационные системы и базы данных  Информационные системы. Базы данных и системы управления базами данных. Стадии разработки программного обеспечения и программной документации. Стандарты разработки. Трудоемкость разработки программного обеспечения.  Темы лекций:  3. Информационные системы  4. Базы данных и системы управления базами данных  5. Стадии разработки ПО и ПД. Стандарты разработки  Раздел 3. Системы счисления Определения, понятия. Перевод чисел между различными СС. Арифметические операции в позиционных системах счисления. Системы счисления и архитектура компьютеров. Темы лекций: 6. Работа с числами в различных системах счисления, перевод чисел между различными системами счисления. Раздел 4. Алгоритмы и технология их разработки, основы программирования и обработки данных Основные понятия теории алгоритмов. Характеристики алгоритмов. Формы представления алгоритмов: словесная, графическая, в псевдокоде. Базовые алгоритмические структуры. Понятие массива, типовые алгоритмы обработки одномерных массивов. Алгоритм суммы бесконечного ряда. Алгоритм табулирования функций. Алгоритмы обработки многомерных массивов. Алгоритмы сортировки. Алгоритм поиска с возвратом. Этапы решения задач с помощью компьютера. Понятие математической модели. Основные этапы разработки программ. Программирование сверху вниз и снизу вверх. Отладка и тестирование программ Темы лекций: 7. Алгоритмизация. Схемы алгоритмов 8. Массивы и списки 9. Простейшие алгоритмы Названия лабораторных работ: 2. Циклические алгоритмы. Итерационные ряды 3. Преобразование одномерных массивов 4. Преобразование многомерных массивов 5. Обработка неупорядоченных данных 6. Использование функций Понятие информации и ее свойства. Измерение информации. Определение и виды систем счисления. Перевод чисел из одной системы счисления в другую. Представление целых чисел со знаком и без знака. Прямой, обратный, дополнительный, модифицированный код числа. Представление чисел в формате с фиксированной запятой. Представление чисел в формате с плавающей запятой. Выполнение арифметических операций с числами с фиксированной и плавающей запятой. Представление символьной, графической и аудио информации. Сжатие данных. Темы лекций: 10. Единицы измерения информации 11. Представление целых чисел 12. Кодирование символьной информации 13. Представление чисел в формате с плавающей запятой. Неочевидные особенности вещественных чисел 14. Кодирование графической информации 15. Кодирование аудио Раздел 6. Надежность хранения и передачи информации Контрольная сумма. Корректирующие и обнаруживающие коды. Хеширование. Коллизии. Целостность передачи информации. Надежность хранения информации. RAID- массивы. Резервное копирование. Полная, добавочная и разностная копии. Шифрование данных. Симметричные и асимметричные алгоритмы шифрования. Криптографическая стойкость. Темы лекций: 16. Сжатие данных 17. Целостность передачи информации 4  18. Надежность хранения информации 5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения о Виды учебной деятельности времени, 4. дисциплине Лекции 4 Раздел 1. Основы теории графов РД-1 Практические занятия 4 Самостоятельная работа 4 Раздел 2. Оптимизационные задачи Лекции 12 аи - афов к ад РД-1,РД-2  Практические занятия 12 рии тр Самостоятельная работа 36 Раздел 3. Булевы функции и их Лекции 8 ACH &gt;. BY yun РД-3 Практические занятия 8 нормальные формы Самостоятельная работа 16 Лекции 8 Р 4. Минимизация вых функций аздел Зак буле функц РД-3, РД-4 Практические занятия 8 и систем булевых функций. Самостоятельная работа 24 Содержание разделов дисциплины: Раздел 1. Основы теории графов  История развития теории графов и область ее применения. Графы, их классификация и способы задания. Изоморфные графы. Подграф. Маршруты в графе, диаметр, радиус и центры графа. Связность простых графов. Теорема об оценке числа ребер в графе и следствие о связном графе. Связность орграфов: сильная, слабая, односторонняя. Выделение компонент сильной связности.  Темы лекций:  1. История развития теории графов и область ее применения. Графы, их классификация и способы задания. Изоморфные графы. Подграф.  2. Маршруты в графе. Связность простых и ориентированных графов.  Темы практических занятий:  1. Постановка задач на языке теории графов. Методы доказательств в теории графов (метод математической индукции, от противного, конструктивное доказательство, подсчет двумя способами).  2. Поиск маршрутов в графе. Алгоритмы выявления компонент сильной связности (алгоритм на основе умножения булевых матриц, алгоритм Уоршалла).  Раздел 2. Оптимизационные задачи теории графов  Обход графа. Поиск кратчайшего и минимального пути. Поиск минимальных путей между всеми парами вершин. Деревья. Теорема о шести эквивалентных утверждениях о дереве. Поиск кратчайшего остова. Ориентированные деревья. Сети и потоки, теорема Форда- Фалкерсона. Поиск максимального потока в сети. Эйлеровы графы. Необходимое и достаточное условие эйлеровости графа. Задача почтальона. Гамильтоновы графы. Теорема Дирака. Задача коммивояжера. Планарность графа, необходимые и достаточные условия планарности. Укладка графа на плоскости. Раскраска графа. Хроматическое число произвольных и планарных графов. Точные и приближенные алгоритмы раскраски.  Темы лекций:  3. Обходы графа: обход в глубину и в ширину. Поиск кратчайших и минимальных путей.  4. Деревья и их применение. Теорема о шести эквивалентных утверждениях о дереве. Задача о кратчайшем остове. Ориентированные, упорядоченные и бинарные деревья.  5. Сети и потоки, теорема Форда-Фалкерсона. Максимальный поток и поток минимальной стоимости.  6. Эйлеровы графы. Необходимое и достаточное условие эйлеровости. Задача почтальона.  7. Гамильтоновы графы. Необходимое условие гамильтоновости: теорема Дирака. Задача коммивояжера.  8. Планарность графов. Теорема Понтрягина-Куратовского. Раскраска графов. Теоремы о хроматическом числе произвольных и планарных графов.  Темы практических занятий:  3. Алгоритмы поиска путей: волновой алгоритм, алгоритмы Дейкстра, Беллмана- Мура, Флойда.  4. Поиск кратчайшего остова: алгоритмы Прима и Краскала. Деревья поиска.  5. Поиск кратчайшего потока: алгоритмы Форда-Фалкерсона, Диница. Поиск потока минимальной стоимости: алгоритмы, основанные на поиске кратчайших путей и циклов отрицательного веса в остаточной сети.  6. Поиск эйлерова цикла: алгоритм Флери и алгоритмы, основанные на объединении простых циклов. Решение задачи почтальона для неориентированного и ориентированного графа.  7. Поиск гамильтонова цикла: поиск с возвратами. Точные и приближенные методы решения задачи коммивояжера.  8 Алгоритм укладки графа на плоскости. Алгоритмы раскраски графа.  Раздел 3. Булевы функции и их нормальные формы  Булевы константы и векторы. Булево пространство. Интервал в булевом пространстве. Булевы переменные. Булева функция, способы ее задания. Фиктивные переменные. Элементарные булевы функции. Формула как способ задания функции. Двойственная функция и двойственная формула. Формула Шеннона, разложение булевой функции по К переменным. Совершенная дизъюнктивная нормальная форма (СовДНФ). Совершенная конъюнктивная нормальная форма (СовКНФ). Дизъюнктивная нормальная форма (ДНФ).  Темы лекций:  9. Булевы константы и векторы. Булево пространство и его задание матрицей Грея. Интервал в булевом пространстве. Теорема о мощности интервала. Способы задания интервала.  10. Булевы переменные. Булева функция, способы ее задания. Теорема о числе булевых функций. Фиктивные переменные, их выявление и удаление. Элементарные булевы функции.  11. Формула как способ задания функции. Равносильность формул, способы доказательства равносильностей. Двойственная функция и двойственная формула. Принцип двойственности.  12. Разложение Шеннона. Разложение функции по К переменным. Совершенные нормальные формы: дизъюнктивная и конъюнктивная. Дизъюнктивная нормальная форма. Теорема о конъюнкции и интервале.  Темы практических занятий:  9. Длина и вес булева вектора, представление подмножеств булевыми векторами. Сравнение векторов. Распознавание интервала.  10. Построение булевых функций. Способы задания булевых функций. Выявление и удаление фиктивных переменных.  11. Проверка равносильностей. Двойственные функции и формулы. Построение двойственной функции.  12. Разложение функции по переменным. Построение ДНФ по таблице истинности и матрице Грея. Построение матрицы Грея по ДНФ.  Раздел 4. Минимизация булевых функций и систем булевых функций.  Сокращенная, минимальная, кратчайшая и безызбыточная ДНФ. Построение ДНФ по формуле. Двухэтапный метод минимизации булевой функции. Поиск сокращенной ДНФ: теорема Квайна и алгоритм Квайна-МакКласки, теорема Блейка и алгоритм Блейка- Порецкого. Поиск кратчайщей ДНФ: таблица Квайна, покрытие, его длина, минимальное, кратчайшее и безызбыточное покрытие. Алгоритмы поиска одного и всех безызбыточных покрытий, кратчайшего покрытия. Приближенная кратчайшая ДНФ, метод Закревского. Определение и способы задания не полностью определенных (частичных) булевых функций, доопределение. Минимизация частичных булевых функций. Системы булевых функций. Кратчайшая и безызбыточная системы ДНФ.  Темы лекций:  13. Импликанты и простые импликанты функции. Сокращенная, кратчайшая, минимальная и безызбыточная ДНФ. Теорема о кратчайшей ДНФ. Теорема о минимальных  ДНФ.  14. Двухэтапный метод минимизации булевой функции. Поиск сокращенной ДНФ: теорема Квайна и алгоритм Квайна-МакКласки, теорема Блейка и алгоритм Блейка- Порецкого.  15. Поиск кратчайщей ДНФ: таблица Квайна, покрытие, его длина, минимальное, кратчайшее и безызбыточное покрытие. Алгоритмы поиска одного и всех безызбыточных покрытий, кратчайшего покрытия.  16. Определение и способы задания не полностью определенных (частичных) булевых функций, доопределение. Минимизация частичных булевых функций. Системы булевых функций. Кратчайшая и безызбыточная системы ДНФ.  Темы практических занятий:  13. Выявление импликант и простых импликант. Визуальный поиск сокращенной, кратчайших, минимальных и безызбыточных ДНФ. Построение ДНФ по формуле.  14. Поиск сокращенной ДНФ: алгоритм Квайна-МакКласки, алгоритм Блейка- Порецкого.  15. Поиск кратчайших и минимальных покрытий таблицы Квайна и построение кратчайшей ДНФ.  16. Минимизация частичных булевых функций и систем булевых функций.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый 06 Разделы дисциплины учения по Виды учебной деятельности pene, a. дисциплине  Раздел 1. Раздел 1. Базовые технологии Лекции 12 коммутации и маршрутизации РД-1, РД-2 Лабораторные занятия 12 инфокоммуникационных сетей Самостоятельная работа 48  Лекции 12 Раздел 2. Раздел 2. Продвинутые „ РД-,РД-2  Лабораторные занятия 12 технологии инфокоммуникационных сетей  Самостоятельная работа 48  Содержание разделов дисциплины: Раздел 1. Раздел 1. Базовые технологии коммутации и маршрутизации  инфокомм уникационных сетей  В разделе изучаются основные технологии сетей коммутации и маршрутизации инфокоммуникационных систем и сетей класса ЗОНО на примере оборудования и технологий Huawei  Темы лекций:  1. Введение, принципы сетевой адресация и протоколов. Протоколы Ethernet, IP, ARP, ICMP.  2. Коммутация, протокол связующего дерева (STP, RSTP)  Статическая маршрутизация в ГР-сетях Динамическая маршрутизация в ГР-сетях (OSPF) Принципы работы VLAN Маршрутизация между УГАМ Названия лабораторных работ: Huawei УКР и основы конфигурирования Адресация ГРу4 Статическая маршрутизация на примере IPv4 Сети коммутации Протокол связующего дерева Динамическая маршрутизация на примере OSPF Основы Ethernet и конфигурирование VLAN . Связь между VLAN  Раздел 2. Раздел 2. Продвинутые технологии инфокоммуникационных сетей  В разделе изучаются продвинутые технологии, распространённые в корпоративных и глобальных сетях класса Enterprise на примере оборудования и технологий Huawei  Темы лекций:  7. Сетевые сервисы (DNS, FTP, DHCP)  3  NAwnrY  © чм  8. Агрегирование каналов коммутации  9. Технология ACL, ААА  10. Технология МАТ  11. Сети IPv6: адресация и маршрутизация  12. Использование беспроводных сетей  Названия лабораторных работ:  9. Настройка ОНСР  10. Настройка ЕТР-сервиса  11. Настройка агрегированных каналов в сетях коммутации и маршрутизации 12. Использование списков доступа (ACL) и механизма ААА 13. Использование технологии МАТ  14. Построение сетей ТРуб  15. Основы сетевого программирования и автоматизации  16. Реализация беспроводных сетей  5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной Объем результат деятельности времени, 4. обучения по дисциплине Раздел (модуль) 1. Основы методологии РД1 Лекции 2 исторической науки РД2 Практические 2 РДЗ занятия РД4 Самостоятельная  2 работа Раздел (модуль) 2. Россия и мир в древности РД1 Лекции 6 и в средние века РД2 Практические 4 РДЗ занятия РД4 Самостоятельная  2 работа Раздел (модуль) 3. Европа в период позднего РД1 Лекции 6 средневековья. Московское царство ХУ- РД? Практические 4 XVII вв. РДЗ занятия РД4 Самостоятельная  2 работа Раздел (модуль) 4. Российская империя в РД1 Лекции 18 контексте европейской цивилизации в ХУШ- РД2 Практические 10 начале ХХ вв. РДЗ занятия РД4 Самостоятельная  2 работа Раздел (модуль) 5. РД1 Лекции 4 Россия в революционных трансформациях РД2 Практические 2 начала ХХ века 1914 -1922 гг. От первой РДЗ занятия мировой войны до окончания Гражданской РД4 Самостоятельная  2 войны. работа Раздел (модуль) 6. Советское государство в РД1 Лекции 12 30- нач. 50-х годах. РД2 Практические 8 РДЗ занятия  Великая Отечественная война. РД4 Самостоятельная  4 работа Раздел (модуль) 7. СССР в 1953-1991 гг. РД1 Лекции 10 Становление российской государственности. РД2 Практические 6 РДЗ занятия РД4 Самостоятельная  4 работа Раздел (модуль) 8. Россия и мир в конце 90rr РД1 Лекции 6 - начале 21 в. РД2 Практические 4 РДЗ занятия РД4 Самостоятельная  2 работа Раздел (модуль) 9. История инженерной РД1 Лекции 8 деятельности РД2 Практические 8 РДЗ занятия РД4 Самостоятельная  4 работа  Содержание разделов дисциплины:  Раздел 1. Основы методологии исторической науки  Тема лекции:  1. История и историческая наука. История в системе социально-гуманитарных наук. Объект и предмет исторической науки. Место истории в системе наук. Теория и методология исторической науки, её методы. Историческое сознание и историческая память. Социальные функции истории. Источники изучения истории, их классификация. История России - неотъемлемая часть всемирной истории. Отечественная историография в прошлом. Выдающиеся представители российской исторической науки. Основные направления современной исторической науки.  Тема практического занятия:  1. Методология истории.  Периодизация истории. Понятие исторического источника. Роль курса «История России» в инженерном образовании (дискуссия). Организация работы над курсом.  Раздел 2. Россия и мир в древности и в средние века  Тема лекции:  2. Восточные славяне в древности. Этногенез и расселение славян. Понятие Древнего мира. Цивилизации Запада и Востока в древности, их сравнительная характеристика. Народы и древнейшие государства на территории нашей страны. Территория России в системе Древнего мира: древнейшие культуры Северной Евразии, киммерийцы, скифы, греческие колонии в Северном Причерноморье. Великое переселение народов. Падение Римской империи. Варварские королевства. Государство франков. Вопрос о славянской прародине и происхождении славян. Расселение славян, их разделение на три ветви: восточных, западных и южных. Славянские общности Восточной Европы. Их соседи: балты и финно-угры. Хозяйство восточных славян, их общественный строй и политическая организация. Возникновение княжеской власти. Религиозные представления.  3. Древнерусское государство и его культурно-цивилизационные характеристики.  Образование Древнерусского государства.  Предпосылки образования Древнерусского государства:  cCOlMasIbHO-9KOHOMHYeCKHe, политические, культурные. Изменения в восточнославянском обществе на рубеже УШ-Х вв. этнокультурные факторы становления государственности. Киев и Новгород - два политических центра восточных славян. Начало династии Рюриковичей.  Формирование политических институтов. Система = управления. Княжеская власть; роль вече. Принятие христианства и его влияние на политические, социальные, культурные процессы.  Русские земли в XII-XIV вв. Эволюция древнерусской государственности в XI-XII вв. Новгородская земля, Галицко-Волынское, Владимиро-Суздальское княжества в период политической раздробленности: формирование различных моделей развития древнерусского общества и государства.  4. Русская культура в ХП-ХУ вв. Ценностно-смысловое единство русской культуры.  Формирование христианской культуры. Появление письменности и литературы. Основные жанры древнерусской литературы. Летописание («Повесть временных лет»). Жития святых. Княжеско-дружинный эпос («Слово о полку Игореве», «Задонщина»). «Поучение» Владимира Мономаха. «Хожение за три моря» Афанасия Никитина. Начало каменного строительства. Софийские соборы в Киеве, Новгороде, Полоцке. Владимиро-суздальские и новгородские храмы. Возобновление каменного строительства после монгольского нашествия. Приглашение Иваном Ш иноземных мастеров. Ансамбль Московского Кремля. Древнерусское изобразительное искусство: мозаики, фрески, иконы. Творчество Феофана Грека, Андрея Рублева. Знания о мире и технологии. Обучение и уровень грамотности в древней Руси, берестяные грамоты, граффити.  Тема практических занятий:  2. Древнерусское государство и общество  Концепции происхождения государства (норманнская, антинорманская, торгово- городская. формационная). Современные подходы к проблеме политогенеза и образования Древнерусского государства. Деятельность первых русских князей. «Русская Правда» как отражение социальных и политических процессов.  3. Русь и Золотая Орда: влияние ордынского фактора на начало объединительных процессов. Начало возвышения Москвы.  Образование монгольской державы. Причины и направления монгольской экспансии. Ордынское нашествие на русские земли. Экспансия Запада. Александр Невский. Взаимоотношения русских княжеств и Золотой Орды. Объединение русских земель вокруг Москвы. Отношения Москвы с русскими княжествами и землями. Дмитрий Донской. Альтернативные варианты объединения русских земель: Тверское княжество; Великое княжество Литовское как претенденты на роль политического центра.  Раздел 3. Раздел (модуль) 3. Европа в период позднего средневековья. Московское царство XV- XVII вв.  Тема лекции:  5. Образование централизованного государства.  Русь между Ордой и Великим княжеством Литовским. Польско-литовская уния и судьбы  западно-русских земель. Иван Ш. Окончание ига. Судебник 1497 г. и начало законодательного оформления процесса государственной централизации. Дворянство как опора центральной власти. Общественно-политическая мысль на рубеже столетий. Первые  приказы. Укрепление власти великого князя московского. Ликвидация удельной системы. Завершение формирования доктрины «Москва — Третий Рим», формула монаха Филофея. Идейно-политическая борьба в Русской православной церкви. Взаимоотношения между светской и церковной властью.Византия эпохи Палеологов. Флорентийская уния. Завоевание Константинополя османами. Падение Византийской империи.  6. Россия XVI-XVII вв. в контексте развития европейской цивилизации  XVI-XVII века в мировой истории. Великие географические открытия и начало Нового  времени в Западной Европе. Эпоха Возрождения. Европейская Реформация: ее причины и значение. Развитие капиталистических отношений. Иван Грозный: поиск альтернативных путей социально-политического развития России. Реформы 50-х гг. XVI в. и складывание элементов сословно-представительной монархии. Избранная рада. «Казанская война». Ливонская война. Опричнина. Укрепление самодержавия. Социально-экономический и политический кризис второй половины XVI в. Изменения в социальной структуре и экономике страны. Начало присоединения Сибири. Оценка деятельности Ивана ГУ в исторической литературе.  7. Государство, церковь и культура в Московском государстве.  Церковь и государство. Церковная реформа Никона и раскол: его социально- политическая сущность и последствия. Вопрос о взаимоотношениях «священства и царства». Старообрядчество. Новые черты русской культуры в 17в. Западное влияние в русской культуре ХУП в. и основные каналы его проникновения.  Тема практических занятий:  4. «Смутное время»: кризис государственности и поиски альтернативных путей развития. Закат династии рюриковичей. Феномен самозванчества. Усиление шляхетско- католической экспансии на Восток. Роль ополчения в освобождении Москвы и изгнании чужеземцев. К. Минин и Д. Пожарский. Земский собор 1613 г. и воцарение династии Романовых.  5. Первые Романовы. Социально-экономические процессы в Московском государстве. Новые явления в хозяйственной жизни. Закрепощение крестьян. Усиление позиций дворянства. Боярская Дума. Земские соборы «Соборное Уложение» 1649 г.: юридическое закрепление крепостного права, сословных функций и самодержавия. Дискуссии о генезисе самодержавия в России.  Раздел (модуль) 4. Российская империя в контексте европейской цивилизации в ХУШ - начале ХХ вв.  Тема лекции:  8. Модернизационные процессы в Мировой и российской истории 18в.  ХУШ в европейской и мировой истории. Формирование колониальной системы и капиталистического хозяйства. Начало промышленного переворота в Европе. «Европейское Просвещение» и влияние его идей на мировое развитие. «Просвещенный абсолютизм». Французская революция и ее влияние на политическое и социокультурное развитие стран Европы.  Необходимость преобразований в Российском государстве. Методы, средства, принципы, цели реформ. Проблема цены преобразований. Вопросы о программе и планомерности преобразований. Роль государства и верховной власти в осуществлении реформ. «Эволюционный» и «революционный» форматы преобразований Петр I: борьба за трансформацию традиционного общества в России. Основные направления «европеизации» страны. 9. Формирование Российской Империи.  Утверждение абсолютизма. Понятие «абсолютной монархии» Провозглашение России империей. Принципы «регулярного государства». Упрочение международного авторитета России. Дискуссия о деятельности Петра I. «Просвещённый абсолютизм»: теория и практическое воплощение  10. Русская культура ХУШ в.: от петровских инициатив к «веку Просвещения».  Преобразования в области культуры и быта. Развитие светской культуры. Перестройка повседневной жизни горожан и знати по европейскому образцу. Появление светских праздников и развлечений. Распространение стиля 2барокко. Перенесение на русскую почву западной архитектуры, живописи и музыки. Открытие первого общедоступного театра. Создание гражданского шрифта и начало книгоиздательства на русском языке. Возникновение прессы. Развитие образования и создание условий для научных исследований и их начало. Открытие первого высшего учебного заведения — Славяно-греко-латинской академии — и ее значение в развитии просвещения в эпоху Петра Г. Создание светских учебных заведений. Перевод научной литературы. Начало научного коллекционирования (Кунсткамера), указ о создании Академии наук. Идеология Просвещения и ее влияние на развитие русской культуры ХУШ в.  11. Россия и мир в первой половине XIX века.  Ускорение процесса индустриализации в XIX в. и его политические, экономические,  социальные и культурные последствия. Европейские революции XIX в. Возникновение марксизма. Секуляризация сознания и развитие науки. Гражданская война в США. Бисмарк и объединение германских земель. Попытки реформирования политической системы России при Александре I: проекты М.М. Сперанского и Н.Н. Новосильцева. Изменение политического курса в 20-х гг. ХХ в.: причины и последствия. Россия в системе международных отношений. Участие в антифранцузских коалициях. Тильзитский мир и его последствия. Участие России в континентальной блокаде. Россия в преддверии столкновения с империей Наполеона  12. «Консервативная модернизация» Николая I.  «Бюрократическая Империя» и ее основные черты.  Начало промышленного переворота. Переход от мануфактуры к фабрике. Строительство железных дорог. Развитие инженерного образования.  Подступы к решению крестьянского вопроса в первой половине XIX в.  13. Русская культура в первой половине ХШХв.  Русская общественная мысль второй четверти XIX в. Реформа народного просвещения в эпоху Александра I. Появление сети университетов. Развитие технических учебных заведений при Николае [.  Западники и славянофилы. Пушкинский период русской культуры. Развитие естественных наук и техники. Географические открытия.  14. Внутренняя и внешняя политика России во второй половине XIX в.  Россия после Крымской войны. Великие реформы Александра П.  Причины отмены крепостного права. Подготовка и ход крестьянской реформы. Манифест 19.02.1861. Значение крестьянской реформы, ее достижения и противоречия. Введение земств, реформа городского самоуправления, Судебная и военная реформы. Университетский устав 1863 г. Временные правила о цензуре и печати 1865 г. Земское движение: лидеры, формы организации. Земский либерализм: программные установки, цели, представители. Принципы национальной политики Российской империи. Центральная власть и национальные движения. Польское восстание 1863 г.  Россия как многоконфессиональное государство.  Европейское направление внешней политики в годы царствования Александра П. Новое соотношение сил как результат образования больших европейских держав (Германии и Италии). Политика России в Средней Азии, ее включение в состав Российской империи. Русско-турецкая война (1877—1878). Берлинский конгресс. Внешнеполитический курс в царствование Александра Ш. Нарастающие конфликты с Германской империей. Русско- французское сближение. Становление блоковой системы в Европе конца XIX — начала XX ВВ.  15. Русская культура XIX - начала ХХ вв.: достижения и противоречия  Влияние на систему образования реформ Александра П. Создание земских школ. Университетское образование. Периодическая печать в XIX — начале ХХ в. Основные направления развития и достижения мировой науки.  Вклад российских ученых в развитие мировой науки (работы Н. И. Лобачевского, периодическая система химических элементов Д. И.Менделеева, открытия И. И. Мечникова и И. П. Павлова, удостоенные Нобелевской премии, и др.).  Формирование городского образа жизни и городской среды — доходные дома, водопровод, канализация. Развитие научных основ в архитектуре. Обращение к национальным основам — от «русско-византийского» стиля К. А. Тона к «русскому стилю» Государственного исторического музея. Золотой век и Серебряный век русской культуры.  Объединения «Мир искусства». Авангард в работах В. В. Кандинского, К. С. Малевича, Н. С. Гончарова. Развитие национальной театральной и музыкальной культуры. Появление «режиссерского» театра — театральная система К. С. Станиславского и В. И. Немировича-Данченко. Мировое признание русской культуры. Произведения П. И. Чайковского. Синтез театра, музыки и живописи в постановках С. П. Дягилева — «Русские сезоны» в Париже. Новые виды искусства — фотография и кино.  16. Россия и мир в начале ХХ в.  Войны конца ХПХ-начала ХХ вв. Завершение раздела мира и борьба за колонии. Основные черты социально-экономического развития Российской Империи на рубеже веков. Экономический рост 1890-х гг.: причины и масштабы. Строительство Транссибирской магистрали. Формирование новых промышленных регионов. Эволюция финансовой политики конца XIX в.: Н. Х. Бунге, И. A. Вышнеградский, С. Ю. Витте. Финансовая реформа 1895— 1897 гг. государства в процессе модернизации по мысли С. Ю. Витте. Привлечение иностранных инвестиций. Русская деревня в начале века. Обострение споров вокруг решения аграрного вопроса.  Тема практических занятий:  6. Реформы ХУШ в.  Основные направления реформ: социальные, военные, экономические, управленческие, административные. Скачок в развитии промышленности. Создание военно-морского флота и регулярной армии. Церковная реформа. Эволюция сословной структуры общества. Внешняя политика. Азовские походы; Северная война.  Итоги и результаты петровских реформ. Дворцовые перевороты ХУШ в. Политика «просвещенного абсолютизма» Екатерины П. Жалованные грамоты дворянству и городам. Введение свободы предпринимательства. Усиление крепостничества и социальные конфликты во второй половине XVIII B. Истоки и сущность дуализма внутренней политики Екатерины П. Расширение границ империи. Походы Румянцева, Суворова, Ушакова. Русско- турецкие войны. Присоединение Крыма. Разделы Польши.  7. Внутренняя и внешняя политика Александра I.  Участие Российской Империи в антифранцузских коалициях при Павле Ги Александре [. Походы А.В.Суворова. Отечественная война 1812 года. Победа России в войне против Наполеона и ее значение. Венский конгресс. Политическая концепция легитимизма. Восстание декабристов. Появление тайных обществ. Программы Северного и Южного общества. Причины поражения и последствия восстания. 8. Внутренняя и внешняя политика Николая I.  Деятельность М.М.Сперанского, реформы П.Д.Киселева и Е.Ф. Канкрина. Внешняя политика: основные направления. «Восточный вопрос». Россия и Кавказ. Крымская война. Ход событий. Оборона Севастополя. Причины поражения в войне, Парижский мирный договор.  9. Государство и общество во второй половине XIX вв.  Идейная борьба и общественные движения в России в 70-80 гг ХГХвв. Русское народничество. Направления и эволюция народнической мысли: М. А. Бакунин, П. Л. Лавров, П. Н. Ткачев. «Земля и воля» 1860-х гг. Хождение в народ. Революционный террор конца 1870 — начала 1880-х гг. Деятельность организации «Народная воля». Убийство народовольцами императора Александра П.  Начало царствования Александра Ш. Вопрос о программе нового царствования: контрреформы или политика стабилизации. Контрреволюционные устремления правительственных кругов. Идеологи консерватизма конца XIX в.: общественная мысль и политика (К. П. Победоносцев, М. Н. Катков). Реформы образования. Университетский устав 1884 г. Цензурная политика. Земское положение 1890 г. Городское самоуправление.  Первые марксистские кружки. Складывание Российской социал-демократической рабочей партии (РСДРП). Народничество 1880—1890-х гг.  10. Революция 1905-1907 гг. Начало российского парламентаризма.  Причины первой русской революции. Влияние русско-японской войны. Этапы революции. Манифест 17.10.1905г. Изменения в политической системе. Политические партии в России в начале ХХ в.: генезис, классификация, программы, тактика. Опыт думского «парламентаризма». Столыпинская аграрная реформа: экономическая, политическая и социальная сущность, итоги, последствия.  Раздел 5. Россия в революционных трансформациях начала ХХ века 1914-1922 гг. От Первой мировой войны до окончания Гражданской войны.  Tema лекции:  17. Первая мировая война и политический кризис в России:  Участие России в Первой мировой войне. Общенациональный кризис в стране и его истоки. Февральская революция. Альтернативы развития России после революции. Временное правительство. Политика новой власти. Петроградский Совет. Двоевластие. Эволюция власти от февраля к октябрю. Кризисы Временного правительства. «Апрельские тезисы» Ленина. Корниловский мятеж.  18. Октябрь 1917 г. Формирование Советского государства.  События 25/26 октября. Первые декреты Советской власти. Разгон Учредительного собрания. Брестский мир. Политическая и экономическая программа большевиков. Начало формирования однопартийной политической системы. Принятие первой Конституции. Гражданская война и интервенция. Первая волна русской эмиграции. Современная отечественная и зарубежная историография о причинах, содержании и последствиях общенационального кризиса в России и революции в России в 1917 г.  Тема практических занятий:  11. Советское государство в 1918-1922 гг.  Гражданская война и интервенция: причины, основные этапы, события, итоги Гражданской войны. Политический кризис в Советском государстве в начале 1920-х гг. Переход от военного коммунизма к нэпу. Образование СССР. Особенности советской национальной политики и модели национально-государственного устройства.  Раздел 6. Советское государство в 20-40 —х годах. Великая Отечественная война.  Тема лекции:  19. Мир между мировыми войнами.  Новая карта Европы. Версальская система международных отношений. Лига наций. Капиталистическая мировая экономика в межвоенный период. Мировой экономический кризис 1929 г. и «великая депрессия». Идеологическое обновление капитализма под влиянием социалистической угрозы. Приход к власти фашистов в Германии. «Новый курс» Ф. Рузвельта. Коминтерн как орган всемирного революционного движения.  20. СССР в 20-30-е годы  Борьба в руководстве партии по вопросам развития страны. Возвышение И.В. Сталина. Курс на строительство социализма в одной стране. Форсированная индустриализация: предпосылки, источники накопления, методы, темпы, итоги. Политика сплошной коллективизации сельского хозяйства, ее социальные и политические последствия. Утверждение тоталитарного политического режима. Экономические основы советского политического режима. Культурная революция в Советском государстве. Конституция СССР 1936 г.  21. СССР во Второй мировой войне.  Международная ситуация в конце 30-х годов. Предпосылки Второй мировой войны. Пакт Молотова-Риббентропа. Начало войны. Советско-финская война и ее итоги.  22-23. Великая Отечественная война советского народа (1941-1945)  Нападение нацистской Германии на СССР. Причины отступления советских войск. Массовый героизм советских воинов. Важнейшие сражения лета — осени 1941 г. Блокада Ленинграда. Победа под Москвой и ее историческое значение. Крах немецкой стратегии блицкрига. Нацистский оккупационный режим. Политика и практика геноцида советского народа нацистами и их пособниками. Генеральный план «Ост» и замыслы гитлеровского руководства относительно населения СССР. Массовые преступления гитлеровцев на временно оккупированной территории.  Становление партизанского движения в тылу противника. Битва под Сталинградом. Советское наступление зимой — весной 1943 г.  Деблокирование Ленинграда. «Дорога Победы». Основные причины успеха советских войск в ходе зимнего контрнаступления.  Сражение на Курской дуге и наступление Красной армии по всем фронтам до весны  1943 г. Причины успеха советского наступления осенью 1943 г. — весной 1944 г. Рост выпуска военной техники в СССР, освоение новых образцов вооружений. Окончательное освобождение территории СССР и освободительный поход в Восточную и Центральную Европу. Важнейшие сражения: операция «Багратион», Ясско-Кишиневская операция, Висло-Одерская операция, Берлинская операция. Освобождение Праги. Капитуляция Германии. Начало восстановления экономики освобожденных регионов СССР.  Итоги Великой Отечественной и Второй мировой войны. Решающий вклад СССР в победу антигитлеровской коалиции. Людские и материальные потери. Изменения политической карты Европы. __  План «Барбаросса». Основные этапы и события Великой Отечественной войны. Создание антигитлеровской коалиции. Решающий вклад СССР в разгром фашизма. Причины и цена победы. Консолидация советского общества в годы войны.  24. От Холодной войны к Новому политическому мышлению»: международные отношения во второй половине ХХ века.  Формирование двух лагерей: социалистического и капиталистического. Состав и характеристика участников. Образование военно-политических блоков: НАТО и ОВД. Гонка вооружения, развитие средств доставки ядерных зарядов. Раздел мира на зоны влияния. Фултонская речь У. Черчилля. «Доктрина Трумэна» и план Маршалла. Берлинский кризис 1948 г. Борьба «с безродным космополитизмом» в СССР и маккартизм в США. Венгерское восстание и Суэцкий кризис. Берлинский кризис (1961 г.). Карибский кризис.  Движение неприсоединения. Противостояние социалистического и капиталистического блока в бывших колониях.  «Доктрина Брежнева». Чехословацкое восстание. Совещание по безопасности и сотрудничеству в Европе. ОСВ-Ги ОСВ-П. Новый виток гонки вооружения. Завершающий этап Холодной войны. «Новое политическое мышление» М.С. Горбачева. Объединение Германии. Распад СССР и роспуск ОВД.  Тема практических занятий:  12. «Большой скачок». Модернизационные процессы 30-х годов. Решения XIV и ХУ съездов. Дискуссии о методах и темпах проведения индустриализации.  и 2 пятилетние планы. Коллективизация как основной источник инвестиций для проведения индустриализации. Особенности культурной революции в СССР. Формирование тоталитарного режима.  13. Великая Отечественная война советского народа. План «Барбаросса». Основные этапы и события Великой Отечественной войны. Создание антигитлеровской коалиции. Решающий вклад СССР в разгром фашизма. Причины и цена победы. Консолидация советского общества в годы войны.  14. Проект «Без срока давности»: памяти геноцида советского народа в годы Великой Отечественной войны.  15. Послевоенное десятилетие.  Социально-экономическое развитие, общественно-политическая жизнь, культура СССР в послевоенный период. Трудности послевоенного переустройства. Восстановление народного хозяйства и ликвидация атомной монополии США. Ужесточение политического режима и идеологического диктата. «Демократический импульс войны» и ужесточение политического режима. «Поздний сталинизм» (1945-1953). XIX съезд партии и его решения. Необходимость нового технологического рывка в свете военно-технического противостояния с Западом. «Атомный проект», переход к турбореактивному самолетостроению, развитие ракетостроения. Новый виток массовых репрессий. «Борьба с космополитизмом». Голод 1946—1947 гг.  Раздел 7. СССР в 1953-1991 гг. Становление Российской государственности.  Тема лекции:  25. Социально-экономическое развитие, внешняя политика, общественно- политическая жизнь, культура СССР в период «Оттепели».  «Оттепель» (вторая половина 1950-х — первая половина 1960-х гг.). Борьба за власть после смерти И. В. Сталина. Причины, обусловившие победу Н. С. Хрущева. Реабилитация жертв политических репрессий. ХХ съезд КПСС. Принятие новой программы партии. Планы построения коммунизма к 1980 году. Успехи в освоении космоса. Завершение в СССР процесса урбанизации и экономические последствия. Аграрная политика: Освоение Целины и другие новации в сельском хозяйстве. Создание Совнархозов. Практические результаты реформ. Важнейшие достижения СССР в этот период: решение жилищной проблемы, лидирующие позиции в исследованиях космоса и компьютерных технологиях. Замедление темпов роста экономики к середине 1960-х гг. Причины отстранения Хрущева от власти.  26. СССР 1970-х-начале 1980-х гг.: курс руководства страны на консервацию советской системы. Застой.  Власть и общество BO второй половине 1960-х — начале 1980-х rr. Приход к власти Л. И. Брежнева. Принцип коллективного руководства. Выбор стратегического пути развития страны в середине 1960-х гг. Реформа по внедрению в экономику принципов экономического стимулирования и причины ее свертывания. Возрастание роли и значения ВПК и ТЭК. Освоение нефтегазовых месторождений Западной Сибири и их значение. Строительство Байкало-Амурской магистрали. Проекты международного сотрудничества с Европой (газопровод «Дружба») и экономические санкции.  Причины снижения темпов экономического развития и появления кризисных явлений к началу 1980-х гг. Отставание в производительности труда, в компьютерных технологиях, в наукоемких отраслях промышленности. Рост «теневой экономики». Ситуация в сельском хозяйстве. Причины неудач в решении продовольственной проблемы. Вынужденное увеличение импорта зерна.  Советское общество в период «позднего социализма». Приоритеты социальной политики. Повышение культурно-образовательного уровня и материального благосостояния граждан. Ликвидация бедности. Формирование советского «среднего класса». Рост потребительских запросов населения и обострение проблемы товарного дефицита. Принятие Конституции СССР 1977 г. Рост влияния КПСС. Увеличение привилегий номенклатуры к началу 1980-х гг.  27-28. 1985-1991 гг.: реформирования советской системы. «Перестройка»  Попытки реформирования СССР во второй половине 1980-х гг.  Формирование идеологии нового курса: «ускорение», «гласность», «перестройка». Реакция населения на политику «перестройки».. Экономическая реформа: кооперативы и государственные предприятия с выборными директорами и СТК. «Явочная» приватизация. Перемены в отношении государства и церкви. Их последствия. 1000-летие Крещения Руси. Съезд народных депутатов 1989г. Становление многопартийности. Учреждение поста Президента.  «Парад суверенитетов» — причины и следствия. Обострение межнациональных конфликтов. «Новоогаревский процесс» и договор об учреждении Союза Суверенных Государств. Путч ГКЧИ, учреждение Содружества Независимых Государств, и роспуск СССР. Непосредственные и долгосрочные последствия распада СССР. Дискуссия о причинах распада СССР и о соотношении в данном случае внешнего и внутреннего факторов.  Внешняя политика периода «перестройки». «Новое мышление». Советско- американский договор о ракетах малой и средней дальности. Роспуск ОВД и СЭВ. Объединение Германии и вопрос о расширении НАТО на восток. «Бархатные революции» в Восточной Европе. Окончание «холодной войны». Вопрос о судьбе советского ядерного оружия. Европейская интеграция. Культура СССР в период «перестройки».  29. Становление российской государственности Россия в 1990-е гг.  Принятие декларации о государственном суверенитете РФ. 12.06.1990. Избрание Президентом РФ Б.Н.Ельцина. Противоречия между исполнительной и законодательной ветвями власти. Политический и конституционный кризис 1993г. Принятие новой Конституции. Демонтаж системы советов.  Становление и развитие российского федерализма, его особенности. Военно-политический кризис в Чечне. Внешняя политика РФ в 1991-1999 гг. Политические партии и общественные движения России.  Тема практических занятий: 16. Общество и культура в 60-70-е гг.  1960-х гг. Изменения в общественных настроениях в период «Оттепели». Феномен «шестидесятников». Ослабление «железного занавеса». Московский фестиваль молодежи и студентов 1957 г. Московские кинофестивали. Антирелигиозная политика. Кампания против «формализма и абстракционизма». Поэзия 60-х как общественный феномен. Расцвет живописи, кинематографа, литературы. «Лагерная проза» А.И.Солженицына и В.Шаламова.  Диссидентское движение в СССР: предпосылки, сущность, основные этапы развития. Уход молодежи в неформальные движения (КСП, хиппи и др.). Снижение доверия к государственным СМИ. «Самиздат» как социальный феномен. Правозащитное движение. Потребительские тенденции в социуме. Рост «теневой экономики». Состояние советского социума к 1985 г.  17. СССР в 1970-1980-rr.  Экономические реформы 1965-1970rr: идеология, программа, реализация. Промышленный рост и достижения 8- пятилетки. Почему «косыгинские» реформы не получили дальнейшего развития? Могли ли они привести к модернизации советского строя? (дискуссия). Курс руководства страны на консервацию советской системы. Стагнация в экономике и нарастание кризисных явлений во всех сферах общественной жизни. Ввод советских войск в Афганистан и его последствия.  18. Россия в 1990-е гг.  Радикальные изменения экономического и политического строя в России. Либеральная концепция российских реформ: переход к рынку, формирование гражданского общества и правового государства. «Шоковая терапия» начала 1990-х гг.: либерализация цен, ваучерная приватизация. Резкая поляризация общества. Наука, культура, образование в рыночных условиях. Социальная цена и первые результаты реформ.  Раздел 8. Россия и мир в начале 21 в.  Тема лекции: 30. Основные тенденции, проблемы и противоречия развития мира в начале XXI в.  Особенности внутри - и внешнеполитического развития отдельных стран Европы и США. Интеграционные процессы в мире. Постиндустриальное общество. Интернет. Информационная революция. Информационная экономика. Экономические кризисы. Глобализация и региональная интеграция. Интеграционные процессы в Евразии, Тихоокеанском и Атлантическом регионах. Новые социальные и культурные проблемы. Проблемы климата, экологии и демографии. Межэтнические конфликты. Миграционный кризис. Пандемия. Нарастание разрыва между богатыми и бедными.  Новая научная картина мира: открытия в области астрономии, физики, биологии, химии, медицины, генной инженерии. Когнитивные науки и искусственный интеллект.  Интеграционные процессы в мире. Модернизационные процессы в странах Латинской Америки, Азии и Африки в конце ХХ в. — начале ХХ] века. Государства на постсоветском пространстве в Европе и Азии. Проблемы формирования новой системы международных отношений. Борьба с международным терроризмом. Расширение НАТО и Европейского союза на восток. Возрастание роли Китая на международной арене. Восстановление лидирующих позиций России в международных отношениях. Последовательное отстаивание Россией концепции многополярного мира.  31. Россия в XXI в.  Избрание в 2000 г. В. В. Путина президентом России. Приоритеты нового руководства страны. Преодоление противостояния парламента и правительства. Укрепление «вертикали власти», создание федеральных округов. «Равноудаление» бизнеса от власти. Восстановление в Чечне конституционного порядка. Разграничение властных полномочий федерального центра и регионов. Приведение местного законодательства в соответствие с федеральным.  Переизбрание В. В. Путина президентом в 2004 г., главные положения </t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине Раздел 1. РД1 Лекции 12 Обыкновенные Практические занятия 12 дифференциальные уравнения РД? Лабораторные занятия 0 PIB Самостоятельная работа 30 Раздел 2. PHI Лекции 12 Числовые и функциональные Практические занятия 12 ряды РД Лабораторные занятия 0 PIB Самостоятельная работа 39 Раздел 3. PHI Лекции 16 Комплексный анализ Практические занятия 16 РД Лабораторные занятия PIB Самостоятельная работа 38 Раздел 4. РД1 Лекции 8 Преобразование Лапласа. Практические занятия 8 Операционный метод решения РД Лабораторные занятия дифференциальных уравнений РЗ Самостоятельная работа 13  Содержание разделов дисциплины:  Раздел 1. Обыкновенные дифференциальные уравнения первого порядка  Дифференциальные уравнения первого порядка: основные определения и понятия.  Существование и единственность решения задачи Коши. Особые решения. Уравнения с разделяющимися переменными и уравнения, приводящиеся к ним. Однородные уравнения. Уравнения, приводящиеся к однородным. Линейные уравнения, уравнение Бернулли и методы решения. Уравнения в полных дифференциалах. Интегрирующий множитель. Простейшие типы уравнений, не разрешенных относительно производной Дифференциальные уравнения высших порядков: основные понятия и определения. Уравнения, допускающие понижение порядка. Линейные однородные дифференциальные уравнения. Линейные однородные дифференциальные уравнения с постоянными коэффициентами, построение фундаментальной системы решений. Уравнение Эйлера. Линейные неоднородные дифференциальные уравнения, методы решения. Системы дифференциальных уравнений: основные определения и понятия, методы решения. Линейные системы дифференциальных уравнений с постоянными коэффициентами.  Темы лекций:  1. ДУ 1-го порядка. ДУ с разделяющимися переменными, однородные. Линейные ДУ 1-го порядка, уравнение Бернулли...  ДУ в полных дифференциалах, интегрирующий множитель. Основные теоремы дифференциального исчисления  N  ДУ высших порядков допускающие понижение порядка. Линейные однородные ДУ. Определитель Вронского. Линейные неоднородные ДУ . Метод Лагранжа. Линейные неоднородные ДУ со специальной правой частью  AWRY  Системы дифференциальных уравнений, основные понятия и определения. Методы решения.  Темы практических занятий:  ДУ 1-го порядка с разделяющимися переменными, однородные ДУ.  Линейные ДУ 1-го порядка, уравнение Бернулли. ДУ в полных дифференциалах. ДУ высших порядков допускающие понижение порядка. Однородные ДУ. Неоднородные линейные ДУ со специальной правой частью.  Неоднородные линейные ДУ. Метод Лагранжа. Системы ДУ.  Контрольная работа по теме «Дифференциальные уранения».  жиров  Раздел 2. Числовые ряды  Понятие числового ряда. Теоремы о свойствах сходящихся рядов. Необходимый признак сходимости ряда. Понятие знакоположительного ряда, необходимое и достаточное условие его сходимости. Достаточные признаки сходимости неотрицательных рядов. Эталонные ряды и их сходимость. Знакопеременные ряды: понятие условной и абсолютной сходимости. Теорема Лейбница. Признак Дирихле.  Определения функционального ряда и области его сходимости. Понятие равномерной сходимости. Признак Вейерштрасса. Свойства равномерно сходящихся рядов. Степенные ряды. Теорема Абеля. Основные свойства степенных рядов. Ряды Тейлора и Маклорена. Разложение основных элементарных функций в ряд Маклорена.  Ортогональные и нормированные системы функций. Тригонометрическая система функций. Понятие тригонометрического ряда Фурье. Сумма ряда Фурье. Теорема Дирихле. Разложение четных и нечетных функций в ряд Фурье. Разложение в ряд Фурье функций, заданных на полуинтервале. Ряд Фурье для функций с произвольным периодом. Понятие об интеграле Фурье  Темы лекций:  ивр  Числовые ряды. Основные теоремы о свойствах сходящихся рядов.  Достаточные признаки сходимости неотрицательных рядов. Знакопеременные ряды Функциональные ряды. Степенные ряды, основные свойства.  Разложение функций в степенные ряды  Ряды Фурье Разложение функций в тригонометрический ряд Фурье  Понятие об интеграле Фурье  Темы практических занятий:  про  Сумма ряда, необходимый признак сходимости ряда. Достаточные признаки сходимости  Знакопеременные ряды.  Функциональные ряды, равномерная сходимость. Область сходимости  Разложение функций в степенные ряды.  Разложение функций в ряд Фурье, условия Дирихле Ряды Фурье для функций с произвольным периодом.  Контрольная работа  Раздел 3. Комплексный анализ  Комплексные числа и действия над ними. Определение ФКП. Основные элементарные функции комплексного переменного и их свойства. Однозначные и многозначные функции. Точки ветвления и их классификация. Производная ФКП. Дифференцируемость. Условия Коши - Римана. Геометрический смысл производной. Понятие аналитичности ФКП. Интеграл от ФКП вдоль кривой и его свойства. Интегральная формула Коши.  Числовые и функциональные ряды с комплексными членами. Степенные ряды. Теорема Абеля. Ряд Тейлора. Теорема о разложении аналитической функции в ряд Тейлора. Ряды Лорана, определение. Теорема Лорана о разложении аналитической функции в кольце в ряд. Понятие аналитического продолжения. Особые точки и их классификация.  Вычет функции в изолированной особой точке. Формулы для вычисления вычетов. Основная теорема о вычетах. Применение вычетов к вычислению определённых интегралов.  Темы лекций:  © чом ичьшр  Введение в ТФКП  Дифференциальное исчисление ФКП  Интегральное исчисление ФКП. Теоремы Коши  Ряды аналитических функций  Ряд Лорана.  Изолированные особые точки и их классификация  Вычет функции в изолированной особой точке, основная теорема теории вычетов. Приложение теории вычетов к вычислению некоторых интегралов  Темы практических занятий:  © чмирьь-  Комплексные числа и действия над ними, ФКП  Условия Коши — Римана. Геометрический смысл производной ФКП. Интегрирование ФКП. Интеграл Коши.  Ряды в комплексной области. Ряды аналитических функций Разложение функций в ряд Лорана.  Теория вычетов, нахождение вычетов.  Приложение теории вычетов к вычислению некоторых интегралов. Контрольная работа  Раздел 4 Преобразование Лапласа. Операционный метод решения дифференциальных уравнений  Операционное исчисление: основные понятия и определения. Свойства преобразования  Лапласа. Таблица оригиналов и изображений. Отыскание оригинала по изображению. Интеграл Меллина. Решение линейных дифференциальных уравнений с постоянными коэффициентами операционным методом. Интеграл Дюамеля и его применение к решению дифференциальных уравнений. Решение систем однородных и неоднородных дифференциальных уравнений операционным методом  Темы лекций:  1. Преобразование Лапласа и его свойства. 2. Обратное преобразование Лапласа  3. Приложения преобразования Лапласа  Темы практических занятий:  Преобразование Лапласа и его свойства  Обратное преобразование Лапласа  Решение ДУ и систем ДУ операционным методом. Контрольная работа  ов  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч.  обучения по  дисциплине  Раздел 1. Общее понимание права. РД-1 Лекции 2  РД-2 Практические занятия 2  Самостоятельная работа 8  Раздел 2. Гражданское право РД-1 Лекции 2  Практические занятия 4  Самостоятельная работа 8  Раздел 3. Трудовое право. РД-1 Лекции 2  РД-2 Практические занятия 2  Самостоятельная работа 8  Раздел 4. Административное и РД-1 Лекции 2  уголовное право в инженерной РД-2 Практические занятия 4  деятельности Самостоятельная работа 8  Раздел 5. Основы экологического РД-1 Лекции 0  права. Практические занятия 2  Самостоятельная работа 8  Раздел 6. Правовые основы РД-1 Лекции 0 предпринимательской РД-2  редпр A Практические занятия 2  деятельности и управления предприятием. Самостоятельная работа 8  Содержание разделов дисциплины:  Раздел 1. Общее понимание права.  Понятие функции и формы государства. Правовое государство. Регуляторы общественного поведения. Мораль, нравственность, право. Понятие и признаки права. Норма права. Правоотношение. Источники права. Механизмы возникновения и развития института права, функции права. Права человека. Правовые принципы, лежащие в основе политики противодействия коррупции. Конституционное право Российской федерации. История  развития государства и права Российской Федерации. Система права Российской Федерации. Отрасли российского права. Темы лекций:  1. Теория государства и права. Конституционное право. Права человека. Темы практических занятий  1. Признаки и методы права.  2. Конституция РФ. Права человека.  Раздел 2. Гражданское право  Понятие гражданского права и гражданского правоотношения. Особенности гражданских правоотношений. Субъекты гражданского права. Дееспособность. Правоспособность. Полномочия и доверенность. Право собственности. Сделки и обязательства в гражданском праве. Гражданско-правовой договор. Исковая давность. Наследственное право. Права на результаты интеллектуальной деятельности и средства индивидуализации. Гражданско- правовая ответственность.  Темы лекций:  1.Методы частного права. Отношения, регулируемые гражданским и семейным правом.  2. Авторское право. Интеллектуальная собственность  Темы практических занятий  1. Гражданское право. Гражданские правоотношения. Право собственности.  2. Договорное право. Обязательственное право. Наследственное право  3. Правовые основы охраны авторских прав и промышленной собственности,  4. Правовые основы охраны средств индивидуализации  Раздел 3. Трудовое право.  Предмет и принципы трудового права. Коллективный договор. Трудовой договор. Порядок заключения и расторжения. Основания прекращения трудового договора. Рабочее время. Время отдыха. Дисциплина труда. Отношения работника и работодателя. Ответственность за несоблюдение техники безопасности. Охрана труда. Трудовые гарантии. Индивидуальные и коллективные трудовые споры. Конфликты интересов и их урегулирование. Профсоюзы и социальное партнерство в сфере труда.  Темы лекций:  1. Правовое регулирование трудовых отношений.  Темы практических занятий  1. Возникновение и прекращение трудовых отношений. Разрешение трудовых споров  Раздел 4. Административное и уголовное право в инженерной деятельности  Административная и уголовная ответственность в профессиональной деятельности инженера. Административное право — функции, цели. Административное правонарушение. Административные правонарушения в промышленном производстве. Уголовное право — функции, цели, принципы. Уголовная ответственность в профессиональной деятельности инженера. Понятие преступления и состава преступления. Обоснованный риск и его пределы при осуществлении испытаний в инженерном деле. Общественная безопасность. Криминологическая характеристика преступлений, угрожающих национальной безопасности и конституционному строю Российской федерации: экстремизм, терроризм, коррупция. Профилактика и предупреждение экстремизма, терроризма, коррупции. Система уголовных наказаний. Уголовные наказания по преступлениям, связанным с экстремизмом, терроризмом и коррупцией.  Темы лекций  1. Административное право. Государственное управление  2. Уголовное право. Противодействие экстремизму. Противодействие коррупции  Темы практических занятий 1. Государственное управление. Административные правонарушения 2. Уголовная ответственность инженера. Противодействие коррупции  Раздел 5. Основы экологического права.  Принципы экологической политики государства. Основы правомерного использования природных ресурсов. Правовое регулирование экологической безопасности промышленных объектов. Требования к очистке и восстановлению почв, вод и воздуха при хозяйственном использовании, утилизации вредных отходов, отработанных технологических реагентов и ТОПЛИВ. Законодательные основы стимулирования использования экологически безопасных видов топлива и энергосбережения. Общество и окружающая среда. Экологический экстремизм.  Темы практических занятий  1. Правовые основы природопользования и охраны окружающей среды  Раздел 6. Правовые основы предпринимательской деятельности и управления предприятием.  Понятие и признаки предпринимательской деятельности, Государственное регулирование и контроль в сфере предпринимательской деятельности. Защита предпринимательской деятельности от коррупции. Лицензирование предпринимательской деятельности, Техническое регулирование предпринимательской деятельности. Организационно-правовые формы предприятий, правовые условия создания и управления предприятием. Правовое положение отдельных предпринимателей. Регулирование финансового оздоровления предприятий. Правовое регулирование стимулирования предпринимательства. Имущество, используемое в предпринимательской деятельности. Ответственность предпринимателей. Правовая защита конкуренции.  Темы практических занятий:  1. Правовые основы предпринимательской деятельности и управления предприятием.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины  Формируемый результат обучения по дисциплине  Виды учебной деятельности  Объем времени, ч.  развитие страны  Раздел 1. Что такое Россия? РД-1 Лекции 4 Практические занятия 8  Лабораторные занятия 0  Самостоятельная работа 4  Раздел 2. Российское РД-2 Лекции 4 государство-цивилизация Практические занятия 6 Лабораторные занятия 0  Самостоятельная работа 4  Раздел 3. Российское РД-3 Лекции 6 мировоззрение и ценности Практические занятия 6 российской цивилизации Лабораторные занятия 0 Самостоятельная работа 4  Раздел 4. Политическое РД-4 Лекции 6 устройство России Практические занятия 6 Лабораторные занятия 0  Самостоятельная работа 2  Лекции 4  Раздел 5. Вызовы будущего и РД-4 Практические занятия 6 0  2  Лабораторные занятия  Самостоятельная работа  Содержание разделов дисциплины:  Раздел 1. Что такое Россия?  Страна в её пространственном, человеческом, ресурсном, идейно-символическом и нормативно-политическом измерении. Население, культура, религии и языки. Современное  положение российских регионов.  Выдающиеся персоналии («герои»).  испытания и победы России, отразившиеся в еб современной истории.  Темы лекций: 1. Россия: цифры и факты. 2. Россия: испытания и герои  Ключевые  Темы практических занятий: 1. Регионы России 2. Народы России: культура, традиции, религия. 3. Российские праздники: история и современность. 4. Выдающиеся личности в истории России.  Раздел 2. Российское государство-цивилизация  Исторические, географические, институциональные основания формирования российской цивилизации. Концептуализация понятия «цивилизация». Что такое цивилизация? Плюсы и минусы цивилизационного подхода. Особенности цивилизационного развития России: история многонационального характера общества, перехода от имперской организации к федеративной, межцивилизационного диалога за пределами России (и внутри неё). Роль и миссия России в работах различных отечественных и зарубежных философов, историков, политиков, деятелей культуры.  Темы лекций: 1. Цивилизационный подход: границы понятий государства-нация и государство- цивилизация, концепции. 2. Развитие России как государства-цивилизации.  Темы практических занятий: 1. Цивилизационные концепции современности: Э. Тоффлер, В.Л. Цымбурский, Ф. Фукуяма, С. Хантингтон. 2. Классические и современные цивилизационные теории: возможности и ограничения. 3. Российская цивилизационная идентичность на современном этапе развития.  Раздел 3. Российское мировоззрение и ценности российской цивилизации  Мировоззрение и его значение для человека, общества, государства. Что такое мировоззрение? Теория вопроса и смежные научные концепты. Мировоззрение как функциональная система. Мировоззренческая система российской цивилизации. Представление ключевых мировоззренческих позиций и понятий, связанных с российской идентичностью, в историческом измерении и в контексте российского федерализма. Рассмотрение этих мировоззренческих позиций с точки зрения ключевых элементов общественно-политической жизни (мифы, ценности и убеждения, потребности и стратегии). Ценностные принципы (константы) российской цивилизации.  Темы лекций: 1. Мировоззрение и идентичность 2. Мировоззренческие принципы (константы) российской цивилизации 3. Ценности российской цивилизации.  Темы практических занятий: 1. Концепт мировоззрения в социальных науках. 2. Системная модель мировоззрения. 3. Типология ценностей и значение ценностей в формировании мировоззрения.  Раздел 4. Политическое устройство России  Основы конституционного строя России. Принцип разделения властей и демократия. Особенности современного российского политического класса. Генеалогия ведущих политических институтов, их история причины и следствия их трансформации. Уровни организации власти в РФ. Государственные проекты и их значение (ключевые отрасли, кадры, социальная сфера)  Темы лекций: 1. Конституционные принципы и разделение властей. 2. Стратегическое планирование: национальные проекты и государственные программы. 3. Гражданское участие и гражданское общество  Темы практических занятий: 1. Уровни и ветви власти. 2. Планирование будущего: национальные проекты и государственные программы. 3. Гражданское участие и гражданское общество в современной России  Раздел 5. Вызовы будущего и развитие страны  Суверенитет страны и его место в сценариях перспективного развития мира и российской цивилизации. Стабильность, миссия, ответственность и справедливость как ценностные ориентиры для развития и процветания России. Солидарность, единство и стабильность российского общества в цивилизационном измерении. Стремление к компромиссу, альтруизм и взаимопомощь как значимые принципы российской политики. Ответственность и миссия как ориентиры личностного и общественного развития.  Темы лекций: 1. Актуальные вызовы и проблемы развития России. 2. Сценарии развития российской цивилизации.  Темы практических занятий: 1. Россия и глобальные вызовы. 2. Внутренние вызовы общественного развития. 3. Глобальные проблемы современности  5.</t>
+  </si>
+  <si>
+    <t>(6 семестр)  Основные виды учебной деятельности  Формируемый &gt;. 06 Разделы дисциплины бучения ю Виды учебной деятельности npenewn, а. дисциплине  Раздел 1. Основы системного мышления РДУ. РД-2,  Практические занятия 6 у РД-3, РД-4 Самостоятельная работа 8 Раздел 2. Инструменты описания и анализа РД-1, РД-2, Практические занятия 10 систем РД-3, РД-4 Самостоятельная работа 12 РД-1, РД-2, Практические занятия 8  Раздел 3. Модели системного мышления РД-3, РД-4, РД-5 Самостоятельная работа 10 РД-1, РД-2, Практические занятия 6  Р 4. -  аздел 4. Синтез систем РД DLs Самостоятельная работа 8  Содержание разделов дисциплины:  Раздел 1. Основы системного мышления  Системное мышление, отличие от редукционизма. История системного мышления. Некоторые примеры несистемного подхода. Основные законы системного мышления. Система и не-система. Компоненты системы: элементы, связи, функция.  Темы практических занятий:  Базовые концепции системного мышления  2. Законы системного мышления  3.  Характеристики и компоненты систем  Раздел 2. Инструменты описания и анализа систем  Виды диаграмм и графиков для описания систем. Как распознать обманчивый график. Статистика и ее применение для анализа систем. Как правильно интерпретировать статистику. Парадокс Симпсона, скрытые переменные, ловушка Байеса. Стоки и источники системы. Обратная связь и ее виды. Причинно-следственная диаграмма: переменные, усиливающие и балансирующие циклы. Причинно-следственная связь и корреляция: как отличить одно от другого. Онлайн-инструменты для построения диаграмм.  Темы практических занятий: Графики и диаграммы для описания систем Статистика для анализа систем Стоки, источники, обратная связь Причинно-следственная диаграмма . Корреляция и причинность  Раздел 3. Модели системного мышления  Модель "айсберг": событие, паттерн, структура, ментальная модель. Виды ментальных моделей. Причинно-следственная диаграмма и ментальная модель. Системная динамика и ее виды. Связь динамики и структуры системы. Системные архетипы. Связь "архетип-структура-динамика". Негативные и позитивные системные архетипы.  Темы практических занятий:  9. Модель "айсберг"  10. Ментальные модели  11. Системная динамика  12. Системные архетипы  13. Негативные и позитивные архетипы  Стейкхолдеры. Классификация стейкхолдеров. Стратегии работы со стейкхолдерами. Основные ошибки в определении стейкхолдеров и работе с ними. Потребности и требования. Альфы системы.  Темы практических занятий:  14. Стейкхолдеры и их классификация  15. Потребности и требования  16. Альфы системы  © чм  5. Структура и содержание дисциплины (7-8 семестры)  Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем вре- результат обу- мени, ч. чения по дис- циплине Раздел (модуль) 1. Теория ком- Лекции 16 пиляции Практические занятия 16 Лабораторные занятия 0 РД-1 Самостоятельная работа 44 Раздел (модуль) 2. Алгоритмы и РД-2 Лекции 16 структуры данных РД-3 Практические занятия 16 РД-4 Лабораторные занятия 0 РД-5 Самостоятельная работа 41 Раздел (модуль) 3. Анализ соци- РД-6 Лекции 16 альных сетей Практические занятия 16 Лабораторные занятия 0 Самостоятельная работа 41  Раздел (модуль) 4. ЕВР-системы Лекции 3 Практические занятия 22 Лабораторные занятия 0 Самостоятельная работа 41  Содержание разделов дисциплины:  Раздел 1.1. Введение в теорию компиляции  Языковой процессор. Транслятор и компилятор. Структура компилятора: фазы анализа и синтеза. Лексический анализ, синтаксический анализ, семантический анализ, оптими- зация и генерация кода.  Темы лабораторных занятий. 1. Структура компилятора.  Раздел 1.2. Лексический анализ.  Основы лексического анализа. Регулярные множества и регулярные выражения. Ко- нечные распознаватели: детерминированные и недетерминированные. Переход от регуляр- ного выражения к НКА u or НКА к ДКА. Таблица переходов. Лексические ошибки.  Темы лекций: 1. Основы лексического анализа. Регулярные множества и регулярные выражения.  Темы лабораторных занятий. 2. Конечные распознаватели.  3. Регулярные выражения и конечные распознаватели.  Основы синтаксического анализа. Контекстно-свободные грамматики и языки. Мага- зинные автоматы. Связь КС-грамматик и магазинных автоматов. Дерево парсинга. Неоднозначные и леворекурсивные грамматики. Ассоциативность и приоритеты. Кор- рекция ошибок. Нисходящий анализ: рекурсивный спуск, нерекурсивный предиктив- ный анализ, LL(1)-rpammatuku. Восходящий анализ: основы, обрезка основ, стековая реализация, активные процессы, конфликты. Синтаксический анализ приоритета опе- раторов. [.В-анализаторы. Генераторы синтаксических анализаторов.  Темы лекций:  1. КС-грамматики и языки.  2. Магазинные автоматы.  3. Дерево парсинга. Неоднозначные и леворекурсивные грамматики.  4. Ошибки парсинга. Коррекция ошибок.  Темы лабораторных занятий. 5. Нисходящий анализ.  6. LL(1)-rpammartuxu.  7. Восходящий анализ  8. ГВ-анализаторы..  Раздел 1.4. Семантический анализ.  Системы типов. Эквивалентность выражений типа. Преобразование типов. Перегрузка функций и операторов. Полиморфные функции. Алгоритм унификации.  Раздел 2.1. Классификация структур данных. Анализ алгоритмов.  Содержание раздела. Введение. Основные понятия и определения алгоритмов и структур данных. Операции над структурами данных. Критерии эффективности алгоритмов. В ходе изучения данного раздела студенты знакомятся с принятой в англоязычной научной литературе терминологией из области алгоритмов и структур данных и изучают программные конструкции и алгоритмы, относящиеся к различным порядкам сложности.  Keywords: data structure, algorithm, linear and non linear data structure, big-O notation.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям:  — Безличные предложения при формировании технических отчетов.  — Формально-логический стиль в технических текстах. Логических связки “therefore”, “thus”, “so”, “so that”, “hence”, “consequently” при формировании технических отчетов.  2  22 Ge 2  Раздел 2.2. Поиск. Сортировка.  Содержание раздела: алгоритмы поиска: прямой поиск, бинарный поиск. Алгоритмы сортировки массивов: сортировка посредством выбора, сортировка вставками, сортировка обменом, быстрая сортировка. Сортировка последовательных файлов.  В процессе изучения данного раздела студенты знакомятся с терминологией, относя- щейся к представлению массивов в памяти компьютера, а так-же с задачами упорядочивания массивов и последовательных файлов.  Keywords: linear search, binary search, insertion, Srirction, Exchange sort, array. Sequential file.  Лабораторные работы:  1. Изучение открытых материалов конференций издательства «Зрипоег шк» (http://link.springer.com/). Пополнение словаря английскими терминами в области структур и алгоритм обработки данных по тематике «Сортировка и поиск». Перевод задания на лабора- торную работу 2 с русского на английский язык с использованием новых слов.  2. Реализация программного приложения в соответствии с вариантами заданий на языке C++ и формирование отчета по лабораторной работе. Пример задания. Реализовать приложение, которое сортирует заданную последовательность чисел с использованием указанного алгоритма сортировки.  Раздел 2.3. Линейные динамические списки.  Содержание раздела: связанные линейные списки: односвязный, двусвязный, цикли- ческий. Стеки, очереди, деки. Применение линейных динамических структур данных.  Задачей данного раздела является изучение лексикона, позволяющего описывать за- дачи, в которых используются динамические линейные структуры и выполняются действия над ними. В дисциплинарной области задачами студентов являются знакомство с структу- рами «стек» и «очередь», с программными способами задания динамических списков и алго- ритмами обработки данных структур.  Keywords: linear linked list, list building, traversing, node, circular list, doubly linked list, stack, queue.  Лабораторные работы:  Реализация программного приложения в соответствии с вариантами заданий на языке С++. По лабораторной работе формируется отчет, и лабораторная работа защищается устно с отчетом. Пример задания. Сформировать динамический список. Удалить из него все чет- ные элементы.  6  При защите лабораторной работы студенты устно обосновывают выбранный алгоритм и pa3- делы представленные в отчете, демонстрируют англоязычный интерфейс разработанного программного приложения и отвечают на вопросы по заданию.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям:  —Формально-логический стиль в технических текстах. Употребление наречий Also, Too, As Well, So, Either, Neither в технических отчетах и при защите лабораторной работы.  2&gt;  —Использование конструкций, позволяющих описать основу чего-либо “base оп”, “basis of’.  Темы лекционных занятий.  1. Системы типов.  Преобразование типов. Перегрузка функций и операторов. Полиморфные функции.  Алгоритм унификации.  RYN  Раздел 2.4. Графы, структуры для задания графов и алгоритмы их обработки.  Содержание раздела. Введение. Графы. Способы задания графов. Алгоритмы обхода графов. Оптимизационные алгоритмы: кратчайшие пути из заданной вершины во все другие вершины. Эйлеровы пути и циклы. Задача коммивояжера. Нахождение центра ориентиро- ванного графа.  В ходе изучения данного раздела студенты знакомятся с принятой в англоязычной научной литературе терминологией из области алгоритмов и структур данных и изучают программные конструкции и алгоритмы, позволяющие корректно задать граф, решить задачу нахождения кратчайшего пути в графе, найти центр графа, решить задачу коммивояжера.  Keywords: data structure, algorithm, graph, optimization, traveling salesman problem, Euler path, Euler loop, center of oriented graph, shortest path.  Лабораторные работы:  3. Изучение открытых материалов конференций издательства «Springerlink» (http://link.springer.com/). Пополнение словаря английскими терминами в области структур и алгоритм обработки данных по тематике «Графы». Перевод задания на лабораторную работу 2 с русского на английский язык с использованием новых слов.  4. Реализация программного приложения в соответствии с вариантами заданий на языке C# и формирование отчета по лабораторной работе. Пример задания. Реализовать приложение, которое позволяет пользователю задать граф (в оперативной памяти или в файле). Пользователь вводит вершину A, В и С. Найти кратчайший путь соединяющий вершину А и В, не проходящий через вершину С.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям:  —Безличные предложения при формировании технических отчетов.  —Формально-логический стиль в технических текстах. Логических связки “therefore”,  22 Ge  “thus”, “so”, “so that”, “hence”, “consequently” при формировании технических отчетов.  Раздел 2.5. Деревья.  Двоичные деревья. Деревья двоичного поиска. Операции обработки двоичных деревь-  7  ев. Сбалансированные, сильноветвящиеся деревья. Алгоритмы обхода деревьев. Сортировка данных при помощи деревьев двоичного поиска.  Задачей данного раздела является изучение лексикона, позволяющего описывать за- дачи, в которых используются древовидные структуры и выполняются действия над ними. В дисциплинарной области задачами студентов являются знакомство с структурой «дерево», с программными способами задания дерева и алгоритмами обработки данных структур.  Keywords: tree, binary trees, trees processing algorithms, much-branched trees, traverse, preorder traverse, in order traverse, post order traverse . Текущий контроль:  Студентам в устной форме дается задание, текст задания дублируется на слайдах на англий- ском языке и выдается материал для выполнения задания на английском языке (презента- ция). Студенты с использованием выданного материала, а также любых англоязычных мате- риалов выполняют задание. При выполнении задания студенты снабжают этапы выполнения задания соответствующими подписями на английском языке. Примеры заданий. 1. Привести пример двоичного дерева поиска (не менее 10 узлов) выполнить прямой обход дерева, обратный обход дерева, симметричный обход дерева. Указать для каждого случая последовательность вершин при обходе.  Лабораторные работы:  Реализация программного приложения в соответствии с вариантами заданий на языке C#. По лабораторной работе формируется отчет, и лабораторная работа защищается устно с отчетом. Пример задания. Построить двоичное дерево поиска из целых чисел. Удалить из него элементы, встречающиеся несколько раз. Результат вывести на экран. Определить глубину дерева OO и после удаления. При защите лабораторной работы студенты устно обосновывают выбранный алгоритм и раз- делы представленные в отчете, демонстрируют англоязычный интерфейс разработанного программного приложения и отвечают на вопросы по заданию.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям:  —Формально-логический стиль в технических текстах. Употребление наречий Also, Too, As Well, So, Either, Neither в технических отчетах и при защите лабораторной работы.  &gt;  —Использование кон кций, позволяющих описать основу чего-либо “base on’, “basis of’. 2  Раздел 3.1. Использование графов и алгоритмов их обработки для анализа социальных сетей.  Лабораторная работа. Реализация программного веб-приложения обрабатывающего данные из социаль- ных сетей, выполняющее визуализацию данных из социальных сетей, решение задачи “Кеу players problem NEG”  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям: — Формально-логический стиль в технических текстах. Изучение чтения сложных формул. Функции, операторы суммирования, интегралы. — Использование конструкций, позволяющих описать графически представленные дан- ные в виде функций и т.д. “with respect to”.  Раздел 3.2. Параллельная обработка данных.  В ходе изучения данного раздела студенты знакомятся с использованием параллель- ной обработкой данных на центральном процессоре при программировании алгорит- мов обработки графов и деревьев. В данном разделе студенты знакомятся с англо- язычными терминами касающиеся параллельной обработки данных. Также, студен- там необходимо продемонстрировать навыки использования лексикона, накопленного при изучении предыдущих разделов.  Keywords: threading, central processing unit, background worker, multitasking algorithms, paral- lelizing.  Лабораторные работы:  1. Программная реализация оптимизационных алгоритмов обработки графов с ис- пользованием параллельной обработки данных. Реализация на языке С#. Пример лабора- торной работы: Усовершенствовать приложение из лабораторной работы раздела 2 и выполнить параллельную реализацию используемых алгоритмов на центральном процессо-  ре.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям:  — Формально-логический стиль в технических текстах. Построение предложений claus- es of result (as a result, therefore, consequently) в технических отчетах и при защите лабора- торной работы.  — Формально-логический стиль в технических текстах. Построение предложений Claus- es of reason (since, the reason Юг, due to) в технических отчетах и при защите лабораторной работы.  Раздел 3.3. Алгоритмы кластеризации данных.  В ходе изучения данного раздела студенты знакомятся с проблемой кластеризацией данных и алгоритмами кластеризации данных. На практике используются графовые алго- ритмы кластеризации данных, основанные на построении минимального основного дерева Студентам необходимо продемонстрировать навыки использования лексикона, накопленного при изучении предыдущих разделов  Keywords: cclustering analysis, Euclidean distance , Prims algorithm, Kruskal algorithm, k- means algorithm.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям: — Формально-логический стиль в технических текстах. Построение предложений связан- ных со сравнением данных. Использование конструкций Like/As.  — Высказывание предложений по использованию какого-либо метода, алгоритма решения задачи и т.д. (Propose, Suggest).  Раздел 3.4. Алгоритмы нечетких множеств при анализе социальных сетей.  В ходе изучения данного раздела студенты знакомятся с основами нечетких множеств, а также алгоритмов на основе использования нечетких множеств для анализа данных из CO- циальных сетей. Студентам необходимо продемонстрировать навыки использования лекси- кона, накопленного при изучении предыдущих разделов  9 Лабораторная работа. Реализация программного веб-приложения обрабатывающего данные из социаль- ных сетей, выполняющее кластеризацию данных из социальных сетейна основе нечеткого алгоритма кластеризации.  В части английского языка студенты получают практические навыки использования ино- странного (английского) языка в будущей профессиональной деятельности по направлениям: — “ Формально-логический стиль в технических текстах. Построение предложений описы- вающих возможности используемых алгоритмов, методов и разработанных приложений (Al- low, may, can, able to)  Раздел 4.1. Введение.  Корпоративная информационная системы. Системы управления ресурсами предприя- тия (ERP). История развития систем управления ресурсами предприятия. Отличие ERP си- стем от КИС. Типовые модули корпоративных систем, их назначение.  В ходе изучения данного раздела студенты знакомятся с принятой в англоязычной научной литературе терминологией, связанной с областью разработки и эксплуатации кор- поративных информационных систем и изучают историю развития корпоративных инфор- мационных систем, историю появления систем управления ресурсами предприятия и отли- чие данной группы систем от КИС.  Keywords: corporate information system; enterprise resource planning system; module, history of ERP.  Раздел 4.2. Архитектура предприятия.  Бизнес-приложение. Необходимость разработки бизнес-приложений в рамках КИС. Этапы разработки бизнес-приложений. Методы принятия решения при проектировании биз- нес-проиложения в КИС. Классификация методов принятия решения. Экспертные методы принятия решения, их назначение, в том числе метод анализа иерархий, метод Делфи.  Данный раздел направлен на изучение лексикона, позволяющего описывать задачи, связанные с проектированием и разработкой бизнес-приложений, в том числе, задачи анали- за предметной области, процессов. В дисциплинарной области задачами студентов является знакомство с понятиями архитектура предприятия, бизнес-приложение, изучение типового процесса разработки бизнес-приложения, этапов разработки приложения, использование ме- тодов экспертных на этапе анализа предметной области при проектировании бизнес- приложения.  Keywords: enterprise architecture; business application; stages business applications develop- ment; expert methods of decision; hierarchy analysis method; Delphi method;  Лабораторные работы: 1. С использованием метода анализа иерархий выбрать альтернативный вариант про- граммного бизнес-решения исходя из заданных исходных условий.  Раздел 4.3. Платформа 1С:Предприятие.  Архитектура платформы. Тонкий, толстый, веб клиент их отличия. Командный ин- терфейс. Метаданные. Настройка командного интерфейса.  При изучении данного раздела студенты знакомятся с лексиконом связанных с описа- нием архитектуры корпоративной информационной системы на примере платформы 1С.Предприятия и конфигураций КИС, разработанных на данной платформе, в том числе изучение лексикона, относящегося к интерфейсу бизнес-приложения В дисциплинарной об-  10 ласти задачами студентов являются изучение архитектуры платформы 1С:Предприятие и настройки командного интерфейса в рамках конфигурации на базе данной платформы.  Keywords: Platform 1C: Enterprise; Architecture; Thin client; thick client; web-client; command interface; Metadata; interface. Лабораторные работы:  1. Реализация бизнес-приложения, содержащего справочники, константы и докумен- ты и настройка командного интерфейса для различных пользователей.  Раздел 4.4. Инструменты, используемые для оптимизации клиент-серверного взаимодействия для бизнес-приложений на базе платформы 1С:Предприятие.  Показатели производительности. Объединение нескольких вызовов сервера в один. Использование внеконтекстных серверных процедур в модуле формы.  Данный раздел направлен на изучение лексикона, позволяющего описывать задачи оптимизации клиент-серверного взаимодействия для бизнес-приложений на примере приложений. Созданных на базе платформы 1С:Предприяятие. В дисциплинарной об- ласти студенты изучают возможности повышения показателей производительности путем объединения нескольких вызовов сервера в один, использования внекон- текстных серверных процедур в модуле формы и др.  Keywords: client-server interaction optimization; business applications; 1C: Enterprise; multiple server calls; server-context procedures; form module.  Лабораторные работы:  2. Реализация бизнес-приложения, в котором при разработке формы (любой) необхо- димо решить задачу получения дополнительной информации об объекте и отображения этой информации в реквизитах формы.  3. Реализация бизнес-приложения, в котором рассматриваются случаи создания вне- контекстных серверных процедур.  6.</t>
+  </si>
+  <si>
+    <t>Содержание этапов реализации дисциплины:  № Этапы реализации дисциплиньь и  семестра краткое содержание (виды работ) ЕЕ  5 Подготовительный этап: РД1 — Выбор темы и обоснование необходимости решения за-дачи. Определение целей и РД4 задач. Формирование программы. Выбор программного обеспечения, средств разработки и т.д. Подготовка отчета и выступление с докладом в виде презентации по результатам работы.  6 Научно-исследовательская и/или проектная работа: РД1 — Изучение литературы. Сбор, обработка данных и обобщение данных. Объяснение РДЗ полученных результатов и новых фактов. Проектирование архитектуры приложения, РД4 информационной системы, разработка алгоритмов и т.д. Формулировка выводов. Подготовка отчета и выступление с докладом в виде презентации по результатам работы.  7 Научно-исследовательская и/или проектная работа.: РД? — Программная реализация и тестирование проекта. Проведение исследования РДЗ разработанных алгоритмов. Обработка новых данных. Подготовка отчета и РД4 выступление с докладом в виде презентации по результатам работы.  8 Заключительный этап: РДЗ — Изучение нормативных требований, формирование структуры и содержания отчёта о РД4 результатах исследования. Написание, редактирование, формирование списка использованных источников информации, оформление приложений. Подготовка заключительного отчета и выступление с докладом в виде презентации по результатам исследований.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности Формируемый Разделы дисциплины  бучения по Виды учебной деятельности ин а. дисциплине Лекции 2 Раздел 1. Цепи с постоянными РД-1, РД-2,  Практические занятия 4 напряжениями и токами РД-3 Лабораторные занятия 2 Самостоятельная работа 10 Лекции 2 Раздел 2. Однофазные цепи переменного РД-1, РД-2,  Практические занятия 6 тока РД-3 Лабораторные занятия 4 Самостоятельная работа 10 Лекции 2 Раздел 3. Переходные процессы в РД-1, РД-2,  Практические занятия 4 линейных электрических цепях РД-3 Лабораторные занятия 2 Самостоятельная работа 8 Лекции 2 Раздел 4. Трехфазные цепи РД-1, РД-2, Практические занятия 2 РД-3 Лабораторные занятия 2 Самостоятельная работа 8 РД-1.РД-2, Лекции 2 Раздел 5. Трансформаторы РД Лабораторные занятия 2 Самостоятельная работа 6 РД-1.РД-2, Лекции 2 Раздел 6. Асинхронные машины РД Лабораторные занятия 2 Самостоятельная работа 6 Раздел 7. Синхронные машины РД. РД-2,  Лекции 2 РД-3 Самостоятельная работа 6 РД-1.РД-2. Лекции 2 Раздел 8. Машины постоянного тока РД-3 Лабораторные занятия 2 Самостоятельная работа 6  Содержание разделов дисциплины:  Раздел 1. Цепи с постоянными напряжениями и токами  Основные элементы и законы электрических цепей. Источники ЭДС и тока. Схемы замещения электрических цепей. Резистивные элементы схем замещения. Основные топологические понятия для схем замещения электрических цепей: ветвь, узел, контур, граф. Постоянные токи и напряжения. Выбор положительных направлений токов и напряжений. Закон Ома. Первый и второй законы Кирхгофа. Методы расчета электрических цепей: метод контурных токов, метод двух узлов, метод эквивалентного генератора, метод наложения, Теорема Телледжена. Баланс мощности в резистивных цепях.  Темы лекций:  1. Электрические цепи постоянного тока  Темы практических занятий:  1. Методы расчета цепей постоянного тока (метод законов Кирхгофа, метод двух узлов)  2. Метод эквивалентного генератора  Названия лабораторных работ:  1. Исследование линейной электрической цепи постоянного тока  Раздел 2. Однофазные цепи переменного тока  Гармонические токи и напряжения. Промышленная частота. Постоянный ток как частный случай гармонического тока. Действующие значения гармонических величин. Символический метод. Топографические и лучевые векторные диаграммы. Резонанс. Несинусоидальные сигналы. Разложение в ряд Фурье.  Темы лекций:  2. Однофазные цепи переменного тока  Темы практических занятий:  3. Символический метод  4. Методы расчета цепей переменного тока  5. Резонанс в линейных цепях  Названия лабораторных работ:  2. Конденсатор и катушка индуктивности в цепи переменного тока  3. Резонанс напряжений  Раздел 3. Переходные процессы в линейных электрических цепях  Законы коммутации. Условия возникновения переходных процессов. Линейные дифференциальные уравнения. Методы расчета переходных процессов.  Темы лекций:  3. Переходные процессы в линейных электрических цепях  Темы практических занятий:  6. Определение независимых и зависимых начальных условий  7. Расчет переходных процессов в линейных цепях при постоянных и гармонических напряжениях и токах  Названия лабораторных работ:  4. Исследование переходных процессов в цепи первого порядка  Раздел 4. Трехфазные цепи  Трехфазные цепи. Соединения обмоток генераторов и трансформаторов. Симметричный и несимметричный режим трехфазных цепей. Вращающееся магнитное поле.  Темы лекций:  4. Трехфазные цепи  Темы практических занятий:  8. Расчет трехфазных цепей при гармонических напряжениях и токах  Названия лабораторных работ:  5. Исследование трехфазной цепи, соединенной “звездой”  4  Раздел 5. Трансформаторы Однофазный, трехфазный и специальные трансформаторы. Назначение, устройство, принцип действия, «Г»- и «Т»- образные схемы замещения и их параметры. Режимы и опыты холостого хода и короткого замыкания. Темы лекций: 5. Трансформаторы в установившемся режиме Названия лабораторных работ: 6. Исследование трансформатора в линейном режиме Раздел 6. Асинхронные машины Асинхронные машины. Устройство, принцип действия и область применения. Режимы работы асинхронных машин. Пуск в ход асинхронных двигателей. Методы регулирования частоты вращения асинхронных двигателей. Основные характеристики асинхронных машин. Потери энергии и КПД асинхронных машин. Темы лекций: 6. Асинхронные машины Названия лабораторных работ: 7. _ Исследование асинхронного двигателя Раздел 7. Синхронные машины Синхронные машины. Устройство и принцип действия. Режимы работы синхронных машин. Основные характеристики синхронных машин. Потери энергии и КПД синхронных машин. Темы лекций: 7. Синхронные машины Машины постоянного тока, их устройство, принцип действия и область применения. Режимы работы машин постоянного тока. Основные характеристики машин постоянного тока. Потери энергии и КПД машин постоянного тока. Темы лекций: 8 Машины постоянного тока Названия лабораторных работ: 8. Исследование машины постоянного тока в двигательном и генераторном режиме  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности и a дисциплине Лекции 4 Раздел 1. Введение РД1 Лабораторные занятия 6 Самостоятельная работа 12 Лекции 4 Раздел 2. Основы проектирования БД РД? Лабораторные занятия 6 Самостоятельная работа 12 Раздел 3. Реляционная модель данных Лекции 6 ДЕЛ &gt;. ECT дель д РДЗ, РД4 Лабораторные занятия 6 (РМД)  Самостоятельная работа 20 Лекции 4 aman т SQL и РДЗ, РД4 Лабораторные занятия 8 трир Самостоятельная работа 20 Лекции 6 Раздел 5. Технологии разработки РД5. РДб Лабораторные занятия 6  корпоративных ИС Самостоятельная работа 20  Содержание разделов дисциплины: Раздел 1. Введение  Предмет курса. Понятия: данные, информация, информационные система, данные, знания, база данных, СУБД. Классификация информационных систем. Функции СУБД. Назначение и место БД и СУБД в информационных системах.  Темы лекций:  1. Основные понятия  2. Функции СУБД  Названия лабораторных работ:  1. Изучение инструментария Microsoft SQL Server.  Раздел 2. Основы проектирования БД  Архитектура системы баз данных. Этапы проектирования баз данных. Концептуальная (инфологическая) модель. Модель «сущность-связь». Классификация бинарных связей. Логическое проектирование и модели данных. САЗЕ-средства для концептуального и логического проектирования.  Темы лекций:  Модели данных  Схема Бахмана. Этапы проектирования баз данных. Концептуальное моделирование. Модель «сущность-связь». Модели данных и логическое проектирование.  7. Физическое проектирование.САЗЕ-средства для концептуального и логического проектирования.  Названия лабораторных работ:  2. Проектирование БД при помощи Toad Data Modeler.  Раздел 3. Реляционная модель данных (РМД)  Структурный аспект РМД. Аспект манипуляции: реляционная алгебра и реляционное исчисление. Ограничения целостности: потенциальные, первичные, альтернативные, внешние ключи. Нормальные формы.  Темы лекций:  8. Структурный аспект РМД: домен, кортеж, отношение, переменная отношения.  9. Аспект манипуляции: реляционная алгебра и реляционное исчисление.  пмьз  10. Ограничения целостности: потенциальные, первичные, альтернативные, внешние ключи.  11. Нормальные формы (НФ): функциональная зависимость (ФЗ), 1НФ, 2НФ, ЗНФ, НФ Бойса-Кодда.  12. Нормальные формы: многозначная ФЗ, зависимость соединения. 4НФ и 5НФ.  Названия лабораторных работ:  3. Написание DML запросов на языке SQL.  4. Написание DDL запросов на языке SQL.  Раздел 4. Основы языка SQL и администрирование БД  Операторы SELECT, INSERT, UPDATE, DELETE. Виды соединений. Запросы с группировкой. Представления, хранимые процедуры и функции. Настройка доступа к данным и объектам БД. Средства администрирования БД в современных СУБД.  Темы лекций:  13. Основные возможности SQL.  14. Администрирование БД и разграничения прав доступа.  Названия лабораторных работ:  5. Администрирование БД под управлением Microsoft SQL Server.  Раздел 5. Технологии разработки корпоративных ИС  Инструменты разработки \УеБ-приложений баз данных. Шаблон проектирования Model-View-Controller. Основы разработки \уеб-приложений. ОКМ-фреймворки.  Темы лекций:  15. Основы разработки \’еБ-приложений.  16. Шаблон проектирования MVC и фреймворк ASP.NET MVC.  17. ОКМ-фреймворки. Entity Framework.  Названия лабораторных работ:  6. Написание приложения на фреймворке АЗР.МЕТ МУС по индивидуальному заданию.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины ни Виды учебной деятельности Обьем учения по времени, ч. дисциплине Лекции - Практические занятия 8 Раздел 1. Когнитивная эргономика  И.ОПК(У)-6.2 P Лабораторные занятия - Самостоятельная работа 10 Лекции - Раздел 2. Дизайн и эргономика И. ОПКС-62 Практические занятия 8 цифровых продуктов ° : Лабораторные занятия - Самостоятельная работа 10  Содержание разделов дисциплины:  Раздел 1. Когнитивная эргономика  Общие понятие когнитивной эргономики и ее особенности, влияющие на характеристики дизайн проектирования и визуальное восприятие продуктов дизайна.  Темы лекций:  1. Понятие о когнитивной эргономике. Ошибки оператора и надежность. Когнитивная нагрузка.  2. Модели переработки информации человеком. Методы когнитивного анализа задач.  3. Когнитивный анализ задач. Дизайн, ориентированный на пользователя.  4. Эргономическая программа проектирования интерфейсов.  5. Эргономика в инклюзивном дизайне.  Темы практических занятий:  1. Проектирование, основанное на эргономике восприятия.  2. Психологические особенности целевой аудитории и восприятие продуктов дизайна.  3. Композиция и восприятие, точки фокуса.  4. Исследование особенностей визуального восприятия.  5. Исследование взаимосвязи психологических законов и восприятия.  Раздел 2. Дизайн и эргономика цифровых продуктов  Исследование особенностей дизайна современной цифровой среды. Темы лекций:  1. Эргономический анализ цифровой среды.  2. Целевая аудитория.  3. Цифровизация образования, особенности проектирования. Темы практических занятий:  1. Исследование целевой аудитории.  2. Визуальный дизайн интерфейсов.  3. Дизайн и эргономика цифровой образовательной среды  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения о Виды учебной деятельности времени, 4. дисциплине Раздел 1. Основные понятия языка РД! Лекции 4 программирования Python Самостоятельная работа 26 Лекции 4 Раздел 2. Операто исвоения, операто аи ратор пр ‚ оператор РД1 Лабораторные занятия 8 if, циклы, итерации и включения Самостоятельная работа 26 Лекции 4 Раздел 3. Функции РД1 Лабораторные занятия 8 Самостоятельная работа 26 Лекции 4 Раздел 4. Области видимости РД1 Лабораторные занятия 8 Самостоятельная работа 26 Содержание разделов дисциплины: Раздел 1. Основные понятия языка программирования Python  Введение. Базовые концепции, необходимые для написания программ на языке Python. Типы данных и операции. Темы лекций: 1. 1. Основные понятия языка программирования Python, типы объектов, числовые типы, динамическая типизация, строки, списки и словари, кортежи, файлы. Операторы и синтаксис. Темы лекций: 2. Оператор присвоения, оператор if, циклы, Итерации и включения. Названия лабораторных работ: 1. Первая программа на Python. Раздел 3. Функции Функции и генераторы. Темы лекций: 3. Функции. Названия лабораторных работ: 2. Работа с одномерным массивом. 3. Двумерные массивы. Раздел 4. Области видимости Области видимости: - глобальная, локальная, нелокальная. Темы лекций: 4. 4. Области видимости. Названия лабораторных работ:  4. Функции. 5. Словари и файлы. 6. Рекурсия.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обуче 7 Виды учебной деятельности времени, 4. дисциплине Лекции 6 Раздел 1. Разработка модели бизнес-плана РД-1 Лабораторные занятия 8 проекта Самостоятельная работа 31 Раздел 2. Моделирование бизнес- Лекции 6 процессов средствами информационных РД-2 Лабораторные занятия 8 технологий Самостоятельная работа 31 Лекции 6 Раздел 3. Оптимизация финансовых .. РД-3 Лабораторные занятия 8 показателей проекта развития бизнеса Самостоятельная работа 31 Раздел 4. Обеспечение на основе Лекции 6 аналитической обработки данных и РД-4 Лабораторные занятия 8 информационной безопасности проекта Самостоятельная работа 31  Содержание разделов дисциплины:  Раздел 1. Разработка модели бизнес-плана проекта  Рассматриваются концепции ВРМ и даются определения таких ключевых понятий, как сквозной процесс, ценность для потребителя, кросс-функциональная работа. Также рассматриваются типы процессов, компоненты процессы, жизненный цикл ВРМ. Этот раздел дает определение BPM и закладывает фундамент для остальных разделов.  Темы лекций:  1. Введение в ВРМ. ВРМ - управленческая дисциплина  Названия лабораторных работ:  1. Выбор процесса, его описание, схема ВРММ  2. Проектирование пользовательских интерфейсов  Раздел 2. Моделирование бизнес-процессов средствами информационных технологий  В данном разделе формируется понимание целей и эффекта моделирования процессов, рассматриваются типы процессных моделей и варианты их использования, описываются средства, методы и стандарты моделирования. Также в данном разделе рассматриваются цели анализа процессов, подходы к декомпозиции процессов и методы анализа, включая такие аспекты как роли, рамки, бизнес-контекст, правила и показатели эффективности. И также в данном разделе рассматриваются принципы правильного проектирования процессов, роли, методики, а также такие общие аспекты как участие высшего руководства, соответствие нормативным требованиям и стратегии.  Темы лекций:  2. Введение в моделирование бизнес-процессов. Основные процессные нотации.  3. Уровни процессных моделей. Фреймворки и референтные модели.  4. Анализ процессов. Роли участников анализа процессов.  5. Подготовка к анализу процессов. Проведение анализа. Рекомендации по результатам анализа.  6. Основы проектирования процессов. Выявление процесса «как есть» или «текущее состояние». Проектирование процессов и потоков работ — модель «как будет».  Названия лабораторных работ:  3. Создание модели данных процесса Создание экранных форм Настройка правил переходов Запуск и отладка процесса  © м &gt;  Раздел 3. Оптимизация финансовых показателей проекта развития бизнеса  В данном разделе изучается значение и эффект таких аспектов, как измерение эффективности, определение ключевых показателей эффективности, мониторинг и контроль операций, увязывание эффективности процессов с эффективностью организации в целом. Также рассматриваются объекты и методы измерения, имитационное моделирование, поддержка принятия решений, факторы успеха.  Темы лекций:  7. Что такое управление эффективностью процесса? Что такое эффективность процесса?  8. Измерение и управление. Развитие способности измерять эффективность. Ключевые определения эффективности процессов.  9. Выстраивание бизнес-процессов исходя из эффективности предприятия.  10. Фреймворк зрелости управления эффективностью процессов.  Названия лабораторных работ:  7. Контроль и мониторинг процесса  8. Улучшение процесса  Раздел 4. Обеспечение на основе аналитической обработки данных и информационной безопасности проекта  В данном разделе рассматривается широкий спектр существующих технологий, обеспечивающих планирование, проектирование, анализ, исполнение и мониторинг бизнес- процессов. Здесь рассмотрены пакеты прикладных программ, средств разработки, инфраструктурные компоненты, хранилища данных и информации, обеспечивающие связанную с ВРМ деятельность. Рассматриваются интегрированные системы управления бизнес-процессами (BPMS) процессные репозитарии, а также изолированные средства моделирования, анализа, проектирования, исполнения и мониторинга. Также рассказывается о стандартах, методологиях и новых трендах ВРМ.  Темы лекций:  11. Эволюция технологий ВРМ. Возможности технологий ВРМ. Эффект от технологий ВРМ.  12. Взгляд в будущее технологий ВРМ. Преимущества и риски автоматизации процессов.  Названия лабораторных работ:  9. Разработка веб-сервиса  10. Интеграция веб-сервис с процессом  11. Разработка автоматизированного робота с помощью технологии RPA  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине Раздел 1. РД1 Лекции 2 Теоретические, правовые, РД? Практические занятия 4 нормативные и Лабораторные занятия 2 организационные основы Самостоятельная работа 14 обеспечения БЖД Раздел 2. РД1 Лекции 2 Производственная санитария Практические занятия 4 Лабораторные занятия 8 Самостоятельная работа 14 Раздел 3. РД1 Лекции 4 Техника безопасности Практические занятия 2 Лабораторные занятия 6 Самостоятельная работа 10 Раздел 4. РД? Лекции 0 Безопасность в чрезвычайных Практические занятия 4 ситуациях мирного и военного Лабораторные занятия 0 времени Самостоятельная работа 15 Раздел 5. Экологическая РДЗ Лекции 0 безопасность Практические занятия 2 Лабораторные занятия 0 Самостоятельная работа 15  Содержание разделов дисциплины:  Раздел 1. Теоретические, правовые, нормативные и организационные основы обеспечения БЖД  Цель и содержание курса БЖД, его комплексный характер. Основные задачи курса.  Среда обитания человека. Понятие опасности. Аксиома о потенциальной опасности. Опасные и вредные факторы: классификация. Критерии безопасности и комфортности. Понятие, классификация и характеристика видов риска. Количественные показатели. Концепция приемлемого риска. Вопросы БЖД в законах и подзаконных актах.  Травматизм и профессиональные заболевания, методы анализа. Несчастные случаи. Первая помощь. Ответственность работодателей.  Трудовое законодательство. Подзаконные акты по охране труда. Нормативно-техническая документация. Инструкции по охране труда. Система стандартов безопасности труда (ССБТ).  Управление охраной труда. Система управления охраной труда. Обучение безопасности труда, виды инструктажа.  Темы лекций: 1.Теоретические основы безопасности жизнедеятельности. Темы практических занятий: 1.Идентификация опасных и вредных факторов. 2.Расследование несчастного случая. Названия лабораторных работ: Оказание первой помощи.  Раздел 2. Производственная санитария  Вредные вещества. Производственный микроклимат, освещение. Акустические и  механические колебания. Ионизирующие излучения.  Источники, действие на организм человека, основные характеристики, классификация, нормирование, мероприятия по уменьшению, средства защиты: коллективные и индивидуальные. Расчет параметров.  Электромагнитные поля (ЭМП) и излучения. Лазерные излучения. Действие ИК-излучения, УФ-излучения. Нормирование ЭМП и излучений. Защита от ЭМП.  Обеспечение безопасности при работе с компьютером.  Темы лекций: 1.Производственный микроклимат, освещение.  Темы практических занятий: 1.Расчет потребного воздухообмена. 2.Расчет искусственного освещения.  Названия лабораторных работ: 1. Исследование микроклимата производственных помещений. 2. Исследование шумов в производственных помещениях. 3. Исследование вибрации и способов защиты от нее. 4. Исследование эффективности и качества искусственного освещения.  Раздел 3. Техника безопасности  Пожаровзрывоопасность. Физико-химические основы горения. Причины пожаров, классификация. Опасные факторы. Показатели пожаровзрывоопасности. Классификация зданий и помещений. Основные мероприятия по профилактике. Огнестойкость. Пути эвакуации. Способы и средства тушения. Первичные средства пожаротушения. Средства пожарной автоматики и сигнализации.  Электробезопасность. Действие электрического тока. Влияние факторов. Классификация помещений по опасности поражения. Статическое электричество. Мероприятия повышения безопасности. Технические средства защиты.  Требования к безопасной эксплуатации сосудов и систем, работающих под давлением. Регистрация и техническое освидетельствование. Безопасность автоматизированного и роботизированного производства.  Темы лекций: 1.Пожаровзрывоопасность. 2.Электробезопасность.  Темы практических занятий: 1.Расчет молниезащитных зон зданий и сооружений.  Названия лабораторных работ: 1.Исследование сопротивления тела человека. 2.Электробезопасность в жилых и офисных помещениях. 3.Пожарная безопасность.  Раздел 4. Безопасность в чрезвычайных ситуациях мирного и военного времени  Классификация и общая характеристика чрезвычайных ситуаций (ЧС) военного и мирного времени. Устойчивость производственных объектов в условиях ЧС и военных конфликтов. Организация и методика исследования устойчивости функционирования, методы и средства повышения устойчивости предприятий. Защита производственного персонала.  Оценка обстановки. Определение параметров очага поражения. Приёмы и способы проведения спасательных работ. Защита и эвакуация населения. Использование защитных сооружений, СИЗ и медицинских средств.  Ликвидация последствий ЧС. Состав спасательных и других неотложных работ. Организация работ по обеззараживанию. Разработка плана ремонтно-восстановительных работ. Региональные особенности возникновения ЧС. Наиболее характерные природные стихийные явления в Томской области. Потенциально опасные техногенные объекты ТО.  Темы практических занятий: 1.Оценка очагов поражения в ЧС. 2.Оценка радиационной обстановки.  Раздел 5. Экологическая безопасность  Источники загрязнения, опасные и вредные факторы окружающей среды. Виды негативного воздействия производственной сферы на биосферу, промышленные выбросы, твёрдые и жидкие отходы, энергетические загрязнения, аварии и катастрофы.  Классификация, основы применения экобиозащитной техники. Определение ПДВ. Аппараты и системы очистки выбросов. Расчёт, конструирование систем и аппаратов. Рассеивание выбросов в атмосфере.  Рациональное водопользование, устройства для очистки жидких отходов. Расчёт выпусков жидких отходов. Очистка сточных вод.  Сброс, утилизация, захоронение твёрдых и жидких промышленных отходов. Радиоактивные отходы. Вторичные ресурсы. Малоотходные технологии и производства.  Темы практических занятий: 1.Расчет рассеивания загрязняющих веществ в атмосферном воздухе.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности Формируемый . 06 Разделы дисциплины  бучения по Виды учебной деятельности  премени, a. дисциплине Раздел 1. Инженер - это... (особенности инженерной РД-1, РД-2  Практические занятия 4 деятельности) РД-1, РД-2 Раздел 2. Найти идею ? Практические занятия 4 ^ a РД-3.РД-4  Р Раздел 3. Проект и команда проекта РД-2, РД-3  Практические занятия 4 Раздел 4. Ресурсы проекта РД-2, РД-3  Практические занятия 4  Раздел 5. Практический блок: Практические занятия 16  " " Р -l, Р -2 Я умею д д Самостоятельная работа 4  Содержание разделов дисциплины  Раздел 1. Инженер — это ... (особенности инженерной деятельности)  Темы практических занятий (практикум, деловая игра, дискуссия, тренинг):  1.1. Портрет современного инженера  1.2. Задачи современного инженера  1.3. Место проекта в деятельности инженера 1.4. Проектная деятельность в ТПУ  Раздел 2. Найти идею  Темы практических занятий (мастер-класс, деловая игра, тренинг, кейс-задание):  2.1. Изобретение VS инновация 2.2. Какой метод выбрать? 2.3. Решаем задачи — это проект?   Раздел 3. Проект и команда проекта  Темы практических занятий (деловая игра, тренинг):  3.1. Цели и задачи проекта  3.2. Этапы выполнения проекта (инициация, планирование, исполнение, заверше- ние)  3.3. Виды проектов (научно-исследовательский, инженерный, предприниматель- ский, организационный, социальный)  3.4. Команда проекта. Коммуникация в проекте. Функциональные и профессио- нальные роли в команде. Ответственность лидера и руководителя проекта  Раздел 4. Ресурсы проекта  4.1. Инфраструктура проектной деятельности в ТПУ. 4.2. Проекты OMT.  Раздел 5. Практический блок: "Я умею"  Темы минипроектов:  1. Анимация в Blender  2. Разработка гиперказуальной игры 3. Чат-бот  4. RPA  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине Раздел 1. Основные понятия РД1 Лекции 4 информатики и информации. Лабораторные занятия 4 Архитектура современных аппаратно-программных Самостоятельная 8 средств работа Раздел 2. Алгоритмы и Лекции 4 проектирование Лабораторные занятия 8 информационных систем Самостоятельная работа 16 Раздел 3. Основы Лекции 4 программирования на языке С# Лабораторные занятия 12 Самостоятельная 24 работа Раздел 4. Хранение и передача Лекции 2 данных Лабораторные занятия 4 Самостоятельная 6 работа Раздел 5. Информационное Лекции 2 общество Лабораторные занятия 4 Самостоятельная 6 работа  Содержание разделов дисциплины:  Раздел 1. Основные понятия информатики и информации. Архитектура современных аппаратно-программных средств  Терминология информатики. Объект и предмет информатики. Приоритетные направления информатики. Информация. Свойства информации. Сбор и хранение  информации. Обработка и  передача  информации. Системы  Представление информации в компьютере. Классификация компьютеров, основы построения и архитектура. Тенденции развития вычислительных систем. Классификация программного обеспечения (ПО).  Системное и прикладное ПО. Темы лекций:  1. Основные понятия информатики и информации.  2. Архитектура современных аппаратно-программных средств.  Названия лабораторных работ:  1. Изучение среды разработки Microsoft Visual Studio. Разработка и отладка простого оконного приложения.  2. Разработка приложения, реализующего линейный алгоритм.  счисления.  Раздел 2. Алгоритмы и проектирование информационных систем  Основные понятия теории алгоритмов. Характеристики алгоритмов. Схемы алгоритмов и программ. Сложность алгоритмов и вычислительные проблемы.  Понятие информационной системы (ИС). Классификация ИС. Стратегии и методы проектирования программного обеспечения (ПО). Основные принципы программирования. Этапы решения задач с помощью компьютера. Основные этапы разработки программ. Отладка и тестирование программ. Языки программирования. Средства программирования.  Темы лекций:  1. Алгоритмы.  2. Проектирование информационных систем.  Названия лабораторных работ:  1. Разработка приложения, реализующего разветвляющийся алгоритм.  2. Разработка приложения, реализующего циклический алгоритм.  3. Разработка приложения для динамического создания объектов в окне  пользователя. 4. Разработка приложения, реализующего работу со строками.  Раздел 3. Основы программирования на языке С#  Основные понятия И принципы объектно-ориентированного программирования. Переменные элементарных типов, объявление и инициализация. Операции и выражения. Приоритет операций. Приведение типов. Управляющие операторы. Методы. Создание объекта. Операция new. Объявление и инициализация массивов. Одномерные и многомерные массивы.  Темы лекций: 1. Основные понятия И принципы объектно-ориентированного программирования. 2. Основы программирования на языке C#. Названия лабораторных работ: 1. Разработка приложения для работы с одномерными массивами. 2. Разработка приложения для работы с многомерными массивами. 3. Разработка приложения для построения на экране графика заданной функции. 4. Разработка приложения для построения на экране различных графических примитивов. Разработка приложения для вывода на экран анимационного изображения. 6. Разработка приложения для обработки изображений.  nn  Раздел 4. Хранение и передача данных  Понятие телекоммуникации. Способы коммутации и передачи данных. Типы каналов связи. Принципы построения и классификация компьютерных сетей. Понятие топологии сети. Основные виды адресаций, используемых в компьютерных сетях. Коммуникационное оборудование, применяемое в компьютерных сетях.  Хранение информации в классических базах данных и современных распределенных системах на основе блокчейн.  Темы лекций:  1. Хранение и передача данных  Названия лабораторных работ:  1. Разработка приложения с использованием методов.  2. Разработка приложения с использованием алгоритмов сортировки и  поиска.  Раздел 5. Информационное общество  Информационная безопасность. Цифровая экономика. Системы умного дома и города. Информационная инфраструктура. Темы лекций: 1. Информационное общество Названия лабораторных работ: 1. Разработка приложения с использованием рекурсии. 2. Разработка приложения для решения геометрических задач.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Объем времени, ч.  Разделы дисциплины Формируемый результат обучения по  дисциплине  Виды учебной деятельности  1 семест  Раздел 1. Education РД 1-3 Лекции 0  Практические занятия 22 Самостоятельная работа 15 Раздел 2. Work and career РД 1-3 Лекции 0 Практические занятия 20 Самостоятельная работа 14 Раздел 3. Employment РД 1-3 Лекции 0 Практические занятия 22 Самостоятельная работа 15 2 семестр Раздел 4. Sciences РД 1-3 Лекции 0 Практические занятия 20 Самостоятельная работа 14 Раздел 5. Technologies РД 1-3 Лекции 0 Практические занятия 24 Самостоятельная работа 16 Раздел 6. Engineering РД 1-3 Лекции 0 Практические занятия 20 Самостоятельная работа 14 Содержание разделов дисциплины: 1 семестр  Раздел 1. Education  Лексический материал:  Система образования в России и за рубежом, необходимость высшего образования, уровни высшего образования, виды образования, лучшие университеты мира, история и традиции ТПУ, инженерное образование, академическая мобильность, предметы и экзамены, жизнь студентов - рутинные заботы, проблемы и пути решения, непрерывное образование.  Темы практических занятий:  . Educational system in Russia and abroad  . Educational system in Russia and abroad  . Educational system in Russia and abroad  . Universities of the world/ TPU  . Universities of the world/ TPU  . Universities of the world/ TPU  . Educational issues (time management, exams) . Educational issues (time management, exams) 9. Educational issues (time management, exams) 10. Life-long learning  11. Life-long learning  © чмилвфь  Грамматический материал:  Модальные глаголы Modal verbs + Perfect Infinitive; повторение времён Revision of tenses: Present tenses (simple/ continuous/ perfect simple/ perfect continuous), Past tenses (simple/ continuous/ perfect simple/ perfect continuous), Future tenses (simple/ continuous/ perfect simple/ perfect continuous); (дополнительно word order, word formation, linking words, phrasal verbs).  Раздел 2. Work and career  Лексический материал: Планирование карьеры, выбор профессии: характеристика профессий, инженерные профессии.  Темы практических занятий:  . Career planning  . Career planning  . Career planning  . Choice of profession: the characteristics of professions . Choice of profession: the characteristics of professions . Choice of profession: the characteristics of professions . Engineering professions  . Engineering professions  9. Engineering professions  10. Engineering professions  CNDNDNBRWN KR  Грамматический материал:  Страдательный залог Passive voice, Passive with get; неличные формы глагола - причастие Participle 1, 2; отглагольные прилагательные Adjectives -ed/ -ing; (дополнительно word order, word formation, linking words, phrasal verbs).  Раздел 3. Employment  Лексический материал:  Основные стадии устройства на работу, поиск вакансий (биржа труда, объявления и т.д.), составление резюме, мотивационного/ сопроводительного письма, виды собеседования при устройстве на работу, типичные вопросы и ошибки, сфера профессиональной деятельности инженера /специалиста на производстве, техническая деятельность и творчество.  Темы практических занятий:  . Job hunting  . Job hunting  . Job hunting  . Job hunting  . Applying Юга job  . Applying for a job  . Applying Юга job  . Applying for a job 9. Engineering career 10. Engineering career  CNDNDNBRWN KR  Грамматический материал: Неличные формы глагола Infinitive, Gerund, Participle; (дополнительно word order, word formation, linking words, phrasal verbs).  2 семестр  Раздел 4. Sciences  Лексический материал:  Науки, значимость наук в современном мире, научный прогресс в современном обществе, влияние прогресса на современное общество, плюсы и минусы, международное сотрудничество, великие учёные прошлых лет и современности, их вклад в развитие наук.  Темы практических занятий:  1. Sciences in the modern society 2. Sciences in the modern society 3. Sciences in the modern society 4. Scientific progress in modern society 5. Scientific progress in modern society 6. Scientific progress in modern society  7. Scientific progress in modern society 8. The greatest scientists  9. The greatest scientists  10. The greatest scientists  Грамматический материал: Страдательный залог Passive voice (Perfect Passive, revision); (дополнительно word order, word formation, linking words, phrasal verbs).  Раздел 5. Technologies  Лексический материал:  Виды технологий (производственные, информационные, нано-) и области их применения, искусственный интеллект, требования к современным технологиям, изобретатели и их изобретения, инновационная деятельность.  Темы практических занятий:  . Types of technologies  . Types of technologies  . Types of technologies  . Types of technologies  . Types of technologies  . Types of technologies  . Inventors and their inventions  . Inventors and their inventions  . Inventors and their inventions 10. Inventors and their inventions 11. Inventors and their inventions 12. Inventors and their inventions  OMmAANIDNABRWN KR  Грамматический материал: Составные существительные Compound nouns; косвенная речь Reported speech; (дополнительно Word order, word formation, linking words, phrasal verbs).  Раздел 6. Engineering  Лексический материал: Отрасли промышленности, рабочее место инженера, безопасность на рабочем месте.  Темы практических занятий:  . Branches of engineering  . Branches of engineering  . Branches of engineering  . Branches of engineering  . Branches of engineering  . Safety at the workplace of an engineer  . Safety at the workplace of an engineer  . Safety at the workplace of an engineer  . Safety at the workplace of an engineer 10. Safety at the workplace of an engineer  OMmAANIDNABRWN KR  Грамматический материал: Повторение пройденного грамматического материала Revision of grammar.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной Объем результат деятельности времени, обучения по ч. дисциплине  Раздел 1. РД1 Лекции 12  Линейная алгебра РД2 Практические занятия 12 РДЗ Лабораторные занятия 0  Самостоятельная работа _ 26 Раздел 2. РД1 Лекции 6 Векторная алгебра РД? Практические занятия 6 РДЗ Лабораторные занятия 0  Самостоятельная работа 14  Раздел 3. РД1 Лекции 12  Элементы теории линейных РД2 Практические занятия 12 пространств и линейных РДЗ Лабораторные занятия 0  операторов Самостоятельная работа __ 34  Раздел 4. РД1 Лекции 12  Аналитическая геометрия РД? Практические занятия 12 РДЗ Лабораторные занятия 0  Самостоятельная работа  30  Раздел 5. РД1 Лекции 10  Введение в анализ РД2 Практические занятия 10 РДЗ Лабораторные занятия 0  Самостоятельная работа _  26  Раздел 6. РД1 Лекции 12  Дифференциальное РД? Практические занятия 12 исчисление функций одной РДЗ Лабораторные занятия 0  переменной Самостоятельная работа __ 30  Содержание разделов дисциплины:  Раздел 1. Линейная алгебра  Матрицы. Основные понятия и определения, основные виды матриц. Операции над матрицами. Определители 2, 3, п — го порядков и их свойства. Обратная матрица. Решение матричных уравнений. Ранг матрицы. Теорема о базисном миноре. Системы линейных алгебраических уравнений, основные понятия и определения. Совместность систем линейных алгебраических уравнений. Теорема Кронекера — Капелли. Методы нахождения решения системы линейных алгебраических уравнений. Однородные системы линейных алгебраических уравнений, основные понятия и определения. Фундаментальная система решений.  Темы лекций:  1. Матрицы и действия над ними.  2. Определители и их свойства.  3. Обратная матрица. Ранг матрицы Системы линейных уравнений. Матричный метод. 4. Системы линейных уравнений. Основные методы решения.  Темы практических занятий:  Матрицы, виды матриц, действия над матрицами. Определители порядка 2,3. Определители порядка п, их свойства. Ранг матрицы.  Обратная матрица. Решение матричных уравнений.  Системы линейных уравнений. Метод Гаусса.  Системы однородных линейных уравнений.  Контрольная работа по теме «Линейная алгебра».  хин  Раздел 2. Векторная алгебра  Понятие вектора. Линейные операции над векторами. Скалярное, векторное, смешанное произведения векторов, их основные свойства, геометрический смысл, вычисление через координаты вектора.  Темы лекций:  1. Понятие вектора. Линейные операции над векторами.  2. Базис на плоскости и в пространстве. Скалярное произведение. Векторное и смешанное произведения.  Темы практических занятий:  1. Линейные операции над векторами.  2. Скалярное произведение векторов.  3. Векторное произведение векторов. Смешанное произведение векторов.  Раздел 3. Элементы теории линейных пространств и линейных операторов  Аксиоматическое определение линейного пространства. Примеры. Линейная  зависимость и независимость векторов. Размерность и базис. Теорема о разложении вектора по базису. Координаты вектора. Преобразование базиса и координат. Критерий подпространства. Линейные операторы. Матрица линейного оператора конечномерного линейного пространства. Переход к новому базису. Собственные векторы и собственные значения. Характеристический многочлен. Диагонализируемость линейного оператора.  Темы лекций: 1. Линейное пространство. Линейная зависимость и независимость векторов 2. — Размерность и базис, разложение вектора по базису. Критерий подпространства  3. Линейные операторы. Матрица линейного оператора конечномерного линейного пространства.  4. Собственные векторы и собственные значения. Характеристический многочлен. Диагонализируемость линейного оператора  Темы практических занятий:  1. _ Линейное пространство. Критерий подпространства.  2. Линейная зависимость и независимость векторов. Базис линейного пространства.  3. — Преобразование базиса и координат. Линейные операторы.  4. — Преобразование матрицы линейного оператора при переходе к новому базису. 5. Собственные векторы и собственные значения. Диагонализируемость  линейного оператора.  6. Контрольная работа по теме «Элементы теории линейных пространств и  линейных операторов».  Раздел 4. Аналитическая геометрия  Общие понятия о линии, поверхности. Уравнения линий и поверхностей. Прямая на плоскости. Взаимное положение прямых на плоскости. Уравнения плоскости и уравнения прямой в пространстве. Взаимное расположение прямых и плоскостей. Геометрические определения кривых второго порядка Вывод канонических уравнений этих кривых, построение кривых второго порядка по их каноническому уравнению. Приведение общего уравнения кривой второго порядка к каноническому виду. Поверхности второго порядка, их канонические уравнения. Метод сечений в исследовании формы поверхностей.  Темы лекций:  Плоскость и прямая в пространстве.  Взаимное расположение прямой и плоскости.  Вычисление расстояний.  Кривые второго порядка.  Приведение кривых второго порядка к каноническому виду. Поверхности второго порядка.  хин  Темы практических занятий:  Прямая на плоскости.  Плоскость. Общее уравнение. Неполное уравнение.  Прямая в пространстве.  Взаимное расположение прямой и плоскости в пространстве.  Кривые второго порядка. Приведение кривых второго порядка к каноническому виду.  6. Контрольная работа по теме «Аналитическая геометрия».  пиров  Раздел 5. Введение в анализ  Понятие множества. Вещественные числа и их основные свойства. Логическая символика. Понятие функции. Обратная функция. Числовые последовательности: определение, свойства. Предел последовательности. Бесконечно малые и бесконечно большие последовательности. Основные теоремы о пределах последовательностей. Теорема о монотонной ограниченной последовательности. Число е. Предел функции. Односторонние пределы. Бесконечно малые и бесконечно большие функции. Основные теоремы о пределах функций. Первый и второй замечательные пределы. Сравнения бесконечно малых величин. Непрерывность функции: определение, геометрическая  интерпретация. Непрерывность в точке и на интервале. Теоремы о свойствах непрерывных функций. Точки разрыва и их классификация.  Темы лекций:  Введение в анализ. Элементы теории множеств. Понятие функции. Числовая последовательность и её предел.  Предел функции. Основные теоремы о пределах.  Замечательные пределы. Сравнение бесконечно малых.  Непрерывность функции. Основные теоремы о непрерывных функциях.  пиров  Темы практических занятий:  Вычисление пределов последовательности.  Предел функции Замечательные пределы.  Сравнение бесконечно малых.  Непрерывность функции. Точки разрыва и их классификация. Контрольная работа по теме «Введение в анализ».  пир  Раздел 6. Дифференциальное исчисление функций одной переменной  Определение и геометрический смысл производной. Односторонние производные. Понятие дифференцируемости функции. Связь дифференцируемых функций с функциями непрерывными. Определение и геометрический смысл дифференциала. Правила дифференцирования. Теоремы о производной обратной и сложной функций. Производные и дифференциалы высших порядков. Формула Лейбница. Основные теоремы дифференциального исчисления: теоремы Ферма, Ролля, Лагранжа, Коши. Правило Лопиталя, применение к раскрытию неопределенностей  0 со  вида  — и —  ието использование при раскрытии неопределенностей других видов. oe)  Формула Тейлора. Остаточный член в форме Лагранжа. Точки экстремума. Теоремы о необходимых и достаточных условиях существования экстремума. Асимптоты: определение, виды (наклонная, вертикальная). Выпуклость, вогнутость функции. Точки перегиба. Теорема о достаточных условиях существования точки перегиба. Полная схема исследования функции и построения ее графика.  Темы лекций:  1. Понятие дифференцируемости функции. Правила дифференцирования. 2. Дифференциал. Производные и дифференциалы высших порядков.  3. Правило Лопиталя. Основные теоремы дифференциального исчисления. 4. Асимптоты. Полная схема исследования функции.  Темы практических занятий: 1. Правила и техника дифференцирования. Дифференцирование параметрических и неявно заданных функций. Производная степенно-показательной функции. Односторонние производные. Производные высших порядков. Дифференциал. Правило Лопиталя. Асимптоты, исследование на монотонность. Полное исследование и построение графиков функций. Контрольная работа по теме «Дифференцирование функции одной переменной». 5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине Раздел 1. РД1 Лекции 8 Неопределенный интеграл РД? Практические занятия 12 РДЗ Лабораторные занятия 0 Самостоятельная работа 26 Раздел 2. РД1 Лекции 6 Определенный и несобственный РД? Практические занятия 10 интеграл РДЗ Лабораторные занятия 0 Самостоятельная работа 14 Раздел 3. РД1 Лекции 8 Дифференциальное исчисление РД? Практические занятия 10 функций нескольких РДЗ Лабораторные занятия 0 переменных Самостоятельная работа 30 Раздел 4. РД1 Лекции 8 Кратные интегралы РД? Практические занятия 6 РДЗ Лабораторные занятия 0 Самостоятельная работа 26 Раздел 5. РД1 Лекции 18 Элементы векторного анализа РД? Практические занятия 10 РДЗ Лабораторные занятия 0 Самостоятельная работа 24  Содержание разделов дисциплины:  Раздел 1. Неопределенный интеграл  Понятие первообразной функции и неопределенного интеграла. Свойства неопределенного интеграла. Таблица интегралов. Непосредственное интегрирование. Метод замены переменной и метод интегрирования по частям. Интегрирование рациональных функций. Простейшие рациональные дроби и их интегрирование. Теорема о представлении правильной рациональной дроби в виде суммы конечного числа простейших дробей. Интегрирование выражений, содержащих тригонометрические функции. Интегрирование некоторых иррациональных функций. Подстановки Чебышева, тригонометрические.  Темы лекций:  1.  2.  [92]  4.  Первообразная и неопределенный интеграл. Общие методы интегрирования Метод подстановки, интегрирование по частям.  Интегрирование рациональных дробей.  Интегрирование тригонометрических функций.  Интегрирование иррациональных функций. Подстановки Чебышева, тригонометрические подстановки.  Темы практических занятий:  пиров  Непосредственное интегрирование. Введение под знак дифференциала. Интегрирование по частям. Простейшие рациональные дроби.  Интегрирование рациональных дробей.  Интегралы от тригонометрических функций.  Интегрирование иррациональностей. Подстановки Чебышева, тригонометрические подстановки.  6. Контрольная работа по теме «Неопределенный интеграл».  Раздел 2. Определенный и несобственный интеграл  Задачи, приводящие к понятию определенного интеграла. Понятие определенного интеграла, его геометрический и физический смысл. Классы интегрируемых функций. Свойства определенного интеграла. Интеграл с переменным верхним пределом. Формула Ньютона-Лейбница. Вычисление определенного интеграла. Геометрические приложения определенного интеграла: вычисление площадей плоских фигур. Определение и вычисление длины дуги плоской кривой. Вычисление объемов тел. Несобственные интегралы с бесконечными пределами. Определение, свойства. Признаки сходимости интегралов от неотрицательных функций. Абсолютная и условная сходимость. Несобственные интегралы от неограниченных функций. Теорема сравнения.  Темы лекций:  1. Понятие и свойства определенного интеграла.  2. Формула Ньютона-Лейбница. Приложения определенного интеграла. 3. Несобственные интегралы I и П рода.  Темы практических занятий:  1. Определенный интеграл: вычисление. Определенный интеграл с переменным верхним пределом.  Вычисление площадей.  Вычисление дуги дуги. Вычисление обьема тела.  Несобственные интегралы Г и П рода: вычисление, признаки сходимости. Контрольная работа по теме «Определенный интеграл».  ров  Раздел 3. Дифференциальное исчисление функций нескольких переменных  ... Определение функции нескольких переменных. Предел и непрерывность функции нескольких переменных. Частные производные функций нескольких переменных. Производная сложной функции и функции заданной неявно. Полный дифференциал ФНП, инвариантность формы первого дифференциала. Частные производные и дифференциалы высших порядков. Скалярное поле, линии и поверхности уровня. Градиент и производная по направлению. Свойства градиента. Касательная плоскость и нормаль к поверхности. Формула Тейлора для функции двух переменных. Экстремум функции нескольких переменных (необходимые и достаточные условия).  Темы лекций:  1. Предел и непрерывность функции двух переменных.  2. Частные производные и дифференциал функций нескольких переменных.  3. Касательная плоскость и нормаль к поверхности. Формула Тейлора для функции двух переменных.  4. Экстремум функции нескольких переменных.  Темы практических занятий:  1. Функции нескольких переменных: область определения, область значений, линии и поверхности уровня.  2. Частные производные первого порядка для функции нескольких переменных. Дифференцирование сложных функций, функций, заданных неявно. Диффернциал. Приближенное вычисление.  3. Производная по направлению. Градиент. Касательная плоскость и нормаль к поверхности.  4. Частные производные и дифференциалы высших порядков. Экстремум функции 5. Контрольная работа по теме «Функции нескольких переменных».  Раздел 4. Кратные интегралы  ... Задачи, приводящие к понятию двойного интеграла. Определение двойного интеграла, геометрический и физический смысл. Теорема существования, свойства. Сведение двойного интеграла от непрерывной функции к повторному интегралу. Теорема о замене переменных в двойном интеграле. Задачи, приводящие к понятию тройного интеграла. Тройной интеграл, определение, свойства, вычисление в декартовой системе координат. Формулировка теоремы о замене переменных в тройном интеграле. Цилиндрические и сферические координаты. Приложение кратных интегралов: вычисление объемов тел и площадей фигур, решение задач механики и физики.  Темы лекций:  1. Двойные интегралы, сведение к повторным интегралам. Свойства двойного  интеграла.  2. Замена переменных в двойном интеграле, его вычисление в полярной системе  координат. Тройные интегралы и их вычисление в ДСК  3. Замена переменных в тройном интеграле, его вычисление в цилиндрических и  сферических координатах  4. Приложения кратных интегралов  Темы практических занятий:  1. Двойные интегралы: вычисление, переход в полярную систему координат.  2. Тройные интегралы: вычисление, переход в цилиндрическую систему координат.  3. Тройные интегралы: переход в сферическую систему координат. Приложения кратных интегралов.  Раздел 5. Элементы векторного анализа  ... Криволинейные интегралы по длине дуги и по координатам. Определение, свойства и вычисление криволинейных интегралов. Теорема Грина. Условия независимости криволинейного интеграла от пути интегрирования. Отыскание функции по ее полному дифференциалу. Поверхностный интеграл по площади поверхности. Определение, формула для вычисления. Определение, свойства и вычисление поверхностного интеграла по координатам. Теорема и формула Остроградского-Гаусса. Ориентация поверхности и направление обхода замкнутого контура. Теорема и формула Стокса. Векторное поле. Векторные линии. Оператор Гамильтона. Дифференциальные операции первого порядка в скалярном и векторных полях. Дивергенция векторного поля, ее физический смысл. Циркуляция и ротор векторного поля. Теорема Гельмгольца. Потенциальные и соленоидальные поля. Дифференциальные операции второго порядка.  Темы лекций:  1. Криволинейные интегралы [-го рода.  2. Криволинейные интегралы П-го рода. Теорема Грина.  3. Условия независимости криволинейного интеграла П-го рода от пути интегрирования.  4. Отыскание функции по ее полному дифференциалу. Приложения криволинейных  интегралов.  Поверхностные интегралы 1-го рода.  Поверхностные интегралы П-го рода.  Теоремы Стокса и Остроградского-Гаусса. Приложения поверхностных интегралов  Векторное поле, работа, поток поля.  Дифференциальные операции первого и второго порядков в скалярном и векторных  хоча  полях.  Темы практических занятий:  пир  Криволинейные интегралы 1-го рода. Криволинейные интегралы П-го рода. Поверхностные интегралы 1-го рода. Поверхностные интегралы П-го рода. Контрольная работа по теме «Кратные, криволинейные и поверхностные интегралы». 5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине  Раздел 1. РД Случайные события РД2  РДЗ Раздел 2. РД! Случайные величины и их РД2 системы РДЗ Раздел 3. РД! Закон больших чисел и РД2 предельные теоремы РДЗ Раздел 4. РД Выборочный методи РД2 оценивание параметров РДЗ Раздел 5. РД Элементы корреляционно - РД2 регрессионного анализа РДЗ Раздел 6. Проверка РД! статистических гипотез РД?  РДЗ  Содержание разделов дисциплины:  Раздел 1. Случайные события.  Понятие пространства элементарных исходов и случайного события, классификация событий, алгебра событий. Вероятность события, статистическое, классическое и геометрическое определения вероятности. Аксиоматическое определение вероятности, основные теоремы теории вероятностей. Условные вероятности, независимость событий, теорема умножения вероятностей. Формулы полной вероятности и Байеса. Схема последовательных испытаний Бернулли, формула Бернулли, приближенные формулы Муавра-Лапласа и Пуассона.  Темы лекций:  1. Алгебра случайных событий. 2. Алгебра вероятностей случайных событий. 3. Схема последовательных испытаний Бернулли.  Темы практических занятий: 1. Алгебра случайных событий. 2. Алгебра вероятностей случайных событий. 3. Схема последовательных испытаний Бернулли.  Раздел 2. Случайные величины и их системы. Понятие случайной величины и ее закона распределения. Случайная величина дискретного типа, ряд распределения. Функция распределения случайной величины и ее свойства. Случайная величина непрерывного типа, плотность распределения и ее свойства. Числовые характеристики случайных величин и их свойства. Основные законы распределения случайных величин (биномиальное, Пуассона, равномерное, показательное, нормальное).  Понятие случайного вектора. Дискретные и непрерывные вектора. Законы распределения случайных векторов. Понятие независимости случайных величин, условные законы распределения. Числовые характеристики системы случайных величин, свойства характеристик. Ковариация и коэффициент корреляции, свойства коэффициента корреляции.  Темы лекций:  1. Случайная величина и ее законы распределения.  2. Числовые характеристики распределения случайной величины. 3. Системы случайных величин.  Темы практических занятий:  1. Случайная величина и ее законы распределения.  2. Числовые характеристики распределения случайной величины. 3. Системы случайных величин.  Раздел 3. Закон больших чисел. Предельные теоремы.  Неравенства Чебышева. Предельные теоремы Чебышева, Бернулли, Ляпунова, Муавра- Лапласа.  Темы лекций: 1. Закон больших чисел и предельные теоремы.  Темы практических занятий: 1. Контрольная работа по ТВ.  Раздел 4. Выборочный метод и оценивание параметров распределения  Представление эмпирических данных. Понятие выборки, генеральной совокупности. Графическое представление эмпирических законов распределения: гистограмма, полигон, кумулятивная кривая. Требования к оценкам параметров (состоятельность, несмещенность, эффективность). Эмпирические моменты. Среднее, дисперсия, стандартное отклонение, эксцесс, асимметрия и их интерпретация. Способ моментов. Интервальные оценки. Понятие доверительной вероятности, уровня значимости, доверительного интервала. Точечное и интервальное оценивание параметров нормального распределения.  Темы лекций: 1. Выборочный метод. Эмпирические законы распределения. Эмпирические моменты. 2. Доверительный интервал. Интервальные оценки.  Темы практических занятий: 1. Выборочный метод. Эмпирические законы распределения. Эмпирические моменты. 2. Интервальные оценки параметров нормального распределения.  Раздел 5. Элементы корреляционно - регрессионного анализа  Понятие стохастической связи между случайными величинами. Корреляционный момент (ковариация). Определение коррелированных величин. Корреляционная таблица. Выборочный парный коэффициент корреляции. Значимость и надежность коэффициента корреляции. Парная полиномиальная регрессия. Уравнение регрессии. Оценивание коэффициентов регрессии. Адекватность (линейность) регрессии. Степень согласованности эмпирических данных.  Темы лекций: 1. Выборочный парный коэффициент корреляции. Парная регрессия.  Темы практических занятий: 1. Выборочный парный коэффициент корреляции. Парная регрессия. Раздел 6. Проверка статистических гипотез  Основные задачи проверки гипотез. Нулевая и альтернативная гипотезы. Односторонний и двусторонний критерий принятия решений. Критическая область. Ошибки первого и второго рода. Параметрические и непараметрические критерии проверки статистических гипотез. Проверка гипотез о равенстве дисперсий и средних значений нормально распределенных совокупностей. Критерий согласия Пирсона.  Темы лекций:  1. Статистическая гипотеза. Критерий проверки статистических гипотез. Критерий согласия Пирсона.  2. Проверка гипотез о равенстве дисперсий и средних значений нормально распределенных совокупностей.  Темы практических занятий: 1. Проверка гипотез о законе распределения и числовых характеристиках. 2. Контрольная работа по МС.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения a Виды учебной деятельности времени, ч. дисциплине Лекции 4 Раздел 1. Введение в теорию оптимизации РД1 Лабораторные занятия 4 Самостоятельная работа 25 Лекции 4 Раздел 2. Методы одномерной д ‚столы од р PA 1, PI 2 Лабораторные занятия 4 безусловной оптимизации Самостоятельная работа 25 .. Лекции 6 Раздел 3. Методы многомерной к о РД РД2 Лабораторные занятия 6 безусловной оптимизации Самостоятельная работа 25 Лекции 8 Раздел 4. Линейное программирование РД 1, РДЗ Лабораторные занятия 8 Самостоятельная работа 25  Содержание разделов дисциплины:  Раздел 1. Введение в теорию оптимизации  Роль методов оптимизации в решении задач повышения эффективности управления технологическими, экономическими объектами и процессами. Содержательные и формализованные постановки задач оптимизации. Критерии оптимальности. Целевая функция и ограничения. Классификация задач оптимизации по виду целевой функции и ограничениям.  Темы лекций:  1. История развития математического программирования. Классификация и постановка задач оптимизации  2. Математика экстремального анализа функций, функционалов. Условия существования экстремума. Характеристики алгоритмов оптимизации  Названия лабораторных работ:  1. Входное задание  2. Анализ экстремальных свойств функций  Раздел 2. Методы одномерной безусловной оптимизации  Анализ экстремальных свойств задач одномерной безусловной оптимизации. Классификация методов одномерной оптимизации.  Темы лекций:  3. Методы оптимизации, основанные на сокращении интервалов неопределенности: метод дихотомии, золотого сечения. Минимаксная стратегия поиска. Сравнительный анализ интервальных методов.  4. Методы точечного оценивания: квадратичной аппроксимации, Пауэлла. Методы одномерного поиска с использованием производных: Ньютона-Рафсона  Названия лабораторных работ:  3. Интервальные методы одномерного поиска оптимума: методы Дихотомии и Золотого сечения.  4. Использование метода Ньютона-Рафсона в задаче одномерного поиска оптимума.  Раздел 3. Методы многомерной безусловной оптимизации  Анализ экстремальных свойств задач многомерной безусловной оптимизации. Классификация методов многомерной оптимизации.  Темы лекций:  5. Методы прямого поиска: покоординатного поиска, оврагов, Хука-Дживса.  6. Градиентные методы безусловной оптимизации: градиентного спуска, наискорейшего спуска (Коши)  7. Сравнительный анализ методов безусловной оптимизации. Графическая интерпретация прямых и градиентных методов многомерной безусловной оптимизации.  Названия лабораторных работ:  5. Прямые методы многомерной безусловной оптимизации: метод Хука-Дживса.  6. Градиентные методы многомерной безусловной оптимизации: метод простых градиентов.  7. Градиентные методы многомерной безусловной оптимизации: метод Коши и с использованием стандарных процедур СКМ MathCad.  Раздел 4. Линейное программирование  Постановка задачи линейного программирования (ЗЛП). Примеры и формы записи ЗЛП.  Темы лекций:  8. Идея и алгебра симплекс метода. Классические задачи линейного программирования: транспортная задача, задача об использовании сырья, задача о диете.  9. Симплекс- метод для решения задачи линейного программирования.  10. Симплекс- метод решения задачи линейного программирования с использованием искусственного базиса.  11. Экономическая трактовка двойственности задачи линейного программирования.  Названия лабораторных работ:  8. Геометрический метод решения задачи линейного программирования.  9. Решение задачи линейного программирования симплекс- методом с использованием искусственного базиса.  10. Решение задачи линейного программирования с использованием стандарных процедур СКМ Ма Сад.  11. Решение двойственной задачи линейного программирования.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины  бучения по Виды учебной деятельности и a дисциплине Лекции 6 Раздел 1. Введение в ВРМ РД-1 Лабораторные занятия 8 Самостоятельная работа 31 Лекции 6 Раздел 2. Моделирование, анализ и проектирование бизнес-процессов PA-2 Лабораторные занятия 8 Самостоятельная работа 31 Лекции 6 Раздел 3. Управление эффективностью РД-3 Лабораторные занятия 3 процессов Самостоятельная работа 31 Лекции 6 Раздел 4. Технологии ВРМ РД-4 Лабораторные занятия 8 Самостоятельная работа 31 Содержание разделов дисциплины: Раздел 1. Введение в ВРМ  Рассматриваются концепции ВРМ и даются определения таких ключевых понятий, как сквозной процесс, ценность для потребителя, кросс-функциональная работа. Также рассматриваются типы процессов, компоненты процессы, жизненный цикл ВРМ. Этот раздел дает определение BPM и закладывает фундамент для остальных разделов.  Темы лекций:  1. Введение в ВРМ. ВРМ - управленческая дисциплина.  Названия лабораторных работ:  1. Выбор процесса, его описание, схема ВРММ.  2. Проектирование пользовательских интерфейсов.  В данном разделе формируется понимание целей и эффекта моделирования процессов, рассматриваются типы процессных моделей и варианты их использования, описываются средства, методы и стандарты моделирования. Также в данном разделе рассматриваются цели анализа процессов, подходы к декомпозиции процессов и методы анализа, включая такие аспекты как роли, рамки, бизнес-контекст, правила и показатели эффективности. И также в данном разделе рассматриваются принципы правильного проектирования процессов, роли, методики, а также такие общие аспекты как участие высшего руководства, соответствие нормативным требованиям и стратегии.  Темы лекций:  2. Введение в моделирование бизнес-процессов. Основные процессные нотации.  3. Уровни процессных моделей. Фреймворки и референтные модели.  4. Анализ процессов. Роли участников анализа процессов.  5. Подготовка к анализу процессов. Проведение анализа. Рекомендации по результатам анализа.  6. Основы проектирования процессов. Выявление процесса «как есть» или «текущее состояние». Проектирование процессов и потоков работ — модель «как будет».  Названия лабораторных работ:  3. Создание модели данных процесса. 4. Создание экранных форм.  5. Настройка правил переходов.  6. Запуск и отладка процесса. Раздел 3. Управление эффективностью процессов  В данном разделе изучается значение и эффект таких аспектов, как измерение эффективности, определение ключевых показателей эффективности, мониторинг и контроль операций, увязывание эффективности процессов с эффективностью организации в целом. Также рассматриваются объекты и методы измерения, имитационное моделирование, поддержка принятия решений, факторы успеха.  Темы лекций:  7. Что такое управление эффективностью процесса? Что такое эффективность процесса?  8. Измерение и управление. Развитие способности измерять эффективность. Ключевые определения эффективности процессов.  9. Выстраивание бизнес-процессов исходя из эффективности предприятия.  10. Фреймворк зрелости управления эффективностью процессов.  Названия лабораторных работ:  7. Контроль и мониторинг процесса.  8. Улучшение процесса.  Раздел 4. Технологии ВРМ  В данном разделе рассматривается широкий спектр существующих технологий, обеспечивающих планирование, проектирование, анализ, исполнение и мониторинг бизнес- процессов. Здесь рассмотрены пакеты прикладных программ, средств разработки, инфраструктурные компоненты, хранилища данных и информации, обеспечивающие связанную с ВРМ деятельность. Рассматриваются интегрированные системы управления бизнес-процессами (ВРМ$) процессные репозитарии, а также изолированные средства моделирования, анализа, проектирования, исполнения и мониторинга. Также рассказывается о стандартах, методологиях и новых трендах ВРМ.  Темы лекций:  11. Эволюция технологий ВРМ. Возможности технологий ВРМ. Эффект от технологий ВРМ.  12. Взгляд в будущее технологий ВРМ. Преимущества и риски автоматизации процессов.  Названия лабораторных работ:  9. Разработка веб-сервиса.  10. Интеграция веб-сервис с процессом.  11. Разработка автоматизированного робота с помощью технологии КРА.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности Разделы дисциплины Формируемый Виды учебной деятельности Объем результат времени, ч. обучения по дисциплине  Раздел (модуль) 1. РД1, РД2, Лекции Начертательная геометрия РДЗ Практические занятия Лабораторные занятия Самостоятельная работа Раздел (модуль) 2. РД1, РД2, Лекции Аксонометрические проекции РДЗ Практические занятия  6 ЕН jo Пабораторные занятия о  Е jo    &lt;  Самостоятельная работа Раздел (модуль) 3. Элементы  РД1, РД2, Лекции  технического черчения РДЗ Практические занятия Пабораторные занятия Самостоятельная работа  &lt;  3  Содержание разделов дисциплины:  Раздел 1. Начертательная геометрия Введение. Методы проецирования, их свойства. Обратимость чертежа. Комплексный чертеж точки. Прямая. Задание и изображение на чертеже. Положение относительно плоскостей проекций. Взаимное положение двух прямых. Задание плоскости на чертеже. Положение относительно плоскостей проекций. Точка и прямая в плоскости. Взаимное положение прямой и плоскости. Взаимное положение двух плоскостей. Поверхность: определение, задание и изображение на чертеже. Классификация. Точки и линии на поверхности. Гранные поверхности, поверхности вращения. Развертка поверхностей. Взаимное пересечение поверхностей.  Темы лекций: 1. Введение, точка, прямая, плоскость, их взаимное положение. 2. Поверхности: многогранники, поверхности вращения. Точки и линии на поверхности. 3. Винтовые поверхности. Взаимное пересечение поверхностей  Темы практических занятий: 1. Основные правила выполнения чертежей. Прямоугольное проецирование. Проекции точки. 2. Проекции прямой. Плоскость. Взаимное положение прямых и плоскостей. 3. Гранные поверхности. Развертка поверхностей. 4. Поверхности вращения. Взаимное пересечение поверхностей.  Раздел 2. Аксонометрия  Краткие сведения по теории аксонометрических проекций. Прямоугольная и косоугольная аксонометрические проекции. Стандартные аксонометрические проекции.  Темы лекций:  1. Аксонометрия. Краткие сведения по теории аксонометрических проекций. Прямоугольная и косоугольная аксонометрические проекции. Стандартные аксонометрические проекции. Темы практических занятий: 1. Изображения. Прямоугольная изометрия.  Раздел 3. Элементы технического черчения  Изображения — виды, разрезы, сечения. Условности и упрощения. Основные правила нанесения размеров на чертежах. Резьбы. Соединения. Детали, сборочные единицы, комплексы, комплекты. Рабочий чертеж детали, эскиз, сборочный чертеж изделия, чертёж общего вида. Текстовый графический документ — спецификация, правила заполнения.  Темы лекций: 1. Изображения - виды, разрезы, сечения. Условности и упрощения. 2. Основные правила нанесения размеров на чертежах. 3. Резьбы. Соединения разъемные и неразъемные. Крепежные изделия. 4. Виды изделий Виды конструкгорской документации.  Темы практических занятий: 1. Изображения. Построение по двум изображениям третьего. Нанесение размеров на чертежах. Выполнение рациональных разрезов и сечений. Резьбы. Соединения. Составление спецификации сборочной единицы. Сборочный чертеж Эскизирование деталей Деталирование по чертежу общего вида  AWRWN  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  3 Формируемый Разделы дисциплины результат Виды учебной деятельности оон ^ им обучения по иль уч ^ времени, ч. дисциплине Лекции 16 РДТ,РД2 Практические занятия 10 Раздел 1. Механика Al, PIL 2, р РДЗ,РД4 Лабораторные занятия 10 Самостоятельная работа 40 Лекции 16 Раздел 2. Молекулярная физика и РД1,РД2, Практические занятия 6 термодинамика РДЗ,РД4 Лабораторные занятия 6 Самостоятельная работа 40  Содержание разделов дисциплины:  Раздел 1. Механика  Предмет физики. Методы физического исследования (опыт, гипотеза, эксперимент, теория). Роль измерения в физике. Физические модели в механике (материальная точка, система частиц, абсолютно твердое тело, сплошная среда). Кинематическое описание движения. Динамика материальной точки. Законы Ньютона, их физическое содержание и взаимная связь. Границы применимости классической механики. Динамика системы материальных точек и твердого тела. Законы сохранения в механике. Основы механики специальной теории относительности. Тяготение. Неинерциальные системы отсчета и силы инерции.  Темы лекций:  1. Кинематика поступательного движения  2. Кинематика вращательного движения твердого тела.  3. Динамика материальной точки  4. Динамика вращательного движения  5. Динамика системы материальных точек. Законы сохранения импульса, момента импульса  6. Работа и энергия. Законы сохранения.  7. Кинематика и динамика СТО  8. Неинерциальные системы отсчета. Движение тел в НСО.  Темы практических занятий: 1. Кинематика поступательного и вращательного движений. 2. Динамика поступательного и криволинейного движений. Силы в механике 3. Работа и энергия. Законы сохранения. 4. Кинематика и динамика СТО 5. Неинерциальные системы отсчета. Движение тел в НСО  Названия лабораторных работ:  1. М-00. Измерительный практикум. Погрешности измерений. Определение линейных величин и углов.  2. М-02. Определение средней силы сопротивления грунта забивке сваи на модели копра.  3. М-03. Определение модуля Юнга из растяжения на приборе Лермантова.  4. М-04. Определение модуля Юнга по изгибу стержней  5. М-18. Определение момента инерции тела по методу крутильных колебаний.  6. М-09. Проверка основного уравнения динамики при вращении твердого тела вокруг неподвижной оси.  7. M-17. Изучение закономерностей центрального удара.  8. М-08. Определение момента инерции стержня из упругого нецентрального удара.  9. М-09а. Маятник Обербека.  10.  11. 12. 13. 14. 15. 16.  17.  18. 19. 20. 21. 22. 23. 24. 25. 26. 27.  М-21а. Определение скорости пули при помощи баллистического крутильного маятника.  М-14. Определение момента силы трения при помощи машины Атвуда.  М-23. Определение ускорения свободного падения на машине Атвуда.  М-07. Определение момента инерции маятника Максвелла.  М-19. Определение коэффициента силы трения скольжения  М-16. Определение ускорения свободного падения.  М-05. Проверка Максвелловского закона распределения скоростей молекул на механической модели  М-06. Экспериментальное изучение Гауссовского закона распределения результатов измерения.  М-07. Исследование колебательного процесса связанных систем.  М-10. Математический маятник  M-11. Физический маятник  МодМ-01. Ускорение свободного падения  МодМ-02. Второй закон Ньютона.  МодМ-03. Закон сохранения импульса.  МодМ-04. Момент инерции твердого тела.  МодМ-05. Работа и энергия.  МодМ-06. Реактивное движение  МодМ-07. Движение инертного тела в гравитационном поле  Раздел 2. Молекулярная физика и термодинамика  Модель идеального газа. Основное уравнение молекулярно-кинетической теории.  Уравнение состояния идеального газа. Физические основы термодинамики. Теплота, работа. Первое начало термодинамики. Теплоемкость газов. 2 начало термодинамики. Обратимые и необратимые тепловые процессы, круговые процессы. Понятия энтропии, микро- и макросостояний системы. Термодинамическая вероятность состояния. Формула Больцмана. Третье начало термодинамики (теорема Нернста). Цикл Карно, теоремы Карно. Распределение Максвелла и Больцмана. Явления переноса: диффузия, теплопроводность, вязкость (внутреннее трение), их уравнения и коэффициенты. Фазовые равновесия и фазовые превращения. Реальные газы. Элементы неравновесной термодинамики.  Темы лекций:  . МКТ, основное уравнение и его следствия  . Статистические распределения. Часть   . Статистические распределения. Часть 2  . Работа и энергия в термодинамике  . Первое начало термодинамики  . Понятия энтропии, микро- и макросостояний системы  . Второе начало термодинамики  . Элементы неравновесных процессов. Фазовые переходы  © чмилффь-  Темы практических занятий: 1. Опытные газовые законы. Графические методы решения задач по МКТ 2. Статистические распределения, определение характеристических скоростей молекул 3. Ти 2 начала термодинамики  Названия лабораторных работ:  1. МФ-12. Определение средней длины свободного пробега и эффективного диаметра молекул воздуха.  2. МФ-13. Определение коэффициента внутреннего трения жидкости методом Пуазейля.  3. МФ-15. Определение отношения молярных теплоемкостей газов Ср/Су способом Клемана и Дезорма.  4. МФ-20. Экспериментальное изучение Гауссовского закона распределения результатов измерения.  5. МФ-01. Законы идеального газа  6. МФ-02. Определение молярной теплоемкости при постоянном давлении и при постоянном объеме  7. МФ-03. Определение показателя адиабаты газов при помощи осциллятора Фламмерсфельда  8. МФ-04. Распределение молекул по скоростям (распределение Максвелла)  9. МФ-09. Изучение циклических процессов  10. МодТ-01. Вытекание жидкости из малого отверстия  11. МодТ-02. Движение тела в вязкой среде.  12. МодТ-04. Распределение Максвелла  13. МодТ-05. Распределение Больцмана  14. МодТ-06. Законы идеального газа  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  3  Формируемый Разделы дисциплины результат Виды учебной деятельности Объем ен обучения по иль уч es времени, 4. дисциплине Лекции 16 РД1,РД2 Практические занятия Раздел 1. Электростатика AI, PIL2, р РДЗ,РД4 Лабораторные занятия 8 Самостоятельная работа 40 Лекции 16 Раздел 2. Электромагнетизм. Колебания и РД1,РД2, Практические занятия 8 волны РДЗ,РД4 Лабораторные занятия 8 Самостоятельная работа 40  Содержание разделов дисциплины:  Раздел 1. Электростатика  Электрический заряд и его свойства. Закон Кулона Электрическое поле. Напряженность электрического поля. Поле диполя. Закон Гаусса в интегральной форме и дифференциальной форме, применение теоремы к расчету полей. Работа, потенциал, связь напряженности и потенциала. Проводники и диэлектрики. Закон Гаусса для вектора электростатической индукции. Электроемкость проводников. Электрический ток. Условие существования тока. Закон Ома в дифференциальной форме. Закон Ома для полной цепи. Классическая теория — электропроводности металлов и ее затруднения. Электропроводность газов. Типы самостоятельных разрядов: тлеющий, коронный, искровой, дуговой. Понятие о плазме. Электропроводность плазмы. Ток в вакууме. Закон Богуславского-Лэнгмюра. Контактные явления.  Темы лекций:  1. Введение. Электрический заряд и его свойства. Методы измерения электрического заряда  . Электростатическое поле в вакууме.  . Теорема Гаусса и ее применение  . Работа, потенциал, связь напряженности и потенциала  . Проводники в электрическом поле. Энергия поля  . Диэлектрики в электрическом поле  . Электрический ток в различных средах  . Теория электропроводности  © чм  Темы практических занятий: 1. Закон Кулона. 2. Теорема Гаусса и ее применение 3. Работа, потенциал, связь напряженности и потенциала. 4. Электрический ток в различных средах 5. Теория электропроводности  Названия лабораторных работ:  1. Э-01. Моделирование и исследование электрических полей.  2. Э-05. Исследование зависимости сопротивления металлов от температуры и определение температурного коэффициента сопротивления металлов.  3. Э-06. Измерения электроемкости с помощью мостика Соти.  4. Э-07. Определение заряда иона водорода.  5. Э-05а. Исследование температурной зависимости сопротивления полупроводников и определение энергии активации проводимости.  9.  10. 11. 12. 13.  14. 15. 16. 17.  18. 19.  3-09. Исследование термоэлектронной эмиссии и определение работы выхода электрона из металла.  Э-11. Определение удельного заряда электрона с помощью вакуумного диода.  Э-12. Определение горизонтальной составляющей напряженности магнитного поля Земли  Э-18. Исследование полупроводниковых приборов.  Э-16. Измерение напряженности магнитного поля соленоида  Э-17. Снятие кривой намагничения и определение характеристик ферромагнетика. Э-21. Исследование плазмы положительного столба тлеющего разряда  Э-23. Измерение больших сопротивлений и емкостей методом релаксационных колебаний  Э-24. Измерение логарифмического декремента и добротности колебательного контура.  Э-25. Изучение вынужденных электромагнитных колебаний в параллельном колебательном контуре.  Э-32. Распределение Максвелла термоэлектронов по скоростям  КЭ-13. Исследование плазмы положительного столба тлеющего разряда.  МодЭ-03. Электростатическое поле.  МодЭ-04. Движение заряженной частицы в кулоновском поле.  Раздел 2. Электромагнетизм. Колебания и волны  Магнитное поле. Вектор магнитной индукции. Поток вектора магнитной индукции.  Закон Гаусса для магнитного потока в интегральной и дифференциальной формах. Закон Био-Савара-Лапласа и его применение. Закон полного тока в интегральной форме и его применение. Ротор векторной функции. Закон полного тока в дифференциальной форме. Действие магнитного поля на проводники с током и заряженные частицы. Явление электромагнитной индукции. Закон электромагнитной индукции. Правило Ленца. Закон электромагнитной индукции, самоиндукции и взаимной индукции. Энергия магнитного  ПОЛЯ.  Магнетики. Понятие о колебательном движении. Гармонические колебания,  затухающие и вынужденные колебания. Волны, электромагнитные волны.  Темы лекций:  . Магнитное поле тока. Закон Био-Савара-Лапласа.  . Закон полного тока и его применение.  . Сила Лоренца и сила Ампера.  . Магнитное поле в веществе.  . Электромагнитная индукция.  . Гармонические ЭМ колебания. Затухающие и вынужденные ЭМ колебания. . Волны, электромагнитные волны  . Уравнения Максвелла.  © чмилвышь  Темы практических занятий:  1. Магнитное поле в вакууме и веществе. 2. Электромагнитная индукция. Энергия магнитного поля. 3. Колебания и волны.  Названия лабораторных работ: Э-15. Определение горизонтальной составляющей напряженности магнитного поля Земли. Э-16. Измерение напряженности магнитного поля соленоида. Э-17. Снятие кривой намагничения и определение характеристик ферромагнетика. 4. КЭ-13. Исследование плазмы положительного столба тлеющего разряда.  5. Э-19. Измерение больших сопротивлений и емкостей методом релаксационных колебаний.  6. Э-22. Измерение логарифмического декремента и добротности колебательного контура.  7. Э-29. Определение скорости звука, модуля Юнга и внутреннего трения  акустическим методом  Э-34. Резонанс токов.  9. МодЭ-01. Движение заряженной частицы во взаимно перпендикулярных электрическом и магнитном полях.  10. МодЭ-02. Движение заряженной частицы в параллельных электрическом и магнитном полях  11. МодК-01. Свободные гармонические колебания  12. Э-[ба. Исследование магнитных полей с помощью измерительной катушки  13. КЭ-05. Распределение Максвелла термоэлектронов по скоростям  14. МодК-02. Затухающие колебания  15. МодК-03. Сложение перпендикулярных колебаний.  16. МодК-04. Сложение колебаний. Биения  17. МодК-06. Гармонический анализ  18. МодК-07. Связанные колебания.  19. МодК-05. Вынужденные колебания.  го  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины результат Виды учебной деятельности ee обучения по иль уч es времени, 4. дисциплине Лекции 16 Раздел 1. Электромагнитные волны. РД1,РД2, Практические занятия Волновая оптика РДЗ,РД4 Лабораторные занятия 8 Самостоятельная работа 40 Лекции 16 Раздел 2. Квантовая физика. Физика РД1,РД2, Практические занятия 8 атомов, молекул, атомного ядра и РДА,РДЗ Лабораторные занятия 8 элементарных частиц Самостоятельная работа 40  Содержание разделов дисциплины:  Раздел 1. Электромагнитные волны. Волновая оптика  Дифференциальное уравнение для электромагнитной волны и его решение. Корпускулярно-волновой дуализм свойств света. Волны оптического диапазона (световые волны) — частный случай электромагнитных волн. Интерференция плоских монохроматических световых волн. Когерентность (временная и пространственная). Методы получения когерентных световых волн и наблюдения интерференции. Дифракция света. Принцип Гюйгенса-Френеля. Дифракция Френеля и Фраунгофера. Дисперсия света. Классическая теория дисперсии. Поглощение света. Рассеяние света. Поляризация света при отражении. Интерференция поляризованных лучей. Тепловое излучение и его характеристики. Законы теплового излучения (Кирхгофа, Стефана-Больцмана, Вина). Квантовая гипотеза Планка. Формула Планка.  Темы лекций:  1. Электромагнитные волны и их свойства  2. Интерференция волн, сложение волн. Энергия волны 3. Интерференция света  4. Дифракция света. Метод зон Френеля  5. Дифракция света, дифракционная решетка  6. Поляризация света  7. Дисперсия, поглощение света  8. Тепловое излучение  Темы практических занятий: 1. Интерференция света 2. Дифракция Френеля и Фраунгофера. 3. Поляризация света 4. Тепловое излучение  Названия лабораторных работ: О-01. Определение главного фокусного расстояния тонких линз. О-03. Измерение показателя преломления жидкости с помощью рефрактометра. О-04. Исследование явления дисперсии света. О-09. Интерферометр Майкельсона. О-07. Измерение постоянной Планка спектрометрическим методом. О-10. Измерение световой волны и радиуса кривизны линзы с помощью колец Ньютона. 7. О-22. Исследование дифракции света на периодических структурах  хин  4  8. O-11. Измерение длины световой волны с помощью дифракционной решетки.  9. O-14. Определение постоянной Стефана-Больцмана и постоянной Планка при помощи оптического пирометра с исчезающей нитью.  10. О-15. Изучение внешнего фотоэлектрического эффекта и определение постоянной Планка.  11. O-23. Опыт Юнга.  12. О-06. Интерференция света от когерентных точечных источников.  13. О-16. Определение скорости света  14. О23. Изучение дифракции света на периодических структурах  15. О-04. Изучение зависимости показателя преломления призмы от длины волны света  16. МодО-01. Нормальная дисперсия.  17. МодО-02. Аномальная дисперсия.  18. О-10. Измерение длины световой волны и радиуса кривизны линзы с помощью колец Ньютона  19. О-12. Определение длины световой волны интерференционным методом с помощью бипризмы Френеля.  Раздел 2. Квантовая физика. Физика атомов, молекул, атомного ядра и элементарных частиц  Световые кванты. Энергия, импульс и масса фотонов. Фотоэффект и его законы. Уравнение Эйнштейна для фотоэффекта и экспериментальные методы его проверки. Эффект Комптона. Давление света. Корпускулярно-волновой дуализм материи и его опытное обоснование. Гипотеза де Бройля. Соотношение неопределенностей. Волновая функция и ее статистический смысл. Уравнение Шредингера (временное и стационарное). Частица в одномерной потенциальной яме. Туннельный эффект. Элементы зонной теории кристаллов. Уровень Ферми. Физические основы методов контроля качества материалов. Ядерная модель атома. Атом водорода по теории Бора. Пространственное квантование. Спин электрона. Атом водорода по теории Шредингера. Многоэлектронные атомы. Принцип Паули. Периодическая система элементов Д.И. Менделеева. Молекулы. Молекулы водорода. Обменное взаимодействие. Радиоактивность. Радиоактивное превращение ядер. Ядерные реакции и их основные типы. Искусственная радиоактивность. Цепная реакция деления. Ядерный реактор. Проблема управляемых термоядерных реакций. Экологические вопросы современной энергетики.  Иерархия структур материи. Частицы и античастицы. Фотоны, лептоны, адроны (мезоны, барионы, гипероны). Фундаментальные взаимодействия. Систематика элементарных частиц.  Темы лекций:  . Элементы квантовой механики  . Уравнение Шредингера и его применение  . Уравнение Шредингера и его применение, туннельный эффект . Классическая теория строения атома  . Элементы физики твердого тела  . Многоэлектронные атомы  . Элементы ядерной физики  . Элементарные частицы и их свойства  © чмилффь-  Темы практических занятий:  1. Фотоэффект, эффект Комптона  2. Атом водорода  3. Состав и характеристики атомных ядер. Радиоактивность.  5 4. Ядерные реакции. Элементарные частицы и их свойства  Названия лабораторных работ: О-07. Измерение постоянной Планка спектрометрическим методом. О-22. Исследование дифракции света на периодических структурах А-01. Опыт Франка и Герца А-02. Статистика счета элементарных частиц О-23. Опыт Юнга. О-06. Интерференция света от когерентных точечных источников. О-16. Определение скорости света 023. Изучение дифракции света на периодических структурах О-04. Изучение зависимости показателя преломления призмы от длины волны света  CRPANDMNRYWN&gt;S  5.</t>
+  </si>
+  <si>
+    <t>учебной деятельности  Основные виды  Формируемый рмиру .. Объем результат Виды учебной Разделы дисциплины времени, обучения по деятельности 4 дисциплине °  Раздел 1. Физическая культура в Лекции 2 общекультурной и профессиональной подготовке РД1 Практические занятия 4 студентов. Социально-биологические основы Самостоятельная работа 12 физической культуры/ Раздел 2. Основы здорового образа жизни Лекции 2 студента. Психофизиологические основы РД1 Практические занятия 4  чебного а и интеллектуальной РДЗ у труд У д Самостоятельная работа 12 деятельности. Раздел 3. Основы методики самостоятельных Лекции  анятий физическими . 3 физичес упражнениями. Общая РД? Практические занятия физическая и специальная подготовка в системе РДЗ физического воспитания Самостоятельная работа 12 Раздел 4. Спорт. Особенности занятий Лекции выбранным видом спорта или системы РД2 Практические занятия физических упражнений.  Профессионально- РДЗ  Самостоятельная работа 12  прикладная физическая подготовка студентов  Содержание разделов дисциплины:  Раздел 1. Физическая культура в общекультурной и профессиональной подготовке студентов. Социально-биологические основы физической культуры  Физическая культура и спорт как социальные феномены общества. Современное состояние физической культуры и спорта. Федеральный закон "О физической культуре и спорте в Российской Федерации. Физическая культура личности. Деятельностная сущность физической культуры в различных сферах жизни. Ценности физической культуры. Физическая культура как учебная дисциплина высшего профессионального образования и  целостного развития личности. Темы лекций:  1. Физическая культура в общекультурной и профессиональной подготовке студентов. Организм человека как единая саморазвивающаяся и саморегулирующаяся биологическая  система. Темы практических занятий:  1. Физическая культура в общекультурной и профессиональной подготовке студентов. 2. Социально-биологические основы физической культуры и спорта.  Раздел 2. Основы здорового образа жизни студента. Психофизиологические основы учебного труда и интеллектуальной деятельности.  Роль физической культуры в обеспечении здоровья. Здоровье человека как ценность и факторы, его определяющие. Здоровый образ жизни и его составляющие. Личное отношение к здоровью как условие формирования здорового образа жизни. Особенности использования средств физической культуры для оптимизации работоспособности, профилактики нервно- эмоционального и психофизического утомления студентов, повышения эффективности учебного труда с учетом возможных физических и функциональных ограниченных возможностей.  Темы лекций:  1. Основы здорового образа жизни студента. Психофизиологические основы учебного труда и интеллектуальной деятельности  Темы практических занятий:  1. Роль физической культуры в обеспечении здоровья.  2. Основные причины изменения психофизического состояния студентов, с учетом в период экзаменационной сессии, критерии нервного, эмоционального и психофизического утомления.  Раздел 3. Основы методики самостоятельных занятий физическими упражнениями. Общая физическая и специальная подготовка в системе физического воспитания  Мотивация и целенаправленность самостоятельных занятий с учетом физических и функциональных особенностей. Формы и содержание самостоятельных занятий. Организация самостоятельных занятий физическими упражнениями различной направленности. Характер содержания занятий в зависимости от возраста. Особенности самостоятельных занятий для женщин. Планирование и управление самостоятельными занятиями. Границы интенсивности нагрузок в условиях самостоятельных занятий у лиц разного возраста. Самоконтроль за эффективностью самостоятельных занятий.  Темы лекций:  1. Мотивация и целенаправленность самостоятельных занятий. Формы и содержание самостоятельных занятий. Организация самостоятельных занятий физическими упражнениями различной направленности  Темы практических занятий:  1. Роль средств физической культуры в регулировании работоспособности.  2. Организация самостоятельных занятий физическими упражнениями различной направленности. в период экзаменационной сессии, критерии нервного, эмоционального и психофизического утомления.  Раздел 4. Спорт. Особенности занятий выбранным видом спорта или системы физических упражнений. Профессионально-прикладная физическая подготовка студентов  Массовый спорт и спорт высших достижений, их цели и задачи. Особенности организации и планирования спортивной подготовки в вузе. Спортивные соревнования как средство и метод общей физической, профессионально-прикладной, спортивной подготовки студентов. обоснование индивидуального выбора студентом вида спорта или системы  4  физических упражнений для регулярных занятий. Краткая психофизиологическая характеристика основных групп видов спорта и систем физических упражнений  Темы лекций:  1. Краткая психофизиологическая характеристика основных групп видов спорта и систем физических упражнений. Массовый спорт и спорт высших достижений, их цели и задачи. Особенности организации и планирования спортивной подготовки в вузе.  Темы практических занятий:  1. Особенности занятий выбранным видом спорта или системы физических упражнений. Методика развития двигательных качеств. 2. Особенности занятий выбранным видом спорта или системы физических  упражнений. Классификация видов спорта. Классификация спортивных соревнований. Параолимпийские виды спорта.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Разделы дисциплины  Формируемый результат обучения по дисциплине  Виды учебной деятельности  Объем времени, ч.  Раздел 1. Организация и РД1 Лекции 4  управление производственными РД?  системами Практические занятия 10 Лабораторные занятия 0 Самостоятельная работа 18  Раздел 2. Бережливое РД1 Лекции 4  производство как основа РД2  системы непрерывных Практические занятия 8  лучшений  yay Лабораторные занятия 0 Самостоятельная работа 22  Раздел 3. Экономика РД1 Лекции 8  предприятия в отраслевом РД?  разрезе Практические занятия 14 Лабораторные занятия 0 Самостоятельная работа 16  Содержание разделов дисциплины:  Раздел 1. Организация и управление производственными системами  Организация производства:  предприятие как система.  Типы,  понятие,  формы  и методы  сущность, задачи. Производственное  организации производства.  Производство как процесс. Принципы организации производственного процесса. Классификация производственных процессов. Движение предметов труда в пространстве и во времени. Понятия: производственный цикл, производственная программа. Поточные линии и их применение в промышленности. Понятие и типы производственных систем.  Темы лекций:  1. Теоретические основы организации производства.Организация производственного процесса на предприятии.  2. Организация труда: понятия, элементы. Трудовой процесс: производственные функции и виды.  Темы практических занятий:  1.Структурное, функциональное описание предприятия.  2. Процессное описание предприятия.  3. Производственный цикл. Производственная программа.  4. Поточные линии на предприятии.Ритмичность производства.  5. Вспомогательные и обслуживающие процессы на предприятии.  Раздел 2. Бережливое производство как основа системы непрерывных улучшений  Основные понятия и принципы бережливого производства. Бережливое производство как основа системы непрерывных улучшений. Ценность и потери в производственных процессах. Система организации рабочего пространства и рабочего места сотрудника 5С. Основные инструменты бережливого производства. Картирование потока создания ценности. Стандартизированная работа. Разработка системы непрерывных улучшений.  Темы лекций:  1. Основные понятия и принципы бережливого производства. Ценность и потери в производственных процессах.  2. Основные инструменты бережливого производства.  Темы практических занятий: (Обучение проводится в имитационном учебном центре по Бережливому производству Фабрика процессов)  1.Система Кайдзен: построение производственного потока на рабочем участке. 2. Определение ценности и потерь в производственных процессах.  3. Система организации рабочего пространства и рабочего места сотрудника 5С. 4. Картирование потока создания ценности.Стандартизированная работа  Раздел 3. Экономика предприятия в отраслевом разрезе  Имущество предприятия и его состав. Понятие и сущность основных фондов предприятия. Состав и классификация основных средств по сферам производства, секторам экономики и отраслям. Оценка основных фондов предприятия. Износ и амортизация основных фондов предприятия. Показатели движения и эффективности использования основных фондов. Понятие и сущность оборотных средств предприятия. Классификация оборотных средств предприятия. Показатели эффективности использования оборотных средств предприятия. Нормирование оборотных средств предприятия. Понятие и сущность трудовых ресурсов, персонала, кадров предприятия. Классификация трудовых ресурсов предприятия. Показатели движения трудовых  ресурсов предприятия. Показатели эффективности использования трудовых ресурсов предприятия. Понятие и сущность заработной платы. Формы оплаты труда. Системы оплаты труда. Сущность понятий «расходы», «затраты», «издержки». Классификации затрат предприятия в отраслевом аспекте. Понятие себестоимости продукции (услуг). Расчет себестоимости по экономическим элементам затрат. Сущность и методы калькулирования себестоимости продукции. Доход предприятия, его сущность и значение. Прибыль и ее виды. Распределение и использование прибыли. Рентабельность предприятия. Сущность экономической эффективности. Виды эффективности. Дисконтированные и статические показатели эффективности. Методы расчета показателей сравнительной эффективности.  Темы лекций:  1. Ресурсы предприятия: состав, характеристика и показатели эффективности их использования.  2. Затраты предприятия, расчет себестоимости продукции  3. Финансовые результаты деятельности предприятия и оценка ее эффективности  4. Экономическая эффективность технических решений  Темы практического занятия:  1. Основные средства предприятия  2. Оборотные средства предприятия  3. Организация и оплата труда  4. Классификации затрат предприятия и калькулирование себестоимости продукции  5. Финансовые результаты деятельности предприятия  7. Основы оценки эффективности вложений в технику и технологию (улучшения на производстве)  Тема курсового проекта: «Планирование ресурсов и расчет финансовых результатов производства продукции»  Структура курсового проекта:  1. Описание технологического процесса и определение объемов производства .  2. Расчет первоначальной стоимости и амортизации оборудования  3. Расчет потребности в трудовых ресурсах и суммы заработной платы  4. Расчет потребности в материальных ресурсах и прямых затрат на материалы  5. Расчет себестоимости продукции  6. Расчет финансовых результатов от производства продукции за период  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения о Виды учебной деятельности времени, 4. дисциплине Лекции 8 Раздел 1. Современные методологии ¥ PAI Лабораторные занятия 12 командной разработки ПО Самостоятельная работа 34 Лекции 8 Раздел 2. Проектирование и реализация д р Ир р к РД2, РДЗ Лабораторные занятия 12 ПО в составе команды Самостоятельная работа 34 Содержание разделов дисциплины: Раздел 1. Современные методологии командной разработки ПО  В рамках раздела рассматриваются общие вопросы командообразования в теории управления. Приводится критический обзор таких методологий командной разработки программного обеспечения как MSF, SCRUM, КАМВАМ и FDD.  Темы лекций:  1. Microsoft Solutions Framework. Основные компоненты и принципы методологии.  Методология Feature Driven Development и АзПе-манифест.  Вопросы командообразования в теории управления.  Названия лабораторных работ:  2. Microsoft Solutions Framework. Управление проектом, рисками и подготовкой. 3. Методология гибкой разработки программного обеспечения SCRUM.  4. Методология KANBAN и критика АэПе-методологий. 5  6  1. Выявление требований к разрабатываемому программному обеспечению. 2. Формирование технического задания на разработку программного обеспечения. 3. Формирование календарного плана работ.  4. Управление рисками. Раздел 2. Проектирование и реализация ПО в составе команды  Раздел формирует навыки проектирование и реализации программного обеспечения в составе команды. Рассматриваются вопросы работы с системами управления версиями, проектирования высокоуровневой архитектуры и отдельных программных модулей.  Темы лекций:  7. Конструирование программного обеспечения. 8. Управление командной разработкой программного обеспечения. Системы  управления версиями. Названия лабораторных работ:  Проектирование модулей ПО. Тестирование и сборка ПО.  юн  Настройка системы управления версиями. Распределение ролей. Проектирование архитектуры разрабатываемого ПО.  Формирование программной документации.  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый Разделы дисциплины бучения no Виды учебной деятельности о а. дисциплине  Раздел 1. Основные положения Лекции 10 системного подхода для . PIU, РД2 Лабораторные занятия 12 формализованного описания предметной ?  области средствами ИТ Самостоятельная работа 40 Раздел 2. Применение методов и средств Лекции 22 ИТ для формализованного описания РДЗ, РД4 Лабораторные занятия 20 предметной области Самостоятельная работа 76  Содержание разделов дисциплины: Раздел 1. Основные положения системного подхода для формализованного описания предметной области средствами ИТ Базовые понятия системного анализа. Понятие информационных технологий (ИТ). ИТ как инструмент для достижения бизнес-целей предприятия. Понятие информационной системы (ИС). Структура и категории ИС. Единое информационное пространство предприятия. Технологии взаимодействия информационных систем. Современные тенденции в развитии ИТ. Темы лекций: 1. Многообразие информационных технологий и систем. Базовые понятия теории систем. 2. Управление проектами. 3. Процессный подход к управлению. 4. Организационная структура предприятия.  Названия лабораторных работ:  1. Разработка проекта ИТ-комплекса предприятия.  2. Разработка плана выполнения индивидуального проекта.  3. Определение бизнес-процессов предприятия.  4. Разработка оргструктуры предприятия.  Раздел 2. Применение методов и средств ИТ для формализованного описания  предметной области  Методологии и виды моделирования предметной области. Основы бизнес- моделирования. Нотации моделирования. Основные понятия и области применения. Система сбалансированных показателей. Стратегические карты. Диаграмма Исикавы. Техническое задание на ИС.  Темы лекций: Структурный анализ и бизнес-моделирование. Методы и средства функционального бизнес-моделирования. Планирование и анализ. Введение в имитационное моделирование и функционально-стоимостный анализ. Автоматизация бизнес-процессов. Названия лабораторных работ: 5. Разработка диаграмм бизнес-процессов в формальных нотациях. 6. Определение показателей процессов. 7. Разработка стратегической карты. 8 9 1  ю®юнчал  Разработка диаграммы Исикавы. . ИМиФСА бизнес-процесса предприятия. 0. Разработка ТЗ на ИС.  5.</t>
+  </si>
+  <si>
+    <t>Содержание этапов реализации дисциплины: № Этапы реализации дисциплины, и семестра краткое содержание (виды работ) обучения 1:2 Подготовительный этап: PAS — Выбор темы и обоснование необходимости решения задачи. Определение целей и РД1 задач. Формирование программы исследования. Выбор программного обеспечения, средств разработки и тд. Подготовка отчета и выступление с докладом в виде презентации по результатам работы. 2; 3 Научно-исследовательская работа: РД5 — Изучение литературы. Сбор, обработка данных и обобщение данных. Объяснение РД2 полученных результатов и новых фактов. Проектирование архитектуры приложения, РДЗ информационной системы, разработка алгоритмов и т.д. Формулировка выводов. РД4 Подготовка отчета и выступление с докладом в виде презентации по результатам работы. 3; 4 Проектная работа: РД? — Программная реализация и тестирование проекта. Проведение исследования РДЗ разработанных алгоритмов. Обработка новых данных. Подготовка отчета и РД4 выступление с докладом в виде презентации по результатам работы. РД5  5.</t>
+  </si>
+  <si>
+    <t>Основные виды учебной деятельности  Формируемый результат . Объем Разделы ДИСЦИПЛИНЫ обучения 7 Виды учебной деятельности времени, 4. дисциплине Лекции 2 Раздел 1. Погрешности численных .. РД-1 Лабораторные занятия 2 решений Самостоятельная работа 12 Лекции 4 Раздел 2. Численное интегрирование РД-2, РД-3 Лабораторные занятия 4 Самостоятельная работа 15 Лекции 6 Раздел 3. Численные методы решения д и дыр РД-2, РД-5 Лабораторные занятия 10 задач линейной алгебры Самостоятельная работа 17 Раздел 4. Численное решение нелинейных Лекции 4 уравнений и систем нелинейных РД-2, РД-4 Лабораторные занятия 6 уравнений Самостоятельная работа 17 Раздел 5. Численные методы решения Лекции 4 обыкновенных дифференциальных РД-2, РД-6 Лабораторные занятия 4 уравнений Самостоятельная работа 12 Лекции 4 Раздел 6. Приближение функций и д р функц РД-2, РД-7 Лабораторные занятия 6 табличных данных Самостоятельная работа 15  Источники и  Содержание разделов дисциплины:  Раздел 1. Погрешности численных решений классификация  погрешностей.  Абсолютная  И  относительная  погрешности. Значащие и верные цифры. Погрешности элементарных вычислительных операций: суммы, разности, произведения, частного. Общий подход к оценке погрешностей  вычислительных алгоритмов. Темы лекций:  1. История развития вычислительной математики. Элементы теории погрешностей Названия лабораторных работ: 1. _ Оценка погрешности результата численного решения  Раздел 2. Численное интегрирование  Квадратурные формулы Ньютона-Котеса. Формулы прямоугольника, трапеции, Симпсона. Погрешность метода. Принцип Рунге для оценки погрешности интегрирования. Вычисление кратных интегралов. Метод статистических испытаний (Монте-Карло) в задаче  численного интегрирования. Темы лекций:  2. Численное интегрирование. Квадратурные формулы, формулы прямоугольников,  трапеций и Симпсона  3. Погрешность численного интегрирования. Вычисление кратных интегралов. Стохастические методы численного интегрирования. Названия лабораторных работ:  2. Численное интегрирование: формулы прямоугольников и трапеций.  3. Численное интегрирование: формулы Симпсона. Метод Монте- Карло.  Раздел 3. Численное решение нелинейных уравнений и систем нелинейных уравнений  Классификация нелинейных уравнений и систем. Трансцендентные и алгебраические уравнения. Схема решения нелинейного уравнения. Интервальные методы и теорема интервалов. Метод половинного деления, метод хорд, метод касательных, метод простой итерации. Алгоритмизация методов, условия применения, скорость сходимости, геометрическая иллюстрация.  Темы лекций:  4. Нелинейные уравнения. Общая схема решения нелинейных уравнений. Концепция интервальных методов. Процедуры ШИТ MathCad для решения уравнений и систем. Составление пользовательских программ в ШИТ MathCad.  5. . Концепция интервальных методов. Методы дихотомии, хорд для решения нелинейных уравнений.  6. Методы простых итераций и Ньютона для решения нелинейных уравнений. Решение систем нелинейных уравнений.  Названия лабораторных работ:  4. Интервальные методы решения нелинейных уравнений.  5. Итерационные методы решения нелинейных уравнений: метод касательных (Ньютона).  6. Итерационные методы решения нелинейных уравнений: и метод простых итераций (Якоби).  Раздел 4. Численные методы решения обыкновенных дифференциальных авнений  Классификация дифференциальных уравнений. Задача Коши и методы ее решения. Обусловленность задачи. Методы Рунге-Кутта - основная идея. Порядок точности методов. Области устойчивости. Методы Эйлера, Эйлера-Коши, Рунге-Кутта 4-го порядка. геометрическая иллюстрация и погрешность методов, автоматический выбор шага дискретизации.  Системы линейных дифференциальных уравнений. Задача Коши для системы дифференциальных уравнений и формулы Рунге-Кутта. Решение дифференциальных уравнений п-го порядка. Многошаговые методы решения дифференциальных уравнений.  Темы лекций:  7. Классификация дифференциальных уравнений. Задача Коши и методы ее решения. Методы РунгеКутта. Геометрическая иллюстрация и погрешность методов, автоматический выбор шага.  8. Системы линейных дифференциальных уравнений. Задача Коши для системы дифференциальных уравнений и формулы Рунге-Кутта. Решение дифференциальных уравнений п-го порядка.  Названия лабораторных работ:  7. Решение дифференциальных уравнений методами Рунге- Кутта 2 порядка.  8. Решение дифференциальных уравнений методами Рунге- Кутта 4 порядка.  9. Решение систем дифференциальных уравнений методами Рунге- Кутта.  Раздел 5. Приближение функций и табличных данных  Классификация задач аппроксимации. Критерий близости. Задача интерполирования. Полиномиальная интерполяция, чебышевские системы. Остаточный член и погрешность полиномиальной интерполяции. Выбор узлов интерполяции. Сплайн-интерполяция. Сглаживание и фильтрация данных. Метод наименьших квадратов. Уравнения регрессии, полиномиальная регрессия. Базисные функции.  Темы лекций:  9. Классификация задач аппроксимации: интерполяция, сглаживание, экстраполяция. Критерии аппроксимации. Показатели эффективности аппроксимации. Полиномиальная интерполяция, сплайн интерполяции.  10. Сглаживание экспериментальных данных регрессионными уравнениями. Сглаживание экспериментальных данных на основе МНК. Экстраполяция данных.  Названия лабораторных работ:  10. Аппроксимация данных на основе полиномиального регрессионного уравнения  11. Аппроксимация данных на основе метода наименьших квадратов  12. Прогнозирование временных рядов.  5.</t>
+  </si>
+  <si>
+    <t>Методология Data Mining; межотраслевой стандарт CRISP-DM; основные задачи обработки табличных данных.,Знакомство с аналитической платформой Loginom CE.,Основы языка Python (типы данных, операторы, объектно-ориентированное программирование, работа с файлами, обработка исключительных ситуаций, импорт модулей); основные структуры данных (кортеж, список, словарь, множество, строка); библиотека для выполнения численных расчётов numpy; библиотека обработки данных pandas; ,графическая библиотека matplotlib.,ABC-анализ, XYZ-анализ, FMR-анализ, RFM-анализ и их сочетания (описание алгоритма, рекомендации по настройке параметров алгоритмов, реализация в Loginom и Python).,Основные понятия теории вероятностей и математической статистики (функция распределения, плотность вероятностей, точечное и интервальное оценивание, проверка статистических гипотез); А/Б-тестирование (основные понятия, различные аспекты планирования А/Б-тестов и интерпретации результатов).,Основные понятия линейной алгебры (линейное пространство, евклидово пространство, линейный оператор, собственные векторы и собственные значения линейного оператора); SVD-декомпозиция; анализ главных компонент (алгоритм, интерпретация результатов, различные аспекты реализации метода главных компонентов).,Постановка задачи; различные варианты решения задачи регрессии; интерпретация результатов и оценка качества построенной модели; различные аспекты решения задачи регрессии (фиктивные переменные, нелинейные модели, анализ остатков).,Постановка задачи классификации; задача бинарной классификации; логистическая регрессия; интерпретация результатов логистической регрессии; оценка качества бинарной классификации; задача многоклассовой классификации; мультиноминальная регрессия; алгоритм наивного Байеса; оценка качества результатов решения задачи многоклассовой классификации.,Идея алгоритма построения дерева решений; методы оценки чистоты подмножеств; различные алгоритмы построения дерева решения (ID3, CART, CHAID); оценка качества работы дерева решения; оценка важности признаков; алгоритм Random Forest и подбор оптимальных значений его параметров.,Алгоритм градиентного спуска (принцип его работы, параметры); модификации алгоритма спуска; модель нейрона; многослойный персептрон; алгоритм обратного распространения ошибки; эвристики процесса построения и обучения нейронных сетей.,Постановка задачи кластеризации; виды расстояний и их свойства; алгоритм кластеризации k-means (описание, настройка параметров, свойства); обзор других популярных алгоритмов кластеризации и их свойства (иерархические алгоритмы, MeanShift, DBSCAN).,Работа с пропусками и выбросами; процедуры отбора факторов для включения в модель; работа с несбалансированными классами.</t>
+  </si>
+  <si>
+    <t>Тема 1. Business Analysis Key Concepts. Stakeholder theory: origin and progress,Тема 2. Stakeholders, their interests and values,Тема 3. Assessment of Stakeholders for Importance and Influence,Тема 4. Stakeholder mapping,Тема 5. Interacting with stakeholders,Тема 6. BPMN in stakeholder management</t>
+  </si>
+  <si>
+    <t>Понятие цепи поставок. Сетевая структура цепи поставок. Концепция управления цепями поставок (SCM – Supply Chain Management). Виды аналитики в управлении цепями поставок. Задачи цепей поставок и уровень абстракции. Аналитическая оптимизация и динамическое имитационное моделирование. Цифровые двойники цепей поставок. Цифровое управление цепями поставок (Digital SCM). Создание цифрового двойника цепи поставок в anyLogistix.,Дизайн сетевой структуры цепей поставок. Важность правильного размещения элементов цепи поставок. Подходы к решению задачи размещения объектов цепи поставок. Гравитационный анализ. Эвристический метод Ардалана. Метод критической точки. Метод калькуляции затрат. Бальная оценка (scoring model). Задача единого среднего (single median problem). Задача охвата (covering problem). Гравитационный анализ в anyLogistix (Greenfield Analysis – GFA). Определение оптимальной сетевой структуры в anyLogistix (Network Optimization – NO).,Запас как объект управления в цепи поставок (понятие запаса, виды запасов, две точки зрения на запас). Движение запаса в звеньях цепи поставок. Анализ статистики поведения запаса. Основные показатели состояния запаса. Группирование запасов, классификация запасов по степени значимости и вариативности потребительского спроса. ABC-анализ и XYZ-анализ, их совместное применение. Прогнозирование потребности в запасе (предиктивная аналитика). Модель Уилсона и ее модификации. Основные типы стратегий управления запасами. Многономенклатурные модели управления запасами. Управление запасами в интегрированных многоуровневых цепях поставок.,Планирование цепи поставок (стратегическое, тактическое, оперативное). Основы оптимизационного моделирования (статическая модель, динамическая модель, модель с неопределенностью). Классическая транспортная задача. Транспортная задача с промежуточными пунктами. Задача о назначениях. Планирование доставки мелкопартийных грузов в условиях крупного города. Интегрированные модели цепи поставок (транспортно-складская задача, производственно-транспортно-складская задача). Планирование материальных потоков в anyLogistix (Network Optimization – NO). Имитационный эксперимент в anyLogistix (Simulation).,Проблема неопределенности и риска в цепях поставок. Эффект хлыста (bullwhip) в цепях поставок и проблема устойчивости. Классификация логистических рисков. Комплексный подход к анализу рисков. Методы оценки рисков. Принятие логистических решений в условиях риска. Методы управления логистическими рисками (перераспределение и диверсификация, страхование, управление рисками финансового рычага в цепях поставок на основе моделей использования заемных средств, хеджирование и резервирование). Анализ рисков цепи поставок в anyLogistix, имитационное моделирование (Simulation).</t>
+  </si>
+  <si>
+    <t>Потребность в цифровой трансформации предприятия и возникающие проблемы. Основы архитектуры предприятия. Обзор основных методологий, стандартов и сводов знаний в области архитектуры предприятия. Языки описания архитектуры предприятия. Программные средства поддержки архитектурного подхода.,Основные элементы архитектурного подхода. Управление постоянными изменениями и трансформацией на основе архитектурного подхода. Повторное использование знаний при описании и разработке архитектуры предприятия.,Онтология предприятия. Аспекты и слои архитектуры как «полки» для размещения объектов. Метамодель и ее роль в практике управления архитектурой предприятия. Объекты бизнес-слоя. Объекты слоя информационных систем. Объекты технологического слоя. Сервисный подход к описанию и разработке архитектуры предприятия. Объекты расширений. Объекты для планирования перехода из текущей в целевую архитектуру предприятия. Объекты для моделирования физических элементов. Связи между объектами. Паттерны и классификации в архитектуре предприятия.,Связь заинтересованных сторон, артефактов и объектов. Начальный этап. Этап идентификации и анализа существующей архитектуры предприятия. Этап проектирования целевой архитектуры предприятия. Этап реализации и перехода. Этап оценки реализации архитектуры.</t>
+  </si>
+  <si>
+    <t>Тема 1. Стандарты аудита,Тема 2. Саморегулируемые организации в аудите (СРО),Тема 3. Виды аудита,Тема 4. Аттестация аудиторов,Тема 5. Внутренний и внешний аудит,Тема 6. Аутсорсинг в аудите,Тема 1. Согласование аудиторского договора,Тема 2. Цель и основные принципы,Тема 3. Оценка аудиторских рисков,Тема 4. Существенность и верификация в аудите,Тема 5. Классификация мошенничества и ошибки в аудите,Тема 1. Система внутреннего контроля (СВК),Тема 2. Использование системы внутреннего контроля для целей аудита,Тема 3. Тесты контролей,Тема 4. Представление отчетов о внутреннем контроле,Тема 1. Использование системы утверждений аудиторами и аудиторские доказательства,Тема 2. Аудиторские процедуры,Тема 3. Аудиторская выборка и иные способы тестирования,Тема 4. Аудит отдельных статей,Тема 5. Аудиторские методики с использованием ИТ-технологий,Тема 6. Работа экспертов,Тема 7.Трансформация финансовой отчётности (исправление ошибок),Тема 1. События после отчетной даты,Тема 2. Концепция непрерывности деятельности,Тема 3. Письменные заявления,Тема 4. Завершение аудита и итоговый обзор,Тема 5. Аудиторские заключения</t>
+  </si>
+  <si>
+    <t>Понятие базы данных. Понятие СУБД. Типы СУБД: настольные и многопользовательские (профессиональные). Примеры СУБД. Основные функции СУБД. Типовая организация СУБД. Понятие модели данных. Основные модели данных: иерархическая, сетевая, реляционная, объектная. Трехуровневая архитектура СУБД, трехуровневое представление данных. Логическая и физическая независимость данных.,Достоинства и недостатки реляционной модели. Базовые понятия: отношение, схема отношения, атрибут, кортеж, домен, первичный ключ, арность отношения, степень отношения. Фундаментальные свойства отношений. Ограничения целостности. Манипуляционная часть: реляционная алгебра и реляционное исчисление.,Цели проектирования. Понятие избыточных данных. Нормальные формы: свойства нормальных форм. Нормализация отношений. I, II, III нормальные формы.,Основные характеристики языка. Диалекты языка. Язык определения данных (DDL). Типы данных. Создание объектов баз данных. Работа с базой данных: создание, удаление, изменение. Работа с доменами. Работа с таблицами: создание, удаление, изменение. Ограничения целостности уровня столбца и уровня таблицы. Работа с индексами.,Работа СУБД в вычислительных сетях. Архитектура построения сетевых СУБД. Архитектура «файл-сервер» и «клиент/сервер». Двухуровневая и трехуровневая архитектура систем баз данных. Распределенная обработка данных. Модель удаленного доступа к данным. Модель сервера баз данных. Модель сервера приложений. Виды схем построение ИС распределенной обработки информации.,Средства создания таблиц баз данных. Организация связи с базами данных. Механизмы доступа к различным файлам базы данных. Современные механизмы организации доступа к базам данных.</t>
+  </si>
+  <si>
+    <t>Тема 1. Введение: История возникновения и исследования глобальных угроз, Базовые понятия безопасной жизнедеятельности,Тема 2. Опасности природного мира: Геолого-атмосферные опасности, Проблемы выживания в природной среде, Опасности животного мира, Микробные угрозы, чума, лепра и сифилис в истории человечества, Туберкулёз, грипп, ВИЧ, холера, тиф, оспа.,Тема 3. Техногенные и антропогенные опасности: Пожары и взрывы, бытовые опасности, Химическое, бактериологическое, ядерное оружие, аварии на техногенных объектах, Массовые беспорядки и криминальные угрозы, терроризм, Рискованный образ жизни.,Тема 4. Первая помощь пострадавшему: Действия при инсульте, инфаркте, травмах, ожогах и обморожениях</t>
+  </si>
+  <si>
+    <t>Тема 1. Основы управления организацией,Тема 2. Методы управления в международной организации.,Тема 3. Структура управления организацией.,Тема 4. Стратегическое управление международной организацией.,Тема 5. Современные тенденции в управлении международной организацией.</t>
+  </si>
+  <si>
+    <t>Цели и задачи образовательной программы. Структура учебного плана. Перечень дисциплин и практик.,Математические модели мотивации.,Социологический опрос на тему мотивации, выбора места обучения и будущих ожиданий. Обратная связь.,Встреча с представителями центра карьеры ИЭМ.,Тема 5. Деятельность центра предпринимательства,Встречи с представителями ведущих томских компаний и успешными выпускниками, направленные на формирование интереса к будущей профессии, осознания особенностей профессии, анализ студентами уровня соответствия личных качеств требованиям, предъявляемым к специальности.,Тема 7. Построение персональных траекторий развития студента.,Мастер класс «Тайм-менеджмент и стресс-менеджмент». Мастер класс по составлению резюме и портфолио</t>
+  </si>
+  <si>
+    <t>Тема 1. Роль языка в жизни людей и социальная значимость речевой культуры.,Тема 2. Речевое общение как форма взаимодействия между людьми. Модель коммуникации. Речевая этика.,Тема 3. Литературный язык как высшая форма национального языка.,Тема 4. Письменная и устная форма речи.,Тема 5. Качества грамотной речи. Выразительность речи.,Тема 6. Официально-деловой стиль языка,Тема 7. Термины и тематическая лексика дело-вой речи. Экономические термины. Клише и канцеляризмы.,Тема 8. Личные документы. Резюме, заявление, автобиография, расписка. Заполнение бланков, анкет и форм.,Тема 9. Служебные документы: типология, образцы, языковое оформление.,Тема 10. Правила и формулы делового этикета.,Тема 11. Лингвистические особенности рекламных текстов. PR-коммуникация.,Тема 12. Искусство публичной речи.,Тема 13. Культура спора. Приемы спора. Разновидности спора: дискуссия, полемика, эклектика и софистика.,Тема 14. Этико-лингвистические особенности телефонной коммуникации. Модели переговоров. Правила телефонных взаимодействий.,Тема 15. Деловое совещание: лингвистический аспект. Подготовка и этапы проведения совещания.,Тема 16. Интервью и собеседование: психолингвистические особенности.,Тема 17. Презентация: устный и письменный компоненты.</t>
+  </si>
+  <si>
+    <t>Идентификация числовых и категориальных переменных. Оценка пропущенных данных. Определение кардинальности категориальных переменных. Выделение редких категорий. Обнаружение линейных зависимостей. Обнаружение нормального распределения. Обнаружение выбросов.,Удаление наблюдений с пропусками. Заполнение средним или медианным значением. Заполнение модой или наиболее часто встречающимся значением. Замено пропусков произвольным значением. Замена пропусков значениями из хвостов распределения. Добавление индикатора пропущенного значения. Алгоритмы заполнения пропусков библиотеки scikit-learn.,Создание двоичных переменных методом one-hot encoding. Нюансы применения метода one-hot encoding для категорий с большим количеством уровней. Замена категорий порядковыми значениями. Замена категорий количеством или частотой встречаемости. Замена категориальных переменных с учётом среднего значения целевой переменной. Замена категорий на основе веса доказательства (Weight of Evidence). Группировка редких уровней. Кодирование на основе хеширования.,Замена значений путём логарифмирования, заменой значений на обратные величины, квадратные и кубические корни. Степенное преобразование числовой переменной. Преобразования Бокса-Кокса и Yeo-Johnson.,Разделение переменных на интервалы равной длины. Разделение переменных на интервалы на основе частоты встречаемости. Дискретизация на основе категориальной переменной. Дискретизация на основе алгоритма k-средних. Дискретизация с помощью деревьев решений.,Усечение выбросов на основе набора данных. Замена выбросов на максимальное/минимальное значения. Замена выбросов нулевыми значениями.,Извлечение компонент даты и/или времени из переменных типа datetime. Работа с временем в разных временных зонах.,Стандартизация на основе среднего и на основе разброса. Стандартизация на основе медианы и квантилей. Стандартизация на основе длины вектора.</t>
+  </si>
+  <si>
+    <t>Основные финансовые понятия; диверсификация портфеля ценных бумаг; определение зависимости между риском и прибылью; построение и интерпретация параметров модели ценообразования на основной капитал.,Основные понятия экономической теории стоимости и производства; вывод функции издержек на основе производственной функции Кобба-Дугласа; анализ эффекта не пропуска переменной.,Обзор методов учета изменений качества в ценовых индексах; анализ зависимости между ценой и качеством товара в данный момент времени, на временном интервале; гедонический метод моделирования индекса цен на компьютеры; различные аспекты, оценивания гедонических уравнений цен.,Модель человеческого капитала; моделирование различий в оплате труда; роль образования в человеческом капитале; моделирование повышение квалификации как инвестиции в человеческий капитал; виды и методы оценки дискриминации заработной платы.</t>
+  </si>
+  <si>
+    <t>Основные понятия системного анализа (модель, моделирование, адекватность модели, классификация моделей, понятие системы, типы моделей систем, статические и динамические свойства системы); основные понятия имитационного моделирования (этапы, модельное время, различные аспекты).,Задача моделирования случайных величин с заданными свойствами и методы её решения; популярные распределения случайных величин и ситуации, в которых они применяются.,Поток случайных событий и его свойства; понятие, состав и классификация систем массового обслуживания; графы состояний случайного процесса; стационарный пуассоновский поток событий и его свойства.,Уравнения Колмогорова в нестационарном и стационарных случаях; процессы гибели и размножения (определение, граф переходов, уравнения Колмогорова и их решение в стационарном случае).,Системы массового обслуживания (с отказами, с ожиданием, с одним и несколькими приборами обслуживания); граф переходов процесса; системы уравнений для финальных вероятностей состояний системы, их решение; вычисление прочих численных характеристик систем массового обслуживания (среднее время ожидания, пропускная способность, …).,Основные понятия языка программирования Java.,Диаграмм причинно-следственных связей (определение, назначение, правила построения); обратные связи и задержки; типовые паттерны развития динамических систем.,Основные понятия системной динамики; диаграммы потоков данных (определение, назначение, накопители, соединители, правила построения).,Основные понятия многоагентного моделирования (понятия агента, внешней среды); методы взаимодействия агентов между собой и с внешней средой; способы построения коллективов агентов.,Виды имитационных экспериментов (простой эксперимент, эксперимент для перебора параметров, оптимизационный эксперимент); подготовка и проведение экспериментов; механизмы протоколирования имитационных экспериментов и обработки полученных данных.</t>
+  </si>
+  <si>
+    <t>Экономическая сущность и виды инвестиций. Классификация инвестиций на макро- и микроуровне.,Инвестиционный процесс. Инвестиционная деятельность: понятие и механизм осуществления. Факторы, влияющие на инвестиционную деятельность. Объекты и субъекты инвестиционной деятельности. Отношения между субъектами инвестиционной деятельности. Инвесторы, заказчики, исполнители работ, пользователи объектов инвестиционной деятельности. Правовое обеспечение инвестиционной деятельности в России. Права и обязанности субъектов инвестиционной деятельности. Стабильность прав, возмещение убытков. Порядок прекращения или приостановления инвестиционной деятельности. Инвестиционные стратегии.,Источники финансирования инвестиционной деятельности, их состав, структура и общая характеристика.,Инвестиционный рынок: понятие и структура. Показатели состояния инвестиционного рынка: инвестиционный спрос, инвестиционное предложение, цена, конкуренция. Особенности изучения рыночной конъюнктуры инвестиционного рынка. Конъюнктурный цикл. Сегменты инвестиционного рынка. Рынок инвестиционного капитала. Рынок инвестиционных товаров. Рынок объектов реального инвестирования и рынок объектов финансового инвестирования. Виды финансовых посредников.,Инвестиционная политика как составная часть экономической политики государства. Цель и задачи инвестиционной политики, механизм ее реализации.,Государственное регулирование инвестиционной деятельности. Методы государственного регулирования и формы поддержки инвестиционной деятельности.,Инвестиционный климат как объект инвестиционного регулирования: сущность и значение. Факторы, оказывающие влияние на инвестиционный климат. Инвестиционная привлекательность. Инвестиционная активность. Методы оценки инвестиционного климата.,Понятие эффективности инвестиций. Методы инвестиционных расчетов, их классификация. Методы оценки инвестиций, не включающие дисконтирование: метод, основанный на расчете сроков окупаемости инвестиций; метод, основанный на определении нормы прибыли на капитал. Методы оценки инвестиций, основанные на дисконтировании: метод чистой текущей стоимости, метод внутренней нормы прибыли, дисконтированный срок окупаемости, индекс доходности. Инвестиционные риски, их виды и классификации, методы расчета.,Сущность и классификация инвестиционных проектов. Жизненный цикл инвестиционного проекта. Фазы развития жизненного цикла инвестиционного проекта. Предынвестиционная, инвестиционная и эксплуатационная фазы развития инвестиционного проекта, их содержание. Документы, включаемые в инвестиционный проект. Бизнес-план инвестиционного проекта, его содержание. Назначение бизнес-плана и его участники. Задачи бизнес планирования. Структура бизнес-плана. Эффективность и риски инвестиционных проектов: особенности анализа и оценки.</t>
+  </si>
+  <si>
+    <t>роль и значимость хобби и увлечений в жизни человека, личное свободное времяпровождение, экстремальные виды спорта.,структура семьи, родственные связи, особенности семейного уклада, распределение семейных обязанностей, семейные традиции.,образование в разных университетах, мотивы личного выбора ТГУ в качестве вуза для обучения, цель и характер высшего образования, структура и деятельность факультетов, история создания ТГУ, старые и новые традиции ТГУ.,значимость современного образования, личные краткие и долгосрочные цели, связанные с высшим образованием, студенческая жизнь, условия проживания в кампусе, расписание дня студента, история основных достопримечательностей Томска, перспективы развития города., личные особенности и предпочтения в питании, наименование продуктов и способов их приготовления, любимые блюда, способы приготовления еды, личная практика по соблюдению здорового питания., привычки в обращении с деньгами, личный жизненный опыт в отношении денег, управление личными финансами., опыт путешествий, проблемы экологии в контексте туризма и путешествий, основные виды городского транспорта и его характеристики, покупка билетов и заказ гостиницы., описание специфики работы друга/знакомого, личностные особенности в контексте выполнения работы, проблемы карьерного роста, карьерные планы, амбиции и умения для успешной профессиональной деятельности., проблемы школьного обучения, сложности изучения различных аспектов иностранного языка, способы/приемы изучения языка, практическое применение иностранного языка в различных коммуникативных ситуациях., благотворительность, социальная помощь в России и в мире, личное отношение к проблеме, описание сложной ситуации из социальной практики, истории успеха., наименования/описание электронных приборов и их функций, опыт использования электронных приборов в повседневной жизни, искусственный интеллект, перспективы его развития и использования., основные проблемы в окружающей среде, климатические изменения и причины загрязнения воды и воздуха на планете, альтернативные виды энергии, глобальное потепление, прогноз погоды., популярные виды спорта в мире, спортивные игры, предпочтения в занятии спортом, проблемы обмана/мошенничества в спорте., личные критерии выбора подходящей карьеры, виды привилегий от компании, преимущества академического отпуска, личностные факторы-характеристики важные для принятия на работу, опыт поиска работы, тактика для подготовки к интервью, собеседование о приеме на работу, правила написания резюме., основные виды организаций, виды статусных привилегий от компании, качественные характеристики стиля управления организации, позиции в компании, должностные обязанности, виды организационной культуры, стили делового общения., виды бизнес идей и критерии их успешности, потенциал разных продуктов, причины и обстоятельства для начала своего дела, правила создания нового бизнеса, характеристики успешного предпринимателя, причины успеха нового бизнеса в современном мире., положительные и отрицательные качества лидера, поведенческие стратегии лидера и участников команды, лидерские стили, поведение лидера в проблемных ситуациях, личностные качества, представления о себе как лидере в будущем., популярные действия и операции с деньгами, онлайн- платежи и перспективы этой формы, описание практики денежных затрат и сбережений, практика пользования банковскими услугами, возможные источники и их преимущества для начала нового бизнеса, правила базовой финансовой грамотности, прогноз событий /действий в экономике/бизнесе., цели и формы проведения рыночного исследования, задачи фокус-группы, маркетинговые стратегии, специфика люксового бренда, преимущества и недостатки онлайн маркетинга., практика поощрения, система мотивации в менеджменте, стили менеджмента, условия успешного и неуспешного проекта, описание стадий проекта, основные проблемы и пути решения в управлении проектом., культурные особенности в отечественном бизнесе/за рубежом, проблемные ситуации при межкультурном взаимодействии, проблемы адаптации к новой культуре, преимущества и недостатки работы/учебы за рубежом, правила делового этикета.</t>
+  </si>
+  <si>
+    <t>Поведенческие предпосылки институционального анализа. Ситуации, ведущие к появлению институтов. Механизмы принуждения. Функции институтов. Формальные и неформальные институты. Экстрактивные и инклюзивные институты. Институциональная среда и институциональные соглашения.,Разнообразие форм сделок: сущность, виды (Коммонс, Поланьи, Уильямсон) и свойства трансакций. Что стоит за трансакционными издержками: варианты определения базовой категории институциональной экономики «трансакционные издержки». Специфичность активов как важная характеристика трансакций. Схема Уильямсона. Неопределенность и формы управления трансакцией. Основные подходы к классификации трансакционных издержек. Факторы, влияющих на структуру и величину трансакционных издержек (Норт). Способы измерения трансакционных издержек на практике.,Специальные механизмы снижения рыночных трансакционных издержек: а) поиска информации об альтернативах сделки; б) измерения; в) ведения переговоров и заключения контракта; г) контроля за соблюдением контракта и предупреждения оппортунистического поведения; д) защиты контакта от третьей стороны,Значение прав собственности. Определение прав собственности. Теорема Коуза. Трагедия общин. Исключительные права собственности. Коллективная собственность. Частная, или эксклюзивная собственность. Государственная собственность. Эволюция прав собственности,Рынок и иерархия как типы контрактов. Какие факторы влияют на выбор типа контракта. Подход Р. Коуза к объяснению природы фирмы: сеть долгосрочных контрактов, центральный агент, границы фирмы. Подход О. Уильямсона: иерархия как механизм защиты от вымогательства. Квазирента и специфичность активов. Проблема вымогательства и факторы её обострения. Типы контрактов (классический, неоклассический и отношенческий) и альтернативные способы организации сделки. Границы вертикальной интеграции в модели фирмы. Трансакционные издержки внутри фирмы. Издержки влияния (П. Мильгром). Подход с позиций прав собственности,Смешанные формы контрактации. Основные формы гибридных соглашений. Модели решения проблемы гарантий специфических инвестиций,Понятие контракта. Контракт в юридическом и экономическом смысле. Понятие совершенного контракта. Причины неполноты контрактов. Проблема принципала-агента. Типы асимметрии информации (скрытые характеристики, скрытые действия/ скрытая информация и скрытые намерения) и виды оппортунистического поведения. Причины возникновения ухудшающего отбора: модель Акерлофа. Методы предотвращения ухудшающего отбора. На рынке труда (модель Спенса): подача сигналов и просеивание. На рынке кредита: рационирование кредитов,Факторы морального риска. Моральный риск на рынке труда и на рынке страхования. Методы противодействия моральному риску. Внешние и внутренние способы борьбы с моральным риском. Влияние эффективной зарплаты на стимулы работника к оппортунистическому поведению.,Агентские проблемы в организациях. Внутрифирменные правомочия по Алчиану и Демсецу. Типы фирм как институциональная альтернатива. Частнопредпринимательская фирма. Партнерство. Фирма, управляемая коллективом. Открытая корпорация. Закрытая корпорация. Государственная организация. Регулируемая фирма. Некоммерческая организация. Решение агентской проблемы с помощью стимулирующих контрактов.,Проблема безбилетника и коллективные действия. Социальные дилеммы. Типология экономических благ. Парадокс коллективных действий и группы интересов. Решение проблемы коллективных действий: уровень институциональных соглашений. Селективные стимулы. Решение проблемы коллективных действий: уровень институциональной среды. Социальный капитал. Компоненты социального капитала и подходы к измерению. Измерение социального капитала на примере доверия. Механизмы изменения социального капитала. Социальный капитал и экономический рост. Эффекты социального капитала. Меры по накоплению социального капитала.,Определение государства и его функций. Необходимость контроля насилия. Спонтанный экономический порядок. Устойчивость анархии: модель Хиршлейфера. Появление государства: бандиты-гастролеры и оседлый бандит. Контрактный подход к происхождению государства («синтетическая» или неоклассическая теория государства Д. Норта). Ограничения монопольной власти правителя. Дилемма присутствия государства в экономике. Переход от диктатуры к демократии.,Социальный контракт. Факторы разнообразия социальных контрактов. Государство и общество: агентские проблемы. Зависимость от налоговой базы. Законодательные ограничения. Угроза переворота или насилия. Политические режимы (авторитарные и демократические) и экономические результаты. Роль политических лидеров.,Экономическое развитие: факты и объяснения. Институциональная гипотеза. Эмпирические исследования институтов и роста. Проблема причинности и гипотеза модернизации. Роль неформальных институтов. Доверие как фактор роста и развития. Экономический рост и неравенство. Экономическое неравенство в разных странах. Взаимосвязь роста и неравенства.</t>
+  </si>
+  <si>
+    <t>Возникновение и развитие процессного подхода. Функциональный подход. Линейно-функциональная организационная структура. Концепции CPI, TQM, BPR, BPM, международные стандарты качества. Процессная организационная структура. Основные понятия процессного подхода. Классификация процессов.,Моделирование бизнеса: понятие модели, виды моделей, языки описания моделей, требования к нотации, классификация методологий моделирования бизнеса. Методологии моделирование бизнеса. Инструментальные средства моделирования бизнеса.,Анализ бизнес-процессов и окружения бизнеса. Анализ рисков бизнес-процесса. Совершенствование бизнес-процессов.</t>
+  </si>
+  <si>
+    <t>Сигналы, данные, информация. Дискретная и непрерывная информация. Средства реализации информационных технологий: алгоритмические, программные и технические.,Понятие системного блока и периферии, системная плата, процессор, шины данных, организация внутренней памяти (ОЗУ, ПЗУ, кэш-память, CMOS-память), ячейка, основы функционирования ЭВМ.,Виды внешней памяти, принципы представления информации в дисковой памяти, форматирование, логические и физические диски.,Понятие количества информации. Формула Хартли. Количество информации, содержащейся в m-разрядном сообщении. Понятие объема информации, единицы измерения объема информации.,Системы счисления. Основные типы данных и их представление: целые типы без знака и со знаком, способы представления целых со знаком (методы дополнительного кода и смещения), вещественные типы (форматы с фиксированной и плавающей точкой, вещественные с одинарной и двойной точностью), текстовые типы (строковые, символьные), логический тип (логические данные, выражения, операции). Кодирование графической информации: растровый принцип, понятие разрешения (оригинала, экранного и печатного изображения), растрирование изображения с амплитудной и частотной модуляцией; векторная графика; фрактальная графика; основные форматы представления графических файлов. Кодирование звуковой информации (методы частотной модуляции и таблично-волнового синтеза.,Основные типы структур данных (линейная, табличная, иерархическая). Файлы, каталоги; маршрут, спецификация файла; размещение файлов во внешней памяти, кластеры. Основные принципы хранения информации о размещении кластеров файлов (на основе таблицы размещения файлов FAT и на основе главной таблицы файлов MFT).,Назначение и виды компьютерных сетей (локальная, глобальная, интрасеть, виртуальная сеть), основные понятия. Структура глобальных сетей. Назначение и виды сетевого программного обеспечения (понятие логической архитектуры сети, одноранговая архитектура, архитектуры на основе сервера и «клиент-сервер»). Основные топологии локальных сетей (полносвязная, моноканальная, кольцевая , звездообразная) и методы доступа.. Основные особенности сети Internet; уровни адресации компьютеров сети (локальный адрес, IP-адресация, доменная система имен).,Определение алгоритма и особенности его описания, формы представления алгоритмов (словесно-формульная и структурная), основные алгоритмические структуры; требования, предъявляемые к алгоритмам.,Краткая характеристика основных классов программных средств (системное программное обеспечение, системы программирования, прикладное программное обеспечение).,Назначение и основные функции ОС, структура и особенности основных компонент ОС, режимы управления программами. Назначение программ технического обслуживания (утилиты). Архиваторы; программные вирусы и антивирусные программы; утилиты обслуживания внешней памяти.,Назначение и состав систем программирования. Назначение и основные особенности языков программирования, основные особенности языков низкого и высокого уровня. Основные принципы, лежащие в основе различных групп языков программирования высокого уровня: алгоритмический, структурный (понятия программы, подпрограммы и функции, модульное программирование), событийно-ориентированный, объектно-ориентированный (понятия класса, объекта, инкапсуляции, наследования и полиморфизма). Особенности специализированных языков программирования: декларативные, языки программирования баз данных, языки разметки, языки программирования для Internet.,Назначение, виды прикладного программного обеспечения, их основные особенности.,Отличительные особенности данных и знаний; понятия экстенсиональной и интенсиональной информации; сильно типизированные и слабо типизированные модели информации. Определение базы данных; внешняя, концептуальная и внутренняя модели; этапы разработки базы данных.,Понятие абстракции, обобщение, агрегация, наследование свойств. Понятия множества и кортежа, требования к их оформлению; понятия домена и атрибута; интенсионал и экстенсионал атрибута; экземпляр, ключи (возможные, составные, первичные, внешние).,Табличное представление данных (реляционные таблицы и таблицы записей, их использование в моделировании данных); представление данных в виде графа (понятие графа, представление типов и экземпляров объектов и связей).,Понятия декартова произведения и отношения. Бинарное, тернарное, n-арное отношение. Интенсиональное и экстенсиональное описание отношения. Применение отношения в моделировании данных. Понятие отображения, прямое и обратное отображение, полное и частичное отображение, кардинальные числа; виды связей (взаимно однозначная, функциональная и “многие-ко-многим”) и их описание.,Реляционная, иерархическая и сетевая модели; их положительные особенности и недостатки; представление интенсионала и экстенсионала этими моделями; распространение ключа.,Внутренние, явные и подразумеваемые ограничения; ограничения, задаваемые на отображениях.,Основные особенности, запуск, структура окна, панель быстрого доступа, лента, контекстное меню, абзац.,Основные режимы, главное меню, управление лентами, настройка панели быстрого доступа, ввод документа, загрузка и сохранение файлов, экспорт и импорт файлов; подготовка документа к печати,Выделение (мышью и клавиатурой), удаление, перемещение и копирование (мышью и с помощью универсального буфера обмена) фрагментов; установка шрифта; форматирование; обрамление и “заливка”; поиск и исправление ошибок; стиль оформления.,Вставка таблицы; вставка, удаление и изменение размеров строк, столбцов и ячеек; оформление таблицы; объединение и разбиение ячеек; использование инструментальных панелей работы с таблицей и рисунком; способы рисования и работы с готовыми рисунками.,Основные особенности, запуск, структура окна, работа с главным меню команд, лентами, листами и окнами, структура таблицы, содержимое и значения ячеек, способы адресации.,Выделение областей (в том числе – мультивыбор) мышью и клавиатурой, копирование и перемещение (мышью и с помощью универсального буфера обмена), форматирование ячеек; автозаполнение; сохранение и загрузка файлов.,Типы данных, формулы, использование относительной и абсолютной адресации, форматирование таблицы.,Функция, Мастер функций, использование имен, локальные и глобальные имена, формула массива.,Основные понятия, формирование базы данных, критерии поиска, поиск и выбор данных, сортировка данных.,Мастер диаграмм, создание и редактирование диаграмм; особенности гистограмм, графиков, круговых диаграмм.,Основные особенности VBA. Типы данных, константы, переменные, массивы, выражения. Особенности работы в среде программирования Visual Basic Editor (VBE).,Понятие оператора, структура оператора, описание переменных, способы организации ввода и вывода данных.,Назначение и структура цикла, виды циклов, описание циклов.,Понятие ветвления, условный оператор, операторы безусловного перехода и выбора.,Понятия подпрограммы и функции, оформление подпрограммы и функции, операторы вызова подпрограммы и функции.,Модуль и его атрибуты, импорт модуля и его атрибутов. Структура инструкции (оператора). Пользовательские функции. Константы и переменные в Python. Способы организации ввода и вывода данных.,Основные типы данных, динамическая типизация, функции преобразования типов. Арифметические и логические выражения. Виды последовательностей (список, кортеж, множество, диапазон, словарь). Понятие среза последовательности. Операторы работы с последовательностями. Способы присваивания (присваивание значения, групповое и позиционное присваивание, присваивание списка части элементов).,Оператор альтернативного ветвления, множественный выбор. Ветвление с присваиванием. Цикл для выполнения действий с элементами последовательностей. Цикл с предусловием. Операторы прерывания цикла и итерации. Генератор списка, вложенные генераторы.</t>
+  </si>
+  <si>
+    <t>Тема 1. Научно-исследовательская деятельность: понятие, содержание и этапы. Критерий FINER.,Тема 2. Экспертные методы сбора информации. Методология поиска и анализа научной и статистической информации. Понятие «информационный суррогат», последствия его использования в научно-исследовательской деятельности. ,Тема 3. Методы научного исследования. Классификация методов экономических исследований. Аналитический и синтетический методы. Исторический метод. Эволюционный метод. Наблюдение и эксперимент. Статистические и математические методы. Метод моделирования.,Тема 4. Принципы и правила представления исследования в виде научной статьи или доклада. Требования к устной презентации с интерактивным сопровождением. Требования к оформлению результатов НИР.,Тема 1. Типы и области экономических исследований. Особенности теоретических, эмпирических и обзорных исследований.,Тема 2. Составные части процесса эмпирического экономического исследования: гипотеза, программа, отчёт.,Тема 3. Сбор, хранение и обработка исходных данных. Протокол обработки данных. Вычислительный эксперимент. Протокол вычислений. Подготовка иллюстраций, таблиц, сводных результатов. Автоматизация подготовки отчёта с результатами вычислительных экспериментов.,Тема 4. Инструменты представления результатов вычислительных экспериментов: язык разметки Markdown, блокноты Jupyter, система подготовки отчётов knitr. Публикация результатов исследований в World Wide Web</t>
+  </si>
+  <si>
+    <t>Предмет истории. Задачи исторической науки. Научные принципы изучения прошлого. Концепции исторического развития. Методы научного познания.,Понятие исторического факта. Классификация фактов. Классификация исторических источников. Проблема подлинности и достоверности исторических источников.,Понятие периодизации. Виды периодизаций в различных концепциях исторического развития. Периодизация истории России. Краткая характеристика основных периодов в истории человечества.,Условия становления российской цивилизации: между Западом и Востоком. Древняя Русь, Запад, Золотая Орда: характер отношений. Становление Русского (Московского) централизованного государства.,Великие географические открытия и их историческое значение. Реформация и контрреформация в Европе. Становление национальных государств. Первые буржуазные революции. Модернизация России в эпоху Петра Великого.,Промышленный переворот в Европе и его экономические, политические и социальные последствия. Великие (буржуазные) реформы в России во второй половине XIX в.,Особенности социально-экономического и политического развития мира и России на рубеже веков. Первая российская буржуазно-демократическая революция. Политические партии в России. Зарождение парламентаризма.,Причины, характер и особенности мировой войны. Февральская революция 1917 г. и крушения монархии. Октябрьская революция 1917 г. и установление Советской власти. Начало советского периода в истории России. Гражданская война в стране.,Новая экономическая политика. Образование СССР. Социалистическая индустриализация. Коллективизация сельского хозяйства. Политический режим. Массовые политические репрессии. Причины Второй мировой войны. Великая Отечественная война 1941-1945 гг. Источники и цена Победы.,Основные тенденции мирового развития во второй половине XX столетия. «Холодная война». «Перестройка» в СССР 1985-1991 гг. и распад Советского Союза. Становление современной Российской Федерации. Мир и Россия в начале XXI в.</t>
+  </si>
+  <si>
+    <t>Типология картин мира. Кто мы? Откуда? Куда идем? Человек в эпоху неопределенности. Проблема будущего. Техногенная цивилизация: вызовы, опасности против возможностей. Как сознание моделирует мир? Когнитивные науки. Когнитивные модели реальности (ментальные карты): “карта и местность”. Системный подход. Эволюция Вселенной: материя – живая материя — мыслящая живая материя.,Физическая картина мира – смена парадигм от античности до 19 века. Классическая механика. Электромагнитная парадигма.,Современная квантово-релятивистская парадигма.,Наука о жизни. Живая материя, науки о жизни. Происхождение и сущность жизни. Теория эволюции.,Генетика. Генные и клеточные биотехнологии. Биоэтика. Биополитика.,Сознание в контексте антропогенеза: коммуникация, труд, культура. Природа и воспитание.,Этология, социобиология. Когнитивные науки о человеке: мозг и сознание.,Понимание техники.Техника, технология, технические науки.Специфика инженерного знания,Виды схем. Метод кейсов. Современные инструменты мультимедиа для презентации и создания схем.,Закономерности развития в природе и технике, технический прогресс и его этапы, революционный и эволюционный путь развития, промышленные революции.,Модель черного ящика, обратная связь, кибернетика как наука, энтропия. Алгоритм, язык, свойства. Управление, алгоритм управления системой.,Прикладной системный анализ, задачи, этапы, методы принятия решений. Пример решения проблемы применением системного анализа.,Признаки 4-й революции, мегатренды - цифровое направление, физическое, биологическое. Естественный и искусственный интеллект - определение, признаки. Сильный и слабый искусственный интеллект - критерии.,Факторы эволюции человечества, биологическая и техногенная составляющая. Джереми Рифкин - анализ книги “Третья промышленная революция”.,Течение трансгуманизма - его значение, путь развития, причины возникновения. Технологическая сингулярность. Дикарь цифровой эпохи. Влияние цифровой эпохи на естественный интеллект.,Становление социологической науки. Социальный факт Э. Дюркгейма. Понимающая социология М. Вебера. Социальное действие.,Понятие модернизации. Глобализация. Мир-системная теория. Глокализация. Социальная идентичность. Экзистенциальный абсурд.,Понятие постмодернизма как состояния общества. Понятие ризомы как модели общества. Понятие сетевого общества. Основы акторно-сетевой теории.,Семиотика искусства. Понятие знака. Типологии знаков. Знаковые системы: код и текст. Понятие рамки.,Структура коммуникации. Интенции автора и интенции текста. Интенциональность реципиента. Методика семиотического анализа художественного текста.,Эстетика как наука. Эстетические эмоции. Эстетическое отношение. Методика эстетического анализа художественного текста.,Искусство первой половины ХХ века в контексте научных открытий, технических изобретений и социальных изменений. Искусство как миромоделирующая система.,Содержание и границы понятия “современное искусство”. Искусство эпохи модерна и постмодерна. Постмодернизм: игры с хаосом. Границы искусства и понятие арт-практик. Концепция тотального искусства.,Феномен Art&amp;Science (SciArt): между искусством, наукой и технологиями. Наука и техника: новые форматы современных арт-практик. Методика анализа “tabula rasa”. Проблема в науке и в искусстве: специфика подходов. Сущность художественного образа. ,Групповая работа над решением кейса,Групповая защита кейса,Инвалид: основные подходы к определению понятия. История отношения к людям с инвалидностью: от античности до современности. Понимание инвалидности через отклонение от нормы. Движения за права инвалидов как фактор смены подхода к пониманию инвалидности,Инвалид: основные подходы к определению понятия. История отношения к людям с инвалидностью: от античности до современности. Понимание инвалидности через отклонение от нормы. Движения за права инвалидов как фактор смены подхода к пониманию инвалидности,Технические средства реабилитации индивидуального пользования: костыли, трости, инвалидные коляски, протезы, слуховые аппараты, кохлеарные импланты, очки. Новые подходы к индивидуальному протезированию: бионические протезы, очки виртуальной реальности, синтезаторы речи. Возможности применения технологий для всех людей. Трансгуманизм: возможности и риски.,Доступная среда: подходы к определению и основные способы организации. Нормативно-правовые основания формирования доступной среды. Критерии оценки уровня доступности среды. Исследование элементов доступности окружающей среды (практическая работа). Универсальный дизайн как перспективный способ организации доступной среды.,Эксклюзия как отражение социокультурных проблем общества. История включения ранее дискриминируемых групп в социум. Политика позитивных действий: преимущества и недостатки. Интеграция и инклюзия: сходства и различия. Перспективы инклюзивной культуры и инклюзивного типа мышления.,Правила взаимодействия с людьми с инвалидностью с учетом контекста взаимодействия. Ситуативная и целенаправленная помощь. Этические дилеммы в контексте проблематики инвалидности. Этические принципы включения людей с инвалидностью в общественные процессы. Основные правила взаимодействия с людьми с инвалидностью.,Значимость образа человека с инвалидностью для формирования инклюзивного общества. Фестиваль «Кино без барьеров». Образы людей с инвалидностью в российском и зарубежном кинематографе. Спортивные достижения людей с инвалидностью.,Общие подходы к подготовке информационных материалов по проблематике инвалидности. Правила и ошибки при подготовке информационного материала: стилистические, графические, художественные возможности оформления.,Представление итогов групповой домашней работы с учетом следующих требований: задание, подготовка информационного материала (контент-план, серия публикаций в социальной сети, информационный плакат, ролик) по одной из тем, изучаемых в рамках курса. Критерии оценки: соответствие проблематике; корректность используемой информации / отсутствие ошибок; полезность / целенаправленность; доступность для читателя / зрителя; оригинальность задумки и подачи.</t>
+  </si>
+  <si>
+    <t>Тема 1 Введение в корпоративную социальную ответственность и этику бизнеса,Тема 2 Модели корпоративной социальной ответственности,Тема 3 Стандарты корпоративной социальной ответственности,Тема 4 Корпоративная социальная политика,Тема 5 Управление корпоративной социальной ответственностью</t>
+  </si>
+  <si>
+    <t>Определение и основные особенности экономической информационной технологии, методы обработки экономической информации; глобальная, базовые и конкретные информационные технологии. Особенности экономической информации.,Определение и основные особенности экономической информационной системы, роль и место автоматизированных информационных систем в экономике; уровни управления (стратегический, управленческий, информационный, операционный).,Объект и субъект управления, информационные взаимосвязи между ними); информационный контур управления; модель управления в компании. Понятие информационного менеджмента. Основные особенности использования внешней и внутренней информации на разных уровнях управления. Основные принципы построения и функционирования экономической информационной системы.,Понятие корпоративной информационной системы. Основные особенности создания и построения корпоративной информационной системы. Основные задачи, решаемые при реализации корпоративной информационной системы. Базовая функциональность корпоративной информационной системы.,Проблемы управления внедрением корпоративной информационной системы, планирование формирования информационной системы. Основные методики оценки информационных потребностей (анализ деятельности предприятия и определение критических факторов успеха), их достоинства и недостатки. Автоматизация, рационализация, реинжиниринг и смена парадигмы как основные способы организационных изменений. Технологии потока работ (Workflow).,Системная разработка и ее основные этапы. Конверсия, параллельная стратегия, стратегия прямого переключения, пилотная стратегия и фазовая стратегия конверсии. Управление эксплуатацией и техническим обслуживанием информационной системы. Методология «жизненного цикла», создание систем с помощью прототипа и пакетов прикладных программ, разработка конечными пользователями, аутсорсинг. Сравнение различных методов разработки и особенности управления системами.,Этапы развития стандартов управления бизнесом. Методология планирования потребностей в материалах MRP. Планирование производственных мощностей CRP. Планирование ресурсов производства MRP II. APICS. Планирование всех ресурсов предприятия ERP и ERP-системы. Планирование ресурсов во взаимодействии с покупателем CSRP и CRM-системы. Управление ресурсами и взаимодействиями предприятия ERP II и SCM-системы.,Инфраструктура и архитектура предприятия, метамодель организации. Основные особенности информационного менеджмента. Способы влияния организации на использование корпоративной информационной системы. Состав информационных служб. ИТ-инфраструктура (инфраструктура данных, техническая инфраструктура, программная инфраструктура), модели вычислительной и сетевой инфраструктуры.,Понятие угрозы безопасности информации; виды угроз; методы и средства защиты; шифрование информации, безопасность проведения расчетов.,Программные системы учета, аналитические системы, системы автоматизации управления.,Обзор базовых модулей ERP систем на примере программного продукта 1С: Предприятие: «1С: Управление предприятием»; «1С: Бухгалтерия»; «1С: Управление торговлей»; «1С: Зарплата и управление персоналом». Реализация корпоративного стиля управления предприятием: ведение разных видов учетов в единой информационной базе, обеспечение обмена данными, синхронизация данных.,Аналитические возможности программного продукта: прибыльность по товарам, направлениям деятельности; контроль денежных потоков и взаиморасчетов с покупателями, поставщиками; учет доходов, расходов и анализ финансового результата работы предприятия; налоги; отчетность.,Настройка программы. Настройка управленческого, налогового и бухгалтерского учетов.,Способы регистрации хозяйственных операций. Корреспонденция счетов (по документу).,Учёт основных средств. Учёт товарно-материальных ценностей. Учёт денежных средств и расчётов. Учёт расчётов с контрагентами. Учёт расчётов с подотчетными лицами. Банк. Касса. Аналитический учет. Операции. Документы. Отчетность.,Спецификация. Анализ информации о движении запасов. Выпуск готовой продукции.,Начисление заработной платы. Анализ расходов на оплату труда и начисленных налогов (взносов) с ФОТ.,Классификация производственных затрат. Аналитический учёт затрат. Учёт выпуска и реализация готовой продукции.,Подготовка к завершению периода. Закрытие счетов. Корректировка стоимости готовой продукции. Детализация регламентных операций.,Стандартные отчёты. Диаграммы. Регистры налогового учёта. Регламентированная отчётность. Создание регламентированных отчётов. Расшифровка показателей регламентированных отчётов. Проверка показателей регламентированных отчётов. Выгрузка регламентированных отчётов в электронном виде.</t>
+  </si>
+  <si>
+    <t>цели и задачи курса «Критическое мышление и письмо», его роль в структуре ядра. Интерактивная игра «Что такое мир?». Проблематизация понятий мир, картина мира, мировоззрение. Естественная и научная картина мира, рефлексия как основа различия естественной и научной картин мира. Типология картин мира: мифологическая, религиозная, философская, научная.,Что такое критическое мышление, быстрое мышление и медленное мышление, мышление солдата и мышление разведчика. Критическое мышление как практика рефлексии. Что значит слушать, что значит слышать. Правила осознанного слушания. Причины коммуникативных неудач. Упражнение «Слушать – слышать».,Краткое содержание темы. Что такое аргументация? Структура аргументации: тезис, аргумент, демонстрация. Логика и аргументация. Логический анализ аргументации. «Красная селедка». «соломенное чучело». Игра «Дилеммы».,Специфика вопроса как одной из основных составляющих рассуждения. Виды вопросов: настоящие и «ненастоящие вопросы». Закрытые и открытые вопросы. Типология вопросов Б. Блума. Пресуппозиции вопросов. Некоректные вопросы. Постановка проблем в виде вопросов. Проблемный и непроблемный вопрос.,Письмо как рефлексивная практика. Рефлексивное эссе. Структура эссе. Свободное письмо и структурирование текста. Ассоциации – как способ генерации облака смыслов. Правила фрирайтинга.,Понятие, слово, вещь. Объем понятия и содержание понятия. Отношение между понятиями: совместимость и несовместимость. операции над понятиями: обобщение и ограничение. определение понятий. Виды определения. правила определения. Ключевые слова и понятия.,Суждение как логическая форма. суждение и предложение. Структура суждения: субъект, предикат, связка. Суждение и тезис. Требования к тезису. Умозаключение и доказательство. Структура умозаключения и доказательства.,Паралогизмы, софизмы, парадоксы. правила аргументации. правила к тезису, правила к аргументу, правила к демонстрации. Некорректные уловки в споре. Логические ошибка, типология логических ошибок. Игра «Софист»,Понятие верификации и фальсификации. Критерии достоверности информации. Когнитивные искажения, виды когнитивных искажений. Правила работы с информационными источниками. Упражнение «Верю – не верю».,Информация, факт, знание. Процедура фактчекинга. Принципы фактчекинга: критерии выявления дезинформации. Командная работа, межгрупповое занятие: работа с информационными источниками. Самостоятельный подбор информационного источника (содержащего достоверную или недостоверную информацию), верификация источника и составление карты аргументов, обосновывающей решение команды. Рефлексия занятия6 система взаимного оценивания.,Аргументативное письменное рассуждение. Проблема, тезис, аргумент, пример. Командная работа, предполагает ряд этапов. 1 этап: анализ цитаты, выделение ключевых понятий, формулировка проблемы. тезиса, аргументов и примеров. 2. Этап: критический анализ работы оппонентов, формулировка контраргументов. 3 этап: взаимное оценивание, чья карта аргументов более обоснованная.,смысл и цель дебатов К. Поппера. Принципы дебатов. Структура и механика дебатов. Этика дебатов. Регламент дебатов. Функции первого спикера.,Карта аргументов. Аргументация и контраргументация. Функции второго спикера. Вопросы в контексте дебатов. Микро-батл по теме предложенной студентами.,Функции третьего спикера. Аналитика дебатов. Судейский протокол, критерии оценивания дебатов.,Игра «Дебаты». Аналитика текущей игры.,Игра «Дебаты». Аналитика текущей игры.</t>
+  </si>
+  <si>
+    <t>Примеры экономических задач, решение которых сводится к решению систем линейных уравнений.,Понятия вектора, линейной зависимости; теоремы о линейной зависимости и признаках линейной зависимости.,Понятия базиса, координат вектора аффинной и декартовой прямоугольной систем координат, проекции точки и вектора на прямую, плоскость и ось.,Определения и свойства скалярного, векторного и смешанного произведений. Запись произведений векторов в декартовой прямоугольной системе координат.,Общие сведения об уравнениях линий на плоскости и в пространстве, поверхностей в пространстве (алгебраические, параметрические, трансцендентные); уравнения, описывающие взаимосвязь координат вектора (точки) в разных системах координат.,Теорема об общем уравнении прямой линии на плоскости и следствия из неё; другие типы уравнений прямой линии на плоскости; пучок прямых.,Теорема об общем уравнении плоскости в пространстве и следствия из неё; другие уравнения плоскости; пучок и связка плоскостей; уравнения прямой линии в пространстве.,Задачи проецирования точки на прямую и плоскость, определения расстояния от точки до прямой и плоскости; методы решения геометрических неравенств.,Уравнения эллипса, гиперболы и параболы и их свойства; классификация линий второго порядка.,Уравнения различных поверхностей второго порядка и их свойства.,Определение матрицы, типы матриц, линейные операции над матрицами; операция умножения матриц и его свойства.,Определение операций элементарных преобразований матриц, их свойства и их матричные аналоги.,Определение обратной матрицы, теорема об обратной матрице, свойства обратных матриц. Определитель матрицы и его свойства; алгебраические дополнения и разложения определителя матрицы по выбранной строке (столбцу); вычисление алгебраических дополнений.,Дополнительные свойства определителя матрицы, определитель произведения квадратных матриц; понятие ранга матрицы; теорема о базисном миноре и следствия из неё.,Определение системы линейных алгебраических уравнений, различны формы записи систем линейных уравнений; теоремы Кронекера-Капелли и Крамера.,Фундаментальная матрица системы линейных алгебраических уравнений; теорема о фундаментальной матрице; теорема об общем решении однородной и неоднородной системах уравнений.,Дополнительные теоремы о существовании и свойствах решений систем линейных уравнений, альтернатива и теорема Фредгольма.,Определение линейного пространства; линейная зависимость векторов, теорема о линейной зависимости векторов; базис линейного пространства; координаты вектора; теорема о линейной зависимости векторов в координатной форме.,Операция смены базиса; определение линейного подпространства; теорема о линейном подпространстве.,Сумма и пересечение линейных подпространств; теоремы о сумме и пересечении линейных подпространств; прямое дополнение линейного подпространства; теорема о прямом дополнении линейного подпространства.,Определение скалярного произведения; определение евклидова пространства; неравенство Коши-Буняковского-Шварца; норма вектора, расстояние и угол между векторами; ортогональное дополнение линейного подпространства; процедура ортогонализации Грама-Шмидта; скалярное произведение в ортонормированном базисе.,Постановка и решение задачи проецирования вектора на подпространство.,Понятие точечно-векторного пространства; прямая, плоскость и гиперплоскость в точечно-векторном пространстве; выпуклые множества и выпуклые оболочки.,Определение комплексных чисел; операции над комплексными числами; различные формы представления комплексных чисел; определение унитарного пространства.,Определение линейного оператора; координатная и матричная форма записи линейного оператора; преобразование матрицы линейного оператора при смене базиса; операции над линейными операторами; геометрические свойства линейного оператора; обратный линейный оператор; теорема о существовании обратного линейного оператора.,Определение собственного значения и соответствующего ему собственного вектора линейного оператора; теорема о характеристическом уравнении; матрица линейного оператора в базисе из собственных векторов.,Определение разностного уравнения. Примеры практических задач, сводимых к разностным уравнениям и их решение с применением аппарата линейных операторов; некоторые свойства решения разностного уравнения.,Определение скалярных функций векторного аргумента: линейной формы, билинейной формы и квадратичной формы; матричная и координатная форма записи этих функций; преобразование матриц линейных функций при смене базиса.,Понятие знакоопределённой квадратичной формы; закон инерции квадратичных форм; критерии Лагранжа и Сильвестра; классификация квадратичных форм.</t>
+  </si>
+  <si>
+    <t>Макроэкономика как раздел экономической теории. Предмет макроэкономики. Методы макроэкономического изучения. Основные задачи, проблемы и понятия макроэкономики. Модель народнохозяйственного кругооборота. Экономическая политика и научные направления в макроэкономике.,Система национальных счетов как система макроэкономических показателей. Валовой внутренний продукт как основной макроэкономический показатель. Способы расчета валового внутреннего продукта. Особенности структуры валового внутреннего продукта России. Валовой внутренний продукт и другие показатели системы национальных счетов. Основные макроэкономические тождества. Номинальные и реальные макроэкономические показатели. Индексы цен. Валовой внутренний продукт и общественное благосостояние.,Предпосылки кейнсианской модели. Функции потребления и сбережений в коротком периоде. Кейнсианская функция инвестиций. Равновесие в двухсекторной модели «кейнсианского креста». Мультипликатор автономных расходов. Трехсекторная модель «кейнсианского креста». Дискреционная бюджетно-налоговая политика в модели «кейнсианского креста». Мультипликаторы бюджетно-налоговой политики. Рецессионный и инфляционный разрывы. Виды бюджетного дефицита.,Совокупный спрос (AD) и его структура. Факторы совокупного спроса. Совокупное предложение (AS) в коротком и долгом периодах. Факторы совокупного предложения. Модель AD — AS. Макроэкономическое равновесие в коротком и длительном периодах. Нарушение и последующее восстановление макроэкономического равновесия. Шоки совокупного спроса и совокупного предложения.,Понятие макроэкономической нестабильности. Деловой цикл. Экономические кризисы. Безработица: определение, виды, показатели. Особенности занятости и безработицы в России. Инфляция: содержание, показатели, формы. Особенности инфляции в России. Взаимосвязь инфляции и безработицы: кривая Филлипса. Экономический рост: содержание, основные показатели. Источники, типы и факторы экономического роста. Экономический рост и экономическое развитие. Кейнсианские модели экономического роста: модель Домара-Харрода. Неоклассические модели экономического роста: модель Р. Солоу.,Денежная база, или деньги повышенной мощности. Денежная масса (предложение денег). Денежные агрегаты. Денежный мультипликатор. Депозитный (кредитный) мультипликатор. Деньги. Кейнсианская теория спроса на деньги. Количественная теория спроса на деньги. Коммерческие банки. Коэффициент депонирования. Коэффициент монетизации ВВП. Кредитно-денежная политика (КДП). Ликвидность денег. Монетарное правило. Мотив предосторожности. Нейтральность денег. Норма избыточных резервов. Норма обязательных резервов. Норма резервов. Портфельная теория спроса на деньги. Спекулятивный мотив. Спрос на деньги. Ставка рефинансирования. Трансакционный мотив. Уравнение обмена И. Фишера. Функции денег. Центральный банк.,Государство в национальной экономике. Экономические функции государства. Государственный бюджет и его структура. Дефицит бюджета и государственный долг. Бюджетно-налоговая политика: содержание, цели и инструменты. Виды бюджетно-налоговой политики. Встроенные (автоматические) стабилизаторы. Циклический и структурный дефициты (профициты) государственного бюджета. Воздействие бюджетного профицита на экономику. Способы финансирования бюджетного дефицита. Государственный долг. Воздействие бюджетно-налоговой политики на совокупное предложение.,Предпосылки модели IS-LM. Кривая IS как кривая равновесия товарного рынка. Кривая LM как кривая равновесия денежного рынка. Макроэкономическое равновесие в модели IS-LM. Воздействие мер бюджетно-налоговой и кредитно-денежной политики на параметры макроэкономического равновесия в модели IS-LM. Ликвидная и инвестиционная ловушки. Модель IS-LM и кривая совокупного спроса.,Валютный рынок. Глобализация. Девальвация и ревальвация. Конвертируемость денежной единицы. Котировка валюты. Либерализация внешнеэкономических связей. Международные экономические отношения. Модели регулирования внешней торговли. Номинальный и реальный валютный курс. Обменный (валютный) курс. Открытая экономика. Паритет покупательной способности (ППС). Плавающий и фиксированный валютные курсы. Платежный баланс. Предельная склонность к импорту. Протекционизм и фритредерство. Системы валютных курсов. Степень открытости экономики. Счет текущих операций. Счет движения капитала. Условия торговли.</t>
+  </si>
+  <si>
+    <t>Вводная лекция. Предмет и содержание дисциплины «Маркетинг». Эволюция форм управления рыночной деятельностью бизнес-субъектов. Базовые определения маркетинговой деятельности, её основных направлений и типов. Типы и виды маркетинга. Концепции маркетинга. Экономическая роль, цели и задачи стратегической и оперативной маркетинговой деятельности бизнес-субъектов. Понятие маркетинговой среды компании. Методы оценки маркетинговой среды компании,Этапы развития маркетинговых исследований. Понятие и сущность маркетинговых исследований. Основные направления маркетинговых исследований. Принципы маркетинговых исследований. Классификации маркетинговых исследований. Процесс разработки маркетингового исследования. Составление брифа маркетингового исследования. Первичная и вторичная маркетинговая информация и её источники. Методы маркетинговых исследований. Генеральная совокупность и выборка исследования. Маркетинговая информационная система (МИС).,Этапы сегментирования рынка: сегментационный анализ, выбор целевого сегмента, рыночное позиционирование, разработка маркетинговой программы. Методы определения границ рынка. Выбор критериев сегментирования. Особенности сегментирования деловых рынков «В2В». Разработка стратегии охвата рынка. Рыночная ниша. Рыночное окно. Понятия целевого сегмента рынка и целевой аудитории покупателей. Стратегии выбора целевых сегментов. Недифференцированный маркетинг. Дифференцированный маркетинг. Концентрированный маркетинг. Факторы, влияющие на поведение потребителей. Типы покупательского поведения. Процесс принятия потребителем решения о покупке.,Понятие «товар», номенклатура, ассортимент. Длина и широта товарного ассортимента. Классификация потребительских товаров. Классификация товаров производственного назначения. Модели товара по Ф.Котлеру. Мультиатрибутивная модель товара Ж.Ж. Ламбена. Продуктовый портфель, товарные стратегии. Жизненный цикл товара (ЖЦТ) и его стадии. Разработка нового товара. Инструментарий анализа товарного ассортимента компании: Методы: АВС-анализ и ХУZ-анализ; матрица БКГ; матрица GE/McKinsey, матрица И.Ансоффа. Марочная политика компании. Бренд и элементы брендинга.,Понятие о цене товара (услуги). Издержки. Постановка задач ценообразования. Определение спроса и оценка издержек. Определение базового уровня цены. Типы и виды цен. Классификация методов установления цены. Адаптация цен. Цены в условиях конкуренции. Государственное регулирование цен. Стратегии ценообразования.,Формирование коммуникационной политики. Понятие и структура комплекса маркетинговых коммуникаций. Классификация и сущность инструментов комплекса продвижения компании. Процесс маркетинговых коммуникаций. Концепция интегрированных маркетинговых коммуникаций (ИМК). Инструментарий цифрового маркетинга в комплексе продвижении компании.,Каналы распределения товаров. Функции каналов товародвижения, издержки товародвижения. Дистрибьюция потребительских и промышленных товаров. Выбор канала распределения. Охват рынка. Прямые и косвенные каналы распределения. Оптовые посредники и их виды. Дилеры. Дистрибьюторы. Брокеры. Торговые агенты. Розничная торговля. Классификация предприятий розничной торговли. Организация сервиса. Уровень обслуживания потребителей. Типы сбытовых стратегий.,Понятие о стратегическом маркетинге и его основные отличия от операционного маркетинга. Состав и функциональная структура комплексов стратегического и операционного маркетингов бизнес-субъекта. Функции и инструменты стратегического маркетинга. Функции и инструменты операционного маркетинга. Стратегическое планирование маркетинга. Виды маркетинговых стратегий. Основные этапы планирования маркетинга. Виды планов маркетинга. Стратегические планы маркетинга. Операционные (текущие) планы маркетинга. Структура плана маркетинга. Маркетинговые программы.</t>
+  </si>
+  <si>
+    <t>Генеральная и выборочная совокупность. Объём совокупности. Типы выборок (повторная, бесповторная). Репрезентативная выборка. Варианты. Вариационный ряд. Частота и относительная частота. Статистическое распределение выборки. Полигон относительных частот выборки. Группированный статистический ряд выборки. Гистограмма. Эмпирическая функция распределения. Числовые характеристики выборки (выборочная средняя, выборочная дисперсия, выборочное среднее квадратическое отклонение, выборочная мода и выборочная медиана).,Формулировка задачи оценки параметров распределения. Понятие оценки параметров. Свойства оценок (несмещенность, состоятельность, эффективность). Оценки точечные и интервальные. Доверительная вероятность и доверительный интервал. Построение доверительных интервалов для параметров нормального распределения.,Метод моментов. Метод максимального правдоподобия.,Понятие статистической гипотезы. Простые и сложные гипотезы. Нулевая и альтернативная гипотезы. Ошибки первого и второго рода, возникающие при проверке гипотез. Статистический критерий. Уровень значимости критерия. Мощность критерия. Статистика критерия. Основной принцип проверки статистических гипотез. Область принятия гипотезы. Критическая область. Виды критических областей (правосторонняя, левосторонняя, двусторонняя). Гипотеза о значении неизвестного параметра нормального распределения.,Гипотеза о равенстве средних значений двух генеральных совокупностей. Гипотеза о равенстве дисперсий двух генеральных совокупностей.,Гипотеза о законе распределения. Критерий согласия хи-квадрат Пирсона. Алгоритм проверки гипотезы о законе распределения. ,Общая, факторная и остаточная суммы квадратов отклонений. Факторная и остаточная дисперсии. Проверка значимости влияния фактора.,Статистическая зависимость. Корреляционная зависимость. Уравнения регрессии. Выборочные линейные уравнения регрессии.,Понятие выборочной ковариации случайных величин. Понятие выборочного коэффициента корреляции. Связь выборочного коэффициента корреляции с выборочными линейными уравнениями регрессии. Свойства выборочного коэффициента корреляции. Проверка значимости выборочного коэффициента корреляции.,Ранги объектов выборки. Выборочный коэффициент ранговой корреляции Спирмена. Свойства выборочного коэффициента ранговой корреляции Спирмена. Проверка значимости выборочного коэффициента ранговой корреляции Спирмена.,Основные понятия. Метод Монте-Карло (метод статистических испытаний). Преобразование равномерного распределения в заданное. Разыгрывание противоположных событий.,Распределение «хи-квадрат». Распределение Стьюдента. Распределение Фишера-Снедекора. Гамма-распределение.</t>
+  </si>
+  <si>
+    <t>Понятие множества, элемента множества. Обозначение множества. Способы задания множеств. Пустое множество. Понятие подмножества множества. Равные множества. Операции над множествами (объединение, пересечение и разность множеств). Числовые множества. Определение рационального и иррационального числа. Модуль действительного числа и его свойства. Понятия верхней и нижней грани множества. Понятия точной верхней и точной нижней грани множества.,Числовая последовательность. Свойства числовых последовательностей (ограниченная, неограниченная, возрастающая, убывающая, монотонная). Понятие окрестности точки. Предел числовой последовательности. Сходящиеся и расходящиеся числовые последовательности. Геометрический смысл предела последовательности. Определение целой части числа и его свойства. Основные теоремы о пределах числовых последовательностей.,Величины постоянные и величины переменные. Функция. Область определения и область значений функции. Частное значение функции. График функции. Графики основных элементарных функций. Основные свойства функций (четная, нечетная, периодическая, возрастающая, убывающая, монотонная, ограниченная, неограниченная). Способы задания функций (аналитический, табличный, графический).,Определение предела функции. Геометрический смысл предела функции. Односторонние пределы. Бесконечно малые и бесконечно большие функции. Свойства бесконечно малых и бесконечно больших функций. Первый и второй замечательные пределы. Основные теоремы о пределах функций.,Непрерывность функции в точке. Понятие приращения аргумента и приращения функции в точке. Эквивалентное определение непрерывности функции в точке. Непрерывность сложной функции. Свойства функций, непрерывных на отрезке (теоремы об ограниченности функции, о наибольшем и наименьшем значении, о переходе через нуль, о промежуточном значении). Точки разрыва функции и их классификация. ,Производная, ее геометрический и механический смысл. Уравнение касательной к кривой. Производная суммы, произведения, частного. Производная сложной функции, обратной функции, неявной функции, функции, заданной параметрически. Производные основных элементарных функций. Понятие дифференцируемости функции в точке. Логарифмическая производная. Производная степенно-показательной функции.,Дифференциал функции и его геометрический смысл. Дифференциал независимой переменной. Теорема о связи дифференциала функции с производной функции. Свойства дифференциала функции. Теорема об инвариантности формы дифференциала. Использование дифференциала в приближенных вычислениях. Производные и дифференциалы высших порядков.,Теоремы Ролля, Лагранжа, Коши. Правило Лопиталя. Порядок раскрытия неопределенностей неосновного вида с помощью правила Лопиталя. Исследование возрастания и убывания функции с помощью производной. Локальный экстремум, его исследование с помощью первой и второй производной. Понятие критических точек первого рода. Схема отыскания наибольшего и наименьшего значения функции на отрезке.,Выпуклость, вогнутость и точки перегиба графика функции. Достаточное условие выпуклости (вогнутости) графика функции. Понятие критических точек второго рода. Необходимое условие существования точки перегиба. Достаточное условие существования точки перегиба. Асимптоты плоских кривых (определение и классификация). Исследование функций, построение графиков.,Первообразная. Неопределенный интеграл и его свойства. Теорема о существовании первообразной и неопределенного интеграла. Таблица основных интегралов. Непосредственное интегрирование.,Метод замены переменной. Метод интегрирования по частям. Понятие рациональной функции (рациональной дроби). Правильные и неправильные рациональные дроби. Теорема о разложении неправильной рациональной дроби. Простейшие дроби. Теорема о разложении правильной рациональной дроби на простейшие. Порядок интегрирования рациональных дробей,Интегрирование иррациональных функций (основные виды интегралов и порядок их нахождения). Интегрирование тригонометрических функций (основные виды интегралов и порядок их нахождения). Замечание о «неберущихся» интегралах.,Понятие интегральной суммы и её геометрический смысл. Определение, геометрический смысл и основные свойства определенного интеграла. Теорема о существовании определенного интеграла. Теорема о среднем значении. Интеграл с переменным верхним пределом.,Формула Ньютона – Лейбница. Основные методы вычисления определенного интеграла (замена переменной, интегрирование по частям). Вычисление площадей плоских фигур. Приближенное вычисление определенного интеграла методом Симпсона.,Несобственные интегралы с бесконечными пределами интегрирования (интегралы I типа). Понятие особой точки для функции. Несобственные интегралы от неограниченных функций (интегралы II типа). Геометрический смысл несобственных интегралов.,Признаки сходимости несобственных интегралов от неотрицательных функций. Абсолютная сходимость несобственных интегралов. Признак сходимости несобственных интегралов от знакопеременных функций.,Использование понятия производной в экономике (предельные издержки производства, предельная выручка, предельный доход, предельная производительность и т.д.). Экономический смыл определенного интеграла. Решение некоторых задач экономического содержания с использованием дифференциального и интегрального исчисления.,Понятие числового ряда. Понятие n-ой частичной суммы ряда. Понятие сходящегося числового ряда. Понятие суммы числового ряда. Геометрический ряд. Свойства числовых рядов. Понятие n-ого остатка ряда. Необходимый признак сходимости ряда. Теорема о «погружении» дискретного аргумента (n) в непрерывный (х).,Первый признак сравнения. Второй (предельный) признак сравнения. Признак Даламбера. Признак Коши. Интегральный признак Коши.,Знакочередующиеся ряды. Признак Лейбница сходимости знакочередующегося ряда. Понятие знакопеременного числового ряда. Абсолютная и условная сходимость рядов. Метод математической индукции.,Понятие степенного ряда. Область сходимости степенного ряда. Теорема Абеля. Нахождение интервала сходимости степенного ряда. Свойства степенных рядов.,Ряд Тейлора. Достаточное условие представления функции ее рядом Тейлора. Ряд Маклорена. Разложение в ряд Маклорена некоторых функций.,Основные понятия. Схема отыскания области определения функции двух переменных. Определение графика функции двух переменных. Линии уровня функции. Предел и непрерывность функции двух переменных. Линии разрыва функции двух переменных.,Частные производные. Правила дифференцирования. Определение полного дифференциала функции двух переменных. Достаточное условие дифференцируемости функции двух переменных. Дифференцирование сложных функций. Частные производные высших порядков.,Абсолютный экстремум функции нескольких переменных. Необходимое условие экстремума функции нескольких переменных. Достаточное условие экстремума функции двух переменных. Алгоритм отыскания экстремума функции двух переменных. Наибольшее и наименьшее значения функции в замкнутой области. Условный экстремум функции нескольких переменных. ,Способы задания плоских линий (линий на плоскости). Локальные элементы плоской линии. Угол между двумя линиями. Огибающая однопараметрического семейства линий. Дискриминантная линия семейства линий.,Понятие скалярного поля. Поверхность уровня скалярного поля. Производная по направлению. Градиент скалярного поля. Свойства градиента скалярного поля. Дифференцирование неявных функций двух переменных.,Понятие двойного интеграла. Теорема о существовании двойного интеграла. Геометрический смысл двойного интеграла. Основные свойства двойного интеграла. Вычисление двойного интеграла в декартовой системе координат. Вычисление двойного интеграла в полярной системе координат.,Двойные интегралы по бесконечной области. Двойные интегралы от неограниченных функций.,Понятие тройного интеграла. Геометрический смысл тройного интеграла. Основные свойства тройного интеграла. Вычисление тройного интеграла в декартовых координатах. Вычисление тройного интеграла в цилиндрических координатах.,Понятие криволинейного интеграла первого рода. Основные свойства криволинейного интеграла первого рода. Вычисление криволинейного интеграла первого рода. Геометрический смысл криволинейного интеграла первого рода.,Понятие криволинейного интеграла второго рода. Основные свойства криволинейного интеграла второго рода. Вычисление криволинейного интеграла второго рода. Геометрический смысл криволинейного интеграла второго рода.,Понятие дифференциального уравнения. Обыкновенное дифференциальное уравнение. Порядок дифференциального уравнения. Решение дифференциального уравнения. Общее решение дифференциального уравнения. Общий интеграл дифференциального уравнения. Частное решение дифференциального уравнения. Особые решения дифференциального уравнения. Задача Коши. Дифференциальные уравнения первого порядка. Уравнения с разделяющимися переменными.,Однородные дифференциальные уравнения. Метод решения однородного дифференциального уравнения. Линейные дифференциальные уравнения первого порядка. Нахождение общего решения линейного неоднородного уравнения первого порядка методом вариации произвольной постоянной (методом Лагранжа).,Уравнение Бернулли. Уравнение в полных дифференциалах. Уравнение, содержащее только независимую переменную и производную второго порядка. Уравнение, не содержащее искомой функции. Уравнение, не содержащее независимой переменной.,Линейные однородные дифференциальные уравнения второго порядка с постоянными коэффициентами. Понятие комплексного числа. Метод решения линейного однородного дифференциального уравнения второго порядка с постоянными коэффициентами. Характеристическое уравнение. Общее решение линейного однородного дифференциального уравнения второго порядка с постоянными коэффициентами. Линейные неоднородные дифференциальные уравнения второго порядка с постоянными коэффициентами. Общее решение линейного неоднородного дифференциального уравнения второго порядка с постоянными коэффициентами. Метод подбора (метод неопределенных коэффициентов).,Общий вид дифференциального уравнения первого порядка, не разрешенного относительно производной. Метод введения параметра. Уравнение Лагранжа. Уравнение Клеро. Особые решения. Алгоритм отыскания особых решений дифференциального уравнения первого порядка, не разрешенного относительно производной. ,Понятие системы дифференциальных уравнений первого порядка. Понятие нормальной системы дифференциальных уравнений. Понятие решения нормальной системы дифференциальных уравнений. Задача Коши для нормальной системы дифференциальных уравнений. Методы решения нормальных систем дифференциальных уравнений (метод исключения неизвестных, метод нахождения интегрируемых комбинаций).,Понятие изоклины. Приближенное построение интегральных кривых дифференциального уравнения методом изоклин. Составление дифференциального уравнения семейства кривых. Решение задачи Коши методом последовательных приближений.,Линейные однородные дифференциальные уравнения второго порядка с переменными коэффициентами. Общее решение линейного однородного дифференциального уравнения второго порядка с переменными коэффициентами. Линейные неоднородные дифференциальные уравнения второго порядка с переменными коэффициентами. Метод вариации произвольных постоянных (метод Лагранжа). Общее решение линейного неоднородного дифференциального уравнения второго порядка с переменными коэффициентами.,Рассмотрение некоторых примеров использования дифференциальных уравнений в моделях экономической динамики, в которых отражается не только зависимость переменных от времени, но и их взаимосвязь во времени.</t>
+  </si>
+  <si>
+    <t>Глобализация мировой экономики. Понятие международной экономики. Предмет курса. Методы анализа международной экономики. Структура международных экономических отношений. Международное разделение труда.,2.1 Теории международной торговли,Классические теории международной торговли: теория абсолютных преимуществ; теория сравнительных преимуществ; теория соотношения факторов производства; парадокс Леонтьева. Альтернативные теории международной торговли: эффект масштаба и несовершенная конкуренция; теории спроса и реверса в международной торговле; теория цикла жизни продукта; теория конкурентных преимуществ Майкла Портера; влияние международной торговли на доходы.,2.2 Динамика и структура международной торговли,Динамика международной торговли. Структура международной торговли. Страны-лидеры по импорту и экспорту в международной торговле товарами и услугами.,2.3 Внешняя торговля России,Динамика основных показателей внешней торговли России. Географическая структура внешней торговли России. Товарная структура экспорта России. Товарная структура импорта России.,2.4 Регулирование международной торговли,Свобода торговли и протекционизм. Тарифные методы регулирования: таможенные тарифы и пошлины, специфические случаи тарифной политики. Нетарифные методы регулирования международной торговли: количественные ограничения, скрытые методы торговой политики, финансовые методы торговой политики, неэкономические методы регулирования. Последствия введения торговых ограничений для экономики малой и большой страны. Наднациональное регулирование международной торговли.,Формы международного движения капитала. Прямые зарубежные инвестиции: теории, экономические эффекты. Международные корпорации: формы; влияние на принимающие страны и страны базирования. Портфельные зарубежные инвестиции: виды портфельных инвестиций, причины. Международное заимствование и кредитование: инструменты международного кредитования.,Теории международной трудовой миграции: виды, экономические эффекты миграции. Масштабы и направления миграции рабочей силы. Государственное регулирование миграции: механизмы контроля миграции; регулирование миграции; стимулирование реэмиграции.,Понятие валюты. Эволюция валютной системы: золотой стандарт, золотодевизный стандарт, современная валютная система. Валютный курс и его разновидности: понятие и котировки валютного курса; виды валютных курсов по степени гибкости; гибридные виды валютного курса. Теории валютного курса: теория паритета покупательной способности; влияние процентных ставок на валютный курс. Факторы, влияющие на валютные курсы. Влияние валютных курсов на экономику страны. Управление валютным риском.,Становление интеграционных процессов: предпосылки и цели интеграции. Типы интеграционных объединений: этапы интеграции; интеграционные объединения; принципы оценки интеграции. Статические и динамические эффекты интеграции.</t>
+  </si>
+  <si>
+    <t>Сущность и содержание понятия «менеджмент». Подходы к определению менеджмента: менеджмент как наука управления; менеджмент как искусство управления; менеджмент как «лицо» или группа лиц, осуществляющих управление; идентификация менеджмента с органами и аппаратом управления; менеджмент как процесс. Соотношение понятий «менеджмент», «управление», «администрирование», «бизнес», «предпринимательство». История возникновения менеджмента и общая характеристика пяти управленческих революций. Развитие научных школ и подходов в менеджменте (школа научного менеджмента, классическая или административная школа, школа человеческих отношений и поведенческих наук, школа науки управления или количественная школа; процессный подход, системный подход, ситуационный подход; характеристика прочих подходов к менеджменту). Современная система взглядов на менеджмент и характеристика новой управленческой парадигмы. Менеджмент XXI века (Менеджмент 2.0). Три орбиты управления организациями.,Общая характеристика функций управления. Подходы к классификации функций управления. Планирование деятельности. Цели и задачи планирования, этапы планирования Постановка целей в планировании и основные области целеполагания. Требования к постановке целей. Организация управленческой деятельности. Два аспекта организационного процесса в менеджменте. Характеристика ключевых элементов процесса организации (делегирование, ответственность, полномочия). Мотивация деятельности и общая характеристика мотивационного процесса. Типы мотиваций. Теории мотивации (содержательные теории мотивации и процессуальные теории мотивации). Контроль в системе управления организацией. Цели контроля и его основные виды. Ключевые факторы успеха (КФУ). Современная система взглядов на управленческие функции (в контексте Менеджмента 2.0).,Понятие управленческого труда. Сущность и содержание управленческого труда (цель, предмет, средства, продукт). Виды разделения управленческого труда: функциональное, иерархическое, технологическое, профессиональное, квалификационное, должностное. Менеджер и предприниматель. Профессионалы в управлении. Различия предпринимателя и менеджера. Содержание труда менеджеров. Основные типы менеджеров (линейные менеджеры и функциональные менеджеры). Руководители низового звена, руководители среднего звена, руководители высшего звена. Требования, предъявляемые к менеджерам. Лидер и менеджер: сравнительные характеристики. Методы развития навыков менеджеров. Менеджер XXI века: характеристика основных качеств.,Общие подходы к понятию «организация». Признаки организаций. Основные параметры организаций и содержание понятия «организация» как социальной системы. Механистический и органический подходы к организации, креативная (гуманистическая) организация. Классификация организаций по Г. Минцбергу. Виды хозяйственных организаций. Интеграция организаций, варианты интеграционных процессов (вертикальная интеграция, горизонтальная интеграция, диверсификация). Формы интеграции. Кризис традиционной организации и характерные признаки организаций XXI века. Признаки Бирюзовых организаций. Человек – главный актив и субъект организационных изменений.,Внешняя среда организации: компоненты макроокружения (экономическая компонента, политическая, правовая, социокультурная, технологическая, географическая, международное окружение) и рыночного окружения (поставщики, потребители, конкуренты, рыночная инфраструктура). Взаимосвязь компонентов и степень воздействия внешней среды на организацию. Внутренняя среда организации (кадровая подсистема, организационная подсистема, производственная подсистема, маркетинговая подсистема, инновационная подсистема, финансовая подсистема). Организационная культура как обобщающая характеристика среды организации., Внешняя и внутренняя среда в цифровую эпоху; стирание границ между внутренней и внешней средой. Организация как экосистема (эко системный подход).,Общее понятие организационной структуры управления (ОСУ). Принципы формирования ОСУ. Ключевые понятия организационного проектирования.,Факторы проектирования организации: зависимость от внешней среды (параметры среды организации и их виляние на организационное проектирование); технология работы (технологии Индустрии 4.0); стратегический выбор руководства. Элементы проектирования организации: разделение труда и специализация; департаментизация и кооперация; связи между частями и координация; масштаб управляемости и контроль; иерархия организации и ее звенность; распределение прав и ответственности; централизация и децентрализация; дифференциация и интеграция.,Общая характеристика бюрократического типа ОСУ. Виды бюрократических структур управления (линейные, функциональные, линейно-функциональные, линейно-штабные), их преимущества и недостатки. Дивизиональная ОСУ как прогрессивный вид бюрократических ОСУ; критерии структурирования организации по дивизионам (отделениям).,Общая характеристика органического типа ОСУ. Основные виды органических структур управления (матричная организация и ее разновидности, проектная организация, временная целевая группа, постоянная комплексная группа, бригадная форма организации труда). Преимущества и недостатки органических структур управления.,Тенденции в эволюции ОСУ. Признаки современного общества и требования, предъявляемые к формированию эффективных ОСУ. Критерии определения «эффективная структура управления». Характеристика новых типов ОСУ (эдхократическая организация; многомерная организация; партисипативная; организации, ориентированные на рынок; организации предпринимательского типа; сетевые организации; виртуальные организации).,Организационные структуры управления в условиях цифровой трансформации компаний.,Общее понятие и содержание методов менеджмента. Эволюция методов менеджмента в отечественной науке управления. Развитие методического инструментария зарубежными школами и подходами менеджмента. Тенденции изменения методов менеджмента и характеристика современных методов менеджмента. Классификация методов менеджмента. Общенаучные методы менеджмента: метод исторического подхода в менеджменте, моделирование и использование экономико-математических методов, экспериментирование, методы социологических исследований. Специфические методы менеджмента: организационно-распорядительные, экономические, социально-психологические, мотивационные методы. Характеристика прочих подходов к классификации методов менеджмента. Формирование фондов методов менеджмента.</t>
+  </si>
+  <si>
+    <t>Оптимизационная задача (задача математического программирования). Общая постановка задачи математического программирования. Понятия целевой функции, области допустимых решений (области ограничений), оптимального решения (оптимального плана). Понятия линейной и нелинейной, выпуклой и вогнутой функции. Разновидности задачи математического программирования (задачи нелинейного и линейного программирования, задачи без ограничений, с ограничениями-равенствами, ограничениями-неравенствами и смешанными ограничениями). Понятие стационарной точки функции. Понятие матрицы Гессе. Понятия квадратичной формы матрицы, положительной (отрицательной) определенности матрицы. Понятия вектор-функции и матрицы Якоби. Понятия производной по направлению и градиента. Теорема о производной по направлению. Теорема о градиенте. Понятия касательной гиперплоскости и нормали. Формула Тейлора (разложение Тейлора) для функции многих переменных. Теорема Вейерштрасса.,Теорема о необходимых условиях экстремума функции без ограничений. Теорема о достаточных условиях экстремума функции без ограничений. Теорема об условиях определенности матрицы (критерий Сильвестра). Классический метод решения ЗЛНП без ограничений Метод множителей Лагранжа (обоснование метода, функция Лагранжа, инструментальные переменные, множители Лагранжа, стационарные точки функции Лагранжа, окаймленная матрица Гессе и достаточные условия существования экстремума функции при наличии ограничений-равенств, алгоритм реализации метода Лагранжа). Интерпретация множителей Лагранжа. Теорема Лагранжа. Метод подстановки решения ЗНЛП с ограничениями-равенствами. Обобщенный метод множителей Лагранжа (обоснование метода, активные и пассивные ограничения, алгоритм реализации обобщенного метода Лагранжа). Условия Куна-Таккера. Задача выпуклого нелинейного программирования. Достаточность условий Куна-Таккера. Теорема о единственности экстремума строго выпуклой (вогнутой) функции. Метод Куна-Таккера решения задач выпукло-вогнутого нелинейного программирования (обоснование метода и алгоритм его реализации).,Общая постановка задачи линейного программирования (ЗЛП) и формы ее представления (каноническая, симметричная и общая). Понятие угловой точки (вершины выпуклого многогранника). Понятие опорного плана ЗЛП. Теорема об эквивалентности форм представления ЗЛП. Теорема о представлении (Каратеодори). Теорема о решении ЗЛП. Графический метод решения ЗЛП. Обоснование метода. Алгоритм реализации графического метода. Симплекс-метод. Обоснование метода. Алгебра симплекс метода. Алгоритм реализации симплекс-метода. Симплекс-таблицы. Правила построения, заполнения и пересчета симплекс-таблиц. Двойственная пара задач линейного программирования (прямая и двойственная ЗЛП). Двойственная лемма. Прямые и двойственные оценки. 1-я, 2-я и 3-я теоремы двойственности. Теорема о представлении оптимального плана прямой ЗЛП. Теорема о представлении оптимального плана двойственной ЗЛП. Экономическая интерпретация двойственных оценок. Двойственный симплекс-метод. Обоснование метода и алгоритм его реализации. Устойчивость решений задач двойственной пары. Теорема об условиях устойчивости прямых оценок. Теорема об условиях устойчивости двойственных оценок. Закрытая транспортная задача (ТЗ). Теорема о разрешимости ТЗ. Открытые ТЗ на недостаток и избыток. Сведение ТЗ открытого типа к закрытой ТЗ. Методы определения опорного плана ТЗ (метод северо-западного угла и метод минимального элемента (минимальных тарифов)). Метод потенциалов решения ТЗ. Теорема об оптимальном плане ТЗ. Задача коммивояжера. Задача о назначениях (выбора). Методы отсечения в решении ЗЛДП. «Правильные» отсечения. Отсечение Гомори. Метод Гомори (обоснование метода и алгоритм его реализации). Методы ветвей и границ, их обоснование и схема реализации. Примеры.,Понятие многошаговой операции, шагового управления, показателя эффективности, целевой функции, области допустимых управлений.,Условие «Отсутствие последействия». Уравнения состояний. Условие аддитивности целевой функции. Принцип оптимальности Беллмана. Понятия условного и безусловного оптимальных управлений. Обоснование метода прогонки. Двухэтапная процедура метода прогонки (1 этап: обратная прогонка, 2-й этап: прямая прогонка). Вычислительная схема метода прогонки. Уравнения Беллмана. Задача распределения ресурсов, задача управления запасами и задача о замене как примеры задач динамического программирования.,Понятия графа и его элементов (вершины, дуги, ребра, цепи, пути, цикла, дерева). Понятие инцидентности и матрицы инцидентности. Критерий пути. Задача построения минимального остовного дерева. Задача поиска минимального и критического путей. Задача о максимальных потоках в сети. Задача о потоке минимальной стоимости. Сведение рассмотренных задач к задачам линейного программирования. Графики Ганта и сетевые модели проектов. События начала и завершения работ проекта и отображения их на графе. Правила построения сетевой модели проекта. Упорядочение во времени элементов сетевой модели проекта. Сетевые графики. Временные параметры сетевых графиков. Понятие критического пути. CPM и PERT – методы оптимизации сетевых графиков,Общая постановка задачи управления запасами. Понятия величины и характера спроса, типа и скорости расхода запасов, объема (размера) заказа, цикла заказа, точки заказа. Статическая детерминированная модель без дефицита. Формула Уилсона. Статическая детерминированная модель с дефицитом. Статическая детерминированная модель с дисконтом. Простейшие стохастические стационарные модели.,Понятие систем массового обслуживания (СМО) и их основные элементы. Области применения СМО. Простейшие модели СМО. Имитационное моделирование. Метод Монте-Карло. Приемы построения и эксплуатации имитационных моделей.,Общая постановка задачи принятия решений в условиях неопределенности и ее интерпретация как игры с природой. Основные элементы и особенности игры с природой, основные формы (нормальная и позиционная) ее представления. Критерии Лапласа, ожидаемого значения (Байеса), Гурвица, гарантированного результата (минимаксный и максиминный), Сэвиджа, Неймана-Пирсона. Геометрическая интерпретация игры с природой.</t>
+  </si>
+  <si>
+    <t>Две трактовки термина «экономика». Понятие «экономическая теория». Предмет экономической теории. Субъекты экономического выбора: домашнее хозяйство, фирма, государство, их цели. Уровни изучения экономики: микроэкономика, мезоэкономика, макроэкономика, мегаэкономика. Методы экономической теории: общенаучные, специфические. Виды моделей. Метод «при прочих равных условиях». Метод предельного анализа. Метод теории игр. Позитивный и нормативный подход к экономическому объекту.,Блага: экономические и свободные, потребительские и производственные, частные и общественные, долговременные и недолговременные. Общественное производство и воспроизводство. Стадии общественного воспроизводства. Простое и расширенное воспроизводство. Факторы производства К. Маркса: средства производства (средства труда, предметы труда), рабочая сила. Теория факторов производства Сея: земля, капитал, труд, предпринимательские способности. Дополнительные факторы производства.,Технологический выбор в экономике. Кривая производственных возможностей: допущения при построении, графическая и табличная формы, движения по кривой и сдвиги кривой производственных возможностей. Закон возрастающих альтернативных издержек. Коэффициент трансформации.,Экономические системы и их виды. Чистые типы экономических систем. Основные экономические вопросы в чистых типах экономической системы. Смешанная экономика. Переходная экономика.,Понятие собственность. Субъекты и объекты собственности. Правомочия права собственности. Формы собственности: 2 классификации.,Понятие и функции рынка. Способы организации производства благ: натуральное и товарное хозяйство. Их основные черты. Условия возникновения товарного хозяйства. Бартерный и денежный обмен, причины перехода к денежному обмену. Субъекты и объекты рынка. Инфраструктура рынка. Механизм рынка.,Виды рынков: по объектам, в пространственном разрезе; по силе конкурентной борьбы,Совершенная конкуренция. Монополистическая конкуренция. Олигополия. Монополия. Характерные черты типов рыночных структур: число фирм, тип продукта, контроль над ценой, условия вступления в отрасль, неценовая конкуренция. Черты совершенной конкуренции.,Достоинства рынка. Недостатки рынка. Внешние эффекты. Общественные блага и их виды. Асимметрия информации.,Товар. Потребительная и меновая стоимость. Услуга и ее свойства.,Спрос. Функция спроса. Кривая спроса. Наклон кривой спроса. Закон спроса. Обоснования закона спроса: закон убывающей предельной полезности, эффект дохода и эффект замены. Виды спроса: рыночный и индивидуальный спрос. Ценовые и неценовые факторы спроса: нормальные и низшие товары, товары-заменители и дополняющие товары. Сдвиг кривой спроса, изменения в спросе. Товар Гиффена. Индивидуальный и рыночный спрос.,Предложение. Функция предложения: прямая и обратная. Кривая предложения. Закон предложения. Кривая предложения. Ценовые и неценовые факторы предложения. Сдвиг кривой предложения, изменения в предложении. Индивидуальное и рыночное предложение.,Равновесие рынка и его восстановление. Цена равновесия, равновесный объем товара.,Излишек потребителя. Графическая и смысловая интерпретация излишка потребителя. Излишек производителя. Графическая и смысловая интерпретация излишка производителя. Рыночные излишки и влияние государства. Чистые потери общества от налогообложения.,Конкуренция. Внутриотраслевая и межотраслевая виды конкуренции. Методы конкурентной борьбы: добросовестная и недобросовестная. Конкуренция по продукту. Конкуренция по условиям продажи.,Понятие эластичности. Эластичность спроса по цене. Интервалы ценовой эластичности: неэластичный, эластичный, единично эластичный, абсолютно неэластичный, абсолютно эластичный спрос. Факторы ценовой эластичности. Практическое значение измерения ценовой эластичности спроса. Эластичность спроса по доходу. Интервалы эластичности спроса по доходу. Практическое значение эластичности спроса по доходу. Перекрестная эластичность спроса. Интервалы перекрестной эластичности спроса. Практическое значение перекрестной эластичности спроса. Ценовая эластичность предложения. Период производства и ценовая эластичность предложения.,Понятие фирмы. Цель деятельности фирмы. Организационно-правовые формы по ОКОПФ.,Понятие «производство». Движение индивидуального капитала. Прибавочный продукт и прибавочная стоимость. Технология производства. Экономическая эффективность производства. Технологическая эффективность производства.,Краткосрочный и долгосрочный периоды в производственной деятельности. Постоянные и переменные ресурсы. Закон убывающей предельной отдачи фактора. Масштаб производства. Верхняя (техническая) граница производства в краткосрочном и долгосрочном периоде. Экономия от масштаба (эффект масштаба). Виды эффекта масштаба.,Продукт и товар. Совокупный продукт. Средний продукт. Предельный продукт. Предельный продукт труда. Виды учета продукта: определение, обозначение, формула, график.,Производственная функция. Общий вид. Замечания. Формы представления: таблица, уравнение, график. Краткосрочная функция производства. Три стадии и изменение общего, среднего и предельного продуктов. Производственная функция и закон убывания предельной отдачи. Долгосрочная производственная функция. Допущения при ее построении. Таблица, формула, график. Изокванта. Карта изоквант. Свойства стандартных изоквант. Предельная норма технологического замещения. Убывание предельной нормы технологического замещения.,Оптимум производителя. Бюджетное ограничение производителя. Уравнение изокосты. Линия изокосты. Наклон линии изокосты. Условие оптимума и его экономический смысл.,Издержки производства. Роль издержек в экономическом процессе. Виды издержек: по источнику образования, по составу, по сфере возникновения, по возможности возмещения,Бухгалтерская прибыль. Нормальная прибыль. Неявные издержки. Альтернативные издержки. Экономическая прибыль. Невозвратные издержки.,Виды издержек в краткосрочном и долгосрочном периодах. По каждому виду издержек понятие, обозначение, формула, график. Постоянные и переменные издержки. Общие (валовые) издержки. Общие постоянные издержки. Общие переменные издержки. Средние общие издержки. Средние постоянные издержки. Средние переменные издержки. Предельные издержки. Соотношения общих издержек по графикам. Соотношения средних издержек по графикам. Значимые точки пересечения на графиках.,Долгосрочный период. Условно-постоянные издержки. Переменные издержки.,Доход и прибыль фирмы при постоянных и переменных ценах. Выручка. Средний доход. Предельный доход. 4 ситуации получения прибыли фирмы по соотношению общих выгод и издержек. Функция прибыли на графике.,Рыночные структуры. Характерные черты совершенной конкуренции. Фирма-ценополучатель. Значение модели совершенной конкуренции.,Краткосрочные кривые фирмы. Кривая спроса на продукцию фирмы-совершенного конкурента. Формулы и кривые совокупного, среднего и предельного дохода фирмы-совершенного конкурента.,Равновесие фирмы. Оптимальный объем выпуска. Метод совокупных издержек. Метод предельных издержек. Совместная динамика предельной и общей прибыли. Соотношения предельных издержек и предельного дохода. Средняя прибыль.,Условие получения краткосрочной прибыли (варианты рыночной конъюнктуры). Условие прекращения производственной деятельности.,Кривая предложения фирмы-совершенного конкурента. Рыночная кривая предложения.,Равновесие в долгосрочном периоде. Специфика положения фирмы в краткосрочном и долгосрочном периодах. Условие равновесия фирмы в долгосрочном периоде. Перелив капитала в случае экономической прибыли, убытка, безубыточности: графики фирмы и отрасли, логика развития ситуации. Несовершенная эластичность рынка на сжатие и расширение.,Кривые долгосрочных издержек и эффект масштаба. Долгосрочные общие издержки (графики). Долгосрочные средние издержки: определение, построение графика. Оптимальный размер предприятия. Минимально эффективный размер предприятия. Положительный эффект масштаба производства и LATC. Причины положительного эффекта масштаба. Отрицательный эффект масштаба производства и LATC. Причины отрицательного эффекта масштаба. Постоянный эффект масштаба производства и LATC.,Рыночная власть и монополия. Понятие рыночной (монопольной) власти. Коэффициент Лернера. Источники монопольной власти. Монополия в узком и широком смысле. Монопсония. Дуополия. Чистая монополия: допущения.,Барьеры для конкуренции. Естественные и искусственные барьеры. Стратегические и нестратегические барьеры. Естественная, временная, открытая, легальная, локальная, административная, закрытая и искусственная виды монополий. Недобросовестная конкуренция: понятие и содержание.,Спрос и доход фирмы-монополиста. Ценопроизводитель. Власть монополиста в сфере назначения цен. Наклон кривой спроса для монополиста. Особенности кривой спроса для монополиста. Кривые общего и предельного дохода. Монополист работает на эластичном участке D (доказательство).,Условия максимизации прибыли для фирмы-монополиста (аналитически и графически): метод совокупных издержек  совокупного дохода, метод предельных издержек  предельного дохода. Отличие нахождения оптимума при совершенной конкуренции и монополии. Точка оптимума и прибыль монополиста (3 случая). Точка закрытия монополиста. Предложение фирмы-монополиста: традиционное и убывающее. Единая кривая предложения монополиста.,Ценовая дискриминация. Дополнительная выручка от дискриминации: 2 эффекта. Условия эффективности ценовой дискриминации. Арбитраж. Ценовая дискриминация первой степени: понятие и график. Ценовая дискриминация второй степени. Примеры. Ценовая дискриминация третьей степени. Примеры.,Олигополия. Свойства олигополистического рынка. Коэффициент Лернера при олигополии. Взаимозависимость олигополистов (особенность рынка). Олигополистическое взаимодействие. Олигополист и кривые спроса на его продукт, предельного дохода, точка равновесия, оптимум MR = MC.,Виды моделей олигополии. Некооперированная и кооперированная олигополия. Дуополия.,Модель Курно. Предпосылки. Основная задача модели. Суть взаимодействия. Кривая остаточного спроса. Общий доход фирмы. Предельный доход фирмы. Оптимальный объем фирмы. Функция реакции (аналитически, графически). Экономический смысл кривых реакции. Точка равновесия Курно. Отраслевой оптимум (вывод). Параметры отраслевого равновесия (аналитически).,Модель картеля. Основная цель образования картеля. Направления сговора. Международные картели. Картели в России. Административная (КОАП) и уголовная (УК) ответственность за организацию картеля.,Параллелизм олигополистов. Понятие параллелизма. Преимущество параллелизма в отличие от картелей. Формы параллелизма. 2 типа фирм в отрасли. Ценовое лидерство. Свойства лидера и виды лидерства. Лидерство доминирующей фирмы. Общий принцип лидерства. Факторы, препятствующие ценовой координации.,Основные черты рынка монополистической конкуренции. Следствие большого количества продавцов. Барьеры вхождения в отрасль. Причины их небольшой высоты. Продуктовая дифференциация. Факторы дифференциации. Критерий дифференциации. Горизонтельная и вертикальная дифференциация продукта. Сегмент рынка. Стратегия дифференциации продукта. Лояльность потребителя. Концепция уникального рыночного предложения. Неценовая конкуренция. Причины неэффективности ценовой конкуренции. Примеры рынков монополистической конкуренции.,Условия максимизации прибыли в краткосрочном периоде. Промежуточное состояние между совершенной конкуренцией и монополией. Отличия от монополиста. Эластичность и степень монопольной власти. Кривая спроса на продукцию монополистического конкурента: свойства и график. Рыночный спрос на монополистически конкурентном рынке и степень замещения продукта. Предельный доход фирмы монополистического конкурента. Преимущества и недостатки рынка монополистической конкуренции.,Понятие рынка ресурсов. Специфика ресурсных рынков. Виды доходов, получаемые от каждого вида ресурсов. Виды рынков ресурсов. Спрос и предложение на рынке ресурсов. Факторы, определяющие спрос на ресурс. Факторы, определяющие эластичность спроса на ресурс. Особенность предложения ресурсов. Выбор сочетания ресурсов: правило минимизации издержек и правило максимизации прибыли.,Рынок труда. Объект продажи на рынке труда: подходы разных экономических школ. Особенности труда как ресурса. Спрос на труд. Предложение труда. Индивидуальная и рыночная кривая предложения труда. Заработная плата. Номинальная и реальная заработная плата.,Рынок капитала. Трактовки понятия «капитал»: натуралистическая концепция, монетаристская концепция, концепция человеческого капитала. Формы капитала: производительная, товарная, денежная. Кругооборот капитала: производственного, торгового, спекулятивного. Основной и оборотный капитал. Доход за использование капитала: прибыль, процент, маржа Зависимость между процентной ставкой, сроком и риском. Номинальная и реальная процентная ставка. Равновесие на рынке капитала. Дисконтирование.,Рынок земли и рынок услуг земли. Цена земли, земельная рента. Предложение земли и его свойства. Абсолютная и дифференциальная рента. Дифференциальная рента 1 и 2. Цена земли.</t>
+  </si>
+  <si>
+    <t>Пространство товаров. Предпочтения потребителя (отношение предпочтения, основные аксиомы теория потребления). Кривые безразличия. Стандартные предпочтения (непрерывность, монотонность, выпуклость). Функция полезности (определение, важные теоремы, свойства, кривые безразличия как уровни функции полезности). Предельная норма замещения товаров в потреблении. Виды функций полезности, их связь с предпочтениями потребителей.,Бюджетное множество потребителя. Задача потребительского выбора (постановка, графический анализ, решение методом Лагранжа, функции обыкновенного спроса). Правило долей для предпочтений Кобба-Дугласа, особые случаи оптимального выбора потребителя. Косвенная функция полезности, предельная полезность по доходу, тождество Роя. Двойственность в теории потребления (задача минимизации расходов, спрос по Хиксу, функция расходов, предельный расход по полезности, лемма Шепарда, связь между прямой и двойственной задачей потребителя).,Влияние дохода на поведение потребителя (нормальные и инфериорные товары), кривая «доход-потребление» и кривые Энгеля. Влияние цены на поведение потребителя (обычные товары и товары Гиффена), кривые «цена-потребление» и кривые спроса. Эластичность спроса. Эффекты дохода и замещения, связанные с изменением цены. Уравнение Слуцкого. Излишек потребителя как мера его благосостояния.,Описание технологии производства (производственные факторы, производственная функция, изокванты, виды производственных функций). Свойства производственной функции (монотонность технологий, убывание предельного продукта, выпуклость технологий, отдача от масштаба). Предельная норма технологического замещения. Эластичность производства и эластичность замещения.,Экономические издержки. Общие издержки производства и изокосты. Короткий и длительный период в экономическом анализе. Минимизация издержек заданного объема выпуска: определение экономически эффективного способа производства (аналитическое и графическое решение). Функция издержек. Траектория роста фирмы. Графический анализ общих, средних и предельных издержек в длительном и коротком периодах. Взаимное расположение краткосрочных и долгосрочных кривых издержек.,Прибыль и условия ее максимизации. Решение задачи максимизации прибыли конкурентной фирмы в коротком и длительном периодах (процедура одношаговой оптимизации). Точка локального рыночного равновесия производителя. Функции спроса на производственные факторы и функция предложения выпуска. Двухэтапное решение задачи максимизации прибыли. Правило максимизации прибыли. Предложение конкурентной фирмы (критерии целесообразности производства, предельные издержки и кривая предложения). Излишек производителя. Равновесие конкурентной отрасли (предложение конкурентной отрасли в длительном периоде, принцип нулевой прибыли, условия долгосрочного равновесия на рынке совершенной конкуренции). Эффективность конкурентного рынка.,Поведение фирмы в условиях монополии. Спрос на продукт монополиста. Общий и предельный доход монополиста. Зависимость общего и предельного дохода от эластичности спроса по цене. Решение задачи монополиста. Монополия в коротком и длительном периоде. Отсутствие функции предложения у монополиста. Индекс Лернера, как показатель рыночной власти. Неэффективность монополии. Ценовая дискриминация.,Олигополия. Задача принятия решений в условиях конфликта сторон. Равновесие Нэша. Дуополия Курно. Дуополия Стекельберга. Конкуренция против сговора: дилемма заключенного. Влияние дилеммы заключенного на олигополистическое ценообразование. Максимизация прибыли в условиях картеля. Модели ценовой олигополии: дуополия Бертрана.,Рынок монополистической конкуренции. Равновесие фирмы на рынке монополистической конкуренции. Избыточная производственная мощность и плата за разнообразие.,Экономика обмена. Начальный запас. Допустимые распределения. Ящик Эджворта. Парето-улучшение и Парето-эффективность. Контрактная кривая (множество Парето) и ядро экономики. Совокупный избыточный спрос и равновесие по Вальрасу. Закон Вальраса. Конкурентное равновесие и эффективность. Эффективность и справедливость. Теоремы благосостояния.,Экономика с производством. Эффективность в сфере производства. Кривая производственных контрактов. Граница производственных возможностей. Предельная норма трансформации. Эффективность в структуре выпуска продукции. Парето-эффективность на рынке совершенной конкуренции. Теоремы благосостояния.,Базовые методы макроэкономического анализа (моделирование, агрегирование). Статика и динамика. Фактор времени (краткосрочный, среднесрочный и долгосрочный периоды в поведении экономики). Экономический рост и деловой цикл. Валовой внутренний продукт, номинальный и реальный ВВП, индекс реального ВВП, темп прироста ВВП, ВВП на душу населения. Уровень цен, ценовые индексы. Темп инфляции, формула Фишера. Уровень безработицы. Неравенство доходов.,Схема межотраслевого баланса. Модель Леонтьева. Коэффициенты прямых и полных материальных затрат. Продуктивность модели Леонтьева. Межотраслевой баланс в анализе экономических показателей (равновесные цены, межотраслевой баланс труда, оценка показателей фондоёмкости). Динамическая модель межотраслевого баланса. Модель Неймана расширяющейся экономики.,Кейнсианская функция потребления. Загадка Кузнеца. Модель межвременного выбора Фишера. Влияние богатства и ставки процента на потребление и сбережения. Модель жизненного цикла Модильяни. Иллюстрация гипотезы жизненного цикла в рамках модели Фишера. Модель перманентного дохода Фридмана. Иллюстрация гипотезы перманентного дохода в рамках модели Фишера.,Макроэкономические инвестиции. Неоклассическая модель инвестиций в основные фонды. Кейнсианский подход. Инвестиции в модели издержек приспособления (модель гибкого акселератора). Теория q-Тобина. Инвестиции в жилищное строительство. Инвестиции в запасы (модель жесткого акселератора). Вопрос отделимости потребительского решения от инвестиционного.,Модель кейнсианского креста для двухсекторной экономики. Мультипликатор автономных расходов, эффект мультипликатора. Парадокс сбережений. Индуцированные инвестиции и их воздействие на равновесие товарного рынка. Разрывы расходов и выпуска в модели кейнсианского креста. Равновесие товарного рынка в трехсекторной и четырехсекторной моделях экономики.,Количественная теория денег, уравнение обмена. Инфляция и ставка процента. Доход государства от эмиссии денег – сеньораж. Модель экзогенного предложения денег: денежная база и денежный мультипликатор. Модели спроса на деньги: портфельный подход, модель Баумоля-Тобина. Равновесие денежного рынка, равновесная ставка процента. Инструменты денежно-кредитной политики.,Предпосылки модели IS-LM. Совокупные расходы и ставка процента. Кривая IS как кривая равновесия товарного рынка. Кривая LM как кривая равновесия денежного рынка. Особые случаи линий IS и LM (ловушка ликвидности, процентная ловушка, инвестиционная ловушка). Макроэкономическое равновесие в модели IS и LM, достижение равновесия. Макроэкономическая политика в модели IS-LM. IS-LM как модель совокупного спроса. Мультипликаторы совокупного спроса. Модель IS-LM для открытой экономики.,Спрос на труд. Предложение труда. Равновесие рынка труда и безработица. Моделирование естественного уровня безработицы. Циклическая (конъюнктурная) безработица. Модель Оукена. Компромисс между инфляцией и безработицей. Кривая Филлипса как модель совокупного предложения.,Общая характеристика модели AD-AS. Краткосрочное, среднесрочное и долгосрочное равновесие в модели AD-AS. Шоки совокупного спроса и совокупного предложения. Стабилизационная политика в закрытой экономике. Парадокс сбережений в закрытой экономике с гибкими ценами и гибкой заработной платой. Монетарная политика. Последствия изменения совокупного предложения.,Факторы экономического роста. Модель экономического роста Солоу. Сравнительная статика в модели Солоу. Оптимальный запас капитала и золотое правило. Экономический рост и технологический прогресс, остаток Солоу.,Циклический характер экономической динамики. Деловой цикл и его фазы. Модель Самуэльсона-Хикса. Модель Тевеса. Практическое использование экономических циклов.</t>
+  </si>
+  <si>
+    <t>Понятие цепи поставок. Сетевая структура цепи поставок. Концепция управления цепями поставок (SCM – Supply Chain Management). Виды аналитики в управлении цепями поставок. Задачи цепей поставок и уровень абстракции. Аналитическая оптимизация и динамическое имитационное моделирование. Цифровые двойники цепей поставок. Цифровое управление цепями поставок (Digital SCM).,Важность размещения объектов цепи поставок. Подходы к решению задачи размещения. Гравитационный анализ. Эвристический метод Ардалана. Метод критической точки. Метод калькуляции затрат. Бальная оценка (scoring model). Задача единого среднего (single median problem). Задача охвата (covering problem).,Планирование цепи поставок (стратегическое, тактическое, оперативное). Основы оптимизационного моделирования (статическая модель, динамическая модель, модель с неопределенностью). Классическая транспортная задача. Транспортная задача с промежуточными пунктами. Задача о назначениях. Планирование доставки мелкопартийных грузов в условиях крупного города. Интегрированные модели цепи поставок (транспортно-складская задача, производственно-транспортно-складская задача).,Запас как объект управления в цепи поставок (понятие запаса, виды запасов, две точки зрения на запас). Движение запаса в звеньях цепи поставок. Модель Уилсона (EOQ-модель) и ее модификации (с задержками поставок, с разрывом цены, с дефицитом запаса, с учетом аккумулируемых в запасах денежных средств, с учетом фактора времени). Основные типы стратегий управления запасами. Многономенклатурные модели управления запасами. Управление запасами в интегрированных многоуровневых цепях поставок.,Ключевые преимущества anyLogistix. Аналитическая оптимизация и динамическое моделирование в anyLogistix. Создание цифрового двойника цепи поставок в anyLogistix. Эксперименты Greenfield Analysis – GFA (определение расположения объектов методом «центра тяжести»), Network Optimization – NO (определение оптимальной сетевой структуры и планирование материальных потоков), Simulation (имитационное моделирование для оценки конфигурации, политик и правил цепи поставок).</t>
+  </si>
+  <si>
+    <t>История возникновения понятий налог и налоговая система. Теоретические основы налогообложения. Принципы налогообложения, типы налоговых систем. Существенные элементы налога и их характеристика. Понятие налоговых обязательств. Возникновение и исполнения налоговых обязательств. Налогоплательщик и налоговый агент.,Виды и формы налогового контроля. Виды налоговых проверок. Порядок проведения налоговых проверок. Обжалование действий налоговых органов.,Административная, налоговая и уголовная ответственность. Виды ответственности и налоговые санкции. Условия и порядок привлечения к ответственности по налоговым преступлениям.,Транспортный налог, налог на имущество. Налогоплательщики, налоговая база, ставки налога, льготы по налогу, порядок расчета налога, налоговая отчетность, порядок взимания налога, порядок и способы уплаты налога в бюджет.,Налог на доходы физических лиц: место и роль в налоговой системе Российской Федерации. Доля налога на доходы физических лиц в структуре доходов бюджета. Налогоплательщики. Доходы от источников в РФ и доходы от источников за пределами РФ. Объект налогообложения. Объекты налогообложения для физических лиц, являющихся и не являющихся налоговыми резидентами РФ. Налоговая база. Доходы, не подлежащие налогообложению. Налоговые вычеты: стандартные, социальные, имущественные и профессиональные. Налоговый период. Налоговые ставки. Порядок определения налоговой базы по доходам налогоплательщиков, облагаемых по различным ставкам. Порядок определения налоговой базы при получении доходов в натуральной форме, доходов в виде материальной выгоды, по договорам страхования, по договорам негосударственного пенсионного обеспечения. Порядок исчисления и сроки уплаты. Порядок определения даты фактического получения доходов. Особенности исчисления сумм налога индивидуальными предпринимателями. Налоговая декларация и порядок ее представления. Санкции за нарушение установленного законодательством порядка уплаты налога физическими лицами.,Налогоплательщики, налоговая база, ставки налога, льготы по налогу, порядок расчета налога, налоговые вычеты, налоговая отчетность, порядок взимания налога, порядок и способы уплаты налога в бюджет.,Порядок перехода на УСНО. Налогоплательщики, объекты налогообложения. Порядок определения налогооблагаемой базы, отчетность по налогу, налоговые вычеты. Порядок и сроки уплаты налога в бюджет и представления отчетности по налогу.,Налог на прибыль, его место и роль в налоговой системе Российской Федерации. Доля налога на прибыль организаций в структуре доходов бюджета. Плательщики налога на прибыль. Объект обложения по налогу на прибыль. Порядок определения доходов. Классификация доходов. Расходы. Группировка расходов. Методика исчисления налоговой базы. Налоговый период и налоговые ставки. Порядок и сроки уплаты налога на прибыль. Налоговая декларация. Налоговый учет.,НДС: место и роль в налоговой системе Российской Федерации. Экономическая сущность НДС. Методы расчета добавленной стоимости. Налогоплательщики. Объект налогообложения. Налоговая база. Перечень товаров (работ, услуг), освобожденных от обложения НДС. Налоговый период. Налоговые ставки. Порядок исчисления налога и налоговые вычеты. Счет-фактура. Порядок и сроки уплаты НДС в бюджет.,Акцизы: сущность, социально-финансовые последствия акцизного налогообложения в Российской Федерации. Виды подакцизных товаров. Налогоплательщики. Порядок формирования объектов налогообложения и налогооблагаемой базы при расчете налога на территории РФ. Порядок исчисления акцизов. Налоговые вычеты. Особенности налогообложения операций с нефтепродуктами. Исчисление акцизных сборов при экспортно-импортных операциях.,Налог на добычу полезных ископаемых: роль НДПИ в системе недропользования в Российской Федерации, классификация полезных ископаемых, налогоплательщики, объект налогообложения, налоговая база, понятие «добытое полезное ископаемое», порядок определения количества добытого полезного ископаемого и оценки его стоимости, налоговый период, налоговые ставки, порядок исчисления и сроки уплаты.,Налогоплательщики, налоговая база, ставки налога, порядок расчета налога, налоговая отчетность, порядок взимания налога, порядок и способы уплаты налога в бюджет.</t>
+  </si>
+  <si>
+    <t>Тема 1. Развитие операционного менеджмента как области знаний и предмета практической деятельности. Базовая терминология и понятийный аппарат,Тема 2. Организация производства ,Тема 3. Организация и планирование производственного процесса во времени,Тема 4. Методы организации производства,Тема 5. Оперативно-производственное планирование,Тема 6. Инфраструктура предприятия/ организации</t>
+  </si>
+  <si>
+    <t>Состав активов бизнеса, предприятия, подлежащего оценке. Подготовка информации, необходимой для оценки бизнеса. Понятие рыночной стоимости. Виды стоимости. Основные подходы и методы оценки стоимости предприятия.,Социальные, экономические факторы. Физические условия объекта. Законодательство и изменения в сфере регулирования рынка в России. Политические факторы, влияющие на стоимость. Стандарты оценочной деятельности в Российской Федерации. Законодательство в сфере оценочной деятельности в Российской Федерации. Требования к оценщику, договору на оказание услуг по оценке. Требования к отчету по оценке имущества. Развитие саморегулируемых организаций в оценочной деятельности. Стандарты саморегулируемых организаций оценщиков.,Принципы оценки как основа аналитической деятельности оценщика. Принципы полезности, замещения, ожидания, добавочной продуктивности, вклада, баланса, экономического размера, разделения (объединения) элементов объекта и прав собственности на него. Определяющая роль соотношения спроса и предложения; принципы зависимости, соответствия, конкуренции, изменения и др. Роль принципа наилучшего и наиболее эффективного использования в оценке объекта. Основные подходы и методы в оценке рыночной стоимости бизнеса, особенности применения методов для оценки разных типов имущества.,Финансовый анализ и его необходимость в оценке бизнеса. Оценка контрольного и неконтрольного пакетов акций. Премия за контроль. Скидки за неконтрольный характер. Скидка за недостаточную ликвидность. Согласование результатов оценки.,Метод дисконтирования денежных потоков. Метод капитализации доходов Доходный подход: отличия метода дисконтированных денежных потоков и метода капитализации доходов. Таблицы сложного процента. Понятие капитализируемой прибыли и ее выбор. Понятия и порядок определения ставки дисконтирования и терминальной капитализации. Кумулятивный и рыночный подход, CAPM, WACC.,Метод сделок. Метод рынка капитала. Метод отраслевых коэффициентов Сравнительный подход к оценке стоимости предприятия: метод сделок, метод рынка капитала, метод отраслевых коэффициентов. Обоснование сравнительного подхода. Критерии отбора предприятий – аналогов. Принципы корректировки. Важнейшие ценовые мультипликаторы. Формирование итоговой величины стоимости.,Затратный подход: метод стоимости чистых активов и метод ликвидационной стоимости. Баланс предприятия и его корректировка. Анализ финансовой отчетности. Активы баланса предприятия: виды и особенности их оценки. Дебиторская и кредиторская задолженность предприятия: анализ и оценка. Значение и особенности оценки нематериальных активов компании.,Обзор отчета оценщика как итогового заключения об оценке стоимости предприятия.,Согласование результатов оценки. Особенности оценки стоимости предприятия для конкретных целей.</t>
+  </si>
+  <si>
+    <t>Определение системного подхода. Определение роли информационных систем в решении задач финансового учета и анализа на предприятии.,Структура и состав информационных систем финансового управления. Классификация информационных систем.,Понятие и характеристика ППП для решения функциональных задач финансового учета и анализа. Классификация ППП.,Примеры задач, которые могут быть решены с использованием ППП финансового учета и анализа.,Общие сведения о системе. Описание разделов Project Expert. Возможности аналитический системы.,Описание процессов построения модели, определения потребности в финансировании, разработки стратегии финансирования, анализа эффективности проекта, формирования отчетов и контроля реализации проекта в Project Expert,Алгоритм ввода общей информации о проекте. Настройка параметров расчета и отображения данных в Project Expert.,Описание финансово-экономического состояния предприятия на момент начала проекта.,Описание финансово-экономической среды, в которой планируется реализация проекта.,Составление календарного план-графика капитальных вложений. Определение этапов работ и расчет необходимых ресурсов. Формирование активов предприятия.,Формирование плана сбыта и производства продукции. Ввод сведений о материалах и комплектующих. Составление плана по персоналу. Расчет издержек.,Подготовка плана финансовой деятельности предприятия. Определение условий привлечения финансовых ресурсов, порядок обслуживания задолженности. Определение условий размещения свободных денежных средств и использования прибыли предприятия.,Формирование финансовых отчетов, таблиц и графиков, отражающих результаты моделирования деятельности предприятия.,Анализ финансовых показателей проекта. Оценка эффективности инвестиций. Анализ чувствительности проекта и его устойчивости к изменениям случайных факторов.,Алгоритм ввода фактической информации о ходе реализации проекта. План-фактный анализ показателей проекта.</t>
+  </si>
+  <si>
+    <t>Понятие хранилища данных (Data Warehouse). Назначение хранилища данных, его отличие от базы данных. Источники данных для хранилища. Основные принципы организации хранилища данных. Основные процессы работы с данными в хранилище.,Понятие OLAP. Основная цель OLAP-средств. Понятия измерения, метки и факта, способы определения фактов. Многомерная модель данных, понятие куба. Поликубическая и гиперкубическая модель данных. Операции, применяемые к кубам (агрегация, детализация, формирования среза, вращение).,Состав хранилища данных (таблицы измерений, таблица фактов). Типовые структурные схемы (схема звезды, схема снежинки), их достоинства и недостатки. Многоуровневые структуры данных для OLAP (сбалансированные, несбалансированные и неровные иерархии).,Требования, предъявляемые к продуктам OLAP (тест FASMI).Особенности OLAP-средств, встроенных в настольные приложения. Особенности сетевых OLAP-систем. Классификация OLAP-средств с точки зрения способа представления данных в хранилище (MOLAP, ROLAP, HOLAP). Достоинства и недостатки средств каждого класса. Физический OLAP и виртуальный OLAP.,Виртуальное хранилище данных, его достоинства и недостатки. Аналитическая пирамида. Краткая характеристика элементов архитектуры хранилища данных. Оперативный склад данных. Витрины данных (принципы построения, источники данных, виды витрин, преимущества и недостатки). Метаданные.,СIF –архитектура ("корпоративная информационная фабрика"). Хранилище данных с архитектурой шины BUS. Гибридная многоуровневая архитектура. Слоистая архитектура хранилища данных. Достоинства и недостатки архитектур каждого вида.,Типовая структура программной системы управления хранилищем данных (подсистема загрузки данных, подсистема представления данных и обработки запросов, подсистема администрирования хранилища).Технология ETL: назначение, процессы, реализуемые в ETL-системах. Особенности выполнения этапа извлечения данных из источников. Особенности выполнения этапа преобразования данных (перевод значений, внешнее и внутреннее обогащение, очистка и агрегирование данных). Особенности выполнения этапа загрузки данных в хранилище.,Уровни управления в организациях, принятие решений и пакеты прикладных программ. Уровни управления и пакеты прикладных программ (системы обработки транзакций; системы информационного уровня; управленческие системы и системы поддержки принятия решений; системы поддержки принятия стратегических решений). Место пакетов прикладных программ оперативного анализа данных в информационной системе предприятия.,Предпроектное обследование предметной области (анализ предметной области, техническое задание, экономическое обоснование, основные виды затрат). Особенности проектирования хранилища данных. Реализация и внедрение (выбор способа представления хранилища, этапы тестирования). Основные виды конверсии (параллельная стратегия, стратегия прямого переключения, пилотная и фазовая стратегии). Особенности эксплуатации и модификации. Основные модели жизненного цикла (каскадная и спиральная модели).,Корпоративная модель данных, особенности спирального подхода к построению корпоративной модели данных. Выбор типовой структурной схемы корпоративного хранилища данных. Методы разработки модели корпоративного хранилища данных (с помощью реконструкции, на основе шаблонов, разработка под заказ).,Уровни архитектуры хранилища данных для больших данных (уровень получения данных, интегрированное ядро, уровень доступа, уровень использования). Модель данных Data Vault: основные особенности, основные компоненты (Hub, Link, Satellite). Особенности организации работы с данными на основе методологии Data Vault (промежуточная область Staging area, разделы Raw Data Vault и Business Vault).,Основные особенности CASE-технологии. Возможности современных CASE-средств. Классификация CASE-средств (по типам, по категориям, вспомогательные типы).,Понятие проекта хранилища данных. Таблицы измерений и таблицы фактов. Типовые структурные схемы «звезда» и «снежинка». Понятие процесса в хранилище данных Deductor Studio.,Основные понятия Deductor Warehouse: семантический слой, измерение, ссылка, атрибут. Структура программного окна Deductor Studio; панель управления и область визуализаторов; подключения и сценарии; основные компоненты Deductor Studio (мастера подключений, импорта, экспорта, обработки и визуализации), последовательность работ.,Создание типовой структуры хранилища данных, формирование метаданных, создание сценариев. Подготовка исходных данных. Импорт данных. Очистка данных (фильтрация, выявление дубликатов и противоречий, обнаружение и редактирование аномалий, сглаживание) и загрузка импортированных данных в хранилище данных.,Очистка процессов и измерений, удаление измерения и процесса в хранилище, добавление атрибута, факта и измерения в процесс.,Создание сценариев импорта измерений с формированием таблиц, кубов, срезов. Назначение и виды визуализаторов, их возможности и использование. Создание сценариев импорта из процесса с формированием таблиц и кубов.,Создание куба в хранилище данных, импорт куба из хранилища данных и построение его среза. Отличие кубов в хранилище данных и в сценарии. Использование кросс-диаграмм и кросс-таблиц.,Настройка кросс-таблицы и куба, фильтрация в таблице и кубе, преобразование даты и времени, настройка набора данных, разбиение области значений непрерывного числового параметра на интервалы (квантование), замена данных, добавление полей, значения которых вычисляются из значений других полей. Объединение (слияние) данных.,Проверка сезонности. Подготовка данных для построения модели. Построение пользовательской модели и ее использование для прогнозирования. Построение модели линейной регрессии и ее использование для прогнозирования. Построение модели нейронной сети и ее использование для прогнозирования.,Ассоциативные правила. Параметры, характеризующие ассоциативные правила (поддержка, достоверность, лифт). Настройка параметров поиска ассоциативных правил. Поиск ассоциативных правил. Визуализаторы, используемые для оперативного анализа ассоциативных правил («правила», «популярные наборы», «что-если», «дерево правил»). Интерпретация ассоциативных правил.,Скрипты (определение термина, настройка скрипта). Использование в сценариях ранее созданных ветвей обработки данных. Использование ранее созданных моделей для анализа новых данных и прогнозирования с помощью скрипта.</t>
+  </si>
+  <si>
+    <t>Тема 1. Традиционная модель рационального поведения. Истоки поведенческой экономики,Тема 2. Теория Перспектив,Тема 3. Причины ошибок при принятии решений,Тема 4. Эвристики суждения,Тема 5. Поведенческие эффекты,Тема 6. Влияние на поведение людей. Концепция Nudge,Тема 7. Грамотный потребитель финансовых услуг</t>
+  </si>
+  <si>
+    <t>Тема 1. Введение в дисциплину «Портфельные инвестиции»,Тема 2. Долевые ценные бумаги как объекты портфельного инвестирования,Тема 3. Облигации как объекты портфельного инвестирования,Тема 4. Финансовые вычисления на рынке ценных бумаг,Тема 5. Производные финансовые инструменты,Тема 6. Инвесторы на рынке ценных бумаг,Тема 7. Формирование и оценка риска портфеля ценных бумаг,Тема 8. Профессиональная деятельность на рынке ценных бумаг,Тема 9. Основы анализа ценных бумаг</t>
+  </si>
+  <si>
+    <t>Причины возникновения государства как особой формы организации общества, как социального механизма, обеспечивающего согласование дел и специальных интересов групп и слоев гражданского общества. Признаки государства: особая публичная (государственная) власть и осуществление этой власти особым аппаратом: территориальная организация населения; налоги и займы, законодательство; государственный суверенитет. Функции государства. Внутренние (охранительные, регулятивные) функции. Внешние функции государства,Форма правления. Парламентарная и президентская республики. Монархия, ее виды и особенности. Форма государственного устройства. Федеративные и унитарные государства. Конфедерация.,Право как совокупность правил поведения, исходящих от государства. Обеспечение правом меры равенства и справедливости, согласования воли общества и гражданина. Взаимодействие права с государством,Общая характеристика законодательной, исполнительной и судебной ветвей государственной власти. Система сдержек и противовесов.,Принципы (основные начала), положенные в основу организации и деятельности органов государства: верховенство закона, принцип децентрализации власти, принцип разделения властей. Разделение государственных органов на законодательные, исполнительные и судебные; на органы власти РФ и государственные органы субъектов РФ.,Президент как гарант охраны независимости государства, целостности территории РФ, соблюдения прав и свобод человека и гражданина, согласованного функционирования органов государственной власти. Порядок выборов и прекращение полномочий Президента РФ. Компетенция Президента РФ.,Федеральное собрание РФ – представительный и законодательный орган РФ. Порядок формирования Совета Федерации и выборов депутатов Государственной Думы – палат Федерального Собрания. Полномочия Совета Федерации и Государственной Думы. Порядок рассмотрения, принятия и обнародования законов.,Порядок формирования и состав правительства. Основные направления деятельности: в сфере управления экономикой, в сфере социальной политики, в сфере обеспечения законности, прав и свобод граждан.,Конституционные принципы осуществления судебной власти: осуществление правосудия только судом; законность; гласность судебного разбирательства; презумпция невиновности; коллегиальность; состязательность и равноправие сторон; независимость судей и подчинение их только Конституции РФ и федеральному закону.,Конституционный суд РФ. Порядок формирования и его полномочия. Верховный Суд РФ. Порядок формирования и его полномочия. Система судов общей юрисдикции и арбитражных судов.,Основные направления деятельности прокуратуры. Полномочия прокуратуры.,Адвокатура. Принципы и формы оказания юридической помощи. Министерство внутренних дел РФ и его органы. Полномочия органов полиции.,Право как совокупность правил поведения, исходящих от государства. Обеспечение правом меры равенства и справедливости, согласования воли общества и гражданина. Взаимодействие права с государством.,Норма права как общеобязательное, формально-определенное, установленное обществом и государством правило поведения, наделяющее участников общественных отношений правами и обязанностями, обеспечиваемое и охраняемое от нарушений государством, Структура правовой нормы – гипотеза, диспозиция, санкция. Виды правовых норм: регулятивные (управомочивающие, обязывающие, запрещающие); охранительные.,Понятие источников права. Виды источников права: письменные правовые акты (нормативные акты); правовые обычаи; судебные прецеденты, нормативные договоры. Деление нормативных актов на законы и подзаконные акты. Закон – нормативный акт, обладающий высшей юридической силой, принятый представительным органом государственной власти. Виды законов: Конституция (Основной закон РФ); федеральные конституционные законы, федеральные законы; законы, принимаемые законодательными органами субъектов РФ.,Признаки Конституции: верховенство в системе права; высшая юридическая сила; первичность норм Конституции по отношению ко всем правовым актам.,Понятие правового отношения как конкретизированной юридической связи между участниками (субъектами) общественного отношения, урегулированного нормами права. Объект, стороны, содержание правоотношения. Возникновение, изменение и прекращение правовых отношений. Юридические факты – события и действия, с которыми закон связывает наступление юридических последствий.,Понятие правонарушения. Признаки правонарушения: причинение вреда интересам личности, общества, государства; противоправность; деяние дееспособных, вменяемых лиц; наличие вины. Состав правонарушения. Объект правонарушения – общественные отношения, которые регулируемые и охраняемые правом. Объективная сторона правонарушения: деяние, направленное на определенный объект; причинная связь между противоправным деянием и его общественно-вредными последствиями. Субъект правонарушения. Субъективная сторона правонарушения. Вина и ее формы. Прямой умысел. Косвенный умысел. Неосторожность в форме легкомыслия или небрежности. Мотив и цель правонарушения. Виды правонарушений: административные, дисциплинарные проступки, гражданские правонарушения, уголовные преступления.,Понятие юридической ответственности. Признаки юридической ответственности: юридическая ответственность предполагает государственное принуждение, связь юридической ответственности с правонарушением; ответственность влечет за собой негативные последствия для правонарушителя. Основания возникновения юридической ответственности – факт совершения правонарушения. Виды юридической ответственности. Дисциплинарная и материальная ответственность по трудовому праву. Административная ответственность как вид административного принуждения. Уголовная ответственность как исходящее от имени государства воздействие на гражданина в виде определенных лишений личного или имущественного характера.,Понятие, признаки, виды субъектов и объектов гражданского права. Понятие сделки, ее форма, виды сделок, недействительные сделки. Обязательства: понятие, общая характеристика договорных и внедоговорных обязательств.,Брак: порядок заключения и прекращения, основные права и обязанности супругов.,Трудовой договор: понятие, признаки, виды, стороны. Порядок заключения, изменения, прекращения трудового договора.,Основные институты административного права. Характеристика источников административного права. Административное правонарушение и административная ответственность.,Преступление: понятие, признаки, виды. Состав преступления: значение и характеристика его элементов. Наказание: понятие, цели, система наказаний, отдельные виды наказаний.,Гражданский процесс: виды судебных производств, понятие и признаки лиц участвующих в деле, их основные права и обязанности, доказательства. Арбитражный процесс: виды судебных производств, понятие и признаки лиц участвующих в деле, их основные права и обязанности, доказательства. Уголовный процесс: досудебное и судебное производство, понятие и виды участников уголовного судопроизводства, их права и обязанности.</t>
+  </si>
+  <si>
+    <t>Статистика ,Человек в пространстве количественной информации,Мир растений,Биотехнологии и общество,Атмосфера, климат, погода,Финансовая математика для чайников,Разработка Web-приложений,Мультимедийные сервисы для современного исследователя,Радиофизика вокруг нас,Игровые решения для образования,Введение в социально-политический мир,Культурная антропология,Экономико-географическая картина мира,Активные процессы в современном русском языке,Мифы и ритуалы третьего тысячелетия,в том числе дополнительные практикумы для иностранных студентов:,Деловая риторика и новая коммуникативная грамотность,Морфология искусства,Живопись. Методы творческой интерпретации,Метаморфозы Овидия и европейское искусство,Дизайн-проектирование и организация креативной работы,Мир как текст. Текст как мир,в том числе дополнительные практикумы для иностранных студентов:,Русский язык как иностранный: творческие практики,1.1 Введение в проблематику мастерской. ,1.2 Совместная постановка проблемы.,1.3 Предпроектный анализ. Работа с теоретическими материалами. Выдвижение замысла проекта (исследования). Разработка карты проблем.,2.1 Работа с проблематикой мастерской, в т.ч. с использованием технологий, программных продуктов, лабораторной базы. темы.,2.2 Планирование проектной деятельности. Согласование требований к результатам. Выдвижение замысла исследования, гипотезы. Распределение ролей в команде,2.3 Работа с теоретическими материалами. Описание гипотезы исследования. Составление перечня необходимых работ и процедур. Составление плана работы.,3.1 Работа с проблематикой мастерской, в т.ч. с использованием технологий, программных продуктов, лабораторной базы,3.2 Мониторинг проведения исследования. Результаты индивидуального исследования. Уточнение плана исследования.,3.3 Мониторинг проведения исследования. Промежуточные результаты групповой работы. Уточнение плана завершения проекта.,3.4 Работа с теоретическими материалами. Разработка проектного решения. Обсуждение результатов в группе. Оформление результатов проекта,4.1 Презентация проекта. Анализ результатов.,4.2 Взаимное рецензирование. Выбор лучшего проекта</t>
+  </si>
+  <si>
+    <t>Тема 1. Предприниматель и предпринимательская деятельность. Предмет и задачи курса. Предприниматель и предпринимательская активность: основные концепции. Деловая среда и ее структура. Отечественное предпринимательство в ретроспективе и современный статус. Экономический инструментарий в предпринимательской деятельности.,Тема 2. Предприятие как хозяйствующий субъект. Предприятие: понятие и концепции. Коммерческие и некоммерческие организации и их виды. Организационно-правовые формы предприятий и их характеристика. Учредительные документы организации. Понятие агентских отношений и их роль в функционировании предприятий различных организационно-правовых форм. Понятие малого предприятия. Учет и налогообложение малого бизнеса. Формы прекращения деятельности организации. Прекращение деятельности в деталях: теоретические концепции. Порядок регистрации и ликвидации коммерческой организации. Предпринимательская экосистема.,Тема 3. Концепция бизнеса и деловое проектирование. Концепция бизнеса и стадии делового проектирования. Бизнес-идея: методы генерации, оценки и документирования. Оценка важности для потребителей отдельных характеристик продукта. Понятие и назначение бизнес-модели, ее структура и содержание. ЦП и УТП. Портрет потребителя и целевая аудитория. Сегментация рынка. Методы ценообразования и оптимизация цены продукта. Емкость рынка продукта и методы ее оценки. Бизнес процессы компании: понятие и описание. Расходы компании: виды и методы оценки. Оценка экономической целесообразности организации бизнеса (содержание, порядок и документальное оформление). Формирование команды бизнес-проекта: подходы и методы. Презентация проекта: виды, назначение, особенности структуры, тактика организации.</t>
+  </si>
+  <si>
+    <t>Тема 1. Предмет региональной экономики и управления. Понятие и типологизация регионов.,Тема 2. Теоретические основы региональной экономики.,Тема 3. Регион как объект хозяйствования и управления.,Тема 4. Природно-ресурсный потенциал региона. Распределение экономической деятельности в пространстве.,Тема 5. Регион как объект макроэкономического анализа.</t>
+  </si>
+  <si>
+    <t>Неопределенность и риск. Определение риска. Качественное и количественное понимание рисков. Особенности проявления риска на практике. Классификация рисков. Теория риска и ее развитие. Подходы к оценке рисков. Связь риска и доходности. Основные методы управления рисками. Международные стандарты управления рисками. Культура управления рисками в организации.,Формализация условий ситуации риска. Измерение риска. Проблема сравнения альтернатив. Отношение к риску. Графическое представление рисковых предпочтений. Функция рискового предпочтения. Критерии оценки рисковых решений. Выбор наилучшего решения в условиях риска на основе метода дерева решений.,Анализ чувствительности как метод оценки устойчивости инвестиционного проекта. Основные меры риска инвестиционного проекта. Поправка на риск коэффициента дисконтирования. Оценка риска инвестиционного проекта на основе дерева событий. Сценарный подход к анализу рисков. Использование дерева решений при оценке риска инвестиционных проектов. Имитационное моделирование в инвестиционной аналитике. Управление рисками инвестиционного проекта.,Риск инвестиций в облигации. Цена и доходность облигации. Временная структура процентных ставок. Кривая доходности. Чувствительность цены облигации к параллельным сдвигам кривой доходности. Показатели рыночного риска облигаций – модифицированная дюрация и выпуклость. Хеджирование портфеля облигаций (иммунизация).,Ожидаемая доходность и риск портфеля ценных бумаг. Диверсификация рисков. Портфель Марковица. Эффективная граница. Роль коротких продаж в формировании эффективного портфеля. Оптимизация Тобина. Касательный портфель. Бета-коэффициент. Премия за риск. Оценка рисков активов на основе модели Шарпа. Концепции рисков в моделях CAPM, SML, ATR, их применимость в современной экономической теории и практике.,Капитал под риском (VaR). Основные методы расчета VaR по рыночным данным. Историческое моделирование. Параметрический VaR. Расчет VaR методом Монте-Карло. Верификация модели расчета VaR по историческим данным (backtesting).</t>
+  </si>
+  <si>
+    <t>Стратегический менеджмент как самостоятельная исследовательская область и управленческая практика. Существующие подходы к стратегическому управлению. Этапы развития стратегического менеджмента. Эволюция парадигм управления. Связь стратегического менеджмента со стратегией. Различия между стратегическим и оперативным управлением. Стратегическое мышление. Эффективный стратегический менеджмент. Ключевые элементы концепции стратегического управления в современных условиях. Индустрия4.0 и стратегическое управление.,Нестабильность внешней среды и деятельность компании. Стратегическая установка. Стратегическое видение. Параметры стратегического видения и его преимущества. Стратегические альтернативы. Ценности и миссия компании. Формулирование миссии: причины и рекомендации. Ключевые цели и задачи организации. Особенности стратегических целей. Постановка целей по SMART. Стратегия компании. Мифы о стратегии. Природа стратегических решений. Запрограммированные и незапрограммированные решения.,Стратегический анализ, стратегический выбор и реализация стратегии как ключевые этапы стратегического управления. Стратегический анализ: понятие и компоненты (цель, задачи, ожидания и полномочия, анализ внешней обстановки, анализ внутренних ресурсов). Стратегический выбор: понятие и компоненты (выработка вариантов стратегии, оценка вариантов стратегии, выбор стратегии, стратегические линии поведения и планы). Реализация стратегии: понятие, проблемы и мероприятия (разработка варианта действий при непредвиденных обстоятельствах, разработка организационной структуры, выбор системы управления организацией, политика организации, выбор организационного объединения и систем контроля).,Стратегия компании. Пирамида разработки стратегии для диверсифицированной компании. Корпоративная стратегия. Бизнес-стратегия. Функциональная стратегия. Операционная стратегия. Пирамида разработки стратегии для однопрофильной компании. Консолидация усилий по выработке стратегии. Критерии успешной стратегии.,Роль изменений в стратегическом управлении. Виды стратегических изменений. Модели стратегических изменений. Стадии реализации. Стратегирование: сущность, преимущества и недостатки. Модель стратегирования.,Микро- и макросреда компании. Роль анализа внешней среды. BANI-мир и лидерство в нем. Вызовы BANI-мира и его влияние на стратегические решения бизнес-структур.,PESTLE-анализ. Количественная и качественная оценка. Отраслевой анализ. Определение доминирующих в отрасли экономических характеристик. Внеотраслевые возможности для бизнес-струткур сегодня. Деятельность экосистем.,Структурный анализ конкурентного окружения. Модель конкуренции М. Портера. Угроза проникновения на рынок потенциальных конкурентов. Власть покупателей. Власть поставщиков. Угрозы со стороны заменителей товара или услуги. Уровень конкурентной борьбы между традиционными конкурентами. Продуктовые и географические границы товарного рынка. Барьеры для входа на рынок (экономические и административные ограничения, стратегия поведения компаний, направления на создание барьеров входа на рынок, наличие среди действующих на рынке хозяйствующих субъектов вертикально-интегрированных компаний). Рыночная власть.,Анализ затрат конкурентов: выявление стратегических факторов, управляющих затратами; анализ затрат, моделирование затрат конкурента.,Карты стратегических групп.,Общие конкурентные стратеги: лидерство по затратам, индивидуализация (дифференциация) и фокусирование. Ключевые факторы успеха.,Ключевые элементы внутренней среды. Цели (задачи). Структура организации. Финансовые ресурсы. Трудовые ресурсы. Производственная деятельность. Сбыт. Исследования и разработки. Системы и процедуры. Информационное обеспечение, необходимое для исследования внутренних факторов. Использование управленческого учета. Анализ ключевых компетенций и конкурентных преимуществ компании. Ключевые факторы успеха и устойчивое конкурентное преимущество. Этапы процесса оценки преимуществ и недостатков. Результативность использования ресурсов. SNW-анализ. Анализ гибкости и навыков. Модель формирования стоимости М.Портера.VRIO-анализ.,Необходимость проведения ситуационного анализа в рамках стратегического управления. Оценка применяемой стратегии. Gap-анализ. SWOT-анализ. Идентификация стратегических походов для выработки дальнейших действий. Метод экспертных оценок.,Определение наиболее выгодного стратегического положения. SPACE-модель. Адаптация и использование лучшего опыта в деятельности компании. Бенчмаркинг. Выявление новых трендов и прогнозирование их востребованности у конечного потребителя в будущем.,Концепция заинтересованных сторон. Существующие определения заинтересованных сторон. Выявление заинтересованных сторон. Составление карты заинтересованных сторон, карты отношений и списка 9С. Анализ заинтересованных сторон: цели, матрица власть и интерес Менделоу/Джонсона, матрица власть и интерес Прайса. Девять карт заинтересованных сторон по Скоулзу. Управление заинтересованными сторонами.,По уровням разработки стратегий. Базовые (базисные, эталонные) стратегии. Конкурентные стратегии. Стратегии слияния и поглощения. Международные стратегии. Стратегические хозяйственные зоны. Стратегические ошибки.,Факторы, влияющие на выбор стратегий внутреннего роста. Виды стратегий внутреннего роста. Концентрация, развитие рынка, разработка (обновление) продукта и диверсификация как стратегии внутреннего роста (понятие, преимущества и недостатки, применение российскими компаниями).,Факторы, влияющие на выбор стратегий внешнего роста. Диверсификация (концентрическая и конгломератная) и интеграция (горизонтальная и вертикальная) как стратегии внешнего роста (понятие, преимущества и недостатки, применение российскими компаниями).,Факторы, влияющие на принятие решений о международной стратегии. Трудности реализации данных стратегий. Направления международного стратегического развития. Международные стратегии и финансовое планирование.,Корпоративные стратегии слияния и приобретения: определение, мотивы, формы. Сопротивление приобретению и разделение компании.,Использование матричного анализа. Матрица Бостонской консалтинговой группы (БКГ). Матрица «Привлекательность отрасли – конкурентоспособность» (матрица GeneralElectric (GE) /McKinsey). Матрица «Продукт – рынок» И.Ансоффа. Признаки дисбаланса и устойчивого развития. Стратегия входа на рынок. Стратегия ухода с рынка. Создание портфеля и выбор оптимальногопортфеля. Корректировка стратегии.,Стратегия голубого океана. Цифровая (диджитал) стратегия. Стратегия в области устойчивого развития, корпоративной социальной ответственности. Климатическая стратегия. Стратегии 2020-2022. Обдуманная и срочная стратегии. Стратегии и действия.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Основные понятия. Операции над событиями. Виды случайных событий. Свойства операций над событиями. Классическое определение вероятности. Свойства вероятности., Элементы комбинаторики. Геометрические вероятности. Условная вероятность. Независимость событий. Теоремы сложения и умножения вероятностей., Полная группа событий. Формула полной вероятности. Гипотезы. Формула Байеса. Аксиоматическое построение теории вероятностей., Последовательность независимых испытаний. Определение схемы Бернулли. Примеры испытаний Бернулли. Формула Бернулли. Наивероятнейшее число наступлений события., Формула Пуассона. Локальная формула Муавра-Лапласа. Интегральная формула Муавра-Лапласа., Определение случайной величины. Типы случайных величин. Закон распределения случайной величины. Ряд распределения дискретной случайной величины. Функция распределения. Свойства функции распределения. Плотность вероятности непрерывной случайной величины. Свойства плотности вероятности., Математическое ожидание случайной величины. Свойства математического ожидания. Дисперсия случайной величины. Свойства дисперсии. Среднее квадратическое отклонение случайной величины. Мода, медиана и моменты случайной величины. Квантиль уровня p случайной величины., Биномиальный закон распределения. Математическое ожидание и дисперсия случайной величины, распределенной по биномиальному закону. Закон распределения Пуассона. Математическое ожидание и дисперсия случайной величины, распределенной по закону Пуассона., Геометрическое распределение. Математическое ожидание и дисперсия случайной величины, имеющей геометрическое распределение. Гипергеометрическое распределение. Математическое ожидание и дисперсия случайной величины, имеющей гипергеометрическое распределение., Равномерный закон распределения. Показательный (экспоненциальный) закон распределения. Нормальный закон распределения., Понятие о системе случайных величин. Типы двумерных случайных величин. Закон распределения вероятностей двумерной случайной величины. Функция распределения двумерной случайной величины и ее свойства., Понятие плотности вероятности двумерной непрерывной случайной величины. Свойства плотности вероятности двумерной непрерывной случайной величины. Равномерное распределение двумерной непрерывной случайной величины., Понятие условного закона распределения. Условные законы распределения составляющих двумерной дискретной случайной величины. Условные законы распределения составляющих двумерной непрерывной случайной величины., Математическое ожидание двумерной случайной величины. Дисперсия двумерной случайной величины. Ковариация и коэффициент корреляции случайных величин., Понятие двумерного нормального закона распределения. Вероятностный смысл параметров двумерного нормального закона. Законы распределения составляющих случайной величины, распределенной по двумерному нормальному закону. Условное математическое ожидание. Регрессия., Лемма Чебышева. Неравенство Чебышева. Теорема Чебышева. Теорема Бернулли. Центральная предельная теорема., Понятие функции случайной величины. Функция дискретной случайной величины. Функция непрерывной случайной величины. Числовые характеристики функции случайной величины., Закон распределения функции двух случайных величин. Распределение суммы двух непрерывных случайных величин. Распределение произведения двух непрерывных случайных величин., Понятие случайной функции. Понятие случайного процесса. Задание случайного процесса. Одномерная и n-я мерная функция распределения случайного процесса. Классификация случайных процессов. , Математическое ожидание случайного процесса. Свойства математического ожидания случайного процесса. Дисперсия случайного процесса. Свойства дисперсии случайного процесса. Корреляционная функция случайного процесса. Свойства корреляционной функции случайного процесса., Предел случайного процесса. Свойства предела в среднеквадратичном. Производная случайного процесса. Интеграл от случайного процесса., Понятие цепи Маркова. Граф состояний. Цепь Маркова с дискретным временем. Цепь Маркова с непрерывным временем. Однородные цепи Маркова. Матрица перехода системы.</t>
+  </si>
+  <si>
+    <t>1.1. Основные понятия теории игр. Игра как математическая модель конфликта. Понятия игрока, хода игрока, чистой стратегии, игровой ситуации, функции выигрыша.,1.2. Классификация игр. Классификация по числу участников (парная, множественная), по числу стратегий (конечная, бесконечная), по возможности кооперации (коалиционная, бескоалиционная), по степени информированности участников (игра с полной информацией, игра с совершенной информацией).,1.3. Формы представления игры. Игра в нормальной форме (стратегическая, статическая). Биматричные игры. Игра в развернутой форме (динамическая игра, многошаговая игра). Дерево игры. Понятие информационного множества. Приведение игры в развернутой форме к игре в нормальной форме.,2.1. Понятие решения игры. Основные принципы, определяющие решение игры. Решение игры как равновесная ситуация. Принципы рациональности, осторожности, уравновешенности.,2.2. Виды игровых равновесий. Равновесие в доминирующих стратегиях. Равновесие Нэша. Равновесие в защитных (осторожных, максиминных) стратегиях. Понятие доминируемости игровывых ситуаций. Множество Парето. Оптимальность по Парето. Равновесие Штакельберга. Равновесие дрожащей руки.,2.3. Антагонистические игры. Платежная матрица игры. Седловая точка в платежной матрице. Значение (цена) игры. Смешанные стратегии и теорема Неймана (теорема о минимаксе) для биматричных игр. Решение игр и . Сведение конечной биматричной игры к задаче линейного программирования.,2.4. Экономические приложения стратегических игр с полной информацией. Дуополия Курно. Олигополия Курно. Дуополия Бертрана с однородной продукцией. Дуополия Бертрана с неоднородной продукцией. Конфликты при распределении общего блага. Стратегические игры на сетях. Парадокс Браэсса. Равновесие Вардропа и эгоистичная маршрутизация. Арбитражные механизмы разрешения конфликтов.,3.1. Динамические игры с полной и совершенной информацией. Модель дуополии Штакельберга. Модель последовательной торговой сделки Рубинштейна. Трехэтапная торговля. Многоэтапная торговля.,3.2. Последовательные игры с полной, но несовершенной информацией. Модифицированная модель Штакельберга.,3.3. Развернутая форма представления игр. Совершенное подыгровое равновесие Нэша. Последовательные игры с участием Природы.,4.1. Многократно повторяемые игры. Двукратно повторяемая игра. Бесконечно повторяемая игра. Стратегии переключения.,4.2. Достижимые платежи. Достижимые платежи и теорема Фридмана. Предельные Парето-оптимальные профили стратегий.,4.3. Экономические приложения повторяемых игр. Модель дуополии Курно (бесконечное число раз повторяемая игра).,5.1. Байесовские игры. Нормальная форма представления статических байесовских игр. Равновесие Байеса-Нэша. Модель Штакельберга при асимметричной информации.,5.2. Аукционы. Закрытый аукцион первой цены. Симметрические стратегии. Форматы аукционов.,6.1. Слабое секвенциальное равновесие. Понятие веры игрока. Понятие последовательной рациональности. Траектории равновесия,6.2. Сигнальные игры. Действие игрока как сигнал. Динамический сценарий сигнальной игры. Отправитель и получатель. Совершенное байесовское равновесие в сигнальных играх.,6.3. Игры с неполной и несовершенной информацией,7.1. Основные понятия и определения. Коалиция. Характеристическая функция игры. Супераддитивность.,7.2. Дележи и их свойства. Понятие дележа. Условие индивидуальной рациональности. Условие групповой рациональности. Доминируемость дележей.,7.3. Решение игры в форме характеристической функции. С-ядро и Н-М-решение. Вектор Шепли</t>
+  </si>
+  <si>
+    <t>Назначение и основные понятия теории экономических механизмов,Дизайн экономических механизмов,Функции согласия и общественного выбора,Принципы выявления предпочтений,Нэш-реализуемость механизмов,Механизмы, оптимальные по Парето,Типы агентов. Теоремы Эрроу ,Аукционы. Дизайн аукционов</t>
+  </si>
+  <si>
+    <t>Тема 1. Современная концепция управления проектами.,Тема 2. Организация проекта.,Тема 3. Планирование проекта.,Тема 4. Руководство и управление исполнением проекта.,Тема 5. Ценности и принципы гибких подходов Agile к управлению проектами</t>
+  </si>
+  <si>
+    <t>Физическая культура и спорт как социальный феномен современного общества. Средства физической культуры. Основные составляющие физической культуры. Социальные функции физической культуры. Формирование физической культуры личности. Физическая культура в структуре профессионального образования. Организационно – правовые основы физической культуры и спорта студенческой молодёжи России.,Воздействие социально-экологических, природно-климатических факторов и бытовых условий жизни на физическое развитие и жизнедеятельность человека. Организм человека как единая саморазвивающаяся биологическая система. Анатомо-морфологическое строение и основные физиологические функции организма, обеспечивающие двигательную активность. Физическое развитие человека. Роль отдельных систем организма в обеспечении физического развития, функциональных и двигательных возможностей организма человека. Двигательная активность и ее влияние на устойчивость, и адаптационные возможности человека к умственным и физическим нагрузкам при различных воздействиях внешней среды. Степень и условия влияния наследственности на физическое развитие и на жизнедеятельность человека.,Обучение в процессе физического воспитания обеспечивает одну из его сторон - физическое образование, содержанием которого является системное освоение человеком рациональных способов управления своими движениями, приобретение необходимого в жизни фонда двигательных умений, навыков, знаний. Основные принципы методики обучения и воспитания (методические принципы). Основные специфические средства физического воспитания - физические упражнения, вспомогательные средства - оздоровительные силы природы и гигиенические факторы. Общепедагогические (применяемые во всех случаях обучения и воспитания) и специфические (характерные только для физического воспитания) методы. Основы обучения движениям и оптимального развития физических качеств (силы, быстроты, выносливости, гибкости, ловкости).,Общая психофизиологическая характеристика интеллектуальной деятельности и учебного труда студента. Общие закономерности и динамика работоспособности студентов в учебном году и основные факторы её определяющие. Признаки и критерии нервно-эмоционального и психофизического утомления. Регулирование работоспособности, профилактики утомления студентов в отдельные периоды учебного года. Оптимизация сопряжённой деятельности студентов в учёбе и спортивном совершенствовании.,Виды диагностики при регулярных занятиях физическими упражнениями и спортом. Врачебный и педагогический контроль. Самоконтроль, его основные методы, показатели. Дневник самоконтроля. Использование отдельных методов контроля при регулярных занятиях физическими упражнениями и спортом. Коррекция содержания и методики занятий по результатам показателей контроля.,Понятия "двигательный навык", "двигательное умение". Обучение в процессе физического воспитания обеспечивает одну из его сторон - физическое образование, содержанием которого является системное освоение человеком рациональных способов управления своими движениями, приобретение необходимого в жизни фонда двигательных умений, навыков и связанных с ними знаний. Этапы обучения двигательному действию. Совершенствование двигательных действий.,Определение понятий "работоспособность", "утомление", "усталость". Прямые косвенные показатели работоспособности. Субъективные и объективные признаки утомления. Методы оценки работоспособности человека с учетом его субъективного и функционального состояний, прямых и косвенных показателей работоспособности. Рекомендации по применению средств физической культуры для направленной коррекции работоспособности, усталости, утомления.,Понятия здоровья, физического развития. Антропометрические измерения: понятия, виды, показатели. Методы антропометрических стандартов. Метод индексов. Методы оценки физического развития.,Общее представление о функциональном состоянии организма. Методика оценки функционального состояния сердечно-сосудистой системы с помощью функциональных проб. Методика оценки функционального состояния дыхательной системы.,Понятие об осанке, виды осанок. Определение правильности осанки. Основные причины нарушения осанки. Основные правила сохранения и исправления дефектов осанки. Методика коррекции осанки. Комплексы упражнений для исправления осанки. Методика коррекции телосложения.,Общее представление о саморегуляции психоэмоционального состояния. Приемы регуляции эмоциональных состояний. Преднамеренная задержка проявления или изменения выразительных движений. Специальные двигательные упражнения. Индивидуализированная разминка. Специальные виды массажа и самомассажа. Дыхательные упражнения. Приемы, основанные на регуляции эмоций через воздействие на различные анализаторы. Аутогенная тренировка. Регулирующее музыкальное воздействие. Психомышечная тренировка. Рекомендации по использованию простейших методов саморегуляции.,Основные физические качества – сила, быстрота, гибкость, выносливость, координационные способности. Методика развития силы. Методика развития быстроты. Методика развития гибкости. Методика развития выносливости. Методика развития ловкости.,Понятие "физическое самовоспитание". Основные этапы процесса физического самовоспитания. Методика оценки уровня физической подготовленности. Методика составления индивидуальных тренировочных программ. Рекреационная направленность использования средств физической культуры. Восстановительная направленность использования средств физической культуры.,Цель, направленность и формы самостоятельных занятий. Методика проведения простейших самостоятельных занятий физическими упражнениями гигиенической направленности. Методика проведения самостоятельных занятий тренировочной направленности. Ходьба, оздоровительный бег, занятия лыжным спортом, плавание.,Определение понятий "массаж", "самомассаж", основные приемы. Различные виды массажа (косметический, спортивный, лечебный, гигиенический). Формы массажа и самомассажа: общий, и частный (местный). Методические основы самомассажа.,Причины возникновения миопии. Коррегирующая гимнастика для глаз. Комплекс специальных упражнений для коррекции зрения. Комплекс общеразвивающих упражнений в сочетании с движением глаз. Комплекс специальных упражнений с элементами спортивных игр. Перечень упражнений, включаемых в физкультурную паузу на рабочем месте при ощущении усталости глаз, тяжести головы. Специальная гимнастика для глаз по У. Бейтсу. Пальминг.,Здоровье человека как ценность. Факторы его определяющие. Влияние образа жизни на здоровье. Здоровый образ жизни и его составляющие. Основные требования к организации здорового образа жизни. Роль и возможности физической культуры в обеспечении здоровья. Физическое самовоспитание и самосовершенствование в здоровом образе жизни. Критерии эффективности здорового образа жизни. Личное отношение к здоровью, общая культура как условие формирования здорового образа жизни.,Физиологические механизмы и закономерности совершенствования отдельных функциональных систем и организма в целом под воздействием направленной физической нагрузки или тренировки. Физиологические основы освоения и совершенствования двигательных действий. Физиологические механизмы использования средств физической культуры и спорта для активного отдыха и восстановления работоспособности. Основы биомеханики естественных локомоций (ходьба, бег, прыжки).,Методические принципы физического воспитания. Основы и этапы обучения движениям. Развитие физических качеств. Формирование психических качеств в процессе физического воспитания. Общая физическая подготовка, её цели и задачи. Зоны интенсивности и энергозатраты при различных физических нагрузках. Значение мышечной релаксации при занятиях физическими упражнениями. Возможность и условия коррекции общего физического развития, телосложения, двигательной и функциональной подготовленности средствами физической культуры и спорта. Специальная физическая подготовка, её цели и задачи. Спортивная подготовка. Структура подготовленности спортсмена. Профессионально-прикладная физическая подготовка как составляющая специальной подготовки. Формы занятий физическими упражнениями. ,Массовый спорт и спорт высших достижений, их цели и задачи. Спортивные соревнования как средство и метод общей и специальной физической подготовки студентов. Спортивная классификация. Система студенческих спортивных соревнований: внутривузовские, межвузовские, всероссийские и международные. Индивидуальный выбор студентом видов спорта или системы физических упражнений для регулярных занятий (мотивация и обоснование). Краткая психофизиологическая характеристика основных групп видов спорта и систем физических упражнений.,Мотивация и целенаправленность самостоятельных занятий, их формы, структура и содержание. Планирование, организация и управление самостоятельными занятиями различной направленности. Взаимосвязь между интенсивностью нагрузок и уровнем физической подготовленности. Самоконтроль за эффективностью самостоятельных занятий. Особенности самостоятельных занятий, направленных на активный отдых, коррекцию физического развития и телосложения, акцентированное развитие отдельных физических качеств.,Личная и социально-экономическая необходимость психофизической подготовки человека к труду. Определение понятия ППФП, её цели, задачи, средства. Место ППФП в системе подготовки будущего бакалавра. Факторы, определяющие конкретное содержание ППФП. Методика подбора средств ППФП, организация и формы её проведения. Контроль эффективности ППФП студентов. Основные и дополнительные факторы, оказывающие влияние на содержание ППФП по избранной профессии. Основное содержание ППФП будущего бакалавра и дипломированного специалиста. ,Основные понятия: спортивная подготовка, общая и специальная физическая подготовка. Оценка специальной физической подготовленности. Оценка технической подготовленности. Оценка тактической подготовленности. Оценка психологического состояния. Методика самоконтроля уровня развития физических качеств.,Понятие "релаксация". Специальные приемы, позволяющие освоить технику релаксации. Динамические упражнения для снятия напряжения мышц и их расслабления. Комплексы упражнений для расслабления мышц.,Методика подбора средств профессионально-прикладной физической подготовки. Методика развития некоторых профессионально важных физических качеств. Способность дозировать силовые напряжения. Развитие статической выносливости и устойчивости к гиподинамии. Тренировка сенсомоторной реакции. Специальные упражнения на равновесие и улучшение функций вестибулярного анализатора. Упражнения на внимание. Развитие оперативного мышления. Тренировка эмоциональной устойчивости.,Производственная физическая культура. Производственная гимнастика. Особенности выбора форм, методов и средств физической культуры и спорта в рабочее и свободное время. Профилактика профессиональных заболеваний средствами физической культуры. Дополнительные средства повышения общей и профессиональной работоспособности. Влияние индивидуальных особенностей и самостоятельных занятий физической культурой.</t>
+  </si>
+  <si>
+    <t>Мировоззрение и картины мира. Что такое философия? Философия как мировоззрение и как рефлексивная деятельность. Основные проблемные разделы философии:онтология, гносеология, антропо-аксиология.,Онтология - философия бытия. Основные проблемы и категории Что существует? Почему существует нечто, а не ничто? Как нечто существует (типы бытия)? Материальный мир и физическая реальность. Этапы становления онтологии.,Что я могу знать? Познание, субъект и объект познания, формы познания. Истина и заблуждение. Концепции истины. Взгляды на познание в истории философии.,Специфика научного познания. Научные революции и смена типов рациональности. Методы научного мышления. Нормы и идеалы научного познания. Что такое техника? Чем занимается философия техники? Техногенная цивилизация: глобальный феномен техники,Что такое философская антропология? Что такое человек? Какова природа человека? Что определяет человека - сущность или существование? Есть ли смысл человеческого существования? Есть ли у человека свобода? Категории философской антропологии?,Ценности: многообразие интерпретаций. Система - иерархия ценностей. Личность как средоточие ценностей.,Этика. Что я должен делать? Свобода воли и нравственный выбор. Проблемы оснований добра и зла.,Что такое искусство? Художественная реальность, художественное сознание, художественная деятельность . Мимезис. Эстетика, опыт восприятия и суждения вкуса. Эстетическое отношение к миру и его отличие от познавательного и нравственного отношения. Эстетические установки и критерии как ценностные ориентации</t>
+  </si>
+  <si>
+    <t>1.1.Финансы и финансовые отношения. Централизованные и децентрализованные финансы.,1.2. Принципы и функции финансов, финансовые ресурсы.,Понятие финансовой системы, ее уровни, типы, функции и элементы.,Финансовая система государства.,Институциональная структура финансовой системы в мире и в РФ.,Сущность, цель, объекты, механизм, формы, виды, уровни управления финансами: финансовое регулирование, прогнозирование и контроль.,Финансовая политика: ее сущность, задачи, типы, направления и методы. Финансовая политика РФ.,Сущность, роль в финансовой системе, функции, виды и элементы финансовых рынков.,Инструменты финансового рынка как объект торговли и инвестирования, их характеристики.,Сегменты, участники и институты финансового рынка,Сущность, принципы и функции финансов организаций (предприятий).,Денежное хозяйство предприятий. Структура оборотного капитала предприятий, источники его воспроизводства. Расходы, доходы и прибыль организаций (предприятий).,Сущность, принципы и функции финансов домохозяйств.,Баланс доходов и расходов домохозяйств, финансовое планирование.</t>
+  </si>
+  <si>
+    <t>Концепция временной стоимости денег. Простые и сложные проценты, m-разовое начисление процентов, эквивалентные ставки, эффективная ставка, непрерывные проценты. Дисконтирование и банковский учет. Сравнение денежных сумм. Расчеты в условиях инфляции.,Определение потока платежей и финансовой ренты. Обобщающие характеристики потоков платежей. Обычная постоянная годовая рента с начислением процентов один раз в год. Обычная постоянная годовая рента с начислением процентов m раз в год. Обычная постоянная p-срочная рента с начислением процентов один раз в год. Обычная постоянная p-срочная рента с начислением процентов m раз в год. Рента с кусочно-постоянными платежами. Ренты с изменением выплат по закону арифметической и геометрической прогрессии. Ренты пренумерандо. Отложенные ренты. Вечные ренты. Непрерывные ренты. Определение параметров финансовых рент (размера платежа, срока, процентной ставки). Изменение условий финансовых контрактов (принцип финансовой эквивалентности обязательств, уравнение эквивалентности). Конверсии рент (выкуп ренты, рассрочка платежей, замена одного потока платежей другим, объединений рент).,Баланс финансово-кредитной операции. Методы погашения долга (погашение основного долга в один срок, погашение основного долга равными платежами, погашение долга равными срочными уплатами, погашение потребительского кредита). Понятие полной доходности финансово-кредитной операции. Расчет эффективной ставки по кредиту (простейший случай кредитной операции с удержанием комиссионных, случаи с дифференцированными и аннуитетными погасительными платежами, эффективная ставка в потребительском кредите). Задача реструктуризации долга.,Денежный поток инвестиционного проекта. Дисконтные методы анализа, выбор ставки дисконтирования. Основные критерии экономической эффективности инвестиционного проекта (чистый приведенный доход, внутренняя норма доходности, срок окупаемости, индекс рентабельности), их преимущества и недостатки. Сравнение альтернативных инвестиционных проектов. Формирование портфеля инвестиционных проектов.,Анализ инвестиций в ценные бумаги с фиксированным доходом (облигации). Базовая модель оценивания облигаций. Доходность к погашению. Выявление неверно оцененных рынком ценных бумаг. Расчет внутренней стоимости и доходности к погашению для разного вида облигаций (облигации с нулевым купоном, облигации с выплатой купонов в момент погашения, облигации без обязательного погашения, облигации с периодической выплатой купонов и погашением в конце срока). Средний срок и дюрация облигации. Оценка риска инвестиций в облигации (ценовая чувствительность облигации, дюрация как мера процентного риска, оценка относительного изменения цены облигации через дюрацию и выпуклость). Портфель облигаций.,Детерминированные модели анализа рискованных ценных бумаг (акций). Внутренняя стоимость и внутренняя доходность акции. Модель нулевого роста дивидендов, модель Гордона, модель переменного роста дивидендов. Оценивание акций с учетом конечного срока владения.</t>
+  </si>
+  <si>
+    <t>Понятие, цели и задачи, предмет и организация финансового менеджмента на предприятии. Стратегия и тактика финансового менеджмента. Сущность и структура финансового менеджмента. Современная постановка глобальной цели предприятия.,Рычаги (леверидж) в управлении предприятием. Финансовый леверидж. Эффект финансового рычага: американская и европейская концепция. Сила воздействия финансового рычага и финансовый риск. Финансовый леверидж и формирование рациональной структуры заимствований. Расчет среднесрочной ставки процента. Финансовые условия кредитования.,Операционный (производственный) леверидж. ,Эффект сопряженного рычага. Эффект операционного рычага и количественная оценка уровня предпринимательского риска, генерируемого предприятием. Пороговая выручка. Приемы расчета точки безубыточности. Аналитический и графический метод определения точки безубыточности, практическое использование для принятия управленческих решений. Валовая маржа. Запас финансовой прочности. Практическое использование операционного анализа в управлении.,Оценка текущего финансового положения предприятия и его активов. Ликвидность. Прогнозирование финансовой устойчивости предприятия.,Чистый оборотный капитал и текущие финансовые потребности предприятия. Системная и переменная часть оборотного капитала. Цели управления оборотным капиталом. Левосторонний и правосторонний риск в формировании оптимальной структуры оборотного капитала.,Управление структурой затрат. Регулирование массы и динамики прибыли. Политика управления текущими активами и текущими пассивами. Матрица выбора типа политики управления текущими активами и текущими пассивами.,Прогнозирование денежных потоков и расчет потребности в краткосрочном финансировании. Разработка бюджета денежных средств. Классические способы преодоления локального денежного дефицита. Учет векселей, факторинг, форфейтинг. Опосредованное финансирование Определение оптимального уровня денежных средств. Модели Баумоля и Миллера-Орра в управлении денежными средствами. Главный парадокс (дилемма) финансового менеджмента., Оптимизация источников финансирования предприятия. Источники и структура средств предприятия. Система противоречий интересов руководителей, кредиторов, акционеров. Определение способов внешнего финансирования. Самофинансирование развития предприятия.,Структура капитала предприятия и ее рационализация. Оценка стоимости использования разных источников финансирования. Рыночная цена предприятия и цена капитала. Выбор инвестиционного проекта на основе определения цены капитала. Предельная цена капитала. Оптимальная структура капитала.,Тема 5. Финансовая политика предприятия. Содержание финансовой политики предприятия. Дивидендная политика фирмы. Теории дивидендной политики Основные цели дивидендной политики предприятия и типы политики. Дивидендная политика и политика развития предприятия. Методы выплат дивидендов. Преимущества и недостатки методов выплаты дивидендов. Политика развития предприятия и устойчивый темп роста. Концепции повышенного и заниженного темпов роста и модели поведения. Ассортиментная политика предприятия. Финансовые цели на разных фазах жизненного цикла товара.,Тема 6. Лабораторный практикум. Учебный план по курсу «Финансовый менеджмент» кроме практических занятий по программе курса предполагает проведение компьютерного практикума. Для проведения практикума используется компьютерная имитационная модель, которая отра¬жает ограниченное количество структурных элементов и внешних связей виртуального предприятия, позволяя, тем не менее, достаточно полно воспро¬извести основные процессы управления предприятием, а также внешние условия, в которых предприятие осуществляет свою деятельность. Методические рекомендации к принятию решений в деловой игре изложены в методическом пособии «Стратегия и тактика управления бизнесом в условиях конкуренции». Пособие размещено на сайте научной библиотеки НИ ТГУ, а также имеется раздаточный материал.</t>
+  </si>
+  <si>
+    <t>Понятие финансового (бухгалтерского) учета. Цели финансового учета. Пользователи финансовой информации. Гармонизация российского учета с международными стандартами. Международные стандарты учета и финансовой отчетности. Реформирование системы бухгалтерского учета в Российской Федерации.,Основные принципы (допущения) учетной политики в Российской Федерации. Допущение временной определенности фактов хозяйственной деятельности. Допущение последовательности применения учетной политики. Требования к учетной политике и финансовой (бухгалтерской) отчетности. Основные элементы учетной политики. Инвентаризация активов и обязательств и порядок отражения ее результатов в учете. Порядок утверждения учетной политики организации.,Критерии отнесения активов к основным средствам в соответствии с российской учетной практикой. Состав и единица учета основных средств. Отражение в учете операций по поступлению основных средств. Оценка основных средств при их первоначальном признании. Переоценка и восстановление основных средств и порядок их отражения в учете. Амортизация основных средств. Методы начисления амортизации и порядок ее отражения в учете. Модернизация, реконструкция и ремонт основных средств. Бухгалтерские записи по выбытию основных средств. Документальное оформление операций с основными средствами. Понятие доходных вложений в материальные ценности. Аренда основных средств. Особенности отражения в учете операционной и финансовой аренды.,Понятие и виды нематериальных активов (НМА). Критерии отнесения активов к нематериальным активам. Единица учета нематериальных активов. Порядок отражения в учете операций по поступлению НМА. Оценка нематериальных активов при первоначальном признании. Переоценка нематериальных активов и порядок ее отражения в учете. Амортизация нематериальных активов и порядок ее отражения в учете. Деловая репутация организации и порядок ее отражения в учете. Учет расходов на научно-исследовательские, опытно-конструкторские и технологические работы. Документальное оформление операций с НМА.,Состав материально-производственных запасов. Порядок и способы учета материалов. Формирование себестоимости материалов. Порядок учета затрат на производство. Порядок и способы учета готовой продукции. Методы калькулирования себестоимости. Методы учета товаров. Методы оценки материально-производственных запасов при их выбытии. Порядок формирования резерва под обесценение материально-производственных запасов. Учет продаж материально-производственных запасов (материалов, товаров, готовой продукции). Документирование хозяйственных операций с материально-производственными запасами.,Порядок ведения и учета кассовых операций. Порядок ведения и учета безналичных расчетов. Денежные средства на валютных счетах организации и порядок их учета. Денежные средства на специальных счетах в банках и порядок их отражения в учете. Переводы в пути. Документирование операций с денежными средствами. Порядок оформления платежного поручения. Очередность платежей.,Состав, критерии признания и единица учета финансовых вложений. Оценка финансовых вложений и финансовых инструментов. Порядок отражения в учете операций с ценными бумагами (акции, облигации, векселя). Производные финансовые инструменты. Методы оценки ценных бумаг при их выбытии. Доходы и расходы по финансовым вложениям. Документальное оформление операций с финансовыми вложениями.,Понятие дебиторской задолженности и ее состав. Резерв по сомнительным долгам. Списание безнадежных долгов. Учет обязательств организации. Операционные обязательства организации. Финансовые обязательства. Списание просроченной кредиторской задолженности. Особенности учета отдельных видов финансовых обязательств. Особенности учета арендных обязательств. Финансовая аренда (лизинг). Учет вознаграждений работникам. Документальное оформление дебиторской и кредиторской задолженности.,Понятие и классификация доходов и расходов организации. Порядок отражения доходов от обычных видов деятельности в соответствии с российскими и международными стандартами (ПБУ 9/99 "Доходы организации", ПБУ 10/99 "Расходы организации"). Формирование конечного финансового результата. Реформирование баланса.,Бухгалтерская прибыль и порядок ее формирования. Особенности формирования налогооблагаемой прибыли. Постоянные и временные разницы между бухгалтерской и налогооблагаемой прибылью. Постоянные налоговые обязательства. Отложенные налоговые обязательства. Отложенные налоговые активы. Условный расход (доход) по налогу на прибыль. Текущий налог на прибыль и порядок его отражения в финансовой отчетности.,Понятие собственного капитала организации. Элементы собственного капитала. Эмиссия акций. Обыкновенные акции. Привилегированные акции. Учет уставного капитала. Учет добавочного капитала. Учет резервного капитала. Отражение собственного капитала в финансовой отчетности.,Понятие финансовой отчетности. Цель создания и назначение Концептуальных основ финансовой отчетности. Пользователи финансовой информации. Качественные характеристики полезной финансовой информации. Основополагающее допущение. Элементы финансовой отчетности (активы, обязательства, капитал, доходы и расходы). Критерия признания в отчетности элементов капитала. Концепции поддержания капитала.,Представление финансовой отчетности в соответствии с российскими и международными стандартами финансовой отчетности. Бухгалтерский баланс и порядок его формирования. Отчет о финансовых результатах и порядок его формирования. Отчет об изменении капитала. Отчет о движении денежных средств. Пояснения к финансовой отчетности. Промежуточная финансовая отчетность.,Понятие консолидированной финансовой отчетности. Правила формирования показателей при составлении консолидированной финансовой отчетности.,Раскрытие в финансовой отчетности информации о прекращенной деятельности. События после отчетной даты и порядок раскрытия информации в учете и отчетности. Раскрытие информации в пояснениях об операционных сегментах. Справедливая Раскрытие информации о связанных сторонах. Использование методов финансового анализа для целей дополнительного раскрытия информации в финансовой отчетности.</t>
+  </si>
+  <si>
+    <t>Тема 1. Общая теория ценообразования. Экономическая сущность цены. Функции цены. Задачи цен. Основные участники ценообразования.,Тема 2. Методология ценообразования. Основные принципы ценообразования. Методика ценообразования. Методы ценообразования.,Тема 3. Структура цены. Элементы цены и их взаимосвязь. Себестоимость продукции, переменные и постоянные издержки. Прибыль компании. Косвенные налоги в цене. Влияние налоговых режимов на цены продукции/услуг: НПД, УСН, ОСН.,Тема 4. Система цен. Общая характеристика системы цен. Классификация цен. Соотношения цен. Динамика цен и факторы ценообразования.,Тема 5. Цены компании. Ценовая политика компании. Ценовая стратегия компании. Алгоритм формирования ценовой стратегии компании.,Тема 6. Государственное регулирование цен. Общая характеристика государственного регулирования цен. Инструменты государственного регулирования цен. Государственное регулирование цен за рубежом.,Тема 7. Мировые цены. Основные виды мировых цен. Влияние мировых цен на национальную систему ценообразования.</t>
+  </si>
+  <si>
+    <t>Понятие математической модели и математического моделирования. Математическое моделирование в экономике. Классификация математических моделей и методов в экономике. Предмет эконометрики и возможности ее применения для количественного анализа социально-экономических процессов. Примеры эконометрических моделей. Эконометрические методы – эффективное средство количественного описания, анализа, моделирования, прогноза социально-экономических процессов и явлений и поддержки принятия решений в бизнесе и управлении. Проблемы, связанные с построением эконометрических моделей. Обзор современных эконометрических методов. Важность качественного информационного обеспечения.,Понятие регрессионной зависимости, виды зависимостей. Предмет регрессионного анализа. Линейная регрессия, классы задач, решаемых с помощью моделей линейной регрессии. Примеры линейной регрессионной зависимости между экономическими переменными. Понятие экзогенных и эндогенных переменных. Основные формально-математические проблемы, возникающие при построении регрессионных моделей. Роль информационного обеспечения моделей. Модель парной линейной регрессии. Примеры парной линейной зависимости. Экономическая интерпретация параметров модели. Оценка параметров модели по методу наименьших квадратов. Метод максимального правдоподобия. Сравнительный содержательный анализ МНК и МП методов. Статистическая проверка предпосылок, лежащих в основе метода наименьших квадратов. Теоретические предпосылки, на основе которых строятся МНК-оценки, их роль и правдоподобность выполнения в реальных практических задачах. Гомоскедастичность. Статистические свойства МНК-оценок: несмещенность, состоятельность, оптимальность (эффективность). Теорема Гаусса-Маркова. Проверка статистических гипотез относительно коэффициентов регрессии. Построение доверительных интервалов для коэффициентов регрессии. Остаточные ошибки модели, их свойства. Статистические критерии проверки адекватности модели. Коэффициент детерминации.,Модель множественной линейной регрессии. Примеры социально-экономических процессов, для описания которых можно использовать модели многомерной линейной регрессии. Содержательная интерпретация коэффициентов и стохастической составляющей. Проблема оценки параметров модели. Многомерный метод наименьших квадратов. Вывод нормальных уравнений. Теоретические предпосылки, на основе которых строятся оценки параметров модели по многомерному МНК. Статистические свойства оценок параметров линейной модели множественной регрессии. Теорема Гаусса-Маркова. Спецификация моделей множественной линейной регрессии. Проверка адекватности моделей множественной линейной регрессии. Остатки модели, их свойства. Коэффициент детерминации. Проверка статистических гипотез относительно коэффициентов. Неоднородность дисперсии остатков: гетероскедастичность. Автокорреляция. Коэффициент автокорреляции. Мультиколлинеарность и методы ее устранения. Корректировка состава объясняющих переменных в регрессионной модели.,Примеры проблемных ситуаций, в которых необходимо построение обобщенных моделей. Обобщенная регрессионная модель. Обобщенный метод наименьших квадратов. Обобщенная линейная модель регрессии с гетероскедастичными остаточными ошибками. Регрессионные модели с переменной структурой. Использование «фиктивных переменных». Нелинейные модели регрессии – методы линеаризации. Линейные модели со стохастическими регрессорами. Метод инструментальных переменных. Примеры применения обобщенных моделей множественной линейной регрессии, обсуждение проблем, связанных с их построением.,Понятие временного ряда. Примеры временных рядов в экономике. Виды временных рядов: одномерные стационарные и нестационарные, многомерные. Примеры. Цели и основные проблемы, связанные с анализом временных рядов. Модели одномерных стационарных временных рядов: авторегрессии, скользящего среднего, авторегрессии-скользящего среднего. Идентификация одномерных стационарных рядов. Проверка адекватности моделей. Методы прогнозирования. Математическое описание нестационарных рядов. Методы выделения трендов, сезонной и регулярной составляющих. Метод последовательных разностей. Модели авторегрессии-проинтегрированного скользящего среднего. Проверка адекватности моделей нестационарных временных рядов. Модели с распределенными лагами. Прогнозирование экономических показателей на основе моделей временных рядов.,Системы линейных одновременных уравнений. Модели динамических процессов в экономике, описываемых системами одновременных уравнений. Структурная и приведенная формы уравнений. Идентификация (статистическое оценивание параметров) систем линейных одновременных уравнений. Косвенный метод наименьших квадратов. Свойства оценок. Неидентифицируемость и сверхидентифицируемость. Двухшаговый и трехшаговый методы наименьших квадратов. Точечный и интервальный прогноз эндогенных переменных. Проблема проверки адекватности моделей, описываемых системами одновременных уравнений.</t>
+  </si>
+  <si>
+    <t>Формирование контуров отдельной науки: название курса и Гарвардская парадигма. Объект анализа отраслевой организации рынков. Предмет науки: подходы к исследованию товарных рынков и субъекты отраслевого рынка. Парадигма теории отраслевых рынков и ее развитие.,Классификации отраслевых рынков. Уровень концентрации на отраслевых рынках. Оценка концентрации на отраслевых рынках.,Организационная структура, размеры и эффективность фирм. Внутренняя структура фирмы. Альтернативные цели фирмы и агентов внутри фирмы. Влияние целей фирмы на рыночное поведение. Технологическая, контрактная и стратегическая концепции поведения фирмы на отраслевом рынке.,Феномен дифференциации продукта. Дифференциация продукта в условиях монополистической конкуренции. Вертикальная дифференциация продукта. Бренд как проявление дифференциации продукта. Реклама: роль и функции. Рекламные расходы: российский опыт в контексте международных сопоставлений.,Понятие барьеров входа-выхода. Классификация рынков по уровню входных барьеров. Виды нестратегических барьеров входа фирм на рынок. Барьеры социально-экономического характера. Разновидности правительственных барьеров. Гражданские барьеры. Барьеры выхода фирм с рынка. Показатели статистики входа-выхода фирм на рынок,Понятие вертикальной интеграции и ее виды. Побудительные мотивы фирм к вертикальной интеграции. Интеграционные процессы на отраслевом рынке: интеграция и аутсоринг, виды интеграции. Вертикальные ограничения. Типы вертикальных ограничений. Следствие вертикальной интеграции. Слияния и поглощения.,Дискриминационное ценообразование в практике продаж. Три степени ценовой дискриминации. Воздействие ценовой дискриминации на экономические процессы.,Ограниченность информации о качестве товара. Возможные пути преодоления ограниченности информации о качестве товара. Ограниченность информации о цене товара. Теория сигналов и информационная роль рекламы.,Регулирование функционирования отраслевого рынка. О формах регулирования естественных монополий. Приватизация и национализация.,Теоретические основы государственной антимонопольной политики. Государственная антимонопольная политика в отношении слияния и поглощения фирм. Особенности государственной политики относительно соглашений о фиксировании цен и ценовой дискриминации.</t>
+  </si>
+  <si>
+    <t>Определение экономической социологии. Сходство и различия между экономико-теоретическим и экономико-социологическим подходами. Предметная область экономической социологии. Методы экономической социологии.,Основные категории экономической социологии. Экономическое действие как центральная категория экономической социологии. Экономическое действие и социальная структура. Две модели поведения: Homo Economicus и Homo Sociologicus.,Основные направления и проблематика современной экономической социологии.,Понятие хозяйственного мотива. Мотивационная структура. Регуляторы экономического поведения в моделях «экономического» и «социологического» человека.,Проблема рациональности и ее интерпретации. Границы рациональности. Множественность типов рационального действия.,Определения рынка. Конституирующие элементы рынка.,Рынок как совокупность социальных сетей. Различные формы сетевых связей. Формирование социального капитала на основе социальных сетей. Этническая экономика.,Институциональный подход к анализу рынка. Фундаментальные порядки вовлеченности и связей. Конвенции координации. Социокультурный подход к анализу рынка. Культура и экономика: формы и способы взаимовлияния. Аспекты рыночной культуры: когнитивный, ценностный и символический.,Проблемы формирования экономической культуры в современной России.,Понятие государства. Эволюция государственного вмешательства в хозяйственную жизнь. Основные функции современного государства. Новая парадигма отношений государства и рынка.,Типы государственного регулирования. Модели взаимодействия государства и рынка. Модели социальной политики. Государство всеобщего благосостояния. Характеристика коррупционных отношений. «Захват государства».,Государственное регулирование в экономике современной России.,Структурный и институциональный подходы к анализу ненаблюдаемой экономики. Неформальная экономика как сегмент хозяйствования. Теневая экономика. Нелегальная (криминальная) экономика. Измерение неформальной экономики. Экономические, этнокультурные и социальные факторы существования неформальной экономики. Причины роста теневой экономики. Влияние государственного регулирования на степень «формализации» экономики. Формальные и неформальные правила. Формализация и деформализация правил.,Ненаблюдаемая экономика в современной России.,Отношения занятости. Спрос и предложение на рынке труда (работодатели и наемные работники). Трудовая мотивация на рынке труда. Сегментация рынка труда (внутренний и внешний рынки труда, первичный и вторичный рынки труда, «ядро» и «периферия»). Факторы сегментации рынка труда.,Социальные механизмы трудового найма и заполнения рабочих мест.,Социально-демографический «портрет» безработных. Последствия безработицы.,Рынок труда и рынок образовательных услуг: проблемы соответствия.,Характеристика российского рынка труда. Особенности рынков труда российских регионов.,Определение предпринимательства. Предприниматель: социально-психологический «портрет». Эволюция предпринимательской функции: собственник капитала, комбинатор экономических ресурсов, носитель риска и неопределённости, инноватор.,Мотивация предпринимательской деятельности. Способы изучения предпринимательского поведения: ресурсные основания деятельности; отношения между группами предпринимателей; взаимодействие с представителями властных структур. Крупный бизнес, малый и средний бизнес. Роль государства в содействии предпринимательству.,Предпринимательская деятельность в современной России.,Домашнее хозяйство, домашний труд. Современная семья: особенности в различных странах. Распределение и использование семейных ресурсов. Внутрисемейная иерархия: принципы распределения труда между супругами в домашнем хозяйстве. Бюджеты времени в современном домашнем хозяйстве.,Экономический и социологический подходы к изучению потребительского поведения. Модели потребительского поведения. Понятие габитуса. Система потребительских предпочтений и стили жизни. Потребление как инновационный процесс.,Структура и функции финансового поведения. Сберегательное и инвестиционное поведение домохозяйств.,Экономико-социологический подход к исследованию социального неравенства и социальной структуры общества. Стратификация и критерии социального статуса общественных групп.,Основные показатели и способы измерения социально-экономической стратификации. Управленческая и хозяйственная и элиты. Средний класс, его место и роль в развитии общества.,Средний класс в России: проблемы идентификации.</t>
+  </si>
+  <si>
+    <t>Тема 1. Организация статистической деятельности в РФ,Тема 2. Источники статистических данных,Тема 3. Статистическое исследование,Тема 4. Сводка и группировка,Тема 5. Анализ полученных результатов,Тема 6. Индексы цен. Измерение инфляции,Тема 7. Система национальных счетов. Измерение ВВП</t>
+  </si>
+  <si>
+    <t>Тема 1. Экономический анализ: наука и практика,Тема 2. Информационное обеспечение экономического анализа,Тема 3. Виды экономического анализа,Тема 4. Методы и приемы экономического анализа,Тема 5. Аспектный экономический анализ,Тема 6. Рейтинговые и скоринговые подходы к аналитическим процедурам,Тема 7. Техника составления аналитического заключения</t>
+  </si>
+  <si>
+    <t>1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Общеразвивающие упражнения. Общеразвивающие упражнения без предметов и с предметами. Строевые упражнения, повороты на месте и в движении, перестроения на месте и в движении. Упражнения, направленные на формирование правильной осанки.,3.2. Прикладные упражнения. Ходьба, бег, прыжки; упражнения в равновесии; подтягивание на перекладине, сгибание и разгибание рук в упоре лежа; упражнения с использованием отягощений, прыжки в длину, прыжки через препятствия, челночный бег. Подвижные игры и эстафеты.,3.3. Плавание. Обучение умению держаться на воде, прыжкам в воду. Обучение классическим стилям плавания.,3.4. Атлетическая гимнастика. Упражнения с отягощениями и на тренажерах для развития силы рук, плечевого пояса, шеи, туловища и ног.,3.5. Волейбол. Обучение стойкам и перемещениям; ходьба, бег, скачок, прыжок, старты, остановки, повороты. Обучение технике подач сверху и снизу, приема мяча сверху и снизу двумя руками. Основы тактики волейбола. Розыгрыш мяча в три касания через игрока зоны 3. Игровая практика.,3.6. Баскетбол. Техника игры в защите: защитная стойка, перемещения обычными, приставными шагами в различных направлениях, передвижение спиной вперед. Обучение технике владения мячом: ловля мяча на месте и в движении, ведение мяча правой и левой рукой в движении шагом и бегом, броски мяча в корзину, штрафные броски. Игровая практика.,3.7. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Техника выполнения упражнений атлетической гимнастики для тренировки отдельных мышечных групп. Обучение основам техники упражнений. Жим штанги лёжа на горизонтальной скамье, разводка гантелей в стороны лёжа, подъем штанги на бицепс стоя, жим лёжа узким хватом, французский жим стоя, жим штанги стоя с груди, приседание со штангой на плечах, становая тяга, тяга штанги в наклоне к поясу, шраги, пресс на наклонной скамье, пресс на консольных брусьях. ,3.2. Развитие отдельных групп мышц на тренажерах. Тяга рукоятки блока к подбородку стоя, тяга рукоятки блока за голову широким хватом сидя, тяга рукоятки блока к животу сидя, сгибание рук со штангой на скамье Скотта, сгибание рук на блочном устройстве, трицепсовый жим на блоке стоя, разгибание рук на блоке сидя, разгибание ног на тренажере сидя, сгибание ног на тренажере сидя, жим ногами на тренажере сидя, сведение рук перед грудью на тренажере сидя, голень в тренажере сидя, пресс на римском стуле, гиперэкстензия, кроссоверы, отжимание на брусьях на блочном устройстве,3.3. Упражнения на увеличение мышечной массы. Для мышц рук: сгибание рук со штангой с «Читингом», подтягивание обратным хватом с отягощением у пояса, жим лежа узким хватом, французский жим узким хватом лежа. Для мышц спины: сведение плеч назад-вверх со штангой в руках, тяга гантелей в наклоне попеременно, тяга спиной со штангой. Для мышц ног: приседание со штангой на плечах (груди), становая тяга с выпрямленными ногами. Для дельтовидных мышц: жим штанги, стоя, широким хватом с груди, тяга штанги к подбородку узким хватом.,3.4. Коррекция отдельных групп мышц. Бицепс: сгибание рук на скамье Скотта, сгибание рук с гантелями, сгибание рук со штангой. Трицепс: французский жим стоя, лежа ото лба, отведение руки с гантелью назад в наклоне. Для мышц спины: вращение плечами с гантелями в руках, тяга на блоке к животу сидя, гиперэкстензия. Квадрицепс: полуприседы со штангой, приседание со штангой в руках за спиной. Бицепс бедра: половинчатое сгибание ног на блоке. Для дельтовидных мышц: жим сидя широким хватом с груди (из-за головы), жим гантелей сидя, локти в стороны. Для мышц груди: разводка гантелей лежа, жим штанги лежа под отрицательным углом.,3.5. Упражнения на тренажерах различных типов. Тяга рукоятки блока к подбородку стоя, тяга рукоятки блока за голову широким хватом сидя, тяга рукоятки блока к животу сидя, сгибание рук со штангой на скамье Скотта, сгибание рук на блочном устройстве, трицепсовый жим на блоке стоя, разгибание рук на блоке сидя, разгибание ног на тренажере сидя, сгибание ног на тренажере сидя, жим ногами на тренажере сидя, сведение рук перед грудью на тренажере сидя, голень в тренажере сидя, пресс на римском стуле, гиперэкстензия, кроссоверы, отжимание на брусьях на блочном устройстве.,3.6. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Техника выполнения обязательных элементов (шагов) аэробики. Обучение технике обязательных элементов в системе нон-стоп (при проведении упражнений поточным методом). Обучение согласованным движениям рук и ног.,3.2. Комплексы упражнений аэробики. Этапы составления комбинаций. Выбор музыкального сопровождения. Подбор упражнений. Логичные переходы между движениями. Перемещения, смена направления. ,3.3. Изучение и совершенствование техники упражнений аэробики. Система нон-стоп. Метод квадрата. Пирамидальный метод. Обучение технике соединений упражнений со сменой ноги в первом упражнении, в последнем упражнении, в середине комбинации.,3.4. Прикладные виды аэробики. Аэробика со снарядами: степ-аэробика, слайд-аэробика, фитбол- аэробика, аква- аэробика.,3.5. Прикладные виды аэробики. Танцевальная аэробика: латиноамериканские танцы, джаз-аэробика, фанк-хип-хоп, классический танец в аэробике.,3.6. Йога в аэробике. Общая характеристика и специфика. Основные понятия. Йога как система физической, умственной и духовной тренировки. Основные ступени йоги. Построение урока. Музыкальное сопровождение занятий. Освоение основных асан: гора, дерево, вытянутый треугольник, воин, тадасан. Методика построения комплексов фитнес - йоги. Освоение техники релаксации и медитации. Дыхание в системе йоги.,3.7. Восточные виды единоборств и аэробика. Исторические аспекты появления программ аэробики соединение с восточными видами единоборств. Основные стили: карате - аэробика, айкидо, дзю- дзюцу, винчунь, кикбоксинг, таеквондо. Физиологические и биохимические основы движений. Взаимосвязь принципов построения хореографии классической аэробики с элементами восточных видов единоборств. Особенности структуры урока. Методика составления программ. Основные положения и движения: основная стойка, нейтральная стойка, удары руками, удары ногами. Практическое выполнение различных шагов, соединений и парной тренировки.,3.8. Закрепление техники, совершенствования различных композиций, достижение высокого уровня спортивной формы и психологической подготовки студентов. Особенности работы опорно-двигательного аппарата, работа мышц. Работа сенсорных систем организма. Основные закономерности управления двигательными действиями при выполнении базовых шагов, скачков, подскоков, прыжков. Особенности опоры при выполнении равновесий. Правильная осанка. Равновесие тела. Центр тяжести тела, угол устойчивости. Техника упражнений, выполняемых на месте. Техника беговых упражнений. Овладение методикой аутотренинга. Методы совершенствования коммуникационных способностей: настройка на дыхание и движения, настройка к интонации, настройка к внутренним ритмам,3.9. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Специальная физическая подготовка. Упражнения для развития физических качеств, необходимых волейболисту: силы, быстроты и координации движений, гибкости, общей и скоростной выносливости, прыгучести.,3.2. Совершенствование техники игры в волейбол. Стойки и перемещения: основная стойка, перемещения – ходьба, бег, скачок, прыжок.,3.3. Техника владения мячом. Подачи: нижняя прямая, нижняя боковая, верхняя прямая. Подачи на точность в различные зоны площадки.,3.4. Передачи мяча. Передачи двумя руками сверху: в стойке, в движении, на месте и после перемещения, вперед, над собой, назад, длинные, средние, короткие передачи.,3.5. Нападающие удары. Нападающие удары: прямой, без перевода, с переводом, с поворотом туловища, по блоку, в обход блока.,3.6. Прием мяча. Прием мяча: сверху двумя руками, снизу двумя руками, одной рукой.,3.7. Блокирование. Блокирование: одиночное, групповое, неподвижное, подвижное.,3.8. Тактика нападения. Индивидуальные тактические действия пасующего, нападающего; групповые и командные тактические действия с пасующим в зоне 3.,3.9. Тактика защиты. Индивидуальные, групповые и командные тактические действия при системе защиты «углом вперед». Страховка нападающего. Страховка блокирующих.,3.10. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Специальная физическая подготовка. Упражнения для развития физических качеств, необходимых баскетболисту: силы, быстроты и координации движений, гибкости, общей и скоростной выносливости, прыгучести.,3.2. Совершенствование техники игры в баскетбол. Техника перемещений: бег обычный и приставными шагами с изменением скорости и направления, прыжки, остановки, повороты, рывки.,3.3. Техника владения мячом. Ловля и передача мяча правой и левой руками, на месте и в движении шагом и бегом; ведение мяча правой и левой рукой на месте и в движении шагом и бегом; броски мяча в корзину; штрафные броски.,3.4. Техника овладения мячом и противодействия. Овладение мячом при отскоке от щита или от корзины; вырывание и выбивание, перехваты мяча; способы противодействия броскам в корзину.,3.5. Элементы тактики игры в нападении. Индивидуальные действия игрока с мячом и без мяча, взаимодействие двух и трех игроков без “противника” и с “противником”.,3.6. Элементы тактики игры в защите. Действия защитника против игрока с мячом и без мяча, взаимодействие двух, трех и более игроков в защите, командные действия, варианты тактических систем в защите.,3.7. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Специальная физическая подготовка. Упражнения для развития физических качеств необходимых футболисту: силы, быстроты, координации движений, гибкости, общей и специальной выносливости,3.2. Техника полевого игрока. Передвижения: бег, прыжки, остановки, повороты. Техника ударов: ногой, головой.,3.3. Техника остановок мяча. Техника ведения мяча. Техника финтов. Упражнения по обучению техники остановки мяча внутренней стороной стопы, подошвой, серединой подъема. Упражнения ударов по мячу ногой различными способами из различных положений, в движении.,3.4. Техника отбора мяча. Владение мячом. Техника вбрасывания мяча. Техника вратаря. Упражнения по ловле, отбиванию, переводам, броскам мяча. Упражнения по технике вбрасывания мяча. Упражнения на ловлю мяча, летящего на уровне колен, бедер, пояса, груди, катящегося по земле.,3.5. Тактика нападения. Индивидуальные действия игрока с мячом и без мяча, взаимодействие двух и трех игроков без “противника” и с “противником”.,3.6. Тактика защиты. Действия защитника против игрока с мячом и без мяча, взаимодействие двух, трех и более игроков в защите, командные действия, варианты тактических систем в защите.,3.7. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Обучение технике попеременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.2. Обучение технике одновременных лыжных ходов. Развитие быстроты, силы, выносливости, скоростно-силовых качеств, координационных способностей.,2.3. Обучение технике спусков и подъемов. Развитие ловкости, силы, скоростно-силовых качеств.,2.4. Контрольное тестирование по лыжной подготовке.,3.1. Развитие и совершенствование сердечно-сосудистой и дыхательной систем организма. Упражнения для развития и совершенствование сердечно-сосудистой и дыхательной систем организма, развития физических качеств: выносливости, гибкости, координации и скоростно-силовой подготовки. Упражнения на координацию, подвижность суставов, имитационные, дыхательные упражнения.,3.2. Подготовительные упражнения для освоения с водой. Специальные и имитационные упражнения на суше, учебные прыжки в воду, игры и развлечения на воде, упражнения для изучения техники спортивных способов плавания.,3.3. Обучение технике плавания кролем на груди и кролем на спине.,3.4. Обучение и совершенствование техники плавания брассом.,3.5. Обучение и совершенствование техники плавания способом баттерфляй.,3.6. Контрольное тестирование уровня спортивно-технической подготовленности.,1.1.,1.2.,1.3.,1.4.,2.1. Специальная физическая подготовка. Комплексы общеразвивающих упражнений, направленные на раз¬витие гибкости, координационных способностей, силовой выносли¬вости. Спортивные и подвижные игры, направленные на развитие ловкости, быстроты, выносливости. Эстафеты и прыжковые упраж¬нения, направленные на развитие скоростно-силовых способностей и быстроты. Циклические упражнения, направленные на развитие выносливости. Имитационные упражнения, кроссовая подготовка, ходьба, преимущественно направленные на увеличение аэробной произ¬водительности организма и развитие волевых качеств, специфи¬ческих для лыжника-гонщика. Комплексы специальных упражне¬ний на лыжах и лыжероллерах для развития силовой выносливо¬сти мышц ног и плечевого пояса.,2.2. Обучение и совершенствование техники лыжных ходов. Ступающий шаг. Скользящий шаг. Обучение ступающему шагу и скольжению на лыжах. Стойка лыжника, повороты, отталкивание ногами, руками при перед¬вижении попеременным двухшажным ходом. Последовательность обучения, фазовый состав и структура движений попеременно двухшажного и одновременного лыжных ходов. Изучение и совершенствова¬ние элементов классического хода (обучение подседанию, отталки¬ванию, махам руками и ногами, активной постановке палок) и формирование целесообразного ритма двигательных действий при передвижении классическими ходами. Классификация коньковых лыжных ходов. Последовательность обучения, фазовый состав и структура движений. Изучение и совершенствова¬ние элементов конь¬кового хода (обучение маховому выносу ноги и постановки ее на опору, подседанию на опорной ноге и отталкиванию боковым сколь¬зящим упором, ударной постановке палок и финальному усилию при отталкивании руками) и формирование целесообразного ритма двигательных действий при передвижении коньковыми ходами.,2.3. Обучение и совершенствование техники подъемов и спусков: «елочкой», «полуелочкой», лесенкой, ступающим шагом. Торможение «плугом» и «полуплугом». Специфичные двигательные действия при прохождении подъемов лыжными ходами. Движения, контролируемые при обучении высокой, средней, низкой стойкам спусков. Своевременное выпрямление траектории движения при обучении технике преодоления неровностей. Характерные двигательные действия при каждом виде торможения лыжами. Особенности обучения торможения палками и управляемым падением. Обучение поворотам в движении: переступанием, «плугом», упором, на параллельных лыжах. Характерные двигательные действия при выполнении различных поворотов в движении и на месте.,2.4. Тренировка на дистанции с применением изученных лыжных ходов. Прохождение дистанции в различном темпе по равнинной или пересеченной местности. Силовая тренировка в подъем. Короткие ускорения на дистанции. Равномерная, интервальная, контрольная и круговая тренировки на лыжах. Игры и игровые упражнения на лыжах.,2.5. Контрольное тестирование уровня спортивно-технической подготовленности.,Тема 1. Активация вестибулярной функциональной системы. ОРУ в ходьбе и на месте с поворотами и вращениями головы и туловища. Бег вращаясь. ОРУ на узкой и ограниченной опорах. Ходьба, бег, прыжки по гимнастической скамейке, по низкому и высокому гимнастических бревнах, ходьба с поворотами на 180 и 360 градусов.,Тема 2. Общеразвивающие, дыхательные, релаксирующие упражнения, ходьба, бег (в сочетании ходьбы с бегом), плавание. Упражнения на месте и в движении (ходьба, бег). Упражнения на координацию и равновесие.,Тема 3. Упражнения с предметами (фитболы, гимнастические палки, малые мячи).,Тема 4. Упражнения на месте, лежа на коврике, в движении (ходьба). Упражнения на координацию и равновесие. Упражнения сидя и лежа на коврике, на укрепление различных мышечных групп, общеразвивающие упражнения в сочетании с дыхательными. Упражнения на тренажерах для укрепления локальных мышечных групп, развития мышечного корсета.,Тема 5. Комплексы лечебной физической культуры по заболеваниям.,Тема 6. Контрольное тестирование.</t>
+  </si>
+  <si>
+    <t>Бизнес-анализ и разработка информационных систем</t>
+  </si>
+  <si>
+    <t>Бизнес-аналитика</t>
+  </si>
+  <si>
     <t>основной вид учебный деятельность раздел дисциплина формировать вид учебный деятельность объем результат время ч обучение дисциплина раздел основа тестирование рд рд лекция тестирование оценка качество лабораторный занятие по самостоятельный работа раздел формирование рдз лекция реализация стратегия лабораторный занятие тестирование по самостоятельный работа содержание раздел дисциплина раздел основа тестирование тестирование оценка качество по рамка раздел рассматриваться общий теоретический основа процесс тестирование программный обеспечение число механизм выявление формирование оценка качество требование стратегия вид тестирование тема лекция тестирование по ретроспектива основа требование выявление анализ документирование проверка вид стратегия тестирование тема практический занятие отчет дефект гостр исо мэк требование оценка качество система программный обеспечение гостр исолмэк требование оценка качество система программный обеспечение элемент показатель качество управление проект планирование отчетность название лабораторный работа требование выявление оценка качество документирование раздел формирование реализация стратегия тестирование по раздел формировать навык разработка реализация стратегия тестирование рассматриваться специализированный вид тестирование автоматизированный регрессионный тестирование удобство использование тема лекция автоматизация тестирование регрессионный тестирование нефункциональный тестирование тестирование удобство использование название лабораторный работа модульный тестирование регрессионный тестирование тема практический занятие неформальный проверка код оценка качество документированность код</t>
   </si>
   <si>
@@ -302,6 +836,201 @@
   </si>
   <si>
     <t>основной вид учебный деятельность формировать результат объем разделы дисциплина обучение вид учебный деятельность время дисциплина лекция раздел погрешность численный рд-1 лабораторный занятие 2 решение самостоятельный работа лекция раздел численный интегрирование рд-2 рд-3 лабораторный занятие самостоятельный работа лекция раздел численный метод решение д дыра рд-2 рд-5 лабораторный занятие задача линейный алгебра самостоятельный работа раздел численный решение нелинейный лекция уравнение система нелинейный рд-2 рд-4 лабораторный занятие 6 уравнение самостоятельный работа раздел численный метод решение лекция обыкновенный дифференциальный рд-2 рд-6 лабораторный занятие 4 уравнение самостоятельный работа лекция раздел приближение функция д р функца рд-2 рд-7 лабораторный занятие табличный данные самостоятельный работа источник содержание раздел дисциплина раздел погрешность численный решение классификация погрешность абсолютный относительный погрешность значащие верный цифра погрешность элементарный вычислительный операция сумма разность произведение частный общий подход оценка погрешность вычислительный алгоритм тема лекция история развитие вычислительный математика элемент теория погрешность название лабораторный работа _ оценка погрешность результат численный решение раздел численный интегрирование квадратурный формула ньютон-котес формула прямоугольник трапеция симпсон погрешность метод принцип рунге оценка погрешность интегрирование вычисление кратный интеграл метод статистический испытание монте-карло задача численный интегрирование тема лекция численный интегрирование квадратурный формула формула прямоугольник трапеция симпсон погрешность численный интегрирование вычисление кратный интеграл стохастические метод численный интегрирование название лабораторный работа численный интегрирование формула прямоугольник трапеция численный интегрирование формула симпсон метод монте- карло раздел численный решение нелинейный уравнение система нелинейный уравнение классификация нелинейный уравнение система трансцендентные алгебраический уравнение схема решение нелинейный уравнение интервальный метод теорема интервал метод половинный деление метод хорда метод касательная метод простой итерация алгоритмизация метод условие применение скорость сходимость геометрический иллюстрация тема лекция нелинейный уравнение общий схема решение нелинейный уравнение концепция интервальный метод процедура шит mathcad решение уравнение система составление пользовательский программа шитый mathcad концепция интервальный метод метод дихотомия хорда решение нелинейный уравнение метод простой итерация ньютон решение нелинейный уравнение решение система нелинейный уравнение название лабораторный работа интервальные метод решение нелинейный уравнение итерационный метод решение нелинейный уравнение метод касательная ньютон итерационный метод решение нелинейный уравнение метод простой итерация якоби раздел численный метод решение обыкновенный дифференциальный авнения классификация дифференциальный уравнение задача кош метод решение обусловленность задача метод рунге-кутта основный идея порядок точность метод область устойчивость метод эйлер эйлера-кош рунге-кутта порядок геометрический иллюстрация погрешность метод автоматический выбор шаг дискретизация система линейный дифференциальный уравнение задача кош система дифференциальный уравнение формула рунге-кутта решение дифференциальный уравнение п-го порядок многошаговые метод решение дифференциальный уравнение тема лекция классификация дифференциальный уравнение задача кош метод решение метод рунгекутта геометрический иллюстрация погрешность метод автоматический выбор шаг система линейный дифференциальный уравнение задача кош система дифференциальный уравнение формула рунге-кутта решение дифференциальный уравнение п-го порядок название лабораторный работа решение дифференциальный уравнение метод рунге- кутта порядок решение дифференциальный уравнение метод рунге- кутта порядок решение система дифференциальный уравнение метод рунге- кутта раздел приближение функция табличный данные классификация задача аппроксимация критерий близость задача интерполирование полиномиальный интерполяция чебышевский система остаточный член погрешность полиномиальный интерполяция выбор узел интерполяция сплайн-интерполяция сглаживание фильтрация данные метод малый квадрат уравнение регрессия полиномиальный регрессия базисный функция тема лекция классификация задача аппроксимация интерполяция сглаживание экстраполяция критерий аппроксимация показатель эффективность аппроксимация полиномиальный интерполяция сплайн интерполяция сглаживание экспериментальный данные регрессионный уравнение сглаживание экспериментальный данные основа мнк экстраполяция данные название лабораторный работа аппроксимация данные основа полиномиальный регрессионный уравнение аппроксимация данные основа метод малый квадрат прогнозирование временной ряд</t>
+  </si>
+  <si>
+    <t>методология data mining межотраслевой стандарт crisp-dm основной задача обработка табличный данные знакомство аналитический платформа loginom ce основа язык python тип данные оператор объектно-ориентированный программирование работа файл обработка исключительный ситуация импорт модуль основной структура данные кортеж список словарь множество строка библиотека выполнение численный расчет numpy библиотека обработка данные pandas графический библиотека matplotlib abc-анализ xyz-анализ fmr-анализ rfm-анализ сочетание описание алгоритм рекомендация настройка параметр алгоритм реализация loginom python основной понятие теория вероятность математический статистика функция распределение плотность вероятность точечный интервальный оценивание проверка статистический гипотеза а б-тестирование основной понятие различный аспект планирование а б-тест интерпретация результат основной понятие линейный алгебра линейный пространство евклидов пространство линейный оператор собственный вектор собственный значение линейный оператор svd-декомпозиция анализ главный компонент алгоритм интерпретация результат различный аспект реализация метод главный компонент постановка задача различный вариант решение задача регрессия интерпретация результат оценка качество построить модель различный аспект решение задача регрессия фиктивный переменный нелинейный модель анализ остаток постановка задача классификация задача бинарный классификация логистический регрессия интерпретация результат логистический регрессия оценка качество бинарный классификация задача многоклассовый классификация мультиноминальный регрессия алгоритм наивный байес оценка качество результат решение задача многоклассовый классификация идея алгоритм построение дерево решение метод оценка чистота подмножество различный алгоритм построение дерево решение id cart chaid оценка качество работа дерево решение оценка важность признак алгоритм random forest подбор оптимальный значение параметр алгоритм градиентный спуск принцип работа параметр модификация алгоритм спуск модель нейрон многослойный персептрон алгоритм обратный распространение ошибка эвристика процесс построение обучение нейронный сеть постановка задача кластеризация вид расстояние свойство алгоритм кластеризация k-means описание настройка параметр свойство обзор другой популярный алгоритм кластеризация свойство иерархический алгоритм meanshift dbscan работа пропуск выброс процедура отбор фактор включение модель работа несбалансированный класс</t>
+  </si>
+  <si>
+    <t>тема business analysis key concepts stakeholder theory origin and progress тема stakeholders their interests and values тема assessment of stakeholders for importance and influence тема stakeholder mapping тема interacting with stakeholders тема bpmn in stakeholder management</t>
+  </si>
+  <si>
+    <t>понятие цепь поставка сетевой структура цепь поставка концепция управление цепь поставка scm supply chain management вид аналитик управление цепь поставка задача цепь поставка уровень абстракция аналитический оптимизация динамический имитационный моделирование цифровой двойник цепь поставка цифровой управление цепь поставка digital scm создание цифровой двойник цепь поставка anylogistix дизайн сетевой структура цепь поставка важность правильный размещение элемент цепь поставка подход решение задача размещение объект цепь поставка гравитационный анализ эвристический метод ардалан метод критический точка метод калькуляция затрата бальный оценка scoring model задача единый средний single median problem задача охват covering problem гравитационный анализ anylogistix greenfield analysis gfa определение оптимальный сетевой структура anylogistix network optimization no запас объект управление цепь поставка понятие запас вид запас точка зрение запас движение запас звено цепь поставка анализ статистика поведение запас основной показатель состояние запас группирование запас классификация запас степень значимость вариативность потребительский спрос abc-анализ xyz-анализ совместный применение прогнозирование потребность запас предиктивный аналитик модель уилсон модификация основный тип стратегия управление запас многономенклатурный модель управление запас управление запас интегрировать многоуровневый цепь поставка планирование цепь поставка стратегический тактический оперативный основа оптимизационный моделирование статический модель динамический модель модель неопределенность классический транспортный задача транспортный задача промежуточный пункт задача назначение планирование доставка мелкопартийный груз условие крупный город интегрировать модель цепь поставка транспортно-складской задача производственно-транспортно-складский задача планирование материальный поток anylogistix network optimization no имитационный эксперимент anylogistix simulation проблема неопределенность риск цепь поставка эффект хлыст bullwhip цепь поставка проблема устойчивость классификация логистический риск комплексный подход анализ риск метод оценка риск принятие логистический решение условие риск метод управление логистический риск перераспределение диверсификация страхование управление риск финансовый рычаг цепь поставка основа модель использование заемный средство хеджирование резервирование анализ риск цепь поставка anylogistix имитационный моделирование simulation</t>
+  </si>
+  <si>
+    <t>потребность цифровой трансформация предприятие возникать проблема основа архитектура предприятие обзор основный методология стандарт свод знание область архитектура предприятие язык описание архитектура предприятие программный средство поддержка архитектурный подход основной элемент архитектурный подход управление постоянный изменение трансформация основа архитектурный подход повторный использование знание описание разработка архитектура предприятие онтология предприятие аспект слой архитектура полка размещение объект метамодель роль практика управление архитектура предприятие объект бизнес-слоя объект слой информационный система объект технологический слой сервисный подход описание разработка архитектура предприятие объект расширение объект планирование переход текущий целевой архитектура предприятие объект моделирование физический элемент связь объект паттерн классификация архитектура предприятие связь заинтересованный сторона артефакт объект начальный этап этап идентификация анализ существовать архитектура предприятие этап проектирование целевой архитектура предприятие этап реализация переход этап оценка реализация архитектура</t>
+  </si>
+  <si>
+    <t>тема стандарт аудит тема саморегулируемый организация аудит сро тема вид аудит тема аттестация аудитор тема внутренний внешний аудит тема аутсорсинг аудит тема согласование аудиторский договор тема цель основный принцип тема оценка аудиторский риск тема существенность верификация аудит тема классификация мошенничество ошибка аудит тема система внутренний контроль свк тема использование система внутренний контроль цель аудит тема тест контроль тема представление отчет внутренний контроль тема использование система утверждение аудитор аудиторский доказательство тема аудиторский процедура тема аудиторский выборка и иной способ тестирование тема аудит отдельный стать тема аудиторский методика использование ит-технология тема работа эксперт тема трансформация финансовый отчетность исправление ошибка тема событие отчетный дата тема концепция непрерывность деятельность тема письменный заявление тема завершение аудит итоговый обзор тема аудиторский заключение</t>
+  </si>
+  <si>
+    <t>понятие база данные понятие субд тип субд настольный многопользовательский профессиональный пример субд основный функция субд типовой организация субд понятие модель данные основной модель данные иерархический сетевой реляционный объектный трехуровневый архитектура субд трехуровневый представление данные логический физический независимость данные достоинство недостаток реляционный модель базовый понятие отношение схема отношение атрибут кортеж домен первичный ключ арность отношение степень отношение фундаментальный свойство отношение ограничение целостность манипуляционный часть реляционный алгебра реляционный исчисление цель проектирование понятие избыточный данные нормальный форма свойство нормальный форма нормализация отношение i ii iii нормальный форма основной характеристика язык диалект язык язык определение данные ddl тип данные создание объект база данные работа база данные создание удаление изменение работа домен работа таблица создание удаление изменение ограничение целостность уровень столбец уровень таблица работа индекс работа субд вычислительный сеть архитектура построение сетевой субд архитектура файл-сервер клиент сервер двухуровневый трехуровневый архитектура система база данные распределенный обработка данные модель удалить доступ данные модель сервер база данные модель сервер приложение вид схема построение иса распределить обработка информация средство создание таблица база данные организация связь база данные механизм доступ различный файл база данные современный механизм организация доступ база данные</t>
+  </si>
+  <si>
+    <t>тема введение история возникновение исследование глобальный угроза базовый понятие безопасный жизнедеятельность тема опасность природный мир геолого-атмосферный опасность проблема выживание природный среда опасность животный мир микробные угроза чума лепра сифилис история человечество туберкулез грипп вич холера тиф оспа тема техногенный антропогенный опасность пожар взрыв бытовой опасность химический бактериологический ядерный оружие авария техногенный объект массовый беспорядок криминальный угроза терроризм рискованный образ жизнь тема первый помощь пострадать действие инсульт инфаркт травма ожог обморожение</t>
+  </si>
+  <si>
+    <t>тема основа управление организация тема метод управление международный организация тема структура управление организация тема стратегический управление международный организация тема современный тенденция управление международный организация</t>
+  </si>
+  <si>
+    <t>цель задача образовательный программа структура учебный план перечень дисциплина практика математический модель мотивация социологический опрос тема мотивация выбор место обучение будущий ожидание обратный связь встреча представитель центр карьера иэм тема деятельность центр предпринимательство встреча представитель ведущий томский компания успешный выпускник направить формирование интерес будущий профессия осознание особенность профессия анализ студент уровень соответствие личный качество требование предъявлять специальность тема построение персональный траектория развитие студент мастер класс тайм-менеджмент стресс-менеджмент мастер класс составление резюме портфолио</t>
+  </si>
+  <si>
+    <t>тема роль язык жизнь человек социальный значимость речевой культура тема речевой общение форма взаимодействие человек модель коммуникация речевой этика тема литературный язык высокий форма национальный язык тема письменный устный форма речь тема качество грамотный речь выразительность речь тема официально-деловой стиль язык тема термин тематический лексика дело-вой речь экономический термин клише канцеляризм тема личный документ резюме заявление автобиография расписка заполнение бланк анкета форма тема служебный документ типология образец языковой оформление тема правило формула деловой этикет тема лингвистический особенность рекламный текст pr-коммуникация тема искусство публичный речь тема культура спор прием спор разновидность спор дискуссия полемика эклектика софистика тема этико-лингвистические особенность телефонный коммуникация модель переговоры правило телефонный взаимодействие тема деловой совещание лингвистический аспект подготовка этап проведение совещание тема интервью собеседование психолингвистический особенность тема презентация устный письменный компонент</t>
+  </si>
+  <si>
+    <t>идентификация числовой категориальный переменный оценка пропустить данные определение кардинальность категориальный переменный выделение редкий категория обнаружение линейный зависимость обнаружение нормальный распределение обнаружение выброс удаление наблюдение пропуск заполнение средний медианный значение заполнение мода наиболее часто встречаться значение заменый пропуск произвольный значение замена пропуск значение хвост распределение добавление индикатор пропустить значение алгоритм заполнение пропуск библиотека scikit-learn создание двоичный переменный метод one-hot encoding нюанс применение метод one-hot encoding категория больший количество уровень замена категория порядковый значение замена категория количество частота встречаемость замена категориальный переменный учет средний значение целевой переменный замена категория основа вес доказательство weight of evidence группировка редкий уровень кодирование основа хеширование замена значение путем логарифмирование замена значение обратный величина квадратный кубический корень степенной преобразование числовой переменный преобразование бокс-кокс yeo-johnson разделение переменный интервал равный длина разделение переменный интервал основа частота встречаемость дискретизация основа категориальный переменный дискретизация основа алгоритм k-средних дискретизация помощь дерево решение усечение выброс основа набор данные замена выброс максимальный минимальный значение замена выброс нулевой значение извлечение компонент дата время переменный тип datetime работа время разный временной зона стандартизация основа средний основа разброс стандартизация основа медиана квантиль стандартизация основа длина вектор</t>
+  </si>
+  <si>
+    <t>основный финансовый понятие диверсификация портфель ценный бумага определение зависимость риск прибыль построение интерпретация параметр модель ценообразование основной капитал основной понятие экономический теория стоимость производство вывод функция издержка основа производственный функция кобба-дуглас анализ эффект не пропуск переменный обзор метод учет изменение качество ценовый индекс анализ зависимость цена качество товар данный момент время временной интервал гедонический метод моделирование индекс цена компьютер различный аспект оценивание гедонический уравнение цена модель человеческий капитал моделирование различие оплата труд роль образование человеческий капиталь моделирование повышение квалификация инвестиция человеческий капитал вид метод оценка дискриминация заработный плата</t>
+  </si>
+  <si>
+    <t>основной понятие системный анализ модель моделирование адекватность модель классификация модель понятие система тип модель система статический динамический свойство система основной понятие имитационный моделирование этап модельный время различный аспект задача моделирование случайный величина задать свойство метод решение популярный распределение случайный величина ситуация применяться поток случайный событие свойство понятие состав классификация система массовый обслуживание графа состояние случайный процесс стационарный пуассоновский поток событие свойство уравнение колмогоров нестационарный стационарный случай процесс гибель размножение определение граф переход уравнение колмогоров решение стационарный случай система массовый обслуживание отказ ожидание прибор обслуживание граф переход процесс система уравнение финальный вероятность состояние система решение вычисление прочий численный характеристика система массовый обслуживание средний время ожидание пропускной способность основной понятие язык программирование java диаграмм причинно-следственный связь определение назначение правило построение обратный связь задержка типовой паттерн развитие динамический система основной понятие системный динамика диаграмма поток данные определение назначение накопитель соединитель правило построение основной понятие многоагентный моделирование понятие агент внешний среда метод взаимодействие агент и внешний среда способ построение коллектив агент вид имитационный эксперимент простой эксперимент эксперимент перебор параметр оптимизационный эксперимент подготовка проведение эксперимент механизм протоколирование имитационный эксперимент обработка получить данные</t>
+  </si>
+  <si>
+    <t>экономический сущность вид инвестиция классификация инвестиция макро- микроуровне инвестиционный процесс инвестиционный деятельность понятие механизм осуществление фактор влиять инвестиционный деятельность объект субъект инвестиционный деятельность отношение субъект инвестиционный деятельность инвестор заказчик исполнитель работа пользователь объект инвестиционный деятельность правовой обеспечение инвестиционный деятельность россия право обязанность субъект инвестиционный деятельность стабильность право возмещение убыток порядок прекращение приостановление инвестиционный деятельность инвестиционный стратегия источник финансирование инвестиционный деятельность состав структура общий характеристика инвестиционный рынок понятие структура показатель состояние инвестиционный рынок инвестиционный спрос инвестиционный предложение цена конкуренция особенность изучение рыночный конъюнктура инвестиционный рынок конъюнктурный цикл сегмент инвестиционный рынок рынок инвестиционный капитал рынок инвестиционный товар рынок объект реальный инвестирование рынок объект финансовый инвестирование вид финансовый посредник инвестиционный политика составной часть экономический политика государство цель задача инвестиционный политика механизм реализация государственный регулирование инвестиционный деятельность метод государственный регулирование форма поддержка инвестиционный деятельность инвестиционный климат объект инвестиционный регулирование сущность значение фактор оказывать влияние инвестиционный климат инвестиционный привлекательность инвестиционный активность метод оценка инвестиционный климат понятие эффективность инвестиция метод инвестиционный расчет классификация метод оценка инвестиция не включать дисконтирование метод основать расчет срок окупаемость инвестиция метод основать определение норма прибыль капитал метод оценка инвестиция основать дисконтирование метод чистый текущий стоимость метод внутренний норма прибыль дисконтировать срок окупаемость индекс доходность инвестиционный риск вид классификация метод расчет сущность классификация инвестиционный проект жизненный цикл инвестиционный проект фаза развитие жизненный цикл инвестиционный проект предынвестиционная инвестиционный эксплуатационный фаза развитие инвестиционный проект содержание документ включать инвестиционный проект бизнес-план инвестиционный проект содержание назначение бизнес-план участник задача бизнес планирование структура бизнес-план эффективность риск инвестиционный проект особенность анализ оценка</t>
+  </si>
+  <si>
+    <t>роль значимость хобби увлечение жизнь человек личный свободный времяпровождение экстремальный вид спорт структура семья родственный связь особенность семейный уклад распределение семейный обязанность семейный традиция образование разный университет мотив личный выбор тгу качество вуз обучение цель характер высокий образование структура деятельность факультет история создание тгу старый новый традиция тгу значимость современный образование личный краткий долгосрочный цель связать высокий образование студенческий жизнь условие проживание кампус расписание день студент история основный достопримечательность томск перспектива развитие город личный особенность предпочтение питание наименование продукт способ приготовление любимый блюдо способ приготовление еда личный практика соблюдение здоровый питание привычка обращение деньга личный жизненный опыт отношение деньга управление личный финансы опыт путешествие проблема экология контекст туризм путешествие основной вид городской транспорт характеристика покупка билет заказ гостиница описание специфика работа друг знакомый личностный особенность контекст выполнение работа проблема карьерный рост карьерный план амбиция умение успешный профессиональный деятельность проблема школьный обучение сложность изучение различный аспект иностранный язык способ прием изучение язык практический применение иностранный язык различный коммуникативный ситуация благотворительность социальный помощь россия мир личный отношение проблема описание сложный ситуация социальный практика история успех наименование описание электронный прибор функция опыт использование электронный прибор повседневный жизнь искусственный интеллект перспектива развитие использование основной проблема окружать среда климатический изменение причина загрязнение вода воздух планета альтернативный вид энергия глобальный потепление прогноз погода популярный вид спорт мир спортивный игра предпочтение занятие спорт проблема обман мошенничество спорт личный критерий выбор подходящий карьера вид привилегия компания преимущество академический отпуск личностный фактор-характеристика важный принятие работа опыт поиск работа тактика подготовка интервью собеседование прием работа правило написание резюме основной вид организация вид статусный привилегия компания качественный характеристика стиль управление организация позиция компания должностной обязанность вид организационный культура стиль деловой общение вид бизнес идея критерий успешность потенциал разный продукт причина обстоятельство начало дело правило создание новый бизнес характеристика успешный предприниматель причина успех новый бизнес современный мир положительный отрицательный качество лидер поведенческий стратегия лидер участник команда лидерский стиль поведение лидер проблемный ситуация личностный качество представление лидер будущее популярный действие операция деньга онлайн- платеж перспектива форма описание практика денежный затрата сбережение практика пользование банковский услуга возможный источник преимущество начало новый бизнес правило базовый финансовый грамотность прогноз событие действие экономика бизнес цель форма проведение рыночный исследование задача фокус-группа маркетинговый стратегия специфика люксовый бренд преимущество недостаток онлайн маркетинг практика поощрение система мотивация менеджмент стиль менеджмент условие успешный неуспешный проект описание стадия проект основной проблема путь решение управление проект культурный особенность отечественный бизнес рубеж проблемный ситуация межкультурный взаимодействие проблема адаптация новый культура преимущество недостаток работа учеба рубеж правило деловой этикет</t>
+  </si>
+  <si>
+    <t>поведенческий предпосылка институциональный анализ ситуация вести появление институт механизм принуждение функция институт формальный неформальный институт экстрактивные инклюзивный институт институциональный среда институциональный соглашение разнообразие форма сделка сущность вид коммонс поланья уильямсон свойство трансакция стоить трансакционный издержка вариант определение базовый категория институциональный экономика трансакционные издержка специфичность актив важный характеристика трансакция схема уильямсон неопределенность форма управление трансакция основный подход классификация трансакционный издержка фактор влиять структура величина трансакционный издержка норт способ измерение трансакционный издержка практика специальный механизм снижение рыночный трансакционный издержка а поиск информация альтернатива сделка б измерение ведение переговоры заключение контракт г контроль соблюдение контракт предупреждение оппортунистический поведение д защита контакт третий сторона значение право собственность определение право собственность теорема коуза трагедия община исключительный право собственность коллективный собственность частный эксклюзивный собственность государственный собственность эволюция право собственность рынок иерархия тип контракт фактор влиять выбор контракт подход р коуз объяснение природа фирма сеть долгосрочный контракт центральный агент граница фирма подход о уильямсон иерархия механизм защита вымогательство квазирента специфичность актив проблема вымогательство фактор обострение тип контракт классический неоклассический отношенческий альтернативный способ организация сделка граница вертикальный интеграция модель фирма трансакционный издержка фирма издержка влияние п мильгром подход позиция право собственность смешанный форма контрактация основной форма гибридный соглашение модель решение проблема гарантия специфический инвестиция понятие контракт контракт юридический экономический смысл понятие совершить контракт причина неполнота контракт проблема принципала-агент тип асимметрия информация скрытый характеристика скрыть действие скрытый информация скрытый намерение вид оппортунистический поведение причина возникновение ухудшать отбор модель акерлофа метод предотвращение ухудшать отбор рынок труд модель спенс подача сигнал просеивание рынок кредит рационирование кредит фактор моральный риск моральный риск рынок труд рынок страхование метод противодействие моральный риск внешний внутренний способ борьба моральный риск влияние эффективный зарплата стимул работник оппортунистический поведение агентский проблема организация внутрифирменный правомочие алчиан демсец тип фирма институциональный альтернатива частнопредпринимательский фирма партнерство фирма управляемый коллектив открытый корпорация закрытый корпорация государственный организация регулируемый фирма некоммерческий организация решение агентский проблема помощь стимулировать контракт проблема безбилетник коллективный действие социальный дилемма типология экономический благо парадокс коллективный действие группа интерес решение проблема коллективный действие уровень институциональный соглашение селективный стимул решение проблема коллективный действие уровень институциональный среда социальный капитал компонент социальный капитал подход измерение измерение социальный капитал пример доверие механизм изменение социальный капитал социальный капитал экономический рост эффект социальный капитал мера накопление социальный капитал определение государство функция необходимость контроль насилие спонтанный экономический порядок устойчивость анархия модель хиршлейфер появление государство бандит-гастролер оседлый бандит контрактный подход происхождение государство синтетический неоклассический теория государство д норт ограничение монопольный власть правитель дилемма присутствие государство экономика переход диктатура демократия социальный контракт фактор разнообразие социальный контракт государство общество агентский проблема зависимость налоговый база законодательный ограничение угроза переворот насилие политический режим авторитарный демократический экономический результат роль политический лидер экономический развитие факт объяснение институциональный гипотеза эмпирический исследование институт рост проблема причинность гипотеза модернизация роль неформальный институт доверие фактор рост развитие экономический рост неравенство экономический неравенство разный страна взаимосвязь рост неравенство</t>
+  </si>
+  <si>
+    <t>возникновение развитие процессный подход функциональный подход линейно-функциональный организационный структура концепция cpi tqm bpr bpm международный стандарт качество процессный организационный структура основной понятие процессный подход классификация процесс моделирование бизнес понятие модель вид модель язык описание модель требование нотация классификация методология моделирование бизнес методология моделирование бизнес инструментальный средство моделирование бизнес анализ бизнес-процесс окружение бизнес анализ риск бизнес-процесс совершенствование бизнес-процесс</t>
+  </si>
+  <si>
+    <t>сигнал данные информация дискретный непрерывный информация средство реализация информационный технология алгоритмический программный технический понятие системный блок периферия системный плата процессор шина данные организация внутренний память оз пзу кэш-память cmos-память ячейка основа функционирование эвм вид внешний память принцип представление информация дисковый память форматирование логические физический диск понятие количество информация формула хартля количество информация содержаться m-разрядном сообщение понятие объем информация единица измерение объем информация система счисление основный тип данные представление целый тип знак знак способ представление целое знак метод дополнительный код смещение вещественный тип формат фиксированный плавать точка вещественный одинарный двойной точность текстовый тип строковый символьный логический тип логические данные выражение операция кодирование графический информация растровый принцип понятие разрешение оригинал экранный печатный изображение растрирование изображение амплитудный частотный модуляция векторный графика фрактальный графика основной формат представление графический файл кодирование звуковой информация метод частотный модуляция таблично-волновой синтез основной тип структура данные линейный табличный иерархический файл каталог маршрут спецификация файл размещение файл внешний память кластер основный принцип хранение информация размещение кластер файл основа таблица размещение файл fat основа главный таблица файл mft назначение вид компьютерный сеть локальный глобальный интрасеть виртуальный сеть основной понятие структура глобальный сеть назначение вид сетевой программный обеспечение понятие логический архитектура сеть одноранговый архитектура архитектура основа сервер клиент-сервер основной топология локальный сеть полносвязный моноканальный кольцевой звездообразный метод доступ основной особенность сеть internet уровень адресация компьютер сеть локальный адрес ip-адресация доменный система имя определение алгоритм особенность описание форма представление алгоритм словесно-формульный структурный основной алгоритмический структура требование предъявлять алгоритм краткий характеристика основный класс программный средство системный программный обеспечение система программирование прикладной программный обеспечение назначение основной функция ос структура особенность основный компонент ос режим управление программа назначение программа технический обслуживание утилита архиватор программный вирус антивирусный программа утилит обслуживание внешний память назначение состав система программирование назначение основной особенность язык программирование основной особенность язык низкий высокий уровень основной принцип лежать основа различный группа язык программирование высокий уровень алгоритмический структурный понятие программа подпрограмма функция модульный программирование событийно-ориентировать объектно-ориентированный понятие класс объект инкапсуляция наследование полиморфизм особенность специализированный язык программирование декларативный язык программирование база данные язык разметка язык программирование internet назначение вид прикладной программный обеспечение основной особенность отличительный особенность данные знание понятие экстенсиональный интенсиональный информация сильно типизировать слабо типизировать модель информация определение база данные внешний концептуальный внутренний модель этап разработка база данные понятие абстракция обобщение агрегация наследование свойство понятие множество кортеж требование оформление понятие домен атрибут интенсионал экстенсионал атрибут экземпляр ключ возможный составной первичный внешний табличный представление данные реляционный таблица таблица запись использование моделирование данные представление данные вид граф понятие граф представление тип экземпляр объект связь понятие декартов произведение отношение бинарный тернарный n-арное отношение интенсиональный экстенсиональный описание отношение применение отношение моделирование данные понятие отображение прямой обратный отображение полный частичный отображение кардинальный число вид связь взаимно однозначный функциональный многие-ко-многий описание реляционный иерархический сетевой модель положительный особенность недостаток представление интенсионал экстенсионать модель распространение ключ внутренний явный подразумевать ограничение ограничение задавать отображение основной особенность запуск структура окно панель быстрый доступ лента контекстный меню абзац основной режим главный меню управление лента настройка панель быстрый доступ ввод документ загрузка сохранение файл экспорт импорт файл подготовка документ печать выделение мыший клавиатура удаление перемещение копирование мышь помощь универсальный буфер обмен фрагмент установка шрифт форматирование обрамление заливка поиск исправление ошибка стиль оформление вставка таблица вставка удаление изменение размер строка столбец ячейка оформление таблица объединение разбиение ячейка использование инструментальный панель работа таблица рисунок способ рисование работа готовый рисунок основной особенность запуск структура окно работа главный меню команда лента лист окно структура таблица содержимое значение ячейка способ адресация выделение область число мультивыбор мышь клавиатура копирование перемещение мыший помощь универсальный буфер обмен форматирование ячейка автозаполнение сохранение загрузка файл тип данные формула использование относительный абсолютный адресация форматирование таблица функция мастер функция использование имя локальный глобальный имя формула массив основной понятие формирование база данные критерий поиск поиск выбор данные сортировка данные мастер диаграмма создание редактирование диаграмма особенность гистограмма график круговой диаграмма основной особенность vba тип данные константа переменный массив выражение особенность работа среда программирование visual basic editor vbe понятие оператор структура оператор описание переменный способ организация ввод вывод данные назначение структура цикл вид цикл описание цикл понятие ветвление условный оператор оператор безусловный переход выбор понятие подпрограмма функция оформление подпрограмма функция оператор вызов подпрограмма функция модуль атрибут импорт модуль атрибут структура инструкция оператор пользовательский функция константа переменный python способ организация ввод вывод данные основной тип данные динамический типизация функция преобразование тип арифметический логический выражение вид последовательность список кортеж множество диапазон словарь понятие срез последовательность оператор работа последовательность способ присваивание присваивание значение групповой позиционный присваивание присваивание список часть элемент оператор альтернативный ветвление множественный выбор ветвление присваивание цикл выполнение действие элемент последовательность цикл предусловие оператор прерывание цикл итерация генератор список вложить генератор</t>
+  </si>
+  <si>
+    <t>тема научно-исследовательский деятельность понятие содержание этап критерий finer тема экспертный метод сбор информация методология поиск анализ научный статистический информация понятие информационный суррогат последствие использование научно-исследовательский деятельность тема метод научный исследование классификация метод экономический исследование аналитический синтетический метод исторический метод эволюционный метод наблюдение эксперимент статистический математический метод метод моделирование тема принцип правило представление исследование вид научный статья доклад требование устный презентация интерактивный сопровождение требование оформление результат нир тема тип область экономический исследование особенность теоретический эмпирический обзорный исследование тема составной часть процесс эмпирический экономический исследование гипотеза программа отчет тема сбор хранение обработка исходный данные протокол обработка данные вычислительный эксперимент протокол вычисление подготовка иллюстрация таблица сводный результат автоматизация подготовка отчет результат вычислительный эксперимент тема инструмент представление результат вычислительный эксперимент язык разметка markdown блокнот jupyter система подготовка отчет knitr публикация результат исследование world wide web</t>
+  </si>
+  <si>
+    <t>предмет история задача исторический наука научный принцип изучение прошлое концепция исторический развитие метод научный познание понятие исторический факт классификация факт классификация исторический источник проблема подлинность достоверность исторический источник понятие периодизация вид периодизация различный концепция исторический развитие периодизация история россия краткий характеристика основный период история человечество условие становление российский цивилизация запад восток древний русь запад золотой орда характер отношение становление русский московский централизовать государство великий географический открытие исторический значение реформация контрреформация европа становление национальный государство первый буржуазный революция модернизация россия эпоха петр великий промышленный переворот европа экономический политический социальный последствие великий буржуазный реформа россия второй половина xix особенность социально-экономический политический развитие мир россия рубеж век первый российский буржуазно-демократический революция политический партия россия зарождение парламентаризм причина характер особенность мировой война февральский революция 1917 г крушение монархия октябрьский революция 1917 г установление советский власть начало советский период история россия гражданский война страна новый экономический политика образование ссср социалистический индустриализация коллективизация сельский хозяйство политический режим массовый политический репрессия причина второй мировой война великий отечественный война 1941-1945 год источник цена победа основной тенденция мировой развитие второй половина xx столетие холодный война перестройка ссср 1985-1991 год распад советский союз становление современный российский федерация мир россия начало xxi</t>
+  </si>
+  <si>
+    <t>типология картина мир откуда куда идти человек эпоха неопределенность проблема будущее техногенный цивилизация вызов опасность возможность как сознание моделировать мир когнитивный наука когнитивный модель реальность ментальный карта карта местность системный подход эволюция вселенная материя живой материя мыслящий живой материя физический картина мир смена парадигма античность век классический механика электромагнитный парадигма современный квантово-релятивистский парадигма наука жизнь живой материя наука жизнь происхождение сущность жизнь теория эволюция генетика генные клеточный биотехнология биоэтика биополитика сознание контекст антропогенез коммуникация труд культура природа воспитание этология социобиология когнитивный наука человек мозг сознание понимание техника техника технология технический наука специфика инженерный знание вид схема метод кейс современный инструмент мультимедиа презентация создание схема закономерность развитие природа техника технический прогресс этап революционный эволюционный путь развитие промышленный революция модель черный ящик обратный связь кибернетика наука энтропия алгоритм язык свойство управление алгоритм управление система прикладной системный анализ задача этап метод принятие решение пример решение проблема применение системный анализ признак 4-й революция мегатренд цифровой направление физический биологический естественный искусственный интеллект определение признак сильный слабый искусственный интеллект критерий фактор эволюция человечество биологический техногенный составлять джереми рифкин анализ книга третий промышленный революция течение трансгуманизм значение путь развитие причина возникновение технологический сингулярность дикарь цифровой эпоха влияние цифровой эпоха естественный интеллект становление социологический наука социальный факт э дюркгейм понимать социология м вебер социальный действие понятие модернизация глобализация мир-системный теория глокализация социальный идентичность экзистенциальный абсурд понятие постмодернизм состояние общество понятие ризом модель общество понятие сетевой общество основа акторно-сетевой теория семиотика искусство понятие знак типологии знак знаковый система код текст понятие рамка структура коммуникация интенция автор интенция текст интенциональность реципиент методика семиотический анализ художественный текст эстетика наука эстетический эмоция эстетический отношение методика эстетический анализ художественный текст искусство первый половина хх век контекст научный открытие технический изобретение социальный изменение искусство миромоделирующий система содержание граница понятие современный искусство искусство эпоха модерн постмодерн постмодернизм игра хаос граница искусство понятие арт-практика концепция тотальный искусство феномен art &amp; science sciart искусство наука технология наука техника новый формат современный арт-практика методика анализ tabula rasa проблема наука искусство специфика подход сущность художественный образ групповой работа решение кейс групповой защита кейс инвалид основной подход определение понятие история отношение человек инвалидность античность современность понимание инвалидность отклонение норма движение право инвалид фактор смена подход понимание инвалидность инвалид основной подход определение понятие история отношение человек инвалидность античность современность понимание инвалидность отклонение норма движение право инвалид фактор смена подход понимание инвалидность технический средство реабилитация индивидуальный пользование костыль трость инвалидный коляска протез слуховой аппарат кохлеарный имплант очки новый подход индивидуальный протезирование бионический протез очки виртуальный реальность синтезаторы речь возможность применение технология человек трансгуманизм возможность риск доступный среда подход определение основный способ организация нормативно-правовой основание формирование доступный среда критерий оценка уровень доступность среда исследование элемент доступность окружать среда практический работа универсальный дизайн перспективный способ организация доступный среда эксклюзия отражение социокультурный проблема общество история включение ранее дискриминировать группа социум политика позитивный действие преимущество недостаток интеграция инклюзия сходство различие перспектива инклюзивный культура инклюзивный тип мышление правило взаимодействие человек инвалидность учет контекст взаимодействие ситуативный целенаправленный помощь этический дилемма контекст проблематика инвалидность этический принцип включение человек инвалидность общественный процесс основной правило взаимодействие человек инвалидность значимость образ человек инвалидность формирование инклюзивный общество фестиваль кино барьер образ человек инвалидность российский зарубежный кинематограф спортивный достижение человек инвалидность общий подход подготовка информационный материал проблематика инвалидность правило ошибка подготовка информационный материал стилистический графический художественный возможность оформление представление итог групповой домашний работа учет следующий требование задание подготовка информационный материал контент-план серия публикация социальный сеть информационный плакат ролик тема изучать рамка курс критерий оценка соответствие проблематика корректность использовать информация отсутствие ошибка полезность целенаправленность доступность читатель зритель оригинальность задумка подача</t>
+  </si>
+  <si>
+    <t>тема введение корпоративный социальный ответственность этика бизнес тема 2 модель корпоративный социальный ответственность тема стандарт корпоративный социальный ответственность тема корпоративный социальный политика тема управление корпоративный социальный ответственность</t>
+  </si>
+  <si>
+    <t>определение основной особенность экономический информационный технология метод обработка экономический информация глобальный базовый конкретный информационный технология особенность экономический информация определение основной особенность экономический информационный система роль место автоматизировать информационный система экономика уровень управление стратегический управленческий информационный операционный объект субъект управление информационный взаимосвязь информационный контур управление модель управление компания понятие информационный менеджмент основный особенность использование внешний внутренний информация разный уровень управление основный принцип построение функционирование экономический информационный система понятие корпоративный информационный система основный особенность создание построение корпоративный информационный система основной задача решать реализация корпоративный информационный система базовый функциональность корпоративный информационный система проблема управление внедрение корпоративный информационный система планирование формирование информационный система основный методика оценка информационный потребность анализ деятельность предприятие определение критический фактор успех достоинство недостаток автоматизация рационализация реинжиниринг смена парадигма основный способ организационный изменение технология поток работа workflow системный разработка основной этап конверсия параллельный стратегия стратегия прямой переключение пилотный стратегия фазовый стратегия конверсия управление эксплуатация технический обслуживание информационный система методология жизненный цикл создание система помощь прототип пакет прикладной программа разработка конечный пользователь аутсорсинг сравнение различный метод разработка особенность управление система этап развитие стандарт управление бизнес методология планирование потребность материал mrp планирование производственный мощность crp планирование ресурс производство mrp ii apics планирование ресурс предприятие erp erp-система планирование ресурс взаимодействие покупатель csrp crm-система управление ресурс взаимодействие предприятие erp ii scm-система инфраструктура архитектура предприятие метамодель организация основной особенность информационный менеджмент способ влияние организация использование корпоративный информационный система состав информационный служба ит-инфраструктура инфраструктура данные технический инфраструктура программный инфраструктура модель вычислительный сетевой инфраструктура понятие угроза безопасность информация вид угроза метод средство защита шифрование информация безопасность проведение расчет программный система учет аналитический система система автоматизация управление обзор базовый модуль erp система пример программный продукт с предприятие с управление предприятие с бухгалтерия с управление торговля с зарплата управление персонал реализация корпоративный стиль управление предприятие ведение разный вид учет единый информационный база обеспечение обмен данные синхронизация данные аналитический возможность программный продукт прибыльность товар направление деятельность контроль денежный поток взаиморасчет покупатель поставщик учет доход расход анализ финансовый результат работа предприятие налог отчетность настройка программа настройка управленческий налоговый бухгалтерский учет способ регистрация хозяйственный операция корреспонденция счет документ учет основный средство учет товарно-материальный ценность учет денежный средство расчет учет расчет контрагент учет расчет подотчетный лицо банк касса аналитический учет операция документ отчетность спецификация анализ информация движение запас выпуск готовый продукция начисление заработный плата анализ расход оплата труд начислить налог взнос фот классификация производственный затрата аналитический учет затрата учет выпуск реализация готовый продукция подготовка завершение период закрытие счет корректировка стоимость готовый продукция детализация регламентный операция стандартный отчет диаграмма регистр налоговый учет регламентировать отчетность создание регламентировать отчет расшифровка показатель регламентировать отчет проверка показатель регламентировать отчет выгрузка регламентировать отчет электронный вид</t>
+  </si>
+  <si>
+    <t>цель задача курс критический мышление письмо роль структура ядро интерактивный игра мир проблематизация понятие мир картина мир мировоззрение естественный научный картина мир рефлексия основа различие естественный научный картина мир типология картина мир мифологический религиозный философский научный критический мышление быстрый мышление медленный мышление мышление солдат мышление разведчик критический мышление практика рефлексия значить слушать значить слышать правило осознанный слушание причина коммуникативный неудача упражнение слушать слышать краткий содержание тема аргументация структура аргументация тезис аргумент демонстрация логика аргументация логический анализ аргументация красный селедка соломенное чучело игра дилемма специфика вопрос основный составлять рассуждение вид вопрос настоящий ненастоящий вопрос закрытый открытый вопрос типология вопрос б блум пресуппозиция вопрос некоректные вопрос постановка проблема вид вопрос проблемный непроблемный вопрос письмо рефлексивный практика рефлексивный эссе структура эссе свободный письмо структурирование текст ассоциация способ генерация облако смысл правило фрирайтинг понятие слово вещь объем понятие содержание понятие отношение понятие совместимость несовместимость операция понятие обобщение ограничение определение понятие вид определение правило определение ключевой слово понятие суждение логический форма суждение предложение структура суждение субъект предикат связка суждение тезис требование тезис умозаключение доказательство структура умозаключение доказательство паралогизм софизм парадокс правило аргументация правило тезис правило аргумент правило демонстрация некорректный уловка спор логический ошибка типология логический ошибка игра софист понятие верификация фальсификация критерий достоверность информация когнитивный искажение вид когнитивный искажение правило работа информационный источник упражнение не верить информация факт знание процедура фактчекинг принцип фактчекинг критерий выявление дезинформация командный работа межгрупповой занятие работа информационный источник самостоятельный подбор информационный источник содержать достоверный недостоверный информация верификация источник составление карта аргумент обосновывать решение команда рефлексия занятие 6 система взаимный оценивание аргументативное письменный рассуждение проблема тезис аргумент пример командный работа предполагать ряд этап этап анализ цитата выделение ключевой понятие формулировка проблема тезис аргумент пример этап критический анализ работа оппонент формулировка контраргумент этап взаимный оценивание карта аргумент более обоснованный смысл цель дебаты к поппер принцип дебаты структура механика дебаты этика дебаты регламент дебаты функция первый спикер карта аргумент аргументация контраргументация функция второй спикер вопрос контекст дебаты микро-батл тема предложить студент функция третий спикер аналитик дебаты судейский протокол критерий оценивание дебаты игра дебаты аналитик текущий игра игра дебаты аналитик текущий игра</t>
+  </si>
+  <si>
+    <t>пример экономический задача решение сводиться решение система линейный уравнение понятие вектор линейный зависимость теорема линейный зависимость признак линейный зависимость понятие базис координата вектор аффинный декартов прямоугольный система координата проекция точка вектор прямой плоскость ось определение свойство скалярный векторный смешанный произведение запись произведение вектор декартов прямоугольный система координата общий сведение уравнение линия плоскость пространство поверхность пространство алгебраический параметрический трансцендентный уравнение описывать взаимосвязь координата вектор точка разный система координата теорема общий уравнение прямой линия плоскость следствие нее другой тип уравнение прямой линия плоскость пучок прямой теорема общий уравнение плоскость пространство следствие нее другой уравнение плоскость пучок связка плоскость уравнение прямой линия пространство задача проецирование точка прямой плоскость определение расстояние точка прямой плоскость метод решение геометрический неравенство уравнение эллипс гипербола парабола свойство классификация линия второй порядок уравнение различный поверхность второй порядок свойство определение матрица тип матрица линейный операция матрица операция умножение матрица свойство определение операция элементарный преобразование матрица свойство матричный аналог определение обратный матрица теорема обратный матрица свойство обратный матрица определитель матрица свойство алгебраический дополнение разложение определитель матрица выбрать строка столбец вычисление алгебраический дополнение дополнительный свойство определитель матрица определитель произведение квадратный матрица понятие ранг матрица теорема базисный минор следствие нее определение система линейный алгебраический уравнение различный форма запись система линейный уравнение теорема кронекер-капелли крамер фундаментальный матрица система линейный алгебраический уравнение теорема фундаментальный матрица теорема общий решение однородный неоднородный система уравнение дополнительный теорема существование свойство решение система линейный уравнение альтернатива теорема фредгольм определение линейный пространство линейный зависимость вектор теорема линейный зависимость вектор базис линейный пространство координата вектор теорема линейный зависимость вектор координатный форма операция смена базис определение линейный подпространство теорема линейный подпространство сумма пересечение линейный подпространство теорема сумма пересечение линейный подпространство прямой дополнение линейный подпространство теорема прямой дополнение линейный подпространство определение скалярный произведение определение евклидов пространство неравенство коши-буняковского-шварц норма вектор расстояние угол вектор ортогональный дополнение линейный подпространство процедура ортогонализация грам-шмидт скалярный произведение ортонормированный базис постановка решение задача проецирование вектор подпространство понятие точечно-векторный пространство прямой плоскость гиперплоскость точечно-векторный пространство выпуклый множество выпуклый оболочка определение комплексный число операция комплексный число различный форма представление комплексный число определение унитарный пространство определение линейный оператор координатный матричный форма запись линейный оператор преобразование матрица линейный оператор смена базис операция линейный оператор геометрический свойство линейный оператор обратный линейный оператор теорема существование обратный линейный оператор определение собственный значение соответствующий собственный вектор линейный оператор теорема характеристический уравнение матрица линейный оператор базис собственный вектор определение разностный уравнение пример практический задача сводить разностный уравнение решение применение аппарат линейный оператор свойство решение разностный уравнение определение скалярный функция векторный аргумент линейный форма билинейный форма квадратичный форма матричный координатный форма запись функция преобразование матрица линейный функция смена базис понятие знакоопределенный квадратичный форма закон инерция квадратичный форма критерий лагранж сильвестр классификация квадратичный форма</t>
+  </si>
+  <si>
+    <t>макроэкономика как раздел экономический теория предмет макроэкономика метод макроэкономический изучение основный задача проблема понятие макроэкономика модель народнохозяйственный кругооборот экономический политика научный направление макроэкономика система национальный счет система макроэкономический показатель валовой внутренний продукт основной макроэкономический показатель способ расчет валовый внутренний продукт особенность структура валовый внутренний продукт россия валовой внутренний продукт другой показатель система национальный счет основной макроэкономический тождество номинальный реальный макроэкономический показатель индекс цена валовой внутренний продукт общественный благосостояние предпосылка кейнсианский модель функция потребление сбережение короткий период кейнсианский функция инвестиция равновесие двухсекторный модель кейнсианский крест мультипликатор автономный расход трехсекторный модель кейнсианский крест дискреционный бюджетно-налоговый политик модель кейнсианский крест мультипликатор бюджетно-налоговый политика рецессионный инфляционный разрыв вид бюджетный дефицит совокупный спрос ad структура фактор совокупный спрос совокупный предложение as короткий долгий период фактор совокупный предложение модель ad as макроэкономический равновесие короткий длительный период нарушение последующий восстановление макроэкономический равновесие шок совокупный спрос совокупный предложение понятие макроэкономический нестабильность деловой цикл экономический кризис безработица определение вид показатель особенность занятость безработица россия инфляция содержание показатель форма особенность инфляция россия взаимосвязь инфляция безработица кривая филлипес экономический рост содержание основной показатель источник тип фактор экономический рост экономический рост экономический развитие кейнсианский модель экономический рост модель домара-харрода неоклассический модель экономический рост модель р солоу денежный база деньга повышенный мощность денежный масса предложение деньга денежный агрегат денежный мультипликатор депозитный кредитный мультипликатор деньга кейнсианский теория спрос деньга количественный теория спрос деньга коммерческий банк коэффициент депонирование коэффициент монетизация ввп кредитно-денежный политика кдп ликвидность деньга монетарный правило мотив предосторожность нейтральность деньга норма избыточный резерв норма обязательный резерв норма резерв портфельный теория спрос деньга спекулятивный мотив спрос деньга ставка рефинансирование трансакционный мотив уравнение обмен и фишер функция деньга центральный банк государство национальный экономика экономический функция государство государственный бюджет структура дефицит бюджет государственный долг бюджетно-налоговый политик содержание цель инструмент вид бюджетно-налоговый политика встроить автоматический стабилизатор циклический структурный дефицит профицит государственный бюджет воздействие бюджетный профицит экономика способ финансирование бюджетный дефицит государственный долг воздействие бюджетно-налоговый политика совокупный предложение предпосылка модель is-lm кривая is кривая равновесие товарный рынок кривая lm кривая равновесие денежный рынок макроэкономический равновесие модель is-lm воздействие мера бюджетно-налоговый кредитно-денежный политика параметр макроэкономический равновесие модель is-lm ликвидный инвестиционный ловушка модель is-lm кривая совокупный спрос валютный рынок глобализация девальвация ревальвация конвертируемость денежный единица котировка валюта либерализация внешнеэкономический связь международный экономический отношение модель регулирование внешний торговля номинальный реальный валютный курс обменный валютный курс открытый экономика паритет покупательный способность ппс плавать фиксированный валютный курс платежный баланс предельный склонность импорт протекционизм фритредерство система валютный курс степень открытость экономика счет текущий операция счет движение капитал условие торговля</t>
+  </si>
+  <si>
+    <t>вводный лекция предмет содержание дисциплина маркетинг эволюция форма управление рыночный деятельность бизнес-субъект базовый определение маркетинговый деятельность основный направление тип тип вид маркетинг концепция маркетинг экономический роль цель задача стратегический оперативный маркетинговый деятельность бизнес-субъект понятие маркетинговый среда компания метод оценка маркетинговый среда компания этап развитие маркетинговый исследование понятие сущность маркетинговый исследование основной направление маркетинговый исследование принцип маркетинговый исследование классификация маркетинговый исследование процесс разработка маркетинговый исследование составление бриф маркетинговый исследование первичный вторичный маркетинговый информация источник метод маркетинговый исследование генеральный совокупность выборка исследование маркетинговый информационный система мис этап сегментирование рынок сегментационный анализ выбор целевой сегмент рыночный позиционирование разработка маркетинговый программа метод определение граница рынок выбор критерий сегментирование особенность сегментирование деловой рынок в разработка стратегия охват рынок рыночный ниша рыночный окно понятие целевой сегмент рынок целевой аудитория покупатель стратегия выбор целевой сегмент недифференцированный маркетинг дифференцированный маркетинг концентрированный маркетинг фактор влиять поведение потребитель тип покупательский поведение процесс принятие потребитель решение покупка понятие товар номенклатура ассортимент длина широта товарный ассортимент классификация потребительский товар классификация товар производственный назначение модель товар ф котлер мультиатрибутивный модель товар ж ж ламбен продуктовый портфель товарный стратегия жизненный цикл товар жцт стадия разработка новый товар инструментарий анализ товарный ассортимент компания метод авс-анализ ху z-анализ матрица бкг матрица ge mckinsey матрица и ансоффа марочный политик компания бренд элемент брендинг понятие цена товар услуга издержка постановка задача ценообразование определение спрос оценка издержка определение базовый уровень цена тип вид цена классификация метод установление цена адаптация цена цена условие конкуренция государственный регулирование цена стратегия ценообразование формирование коммуникационный политика понятие структура комплекс маркетинговый коммуникация классификация сущность инструмент комплекс продвижение компания процесс маркетинговый коммуникация концепция интегрировать маркетинговый коммуникация имк инструментарий цифровой маркетинг комплекс продвижение компания канал распределение товар функция канал товародвижение издержка товародвижение дистрибьюция потребительский промышленный товар выбор канал распределение охват рынок прямой косвенный канал распределение оптовый посредник вид дилер дистрибьютор брокер торговый агент розничный торговля классификация предприятие розничный торговля организация сервис уровень обслуживание потребитель тип сбытовый стратегия понятие стратегический маркетинг основный отличие операционный маркетинг состав функциональный структура комплекс стратегический операционный маркетинговый бизнес-субъект функция инструмент стратегический маркетинг функция инструмент операционный маркетинг стратегический планирование маркетинг вид маркетинговый стратегия основный этап планирование маркетинг вид план маркетинг стратегический план маркетинг операционный текущий план маркетинг структура план маркетинг маркетинговый программа</t>
+  </si>
+  <si>
+    <t>генеральный выборочный совокупность объем совокупность тип выборка повторный бесповторный репрезентативный выборка вариант вариационный ряд частота относительный частота статистический распределение выборка полигон относительный частота выборка группировать статистический ряд выборка гистограмма эмпирический функция распределение числовые характеристика выборка выборочный средний выборочный дисперсия выборочный средний квадратический отклонение выборочный мода выборочный медиана формулировка задача оценка параметр распределение понятие оценка параметр свойство оценка несмещенность состоятельность эффективность оценка точечный интервальный доверительный вероятность доверительный интервал построение доверительный интервал параметр нормальный распределение метод момент метод максимальный правдоподобие понятие статистический гипотеза простой сложный гипотеза нулевой альтернативный гипотеза ошибка первый второй род возникать проверка гипотеза статистический критерий уровень значимость критерий мощность критерий статистика критерий основной принцип проверка статистический гипотеза область принятие гипотеза критический область вид критический область правосторонний левосторонний двусторонний гипотеза значение неизвестный параметр нормальный распределение гипотеза равенство средний значение генеральный совокупность гипотеза равенство дисперсия генеральный совокупность гипотеза закон распределение критерий согласие хи-квадрат пирсон алгоритм проверка гипотеза закон распределение общий факторный остаточный сумма квадрат отклонение факторный остаточный дисперсия проверка значимость влияние фактор статистический зависимость корреляционный зависимость уравнение регрессия выборочный линейный уравнение регрессия понятие выборочный ковариация случайный величина понятие выборочный коэффициент корреляция связь выборочный коэффициент корреляция выборочный линейный уравнениями регрессия свойство выборочный коэффициент корреляция проверка значимость выборочный коэффициент корреляция ранги объект выборка выборочный коэффициент ранговый корреляция спирмена свойство выборочный коэффициент ранговый корреляция спирмена проверка значимость выборочный коэффициент ранговый корреляция спирмена основной понятие метод монте-карло метод статистический испытание преобразование равномерный распределение задать разыгрывание противоположный событие распределение хи-квадрат распределение стьюдент распределение фишер-снедекор гамма-распределение</t>
+  </si>
+  <si>
+    <t>понятие множество элемент множество обозначение множество способ задание множество пустой множество понятие подмножество множество равный множество операция множество объединение пересечение разность множество числовые множество определение рациональный иррациональный число модуль действительный число свойство понятие верхний нижний грань множество понятие точный верхний точный нижний грань множество числовой последовательность свойство числовой последовательность ограничить неограниченный возрастать убывать монотонный понятие окрестность точка предел числовой последовательность сходящиеся расходиться числовой последовательность геометрический смысл предел последовательность определение целый часть число свойство основной теорема предел числовой последовательность величина постоянный величина переменные функция область определение область значение функция частный значение функция график функция график основный элементарный функция основный свойство функция четный нечетный периодический возрастать убывать монотонный ограничить неограниченный способ задание функция аналитический табличный графический определение предел функция геометрический смысл предел функция односторонний предел бесконечно малый бесконечно больший функция свойство бесконечно малый бесконечно больший функция первый второй замечательный предел основной теорема предел функция непрерывность функция точка понятие приращение аргумент приращение функция точка эквивалентный определение непрерывность функция точка непрерывность сложный функция свойство функция непрерывный отрезок теорема ограниченность функция больший малый значение переход нуль промежуточный значение точка разрыв функция классификация производная геометрический механический смысл уравнение касательная кривая производная сумма произведение частный производная сложный функция обратный функция неявный функция функция задать параметрически производная основный элементарный функция понятие дифференцируемость функция точка логарифмический производная производная степенно-показательный функция дифференциал функция геометрический смысл дифференциал независимый переменный теорема связь дифференциал функция производный функция свойство дифференциал функция теорема инвариантность форма дифференциал использование дифференциал приближенный вычисление производный дифференциал высокий порядок теорема ролль лагранж кош правило лопиталя порядок раскрытие неопределенность неосновной вид помощь правило лопиталь исследование возрастание убывание функция помощь производная локальный экстремум исследование помощь первый второй производный понятие критический точка первый род схема отыскание больший малый значение функция отрезок выпуклость вогнутость точка перегиб график функция достаточный условие выпуклость вогнутость графика функция понятие критический точка второй род необходимый условие существование точка перегиб достаточный условие существование точка перегиб асимптота плоский кривая определение классификация исследование функция построение график первообразный неопределенный интеграл свойство теорема существование первообразный неопределенный интеграл таблица основный интеграл непосредственный интегрирование метод замена переменный метод интегрирование часть понятие рациональный функция рациональный дробь правильный неправильный рациональный дробь теорема разложение неправильный рациональный дробь простой дробь теорема разложение правильный рациональный дробь простой порядок интегрирование рациональный дробь интегрирование иррациональный функция основной вид интеграл порядок нахождение интегрирование тригонометрический функция основной вид интеграл порядок нахождение замечание небраться интеграл понятие интегральный сумма геометрический смысл определение геометрический смысл основный свойство определенный интеграл теорема существование определенный интеграл теорема средний значение интеграл переменный верхний предел формула ньютон лейбниц основной метод вычисление определить интеграл замена переменный интегрирование часть вычисление площадь плоский фигура приближенный вычисление определить интеграл метод симпсон несобственный интеграл бесконечный предел интегрирование интеграл i тип понятие особый точка функция несобственный интеграл неограниченный функция интеграл ii тип геометрический смысл несобственный интеграл признак сходимость несобственный интеграл неотрицательный функция абсолютный сходимость несобственный интеграл признак сходимость несобственный интеграл знакопеременный функция использование понятие производная экономика предельный издержка производство предельный выручка предельный доход предельный производительность так далее экономический смыть определенный интеграл решение задача экономический содержание использование дифференциальный интегральный исчисление понятие числовой ряд понятие n-ой частичный сумма ряд понятие сходиться числовой ряд понятие сумма числовой ряд геометрический ряд свойство числовой ряд понятие n-ого остаток ряд необходимый признак сходимость ряд теорема погружение дискретный аргумент n непрерывный х первый признак сравнение второй предельный признак сравнение признак даламбер признак кош интегральный признак кош знакочередующийся ряд признак лейбниц сходимость знакочередующийся ряд понятие знакопеременный числовой ряд абсолютный условный сходимость ряд метод математический индукция понятие степенной ряд область сходимость степенной ряд теорема абель нахождение интервал сходимость степенной ряд свойство степенной ряд ряд тейлор достаточный условие представление функция ряд тейлор ряд маклорен разложение ряд маклорена функция основной понятие схема отыскание область определение функция переменный определение график функция переменный линия уровень функция предел непрерывность функция переменный линия разрыв функция переменный частный производная правило дифференцирование определение полный дифференциал функция переменный достаточный условие дифференцируемости функция переменный дифференцирование сложный функция частный производная высокий порядок абсолютный экстремум функция переменный необходимый условие экстремума функция переменный достаточный условие экстремума функция переменный алгоритм отыскание экстремума функция переменный больший малый значение функция замкнутый область условный экстремум функция переменный способ задание плоский линия линия плоскость локальный элемент плоский линия угол линия огибающая однопараметрический семейство линия дискриминантный линия семейство линия понятие скалярный поле поверхность уровень скалярный поле производная направление градиент скалярный поле свойство градиент скалярный поле дифференцирование неявный функция переменный понятие двойной интеграл теорема существование двойной интеграл геометрический смысл двойной интеграл основной свойство двойной интеграл вычисление двойной интеграл декартов система координата вычисление двойной интеграл полярный система координата двойной интеграл бесконечный область двойной интеграл неограниченный функция понятие тройной интеграл геометрический смысл тройной интеграл основный свойство тройной интеграл вычисление тройной интеграл декартов координата вычисление тройной интеграл цилиндрический координата понятие криволинейный интеграл первый род основной свойство криволинейный интеграл первый род вычисление интеграл первый род геометрический смысл криволинейный интеграл первый род понятие криволинейный интеграл второй род основной свойство криволинейный интеграл второй род вычисление интеграл второй род геометрический смысл криволинейный интеграл второй род понятие дифференциальный уравнение обыкновенный дифференциальный уравнение порядок дифференциальный уравнение решение дифференциальный уравнение общий решение дифференциальный уравнение общий интеграл дифференциальный уравнение частный решение дифференциальный уравнение особый решение дифференциальный уравнение задача кош дифференциальный уравнение первый порядок уравнение разделяться переменный однородный дифференциальный уравнение метод решение однородный дифференциальный уравнение линейный дифференциальный уравнение первый порядок нахождение общий решение линейный неоднородный уравнение первый метод вариация произвольный постоянный метод лагранж уравнение бернулли уравнение полный дифференциал уравнение содержать только независимый переменный производная второй порядок уравнение не содержать искомый функция уравнение не содержать независимый переменный линейный однородный дифференциальный уравнение второй порядок постоянный коэффициент понятие комплексный число метод решение линейный однородный дифференциальный уравнение второй порядок постоянный коэффициент характеристический уравнение общий решение линейный однородный дифференциальный уравнение второй порядок постоянный коэффициент линейный неоднородный дифференциальный уравнение второй порядок постоянный коэффициент общий решение линейный неоднородный дифференциальный уравнение второй порядок постоянный коэффициент метод подбор метод неопределенный коэффициент общий вид дифференциальный уравнение первый порядок не разрешить производная метод введение параметр уравнение лагранж уравнение клеро особый решение алгоритм отыскание особый решение дифференциальный уравнение первый порядок не разрешить производная понятие система дифференциальный уравнение первый порядок понятие нормальный система дифференциальный уравнение понятие решение нормальный система дифференциальный уравнение задача кош нормальный система дифференциальный уравнение метод решение нормальный система дифференциальный уравнение метод исключение неизвестный метод нахождение интегрировать комбинация понятие изоклина приближенный построение интегральный кривая дифференциальный уравнение метод изоклина составление дифференциальный уравнение семейство кривой решение задача кош метод последовательный приближение линейный однородный дифференциальный уравнение второй порядок переменный коэффициент общий решение линейный однородный дифференциальный уравнение второй порядок переменный коэффициент линейный неоднородный дифференциальный уравнение второй порядок переменный коэффициент метод вариация произвольный постоянный метод лагранж общий решение линейный неоднородный дифференциальный уравнение второй порядок переменный коэффициент рассмотрение пример использование дифференциальный уравнение модель экономический динамика отражаться не только зависимость переменный время взаимосвязь время</t>
+  </si>
+  <si>
+    <t>глобализация мировой экономика понятие международный экономика предмет курс метод анализ международный экономика структура международный экономический отношение международный разделение труд 2.1 теория международный торговля классический теория международный торговля теория абсолютный преимущество теория сравнительный преимущество теория соотношение фактор производство парадокс леонтьев альтернативный теория международный торговля эффект масштаб несовершенный конкуренция теория спрос реверс международный торговля теория цикл жизнь продукт теория конкурентный преимущество майкл портер влияние международный торговля доход 2.2 динамика структура международный торговля динамика международный торговля структура международный торговля страны-лидер импорт экспорт международный торговля товар услуга внешний торговля россия динамика основный показатель внешний торговля россия географический структура внешний торговля россия товарный структура экспорт россия товарный структура импорт россия регулирование международный торговля свобода торговля протекционизм тарифный метод регулирование таможенный тариф пошлина специфический случай тарифный политика нетарифный метод регулирование международный торговля количественный ограничение скрыть метод торговый политика финансовый метод торговый политика неэкономические метод регулирование последствие введение торговый ограничение экономика малый большой страна наднациональный регулирование международный торговля форма международный движение капитал прямой зарубежный инвестиция теория экономический эффект международный корпорация форма влияние принимать страна страна базирование портфельный зарубежный инвестиция вид портфельный инвестиция причина международный заимствование кредитование инструмент международный кредитование теория международный трудовой миграция вид экономический эффект миграция масштаб направление миграция рабочий сила государственный регулирование миграция механизм контроль миграция регулирование миграция стимулирование реэмиграция понятие валюта эволюция валютный система золотой стандарт золотодевизный стандарт современный валютный система валютный курс разновидность понятие котировка валютный курс вид валютный курс степень гибкость гибридный вид валютный курс теория валютный курс теория паритет покупательный способность влияние процентный ставка валютный курс фактор влиять валютный курс влияние валютный курс экономика страна управление валютный риск становление интеграционный процесс предпосылка цель интеграция тип интеграционный объединение этап интеграция интеграционный объединение принцип оценка интеграция статический динамический эффект интеграция</t>
+  </si>
+  <si>
+    <t>сущность содержание понятие менеджмент подход определение менеджмент менеджмент наука управление менеджмент искусство управление менеджмент лицо группа лицо осуществлять управление идентификация менеджмент орган аппарат управление менеджмент процесс соотношение понятие менеджмент управление администрирование бизнес предпринимательство история возникновение менеджмент общий характеристика управленческий революция развитие научный школа подход менеджмент школа научный менеджмент классический административный школа школа человеческий отношение поведенческий наука школа наука управление количественный школа процессный подход системный подход ситуационный подход характеристика прочий подход менеджмент современный система взгляд менеджмент характеристика новый управленческий парадигма менеджмент xxi век менеджмент орбита управление организация общий характеристика функция управление подход классификация функция управление планирование деятельность цель задача планирование этап планирование постановка цель планирование основный область целеполагание требование постановка цель организация управленческий деятельность аспект организационный процесс менеджмент характеристика ключевой элемент процесс организация делегирование ответственность полномочие мотивация деятельность общий характеристика мотивационный процесс тип мотивация теория мотивация содержательный теория мотивация процессуальный теория мотивация контроль система управление организация цель контроль основный вид ключевой фактор успех кфу современный система взгляд управленческий функция контекст менеджмент понятие управленческий труд сущность содержание управленческий труд цель предмет средство продукт вид разделение управленческий труд функциональный иерархический технологический профессиональный квалификационный должностной менеджер предприниматель профессионал управление различие предприниматель менеджер содержание труд менеджер основной тип менеджер линейный менеджер функциональный менеджер руководитель низовой звено руководитель средний звено руководитель высокий звено требование предъявлять менеджер лидер менеджер сравнительный характеристика метод развитие навык менеджер менеджер xxi век характеристика основный качество общий подход понятие организация признак организация основный параметр организация содержание понятие организация социальный система механистический органический подход организация креативный гуманистический организация классификация организация г минцберг вид хозяйственный организация интеграция организация вариант интеграционный процесс вертикальный интеграция горизонтальный интеграция диверсификация форма интеграция кризис традиционный организация характерный признак организация xxi век признак бирюзовый организация человек главный актив субъект организационный изменение внешний среда организация компонент макроокружение экономический компонента политический правовой социокультурный технологический географический международный окружение рыночный окружение поставщик потребитель конкурент рыночный инфраструктура взаимосвязь компонент степень воздействие внешний среда организация внутренний среда организация кадровый подсистема организационный подсистема производственный подсистема маркетинговый подсистема инновационный подсистема финансовый подсистема организационный культура обобщать характеристика среда организация внешний внутренний среда цифровой эпоха стирание граница внутренний внешний среда организация экосистема эко системный подход общий понятие организационный структура управление оса принцип формирование оса ключевой понятие организационный проектирование фактор проектирование организация зависимость внешний среда параметр среда организация виляние организационный проектирование технология работа технология индустрия стратегический выбор руководство элемент проектирование организация разделение труд специализация департаментизация кооперация связь часть координация масштаб управляемость контроль иерархия организация звенность распределение право ответственность централизация децентрализация дифференциация интеграция общий характеристика бюрократический тип оса вид бюрократический структура управление линейный функциональный линейно-функциональный линейно-штабной преимущество недостаток дивизиональный оса прогрессивный вид бюрократический оса критерий структурирование организация дивизион отделение общий характеристика органический тип оса основной вид органический структура управление матричный организация разновидность проектный организация временной целевой группа постоянный комплексный группа бригадный форма организация труд преимущество недостаток органический структура управление тенденция эволюция оса признак современный общество требование предъявлять формирование эффективный оса критерий определение эффективный структура управление характеристика новый тип оса эдхократический организация многомерный организация партисипативная организация ориентировать рынок организация предпринимательский тип сетевой организация виртуальный организация организационный структура управление условие цифровой трансформация компания общий понятие содержание метод менеджмент эволюция метод менеджмент отечественный наука управление развитие методический инструментарий зарубежный школа подход менеджмент тенденция изменение метод менеджмент характеристика современный метод менеджмент классификация метод менеджмент общенаучные метод менеджмент метод исторический подход менеджмент моделирование использование экономико-математический метод экспериментирование метод социологический исследование специфический метод менеджмент организационно-распорядительный экономический социально-психологический мотивационный метод характеристика прочий подход классификация метод менеджмент формирование фонд метод менеджмент</t>
+  </si>
+  <si>
+    <t>оптимизационный задача задача математический программирование общий постановка задача математический программирование понятие целевой функция область допустимый решение область ограничение оптимальный решение оптимальный план понятие линейный нелинейный выпуклый вогнутый функция разновидность задача математический программирование задача нелинейный линейный программирование задача ограничение ограничение-равенство ограничение-неравенство смешанный ограничение понятие стационарный точка функция понятие матрица гесс понятие квадратичный форма матрица положительный отрицательный определенность матрица понятие вектор-функция матрица якоби понятие производная направление градиент теорема производный направление теорема градиент понятие касательная гиперплоскость нормаль формула тейлор разложение тейлор функция переменный теорема вейерштрасса теорема необходимый условие экстремум функция ограничение теорема достаточный условие экстремум функция ограничение теорема условие определенность матрица критерий сильвестр классический метод решение злнп ограничение метод множитель лагранж обоснование метод функция лагранж инструментальный переменный множитель лагранж стационарный точка функция лагранж окаймить матрица гесс достаточный условие существование экстремума функция наличие ограничение-равенство алгоритм реализация метод лагранж интерпретация множителей лагранж теорема лагранж метод подстановка решение знлп ограничение-равенство обобщенный метод множитель лагранж обоснование метод активный пассивный ограничение алгоритм реализация обобщенный метод лагранж условие кун-таккер задача выпуклый нелинейный программирование достаточность условие кун-таккер теорема единственность экстремум строго выпуклый вогнутый функция метод кун-таккер решение задача выпукло-вогнутый нелинейный программирование обоснование метод алгоритм реализация общий постановка задача линейный программирование злп форма представление канонический симметричный общий понятие угловой точка вершина выпуклый многогранник понятие опорный план злп теорема эквивалентность форма представление злп теорема представление каратеодори теорема решение злп графический метод решение злп обоснование метод алгоритм реализация графический метод симплекс-метод обоснование метод алгебра симплекс метод алгоритм реализация симплекс-метод симплекс-таблица правило построение заполнение пересчет симплекс-таблица двойственный пара задача линейный программирование прямой двойственный злп двойственный лемма прямой двойственный оценка теорема двойственность теорема представление оптимальный план прямой злп теорема представление оптимальный план двойственный злп экономический интерпретация двойственный оценка двойственный симплекс-метод обоснование метод алгоритм реализация устойчивость решение задача двойственный пара теорема условие устойчивость прямой оценка теорема условие устойчивость двойственный оценка закрытый транспортный задача тз теорема разрешимость тз открытый тз недостаток избыток сведение тз открытый тип закрыть тз метод определение опорный план тз метод северо-западный угол метод минимальный элемент минимальный тариф метод потенциал решение тз теорема оптимальный план тз задача коммивояжер задача назначение выбор метод отсечение решение злдп правильный отсечение отсечение гоморь метод гоморь обоснование метод алгоритм реализация метод ветвь граница обоснование схема реализация пример понятие многошаговый операция шаговый управление показатель эффективность целевой функция область допустимый управление условие отсутствие последействие уравнение состояние условие аддитивность целевой функция принцип оптимальность беллман понятие условный безусловный оптимальный управление обоснование метод прогонка двухэтапный процедура метод прогонка 1 этап обратный прогонка 2-й этап прямой прогонка вычислительный схема метод прогонка уравнение беллман задача распределение ресурс задача управление запас задача замена пример задача динамический программирование понятие граф элемент вершина дуга ребро цепь путь цикл дерево понятие инцидентность матрица инцидентность критерий путь задача построение минимальный остовный дерево задача поиск минимальный критический путь задача максимальный поток сеть задача поток минимальный стоимость сведение рассмотреть задача задача линейный программирование график гант сетевой модель проект событие начало завершение работа проект отображение графа правило построение сетевой модель проект упорядочение время элемент сетевой модель проект сетевой график временной параметр сетевой график понятие критический путь cpm pert метод оптимизация сетевой график общий постановка задача управление запас понятие величина характер спрос тип скорость расход запас объем размер заказ цикл заказ точка заказ статический детерминировать модель дефицит формула уилсон статический детерминированный модель дефицит статический детерминированный модель дисконт простой стохастический стационарный модель понятие система массовый обслуживание смо основной элемент область применение смо простой модель смо имитационный моделирование метод монте-карло прием построение эксплуатация имитационный модель общий постановка задача принятие решение условие неопределенность интерпретация игра природа основной элемент особенность игра природа основной форма нормальный позиционный представление критерий лаплас ожидать значение байес гурвица гарантировать результат минимаксный максиминный сэвидж нейман-пирсон геометрический интерпретация игра природа</t>
+  </si>
+  <si>
+    <t>трактовка термин экономика понятие экономический теория предмет экономический теория субъект экономический выбор домашний хозяйство фирма государство цель уровень изучение экономика микроэкономика мезоэкономика макроэкономика мегаэкономика метод экономический теория общенаучный специфический вид модель метод прочий равный условие метод предельный анализ метод теория игра позитивный нормативный подход экономический объект благо экономический свободный потребительский производственный частный общественный долговременный недолговременный общественный производство воспроизводство стадия общественный воспроизводство простой расширить воспроизводство фактор производство к маркс средство производство средство труд предмет труд рабочий сила теория фактор производство сея земля капитал труд предпринимательский способность дополнительный фактор производство технологический выбор экономика кривая производственный возможность допущение построение графический табличный форма движение кривая сдвиг кривая производственный возможность закон возрастать альтернативный издержка коэффициент трансформация экономический система вид чистый тип экономический система основной экономический вопрос чистый тип экономический система смешанный экономика переходный экономика понятие собственность субъект объект собственность правомочие право собственность форма собственность классификация понятие функция рынок способ организация производство благо натуральный товарный хозяйство основной черта условие возникновение товарный хозяйство бартерный денежный обмен причина переход денежный обмен субъект объект рынок инфраструктура рынок механизм рынок вид рынок объект пространственный разрез сила конкурентный борьба совершенный конкуренция монополистический конкуренция олигополия монополия характерный черта тип рыночный структура число фирма тип продукт контроль цена условие вступление отрасль неценовой конкуренция черта совершенный конкуренция достоинство рынок недостаток рынок внешний эффект общественный благо вид асимметрия информация товар потребительный меновой стоимость услуга свойство спрос функция спрос кривая спрос наклон кривая спрос закон спрос обоснование закон спрос закон убывать предельный полезность эффект доход эффект замена вид спрос рыночный индивидуальный спрос ценовый неценовой фактор спрос нормальный низкий товар товар-заменитель дополнять товар сдвиг кривая спрос изменение спрос товар гиффен индивидуальный рыночный спрос предложение функция предложение прямой обратный кривой предложение закон предложение кривой предложение ценовый неценовой фактор предложение сдвиг кривой предложение изменение предложение индивидуальный рыночный предложение равновесие рынок восстановление цена равновесие равновесный объем товар излишек потребитель графический смысловой интерпретация излишек потребитель излишек производитель графический смысловой интерпретация излишек производитель рыночный излишек влияние государство чистый потеря общество налогообложение конкуренция внутриотраслевой межотраслевой вид конкуренция метод конкурентный борьба добросовестный недобросовестный конкуренция продукт конкуренция условие продажа понятие эластичность эластичность спрос цена интервал ценовый эластичность неэластичный эластичный единичный эластичный абсолютно неэластичный абсолютно эластичный спрос фактор ценовый эластичность практический значение измерение ценовый эластичность спрос эластичность спрос доход интервал эластичность спрос доход практический значение эластичность спрос доход перекрестный эластичность спрос интервал перекрестный эластичность спрос практический значение перекрестный эластичность спрос ценовый эластичность предложение период производство ценовый эластичность предложение понятие фирма цель деятельность фирма организационно-правовой форма окопф понятие производство движение индивидуальный капитал прибавочный продукт прибавочный стоимость технология производство экономический эффективность производство технологический эффективность производство краткосрочный долгосрочный период производственный деятельность постоянный переменный ресурс закон убывать предельный отдача фактор масштаб производство верхний технический граница производство краткосрочный долгосрочный период экономия масштаб эффект масштаб вид эффект масштаб продукт товар совокупный продукт средний продукт предельный продукт предельный продукт труд вид учет продукт определение обозначение формула график производственный функция общий вид замечание форма представление таблица уравнение график краткосрочный функция производство стадия изменение общий средний предельный продукт производственный функция закон убывание предельный отдача долгосрочный производственный функция допущение построение таблица формула график изоквант карта изоквант свойство стандартный изоквант предельный норма технологический замещение убывание предельный норма технологический замещение оптимум производитель бюджетный ограничение производитель уравнение изокоста линия изокоста наклон линия изокоста условие оптимум экономический смысл издержка производство роль издержка экономический процесс вид издержка источник образование состав сфера возникновение возможность возмещение бухгалтерский прибыль нормальный прибыль неявный издержка альтернативный издержка экономический прибыль невозвратный издержка вид издержка краткосрочный долгосрочный период вид издержка понятие обозначение формула график постоянный переменный издержка общий валовый издержка общий постоянный издержка общий переменный издержка средний общий издержка средний постоянный издержка средний переменный издержка предельный издержка соотношение общий издержка графика соотношение средний издержка графика значимый точка пересечение график долгосрочный период условно-постоянный издержка переменный издержка доход прибыль фирма постоянный переменный цена выручка средний доход предельный доход ситуация получение прибыль фирма соотношение общий выгода издержка функция прибыль график рыночный структура характерный черта совершенный конкуренция фирма-ценополучатель значение модель совершенный конкуренция краткосрочный кривой фирма кривая спрос продукция фирмы-совершенный конкурент формула кривой совокупный средний предельный доход фирмы-совершенный конкурент равновесие фирма оптимальный объем выпуск метод совокупный издержка метод предельный издержка совместный динамика предельный общий прибыль соотношение предельный издержка предельный доход средний прибыль условие получение краткосрочный прибыль вариант рыночный конъюнктура условие прекращение производственный деятельность кривой предложение фирмы-совершенный конкурент рыночный кривая предложение долгосрочный период специфика положение фирма краткосрочный долгосрочный период условие равновесие фирма долгосрочный период перелив капитал случай экономический прибыль убыток безубыточность график фирма отрасль логика развитие ситуация несовершенный эластичность рынок сжатие расширение кривая долгосрочный издержка эффект масштаб долгосрочный общий издержка график долгосрочный средний издержка определение построение график оптимальный размер предприятие минимально эффективный размер предприятие положительный эффект масштаб производство latc причина положительный эффект масштаб отрицательный эффект масштаб производство latc причина отрицательный эффект масштаб постоянный эффект масштаб производство latc рыночный власть монополия понятие рыночный монопольный власть коэффициент лернер источник монопольный власть монополия узкий широкий смысл монопсония дуополия чистый монополия допущение барьер конкуренция естественный искусственный барьер стратегический нестратегический барьер естественный временной открытый легальный локальный административный закрытый искусственный вид монополия недобросовестный конкуренция понятие содержание спрос доход фирмы-монополист ценопроизводитель власть монополист сфера назначение цена наклон кривая спрос монополист особенность кривая спрос монополист кривой общий предельный доход монополист работать эластичный участок d доказательство условие максимизация прибыль фирмы-монополист аналитически графически метод совокупный издержка совокупный доход метод предельный издержка предельный доход отличие нахождение оптимум совершенный конкуренция монополия точка оптимум прибыль монополист случай точка закрытие монополист предложение фирма-монополист традиционный убывать единый кривая предложение монополист ценовый дискриминация дополнительный выручка дискриминация эффект условие эффективность ценовый дискриминация арбитраж ценовый дискриминация первый степень понятие график ценовый дискриминация второй степень пример ценовый дискриминация третий степень пример олигополия свойство олигополистический рынок коэффициент лернер олигополия взаимозависимость олигополист особенность рынок олигополистический взаимодействие олигополист кривой спрос продукт предельный доход точка равновесие оптимум mr mc вид модель олигополия некооперированный кооперировать олигополия дуополия модель курно предпосылка основный задача модель суть взаимодействие кривая остаточный спрос общий доход фирма предельный доход фирма оптимальный объем фирма функция реакция аналитически графически экономический смысл кривая реакция точка равновесие курно отраслевой оптимум вывод параметр отраслевой равновесие аналитически модель картель основный цель образование картель направление сговор международный картель картель россия административный коап уголовный ук ответственность организация картель параллелизм олигополистовый понятие параллелизм преимущество параллелизм отличие картель форма параллелизм тип фирма отрасль ценовый лидерство свойство лидер вид лидерство лидерство доминировать фирма общий принцип лидерство фактор препятствовать ценовый координация основной черта рынок монополистический конкуренция следствие большой количество продавец барьер вхождение отрасль причина небольшой высота продуктовый дифференциация фактор дифференциация критерий дифференциация горизонтельная вертикальный дифференциация продукт сегмент рынок стратегия дифференциация продукт лояльность потребитель концепция уникальный рыночный предложение неценовой конкуренция причина неэффективность ценовый конкуренция пример рынок монополистический конкуренция условие максимизация прибыль краткосрочный период промежуточный состояние совершенный конкуренция монополия отличие монополист эластичность степень монопольный власть кривая спрос продукция монополистический конкурент свойство график рыночный спрос монополистическа конкурентный рынок степень замещение продукт предельный доход фирма монополистический конкурент преимущество недостаток рынок монополистический конкуренция понятие рынок ресурс специфика ресурсный рынок вид доход получать вид ресурс вид рынок ресурс спрос предложение рынок ресурс фактор определять спрос ресурс фактор определять эластичность спрос ресурс особенность предложение ресурс выбор сочетание ресурс правило минимизация издержка правило максимизация прибыль рынок труд объект продажа рынок труд подход разный экономический школа особенность труд ресурс спрос труд предложение труд индивидуальный рыночный кривая предложение труд заработный плата номинальный реальный заработный плата рынок капитал трактовка понятие капитал натуралистический концепция монетаристский концепция концепция человеческий капитал форма капитал производительный товарный денежный кругооборот капитал производственный торговый спекулятивный основной оборотный капитал доход использование капитал прибыль процент маржа зависимость процентный ставка срок риск номинальный реальный процентный ставка равновесие рынок капитал дисконтирование рынок земля рынок услуга земля цена земля земельный рента предложение земля свойство абсолютный дифференциальный рента дифференциальный рента цена земля</t>
+  </si>
+  <si>
+    <t>пространство товар предпочтение потребитель отношение предпочтение основной аксиома теория потребление кривой безразличие стандартный предпочтение непрерывность монотонность выпуклость функция полезность определение важный теорема свойство кривой безразличие уровень функция полезность предельный норма замещение товар потребление вид функция полезность связь предпочтение потребитель бюджетный множество потребитель задача потребительский выбор постановка графический анализ решение метод лагранж функция обыкновенный спрос правило доля предпочтение кобба-дуглас особый случай оптимальный выбор потребитель косвенный функция полезность предельный полезность доход тождество рой двойственность теория потребление задача минимизация расход спрос хикс функция расход предельный расход полезность лемма шепард связь прямой двойственный задача потребитель влияние доход поведение потребитель нормальный инфериорный товар кривая доход-потребление кривой энгель влияние цена поведение потребитель обычный товар товар гиффен кривой цена-потребление кривой спрос эластичность спрос эффект доход замещение связать изменение цена уравнение слуцкий излишек потребитель мера благосостояние описание технология производство производственный фактор производственный функция изокванта вид производственный функция свойство производственный функция монотонность технология убывание предельный продукт выпуклость технология отдача масштаб предельный норма технологический замещение эластичность производство эластичность замещение экономический издержка общий издержка производство изокоста короткий длительный период экономический анализ минимизация издержка задать объем выпуск определение экономически эффективный способ производство аналитический графический решение функция издержка траектория рост фирма графический анализ общий средний предельный издержка длительный короткий период взаимный расположение краткосрочный долгосрочный кривой издержка прибыль условие максимизация решение задача максимизация прибыль конкурентный фирма короткий длительный период процедура одношаговый оптимизация точка локальный рыночный равновесие производитель функция спрос производственный фактор функция предложение выпуск двухэтапной решение задача максимизация прибыль правило максимизация прибыль предложение конкурентный фирма критерий целесообразность производство предельный издержка кривая предложение излишек производитель равновесие конкурентный отрасль предложение конкурентный отрасль длительный период принцип нулевой прибыль условие долгосрочный равновесие рынок совершенный конкуренция эффективность конкурентный рынок поведение фирма условие монополия спрос продукт монополист общий предельный доход монополист зависимость общий предельный доход эластичность спрос цена решение задача монополист монополия короткий длительный период отсутствие функция предложение монополист индекс лернер показатель рыночный власть неэффективность монополия ценовый дискриминация олигополия задача принятие решение условие конфликт сторона равновесие нэш дуополия курно дуополия стекельберг конкуренция сговор дилемма заключить влияние дилемма заключить олигополистический ценообразование максимизация прибыть условие картель модель ценовый олигополия дуополия бертран рынок монополистический конкуренция равновесие фирма рынок монополистический конкуренция избыточный производственный мощность плата разнообразие экономика обмен начальный запас допустимый распределение ящик эджворт парето-улучшение парето-эффективность контрактный кривая множество парето ядро экономика совокупный избыточный спрос равновесие вальрасу закон вальрас конкурентный равновесие эффективность эффективность справедливость теорема благосостояние экономика производство эффективность сфера производство кривая производственный контракт граница производственный возможность предельный норма трансформация эффективность структура выпуск продукция парето-эффективность рынок совершенный конкуренция теорема благосостояние базовый метод макроэкономический анализ моделирование агрегирование статика динамика фактор время краткосрочный среднесрочный долгосрочный период поведение экономика экономический рост деловой цикл валовой внутренний продукт номинальный реальный ввп индекс реальный ввп темп прирост ввп ввп душа население уровень цена ценовый индекс темп инфляция формула фишер уровень безработица неравенство доход схема межотраслевой баланс модель леонтьев коэффициент прямой полный материальный затрата продуктивность модель леонтьев межотраслевой баланс анализ экономический показатель равновесный цена межотраслевой баланс труд оценка показатель фондоемкость динамический модель межотраслевой баланс модель нейман расширяться экономика кейнсианский функция потребление загадка кузнец модель межвременной выбор фишер влияние богатство ставка процент потребление сбережение модель жизненный цикл модильяни иллюстрация гипотеза жизненный цикл рамка модель фишер модель перманентный доход фридман иллюстрация гипотеза перманентный доход рамка модель фишер макроэкономический инвестиция неоклассический модель инвестиция основный фонд кейнсианский подход инвестиция модель издержка приспособление модель гибкий акселератор теория q-тобин инвестиция жилищный строительство инвестиция запас модель жесткий акселератор вопрос отделимость потребительский решение инвестиционный модель кейнсианский крест двухсекторный экономика мультипликатор автономный расход эффект мультипликатор парадокс сбережение индуцировать инвестиция воздействие равновесие товарный рынок разрыв расход выпуск модель кейнсианский крест равновесие товарный рынок трехсекторная четырехсекторный модель экономика количественный теория деньга уравнение обмен инфляция ставка процент доход государство эмиссия деньга сеньораж модель экзогенный предложение деньга денежный база денежный мультипликатор модель спрос деньга портфельный подход модель баумоль-тобин равновесие денежный рынок равновесный ставка процент инструмент денежно-кредитный политика предпосылка модель is-lm совокупный расход ставка процент кривая is кривая равновесие товарный рынок кривая lm кривая равновесие денежный рынок особый случай линия is lm ловушка ликвидность процентный ловушка инвестиционный ловушка макроэкономический равновесие модель is lm достижение равновесие макроэкономический политика модель is-lm is-lm модель совокупный спрос мультипликатор совокупный спрос модель is-lm открытый экономика спрос труд предложение труд равновесие рынок труд безработица моделирование естественный уровень безработица циклический конъюнктурный безработица модель оукен компромисс инфляция безработица кривая филлипес модель совокупный предложение общий характеристика модель ad-as краткосрочный среднесрочный долгосрочный равновесие модель ad-as шок совокупный спрос совокупный предложение стабилизационный политика закрытый экономика парадокс сбережение закрыть экономика гибкий цена гибкий заработный плата монетарный политика последствие изменение совокупный предложение фактор экономический рост модель экономический рост солоу сравнительный статика модель солоу оптимальный запас капитал золотой правило экономический рост технологический прогресс остаток солоу циклический характер экономический динамика деловой цикл фаза модель самуэльсона-хикса модель тевес практический использование экономический цикл</t>
+  </si>
+  <si>
+    <t>понятие цепь поставка сетевой структура цепь поставка концепция управление цепь поставка scm supply chain management вид аналитик управление цепь поставка задача цепь поставка уровень абстракция аналитический оптимизация динамический имитационный моделирование цифровой двойник цепь поставка цифровой управление цепь поставка digital scm важность размещение объект цепь поставка подход решение задача размещение гравитационный анализ эвристический метод ардалан метод критический точка метод калькуляция затрата бальный оценка scoring model задача единый средний single median problem задача охват covering problem планирование цепь поставка стратегический тактический оперативный основа оптимизационный моделирование статический модель динамический модель модель неопределенность классический транспортный задача транспортный задача промежуточный пункт задача назначение планирование доставка мелкопартийный груз условие крупный город интегрировать модель цепь поставка транспортно-складской задача производственно-транспортно-складский задача запас объект управление цепь поставка понятие запас вид запас точка зрение запас движение запас звено цепь поставка модель уилсон eoq-модель модификация задержка поставка разрыв цена дефицит запас учет аккумулировать запас денежный средство учет фактор время основный тип стратегия управление запас многономенклатурный модель управление запас управление запас интегрировать многоуровневый цепь поставка ключевой преимущество anylogistix аналитический оптимизация динамический моделирование anylogistix создание цифровой двойник цепь поставка anylogistix эксперимент greenfield analysis gfa определение расположение объект метод центр тяжесть network optimization no определение оптимальный сетевой структура планирование материальный поток simulation имитационный моделирование оценка конфигурация политик правило цепь поставка</t>
+  </si>
+  <si>
+    <t>история возникновение понятие налог налоговый система теоретический основа налогообложение принцип налогообложение тип налоговый система существенный элемент налог характеристика понятие налоговый обязательство возникновение исполнение налоговый обязательство налогоплательщик налоговый агент вид форма налоговый контроль вид налоговый проверка порядок проведение налоговый проверка обжалование действие налоговый орган административный налоговый уголовный ответственность вид ответственность налоговый санкция условие порядок привлечение ответственность налоговый преступление транспортный налог налог имущество налогоплательщик налоговый база ставка налог льгота налог порядок расчет налог налоговый отчетность порядок взимание налог порядок способ уплата налог бюджет налог доход физический лицо место роль налоговый система российский федерация доля налог доход физический лицо структура доход бюджет налогоплательщик доход источник рф доход источник предел рф объект налогообложение объект налогообложение физический лицо являться не являться налоговый резидент рф налоговый база доход не подлежать налогообложение налоговый вычет стандартный социальный имущественный профессиональный налоговый период налоговый ставка порядок определение налоговый база доход налогоплательщик облагать различный ставка порядок определение налоговый база получение доход натуральный форма доход вид материальный выгода договор страхование договор негосударственный пенсионный обеспечение порядок исчисление срок уплата порядок определение дата фактический получение доход особенность исчисление сумма налог индивидуальный предприниматель налоговый декларация порядок представление санкция нарушение установить законодательство порядок уплата налог физический лицо налогоплательщик налоговый база ставка налог льгота налог порядок расчет налог налоговый вычет налоговый отчетность порядок взимание налог порядок способ уплата налог бюджет порядок переход усный налогоплательщик объект налогообложение порядок определение налогооблагаемый база отчетность налог налоговый вычет порядок срок уплата налог бюджет представление отчетность налог налог прибыль место роль налоговый система российский федерация доля налог прибыль организация структура доход бюджет плательщик налог прибыль объект обложение налог прибыль порядок определение доход классификация доход расход группировка расход методика исчисление налоговый база налоговый период налоговый ставка порядок срок уплата налог прибыль налоговый декларация налоговый учет ндс место роль налоговый система российский федерация экономический сущность ндс метод расчет добавить стоимость налогоплательщик объект налогообложение налоговый база перечень товар работа услуга освободить обложение ндс налоговый период налоговый ставка порядок исчисление налог налоговый вычет счет-фактура порядок срок уплата ндс бюджет акциз сущность социально-финансовый последствие акцизный налогообложение российский федерация вид подакцизный товар налогоплательщик порядок формирование объект налогообложение налогооблагаемый база расчет налог территория рф порядок исчисление акциз налоговый вычет особенность налогообложение операция нефтепродукт исчисление акцизный сбор экспортно-импортный операция налог добыча полезный ископаемое роль ндпь система недропользование российский федерация классификация полезный ископаемое налогоплательщик объект налогообложение налоговый база понятие добыть полезный ископаемое порядок определение количество добыть полезный ископаемый оценка стоимость налоговый период налоговый ставка порядок исчисление срок уплата налогоплательщик налоговый база ставка налог порядок расчет налог налоговый отчетность порядок взимание налог порядок способ уплата налог бюджет</t>
+  </si>
+  <si>
+    <t>тема развитие операционный менеджмент область знание предмет практический деятельность базовый терминология понятийный аппарат тема организация производство тема организация планирование производственный процесс время тема метод организация производство тема оперативно-производственный планирование тема инфраструктура предприятие организация</t>
+  </si>
+  <si>
+    <t>состав актив бизнес предприятие подлежать оценка подготовка информация необходимый оценка бизнес понятие рыночный стоимость вид стоимость основной подход метод оценка стоимость предприятие социальный экономический фактор физический условие объект законодательство изменение сфера регулирование рынок россия политический фактор влиять стоимость стандарт оценочный деятельность российский федерация законодательство сфера оценочный деятельность российский федерация требование оценщик договор оказание услуга оценка требование отчет оценка имущество развитие саморегулируемый организация оценочный деятельность стандарт саморегулируемый организация оценщик принцип оценка основа аналитический деятельность оценщик принцип полезность замещение ожидание добавочный продуктивность вклад баланс экономический размер разделение объединение элемент объект право собственность определять роль соотношение спрос предложение принцип зависимость соответствие конкуренция изменение др роль принцип хороший наиболее эффективный использование оценка объект основной подход метод оценка рыночный стоимость бизнес особенность применение метод оценка разный тип имущество финансовый анализ необходимость оценка бизнес оценка контрольный неконтрольный пакет акция премия контроль скидка неконтрольный характер скидка недостаточный ликвидность согласование результат оценка метод дисконтирование денежный поток метод капитализация доход доходный подход отличие метод дисконтированный денежный поток метод капитализация доход таблица сложный процент понятие капитализировать прибыть и выбор понятие порядок определение ставка дисконтирование терминальный капитализация кумулятивный рыночный подход capm wacc метод сделка метод рынок капитал метод отраслевой коэффициент сравнительный подход оценка стоимость предприятие метод сделка метод рынок капитал метод отраслевой коэффициент обоснование сравнительный подход критерий отбор предприятие аналог принцип корректировка важный ценовый мультипликатор формирование итоговый величина стоимость затратный подход метод стоимость чистый актив метод ликвидационный стоимость баланс предприятие корректировка анализ финансовый отчетность актив баланс предприятие вид особенность оценка дебиторский кредиторский задолженность предприятие анализ оценка значение особенность оценка нематериальный актив компания обзор отчет оценщик итоговый заключение оценка стоимость предприятие согласование результат оценка особенность оценка стоимость предприятие конкретный цель</t>
+  </si>
+  <si>
+    <t>определение системный подход определение роль информационный система решение задача финансовый учет анализ предприятие структура состав информационный система финансовый управление классификация информационный система понятие характеристика ппп решение функциональный задача финансовый учет анализ классификация ппп пример задача мочь быть решить использование ппп финансовый учет анализ общий сведение система описание раздел project expert возможность аналитический система описание процесс построение модель определение потребность финансирование разработка стратегия финансирование анализ эффективность проект формирование отчет контроль реализация проект project expert алгоритм ввод общий информация проект настройка параметр расчет отображение данные project expert описание финансово-экономический состояние предприятие момент начало проект описание финансово-экономический среда планироваться реализация проект составление календарный план-график капитальный вложение определение этап работа расчет необходимый ресурс формирование актив предприятие формирование план сбыт производство продукция ввод сведение материал комплектующие составление план персонал расчет издержка подготовка план финансовый деятельность предприятие определение условие привлечение финансовый ресурс порядок обслуживание задолженность определение условие размещение свободный денежный средство использование прибыль предприятие формирование финансовый отчет таблица график отражать результат моделирование деятельность предприятие анализ финансовый показатель проект оценка эффективность инвестиция анализ чувствительность проект устойчивость изменение случайный фактор алгоритм ввод фактический информация ход реализация проект план-фактный анализ показатель проект</t>
+  </si>
+  <si>
+    <t>понятие хранилище данные data warehouse назначение хранилище данные отличие база данные источник данные хранилище основной принцип организация хранилище данные основной процесс работа данные хранилище понятие olap основный цель olap-средство понятие измерение метка факт способ определение факт многомерный модель данные понятие куб поликубический гиперкубический модель данные операция применять куб агрегация детализация формирование срез вращение состав хранилище данные таблица измерение таблица факт типовой структурный схема схема звезда схема снежинка достоинство недостаток многоуровневый структура данные olap сбалансированный несбалансированный неровный иерархия требование предъявлять продукт olap тест fasmi особенность olap-средство встроить настольный приложение особенность сетевой olap-система классификация olap-средство точка зрение способ представление данные хранилище molap rolap holap достоинство недостаток средство класс физический olap виртуальный olap виртуальный хранилище данные достоинство недостаток аналитический пирамида краткий характеристика элемент архитектура хранилище данные оперативный склад данные витрина данные принцип построение источник данные вид витрина преимущество недостаток метаданные if корпоративный информационный фабрика хранилище данные архитектура шина bus гибридный многоуровневый архитектура слоистый архитектура хранилище данные достоинство недостаток архитектура вид типовой структура программный система управление хранилище данные подсистема загрузка данные подсистема представление данные обработка запрос подсистема администрирование хранилище технология etl назначение процесс реализовать etl-система особенность выполнение этап извлечение данные источник особенность выполнение этап преобразование данные перевод значение внешний внутренний обогащение очистка агрегирование данные особенность выполнение этап загрузка данные хранилище уровень управление организация принятие решение пакет прикладной программа уровень управление пакет прикладной программа система обработка транзакция система информационный уровень управленческий система система поддержка принятие решение система поддержка принятие стратегический решение место пакет прикладной программа оперативный анализ данные информационный система предприятие предпроектный обследование предметный область анализ предметный область технический задание экономический обоснование основной вид затрата особенность проектирование хранилище данные реализация внедрение выбор способ представление хранилище этап тестирование основной вид конверсия параллельный стратегия стратегия прямой переключение пилотный фазовый стратегия особенность эксплуатация модификация основной модель жизненный цикл каскадный спиральный модель корпоративный модель данные особенность спиральный подход построение корпоративный модель данные выбор типовой структурный схема корпоративный хранилище данные метод разработка модель корпоративный хранилище данные помощь реконструкция основа шаблон разработка заказ уровень архитектура хранилище данные больший данные уровень получение данные интегрировать ядро уровень доступ уровень использование модель данные data vault основной особенность основной компонент hub link satellite особенность организация работа данные основа методология data vault промежуточный область staging area раздел raw data vault business vault основной особенность case-технология возможность современный case-средство классификация case-средство тип категория вспомогательный тип понятие проект хранилище данные таблица измерение таблица факт типовой структурный схема звезда снежинка понятие процесс хранилище данные deductor studio основной понятие deductor warehouse семантический слой измерение ссылка атрибут структура программный окно deductor studio панель управление область визуализатор подключение сценарий основной компонент deductor studio мастер подключение импорт экспорт обработка визуализация последовательность работа создание типовой структура хранилище данные формирование метаданные создание сценарий подготовка исходный данные импорт данные очистка данные фильтрация выявление дубликат противоречие обнаружение редактирование аномалия сглаживание загрузка импортировать данные хранилище данные очистка процесс измерение удаление измерение процесс хранилище добавление атрибут факт измерение процесс создание сценарий импорт измерение формирование таблица куб срез назначение вид визуализатор возможность использование создание сценарий импорт процесс формирование таблица куб создание куб хранилище данные импорт куб хранилище данные построение срез отличие куб хранилище данные сценарий использование кросс-диаграмма кросс-таблица настройка кросс-таблица куба фильтрация таблица куба преобразование дата время настройка набор данные разбиение область значение непрерывный числовой параметр интервал квантование замена данные добавление поле значение вычисляться значение другой поле объединение слияние данные проверка сезонность подготовка данные построение модель построение пользовательский модель использование прогнозирование построение модель линейный регрессия использование прогнозирование построение модель нейронный сеть использование прогнозирование ассоциативный правило параметр характеризовать ассоциативный правило поддержка достоверность лифт настройка параметр поиск ассоциативный правило поиск ассоциативный правило визуализатор использовать оперативный анализ ассоциативный правило правило популярный набор что-если дерево правило интерпретация ассоциативный правило скрипт определение термин настройка скрипт использование сценарий ранее создать ветвь обработка данные использование ранее создать модель анализ новый данные прогнозирование помощь скрипт</t>
+  </si>
+  <si>
+    <t>тема традиционный модель рациональный поведение исток поведенческий экономика тема теория перспектива тема причина ошибка принятие решение тема эвристика суждение тема поведенческий эффект тема влияние поведение человек концепция nudge тема грамотный потребитель финансовый услуга</t>
+  </si>
+  <si>
+    <t>тема введение дисциплина портфельный инвестиция тема долевые ценный бумага объект портфельный инвестирование тема облигация объект портфельный инвестирование тема финансовый вычисление рынок ценный бумага тема производный финансовый инструмент тема инвестор рынок ценный бумага тема формирование оценка риск портфель ценный бумага тема профессиональный деятельность рынок ценный бумага тема основа анализ ценный бумага</t>
+  </si>
+  <si>
+    <t>причина возникновение государство особый форма организация общество социальный механизм обеспечивать согласование дело специальный интерес группа слой гражданский общество признак государство особый публичный государственный власть осуществление власть особый аппарат территориальный организация население налог заем законодательство государственный суверенитет функция государство внутренний охранительный регулятивный функция внешний функция государство форма правление парламентарный президентский республика монархия вид особенность форма государственный устройство федеративные унитарный государство конфедерация право совокупность правило поведение исходить государство обеспечение право мера равенство справедливость согласование воля общество гражданин взаимодействие право государство общий характеристика законодательный исполнительный судебный ветвь государственный власть система сдержка противовес принцип основной начало положить основа организация деятельность орган государство верховенство закон принцип децентрализация власть принцип разделение власть разделение государственный орган законодательный исполнительный судебный орган власть рф государственный орган субъект рф президент гарант охрана независимость государство целостность территория рф соблюдение право свобода человек гражданин согласовать функционирование орган государственный власть порядок выбор прекращение полномочие президент рф компетенция президент рф федеральный собрание рф представительный законодательный орган рф порядок формирование совет федерация выбор депутат государственный дума палата федеральный собрание полномочие совет федерация государственный дума порядок рассмотрение принятие обнародование закон порядок формирование состав правительство основной направление деятельность сфера управление экономика сфера социальный политика сфера обеспечение законность право свобода гражданин конституционный принцип осуществление судебный власть осуществление правосудие только суд законность гласность судебный разбирательство презумпция невиновность коллегиальность состязательность равноправие сторона независимость судья подчинение только конституция рф федеральный закон конституционный суд рф порядок формирование полномочие верховный суд рф порядок формирование полномочие система суд общий юрисдикция арбитражный суд основной направление деятельность прокуратура полномочие прокуратура адвокатура принцип форма оказание юридический помощь министерство внутренний дело рф орган полномочие орган полиция право совокупность правило поведение исходить государство обеспечение право мера равенство справедливость согласование воля общество гражданин взаимодействие право государство норма право общеобязательный формально-определенный установить общество государство правило поведение наделять участник общественный отношение право обязанность обеспечиваемое охранять нарушение государство структура правовой норма гипотеза диспозиция санкция вид правовой норма регулятивный управомочивающий обязывать запрещать охранительный понятие источник право вид источник право письменный правовой акт нормативный акт правовой обычай судебный прецедент нормативный договор деление нормативный акт закон подзаконный акт закон нормативный акт обладать высокий юридический сила принять представительный орган государственный власть вид закон конституция основной закон рф федеральный конституционный закон федеральный закон закон принимать законодательный орган субъект рф признак конституция верховенство система право высокий юридический сила первичность норма конституция отношение правовой акт понятие правовой отношение конкретизированной юридический связь участник субъект общественный отношение урегулированного норма право объект сторона содержание правоотношение возникновение изменение прекращение правовой отношение юридический факт событие действие закон связывать наступление юридический последствие понятие правонарушение признак правонарушение причинение вред интерес личность общество государство противоправность деяние дееспособный вменять лицо наличие вина состав правонарушение объект правонарушение общественный отношение регулировать охранять право объективный сторона правонарушение деяние направить определенный объект причинный связь противоправный деяние общественно-вредный последствие субъект правонарушение субъективный сторона правонарушение вино форма прямой умысел косвенный умысел неосторожность форма легкомыслие небрежность мотив цель правонарушение вид правонарушение административный дисциплинарный проступок гражданский правонарушение уголовный преступление понятие юридический ответственность признак юридический ответственность юридический ответственность предполагать государственный принуждение связь юридический ответственность правонарушение ответственность влечь негативный последствие правонарушитель основание возникновение юридический ответственность факт совершение правонарушение вид юридический ответственность дисциплинарный материальный ответственность трудовой право административный ответственность вид административный принуждение уголовный ответственность исходящий имя государство воздействие гражданин вид определенный лишение личный имущественный характер понятие признак вид субъект объект гражданский право понятие сделка форма вид сделка недействительный сделка обязательство понятие общий характеристика договорный внедоговорный обязательство брак порядок заключение прекращение основный право обязанность супруг трудовой договор понятие признак вид сторона порядок заключение изменение прекращение трудовой договор основной институт административный право характеристика источник административный право административный правонарушение административный ответственность преступление понятие признак вид состав преступление значение характеристика элемент наказание понятие цель система наказание отдельный вид наказание гражданский процесс вид судебный производство понятие признак лицо участвовать дело основной право обязанность доказательство арбитражный процесс вид судебный производство понятие признак лицо участвовать дело основной право обязанность доказательство уголовный процесс досудебный судебный производство понятие вид участник уголовный судопроизводство право обязанность</t>
+  </si>
+  <si>
+    <t>статистика человек пространство количественный информация мир растение биотехнология общество атмосфера климат погода финансовый математика чайник разработка web-приложение мультимедийный сервис современный исследователь радиофизика игровой решение образование введение социально-политический мир культурный антропология экономико-географический картина мир активный процесс современный русский язык миф ритуал третий тысячелетие число дополнительный практикум иностранный студент деловой риторика новый коммуникативный грамотность морфология искусство живопись метод творческий интерпретация метаморфоза овидий европейский искусство дизайн-проектирование организация креативный работа мир текст текст мир число дополнительный практикум иностранный студент русский язык иностранный творческий практика введение проблематика мастерская совместный постановка проблема 1.3 предпроектный анализ работа теоретический материал выдвижение замысел проект исследование разработка карта проблема 2.1 работа проблематика мастерская т ч использование технология программный продукт лабораторный база тема планирование проектный деятельность согласование требование результат выдвижение замысел исследование гипотеза распределение роль команда работа теоретический материал описание гипотеза исследование составление перечень необходимый работа процедура составление план работа 3.1 работа проблематика мастерская т ч использование технология программный продукт лабораторный база мониторинг проведение исследование результат индивидуальный исследование уточнение план исследование 3.3 мониторинг проведение исследование промежуточный результат групповой работа уточнение план завершение проект 3.4 работа теоретический материал разработка проектный решение обсуждение результат группа оформление результат проект 4.1 презентация проект анализ результат взаимный рецензирование выбор хороший проект</t>
+  </si>
+  <si>
+    <t>тема предприниматель предпринимательский деятельность предмет задача курс предприниматель предпринимательский активность основной концепция деловой среда структура отечественный предпринимательство ретроспектива современный статус экономический инструментарий предпринимательский деятельность тема предприятие хозяйствовать субъект предприятие понятие концепция коммерческий некоммерческий организация вид организационно-правовой форма предприятие характеристика учредительный документ организация понятие агентский отношение роль функционирование предприятие различный организационно-правовой форма понятие малый предприятие учет налогообложение малый бизнес форма прекращение деятельность организация прекращение деятельность деталь теоретический концепция порядок регистрация ликвидация коммерческий организация предпринимательский экосистема тема концепция бизнес деловой проектирование концепция бизнес стадия деловой проектирование бизнес-идея метод генерация оценка документирование оценка важность потребитель отдельный характеристика продукт понятие назначение бизнес-модель структура содержание цп утп портрет потребитель целевой аудитория сегментация рынок метод ценообразование оптимизация цена продукт емкость рынок продукт метод оценка бизнес процесс компания понятие описание расход компания вид метод оценка оценка экономический целесообразность организация бизнес содержание порядок документальный оформление формирование команда бизнес-проект подход метод презентация проект вид назначение особенность структура тактика организация</t>
+  </si>
+  <si>
+    <t>тема предмет региональный экономика управление понятие типологизация регион тема теоретический основа региональный экономика тема регион объект хозяйствование управление тема природно-ресурсный потенциал регион распределение экономический деятельность пространство тема регион объект макроэкономический анализ</t>
+  </si>
+  <si>
+    <t>неопределенность риск определение риск качественный количественный понимание риск особенность проявление риск практика классификация риск теория риск развитие подход оценка риск связь риск доходность основной метод управление риск международный стандарт управление риск культура управление риск организация формализация условие ситуация риск измерение риск проблема сравнение альтернатива отношение риск графический представление рисковой предпочтение функция рисковой предпочтение критерий оценка рисковой решение выбор хороший решение условие риск основа метод дерево решение анализ чувствительность метод оценка устойчивость инвестиционный проект основной мера риск инвестиционный проект поправка риск коэффициент дисконтирование оценка риск инвестиционный проект основа дерево событие сценарный подход анализ риск использование дерево решение оценка риск инвестиционный проект имитационный моделирование инвестиционный аналитика управление риск инвестиционный проект риск инвестиция облигация цена доходность облигация временной структура процентный ставка кривая доходность чувствительность цена облигация параллельный сдвиг кривой доходность показатель рыночный риск облигация модифицировать дюрация выпуклость хеджирование портфель облигация иммунизация ожидать доходность риск портфель ценный бумага диверсификация риск портфель марковица эффективный граница роль короткий продажа формирование эффективный портфель оптимизация тобин касательный портфель бета-коэффициент премия риск оценка риск актив основа модель шарп концепция риск модель capm sml atr применимость современный экономический теория практика капитал риск var основный метод расчет var рыночный данные исторический моделирование параметрический var расчет var метод монте-карло верификация модель расчет var исторический данные backtesting</t>
+  </si>
+  <si>
+    <t>стратегический менеджмент самостоятельный исследовательский область управленческий практика существовать подход стратегический управление этап развитие стратегический менеджмент эволюция парадигм управление связь стратегический менеджмент стратегия различие стратегический оперативный управление стратегический мышление эффективный стратегический менеджмент ключевой элемент концепция стратегический управление современный условие индустрия стратегический управление нестабильность внешний среда деятельность компания стратегический установка стратегический видение параметр стратегический видение преимущество стратегический альтернатива ценность миссия компания формулирование миссия причина рекомендация ключевой цель задача организация особенность стратегический цель постановка цель smart стратегия компания миф стратегия природа стратегический решение запрограммированные незапрограммировать решение стратегический анализ стратегический выбор реализация стратегия ключевой этап стратегический управление стратегический анализ понятие компонент цель задача ожидание полномочие анализ внешний обстановка анализ внутренний ресурс стратегический выбор понятие компонент выработка вариант стратегия оценка вариант стратегия выбор стратегия стратегический линия поведение план реализация стратегия понятие проблема мероприятие разработка вариант действие непредвиденный обстоятельство разработка организационный структура выбор система управление организация политика организация выбор организационный объединение система контроль стратегия компания пирамида разработка стратегия диверсифицировать компания корпоративный стратегия бизнес-стратегия функциональный стратегия операционный стратегия пирамида разработка стратегия однопрофильный компания консолидация усилие выработка стратегия критерий успешный стратегия роль изменение стратегический управление вид стратегический изменение модель стратегический изменение стадия реализация стратегирование сущность преимущество недостаток модель стратегирование микро- макросреда компания роль анализ внешний среда bani-мир лидерство вызов bani-мир влияние стратегический решение бизнес-структура pestle-анализ количественный качественный оценка отраслевой анализ определение доминировать отрасль экономический характеристика внеотраслевые возможность бизнес-струткур сегодня деятельность экосистема структурный анализ конкурентный окружение модель конкуренция м портер угроза проникновение рынок потенциальный конкурент власть покупатель власть поставщик угроза сторона заменитель товар услуга уровень конкурентный борьба традиционный конкурент продуктовый географический граница товарный рынок барьер вход рынок экономический административный ограничение стратегия поведение компания направление создание барьер вход рынок наличие действовать рынок хозяйствовать субъект вертикально-интегрированный компания рыночный власть анализ затрата конкурент выявление стратегический фактор управлять затрата анализ затрата моделирование затрата конкурент карта стратегический группа общий конкурентный стратег лидерство затрата индивидуализация дифференциация фокусирование ключевой фактор успех ключевой элемент внутренний среда цель задача структура организация финансовый ресурс трудовой ресурс производственный деятельность сбыт исследование разработка система процедура информационный обеспечение необходимый исследование внутренний фактор использование управленческий учет анализ ключевой компетенция конкурентный преимущество компания ключевой фактор успех устойчивый конкурентный преимущество этап процесс оценка преимущество недостаток результативность использование ресурс snw-анализ анализ гибкость навык модель формирование стоимость м портер vrio-анализ необходимость проведение ситуационный анализ рамка стратегический управление оценка применять стратегия gap-анализ swot-анализ идентификация стратегический поход выработка дальнейший действие метод экспертный оценка определение наиболее выгодный стратегический положение space-модель адаптация использование хороший опыт деятельность компания бенчмаркинг выявление новый тренд прогнозирование востребованность конечный потребитель будущее концепция заинтересованный сторона существовать определение заинтересованный сторона выявление заинтересованный сторона составление карта заинтересованный сторона карта отношение список с анализ заинтересованный сторона цель матрица власть интерес менделоу джонсон матрица власть интерес прайс карта заинтересованный сторона скоулза управление заинтересованный сторона уровень разработка стратегия базовый базисный эталонный стратегия конкурентный стратегия стратегия слияние поглощение международный стратегия стратегический хозяйственный зона стратегический ошибка фактор влиять выбор стратегия внутренний рост вид стратегия внутренний рост концентрация развитие рынок разработка обновление продукт диверсификация стратегия внутренний рост понятие преимущество недостаток применение российский компания фактор влиять выбор стратегия внешний рост диверсификация концентрический конгломератный интеграция горизонтальный вертикальный стратегия внешний рост понятие преимущество недостаток применение российский компания фактор влиять принятие решение международный стратегия трудность реализация данный стратегия направление международный стратегический развитие международный стратегия финансовый планирование корпоративный стратегия слияние приобретение определение мотив форма сопротивление приобретение разделение компания использование матричный анализ матрица бостонский консалтинговый группа бкг матрица привлекательность отрасль конкурентоспособность матрица generalelectric ge mckinsey матрица продукт рынок и ансоффа признак дисбаланс устойчивый развитие стратегия вход рынок стратегия уход рынок создание портфель выбор оптимальногопортфель корректировка стратегия стратегия голубой океан цифровой диджитал стратегия стратегия область устойчивый развитие корпоративный социальный ответственность климатический стратегия стратегия обдуманный срочный стратегия стратегия действие</t>
+  </si>
+  <si>
+    <t>основный понятие операция событие вид случайный событие свойство операция событие классический определение вероятность свойство вероятность элемент комбинаторика геометрический вероятность условный вероятность независимость событие теорема сложение умножение вероятность полный группа событие формула полный вероятность гипотеза формула байес аксиоматический построение теория вероятность последовательность независимый испытание определение схема бернулли пример испытание бернулли формула бернулли наивероятный число наступление событие формула пуассон локальный формула муавр-лаплас интегральный формула муавр-лаплас определение случайный величина тип случайный величина закон распределение случайный величина ряд распределение дискретный случайный величина функция распределение свойство функция распределение плотность вероятность непрерывный случайный величина свойство плотность вероятность математический ожидание случайный величина свойство математический ожидание дисперсия случайный величина свойство дисперсия средний квадратический отклонение случайный величина мода медиана момент случайный величина квантиль уровень p случайный величина биномиальный закон распределение математический ожидание дисперсия случайный величина распределить биномиальный закон закон распределение пуассон математический ожидание дисперсия случайный величина распределить закон пуассон геометрический распределение математический ожидание дисперсия случайный величина иметь геометрический распределение гипергеометрический распределение математический ожидание дисперсия случайный величина иметь гипергеометрический распределение равномерный закон распределение показательный экспоненциальный закон распределение нормальный закон распределение понятие система случайный величина тип двумерный случайный величина закон распределение вероятность двумерный случайный величина функция распределение двумерный случайный величина свойство понятие плотность вероятность двумерный непрерывный случайный величина свойство плотность вероятность двумерный непрерывный случайный величина равномерный распределение двумерный непрерывный случайный величина понятие условный закон распределение условный закон распределение составлять двумерный дискретный случайный величина условный закон распределение составлять двумерный непрерывный случайный величина математический ожидание двумерный случайный величина дисперсия двумерный случайный величина ковариация коэффициент корреляция случайный величина понятие двумерный нормальный закон распределение вероятностный смысл параметр двумерный нормальный закон закон распределение составлять случайный величина распределить двумерный нормальный закон условный математический ожидание регрессия лемма чебышев неравенство чебышев теорема чебышев теорема бернулли центральный предельный теорема понятие функция случайный величина функция дискретный случайный величина функция непрерывный случайный величина числовой характеристика функция случайный величина закон распределение функция случайный величина распределение сумма непрерывный случайный величина распределение произведение непрерывный случайный величина понятие случайный функция понятие случайный процесс задание случайный процесс одномерный n-я мерный функция распределение случайный процесс классификация случайный процесс математический ожидание случайный процесс свойство математический ожидание случайный процесс дисперсия случайный процесс свойство дисперсия случайный процесс корреляционный функция случайный процесс свойство корреляционный функция случайный процесс предел случайный процесс свойство предел среднеквадратичный производная случайный процесс интеграл случайный процесс понятие цепь марков граф состояние цепь марков дискретный время цепь марков непрерывный время однородный цепь марков матрица переход система</t>
+  </si>
+  <si>
+    <t>основной понятие теория игра игра математический модель конфликт понятие игрок ход игрок чистый стратегия игровой ситуация функция выигрыш классификация игра классификация число участник парный множественный число стратегия конечный бесконечный возможность кооперация коалиционный бескоалиционный степень информированность участник игра полный информация игра совершенный информация форма представление игра игра нормальный форма стратегический статический биматричные игра игра развернуть форма динамический игра многошаговый игра дерево игра понятие информационный множество приведение игра развернуть форма игра нормальный форма понятие решение игра основной принцип определять решение игра решение игра равновесный ситуация принцип рациональность осторожность уравновешенность вид игровой равновесие равновесие доминирующий стратегия равновесие нэш равновесие защитный осторожный максиминный стратегия понятие доминируемость игровывый ситуация множество парето оптимальность парето равновесие штакельберг равновесие дрожать рука антагонистические игра платежный матрица игра седловой точка платежный матрица значение цена игра смешанный стратегия теорема нейман теорема минимакс биматричный игра решение игра сведение конечный биматричный игра задача линейный программирование экономический приложение стратегический игра полный информация дуополия курно олигополия курно дуополия бертран однородный продукция дуополия бертран неоднородный продукция конфликт распределение общий благо стратегический игра сеть парадокс браэсс равновесие вардроп эгоистичный маршрутизация арбитражный механизм разрешение конфликт динамический игра полный совершенный информация модель дуополия штакельберг модель последовательный торговый сделка рубинштейн трехэтапный торговля многоэтапный торговля последовательный игра полный несовершенный информация модифицированный модель штакельберг развернуть форма представление игра совершенный подыгровый равновесие нэш последовательный игра участие природа многократно повторять игра двукратно повторять игра бесконечно повторять игра стратегия переключение достижимый платеж достижимый платеж теорема фридман предельный парето-оптимальные профиль стратегия экономический приложение повторять игра модель дуополия курно бесконечный число раз повторять игра байесовские игра нормальный форма представление статический байесовский игра равновесие байес-нэш модель штакельберг асимметричный информация аукцион закрытый аукцион первый цена симметрический стратегия формат аукцион слабый секвенциальный равновесие понятие вера игрок понятие последовательный рациональность траектория равновесие сигнальный игра действие игрок сигнал динамический сценарий сигнальный игра отправитель получатель совершенный байесовский равновесие сигнальный игра игра неполный несовершенный информация основной понятие определение коалиция характеристический функция игра супераддитивность дележ свойство понятие дележ условие индивидуальный рациональность условие групповой рациональность доминируемость дележ решение игра форма характеристический функция с-ядро н-м-решение вектор шепать</t>
+  </si>
+  <si>
+    <t>назначение основной понятие теория экономический механизм дизайн экономический механизм функция согласие общественный выбор принцип выявление предпочтение нэш-реализуемость механизм механизм оптимальный парето тип агент теорема эрроу аукцион дизайн аукцион</t>
+  </si>
+  <si>
+    <t>тема современный концепция управление проект тема организация проект тема планирование проект тема руководство управление исполнение проект тема ценность принцип гибкий подход agile управление проект</t>
+  </si>
+  <si>
+    <t>физический культура спорт социальный феномен современный общество средство физический культура основной составлять физический культура социальный функция физический культура формирование физический культура личность физический культура структура профессиональный образование организационно правовой основа физический культура спорт студенческий молодежь россия воздействие социально-экологический природно-климатический фактор бытовой условие жизнь физический развитие жизнедеятельность человек организм человек единый саморазвивающийся биологический система анатомо-морфологический строение основной физиологический функция организм обеспечивать двигательный активность физический развитие человек роль отдельный система организм обеспечение физический развитие функциональный двигательный возможность организм человек двигательный активность влияние устойчивость адаптационный возможность человек умственный физический нагрузка различный воздействие внешний среда степень условие влияние наследственность физический развитие и жизнедеятельность человек обучение процесс физический воспитание обеспечивать сторона физический образование содержание являться системный освоение человек рациональный способ управление движение приобретение необходимый жизнь фонд двигательный умение навык знание основный принцип методика обучение воспитание методический принцип основный специфический средство физический воспитание физический упражнение вспомогательный средство оздоровительный сила природа гигиенический фактор общепедагогические применять случай обучение воспитание специфический характерный только физический воспитание метод основа обучение движение оптимальный развитие физический качество сила быстрота выносливость гибкость ловкость общий психофизиологический характеристика интеллектуальный деятельность учебный труд студент общий закономерность динамика работоспособность студент учебный год основной фактор определять признак критерий нервно-эмоциональный психофизический утомление регулирование работоспособность профилактика утомление студент отдельный период учебный год оптимизация сопрячь деятельность студент учеба спортивный совершенствование вид диагностика регулярный занятие физический упражнение спорт врачебный педагогический контроль самоконтроль основной метод показатель дневник самоконтроль использование отдельный метод контроль регулярный занятие физический упражнение спорт коррекция содержание методика занятие результат показатель контроль понятие двигательный навык двигательный умение обучение процесс физический воспитание обеспечивать сторона физический образование содержание являться системный освоение человек рациональный способ управление движение приобретение необходимый жизнь фонд двигательный умение навык связать знание этап обучение двигательный действие совершенствование двигательный действие определение понятие работоспособность утомление усталость прямой косвенный показатель работоспособность субъективный объективный признак утомление метод оценка работоспособность человек учет субъективный функциональный состояние прямой косвенный показатель работоспособность рекомендация применение средство физический культура направить коррекция работоспособность усталость утомление понятие здоровье физический развитие антропометрический измерение понятие вид показатель метод антропометрический стандарт метод индекс метод оценка физический развитие общий представление функциональный состояние организм методика оценка функциональный состояние сердечно-сосудистый система помощь функциональный проба методика оценка функциональный состояние дыхательный система понятие осанка вид осанка определение правильность осанка основной причина нарушение осанка основной правило сохранение исправление дефект осанка методика коррекция осанка комплекс упражнение исправление осанка методика коррекция телосложение общий представление саморегуляция психоэмоциональный состояние прием регуляция эмоциональный состояние преднамеренный задержка проявление изменение выразительный движение специальный двигательный упражнение индивидуализировать разминка специальный вид массаж самомассаж дыхательный упражнение прием основать регуляция эмоция воздействие различный анализатор аутогенный тренировка регулировать музыкальный воздействие психомышечный тренировка рекомендация использование простой метод саморегуляция основной физический качество сила быстрота гибкость выносливость координационный способность методика развитие сила методика развитие быстрота методика развитие гибкость методика развитие выносливость методика развитие ловкость понятие физический самовоспитание основной этап процесс физический самовоспитание методика оценка уровень физический подготовленность методика составление индивидуальный тренировочный программа рекреационный направленность использование средство физический культура восстановительный направленность использование средство физический культура цель направленность форма самостоятельный занятие методика проведение простой самостоятельный занятие физический упражнение гигиенический направленность методика проведение самостоятельный занятие тренировочный направленность ходьба оздоровительный бег занятие лыжный спорт плавание определение понятие массаж самомассаж основной прием различный вид массаж косметический спортивный лечебный гигиенический форма массаж самомассаж общий частный местный методический основа самомассаж причина возникновение миопия коррегирующий гимнастика глаз комплекс специальный упражнение коррекция зрение комплекс общеразвивать упражнение сочетание движение глаз комплекс специальный упражнение элемент спортивный игра перечень упражнение включать физкультурный пауза рабочий место ощущение усталость глаз тяжесть голова специальный гимнастика глаз у бейтс пальминг здоровье человек ценность фактор определять влияние образ жизнь здоровье здоровый образ жизнь составлять основный требование организация здоровый образ жизнь роль возможность физический культура обеспечение здоровье физический самовоспитание самосовершенствование здоровый образ жизнь критерий эффективность здоровый образ жизнь личный отношение здоровье общий культура условие формирование здоровый образ жизнь физиологический механизм закономерность совершенствование отдельный функциональный система организм целое воздействие направить физический нагрузка тренировка физиологический основа освоение совершенствование двигательный действие физиологический механизм использование средство физический культура спорт активный отдых восстановление работоспособность основа биомеханика естественный локомоция ходьба бег прыжок методический принцип физический воспитание основа этап обучение движение развитие физический качество формирование психический качество процесс физический воспитание общий физический подготовка цель задача зона интенсивность энергозатраты различный физический нагрузка значение мышечный релаксация занятие физический упражнение возможность условие коррекция общий физический развитие телосложение двигательный функциональный подготовленность средство физический культура спорт специальный физический подготовка цель задача спортивный подготовка структура подготовленность спортсмен профессионально-прикладной физический подготовка составлять специальный подготовка форма занятие физический упражнение массовый спорт спорт высокий достижение цель задача спортивный соревнование средство метод общий специальный физический подготовка студент спортивный классификация система студенческий спортивный соревнование внутривузовский межвузовский всероссийский международный индивидуальный выбор студент вид спорт система физический упражнение регулярный занятие мотивация обоснование краткий психофизиологический характеристика основный группа вид спорт система физический упражнение мотивация целенаправленность самостоятельный занятие форма структура содержание планирование организация управление самостоятельный занятие различный направленность взаимосвязь интенсивность нагрузка уровень физический подготовленность самоконтроль эффективность самостоятельный занятие особенность самостоятельный занятие направить активный отдых коррекция физический развитие телосложение акцентировать развитие отдельный физический качество личный социально-экономический необходимость психофизический подготовка человек труд определение понятие ппфп цель задача средство место ппфп система подготовка будущий бакалавр фактор определять конкретный содержание ппфп методика подбор средство ппфп организация форма проведение контроль эффективность ппфп студент основный дополнительный фактор оказывать влияние содержание ппфп избрать профессия основный содержание ппфп будущий бакалавр дипломированный специалист основной понятие спортивный подготовка общий специальный физический подготовка оценка специальный физический подготовленность оценка технический подготовленность оценка тактический подготовленность оценка психологический состояние методика самоконтроль уровень развитие физический качество понятие релаксация специальный прием позволять освоить техника релаксация динамический упражнение снятие напряжение мышца расслабление комплекс упражнение расслабление мышца методика подбор средство профессионально-прикладной физический подготовка методика развитие профессионально важный физический качество способность дозировать силовой напряжение развитие статический выносливость устойчивость гиподинамия тренировка сенсомоторный реакция специальный упражнение равновесие улучшение функция вестибулярный анализатор упражнение внимание развитие оперативный мышление тренировка эмоциональный устойчивость производственный физический культура производственный гимнастика особенность выбор форма метод средство физический культура спорт рабочий свободный время профилактика профессиональный заболевание средство физический культура дополнительный средство повышение общий профессиональный работоспособность влияние индивидуальный особенность самостоятельный занятие физический культура</t>
+  </si>
+  <si>
+    <t>мировоззрение картина мир философия философия мировоззрение рефлексивный деятельность основной проблемный раздел философия онтология гносеология антропо-аксиология онтология философия бытие основной проблема категория существовать почему существовать не как существовать тип бытие материальный мир физический реальность этап становление онтология мочь знать познание субъект объект познание форма познание истина заблуждение концепция истина взгляд познание история философия специфика научный познание научный революция смена тип рациональность метод научный мышление норма идеал научный познание техника заниматься философия техника техногенный цивилизация глобальный феномен техника философский антропология человек каков природа человек определять человек сущность существование быть ли смысл человеческий существование быть ли человек свобода категория философский антропология ценность многообразие интерпретация система иерархия ценность личность средоточие ценность этика должный делать свобода воля нравственный выбор проблема основание добро зло искусство художественный реальность художественный сознание художественный деятельность мимезис эстетика опыт восприятие суждение вкус эстетический отношение мир отличие познавательный нравственный отношение эстетический установка критерий ценностный ориентация</t>
+  </si>
+  <si>
+    <t>финансы финансовый отношение централизованный децентрализованный финансы принцип функция финансы финансовый ресурс понятие финансовый система уровень тип функция элемент финансовый система государство институциональный структура финансовый система мир рф сущность цель объект механизм форма вид уровень управление финансы финансовый регулирование прогнозирование контроль финансовый политика сущность задача тип направление метод финансовый политика рф сущность роль финансовый система функция вид элемент финансовый рынок инструмент финансовый рынок объект торговля инвестирование характеристика сегмент участник институт финансовый рынок сущность принцип функция финансы организация предприятие денежный хозяйство предприятие структура оборотный капитал предприятие источник воспроизводство расход доход прибыль организация предприятие сущность принцип функция финансы домохозяйство баланс доход расход домохозяйство финансовый планирование</t>
+  </si>
+  <si>
+    <t>концепция временной стоимость деньга простой сложный процент m-разовое начисление процент эквивалентный ставка эффективный ставка непрерывный процент дисконтирование банковский учет сравнение денежный сумма расчет условие инфляция определение поток платеж финансовый рента обобщающие характеристика поток платеж обычный постоянный годовой рента начисление процент раз год обычный постоянный годовой рента начисление процент m раз год обычный постоянный p-срочная рента начисление процент раз год обычный постоянный p-срочная рента начисление процент m раз год рента кусочно-постоянный платеж рента изменение выплата закон арифметический геометрический прогрессия рента пренумерандо отложить рента вечный рента непрерывный рента определение параметр финансовый рента размер платеж срок процентный ставка изменение условие финансовый контракт принцип финансовый эквивалентность обязательство уравнение эквивалентность конверсия рента выкуп рента рассрочка платеж замена поток платеж другой объединение рента баланс финансово-кредитный операция метод погашение долг погашение основный долг срок погашение основный долг равный платеж погашение долг равный срочный уплата погашение потребительский кредит понятие полный доходность финансово-кредитный операция расчет эффективный ставка кредит простой случай кредитный операция удержание комиссионный случай дифференцированный аннуитетный погасительный платеж эффективный ставка потребительский кредит задача реструктуризация долг денежный поток инвестиционный проект дисконтный метод анализ выбор ставка дисконтирование основной критерий экономический эффективность инвестиционный проект чистый привести доход внутренний норма доходность срок окупаемость индекс рентабельность преимущество недостаток сравнение альтернативный инвестиционный проект формирование портфель инвестиционный проект анализ инвестиция ценный бумага фиксированный доход облигация базовый модель оценивание облигация доходность погашение выявление неверно оценить рынок ценный бумага расчет внутренний стоимость доходность погашение разный вид облигация облигация нулевой купон облигация выплата купон момент погашение облигация обязательный погашение облигация периодический выплата купон погашение конец срок средний срок дюрация облигация оценка риск инвестиция облигация ценовый чувствительность облигация дюрация мера процентный риск оценка относительный изменение цена облигация дюрация выпуклость портфель облигация детерминированный модель анализ рискованный ценный бумага акция внутренний стоимость внутренний доходность акция модель нулевой рост дивиденд модель гордон модель переменный рост дивиденд оценивание акция учет конечный срок владение</t>
+  </si>
+  <si>
+    <t>понятие цель задача предмет организация финансовый менеджмент предприятие стратегия тактика финансовый менеджмент сущность структура финансовый менеджмент современный постановка глобальный цель предприятие рычаг леверидж управление предприятие финансовый леверидж эффект финансовый рычаг американский европейский концепция сила воздействие финансовый рычаг финансовый риск финансовый леверидж формирование рациональный структура заимствование расчет среднесрочный ставка процент финансовый условие кредитование операционный производственный леверидж эффект сопрячь рычаг эффект операционный рычаг количественный оценка уровень предпринимательский риск генерировать предприятие пороговый выручка прием расчет точка безубыточность аналитический графический метод определение точка безубыточность практический использование принятие управленческий решение валовый маржа запас финансовый прочность практический использование операционный анализ управление оценка текущий финансовый положение предприятие актив ликвидность прогнозирование финансовый устойчивость предприятие чистый оборотный капитал текущий финансовый потребность предприятие системный переменный часть оборотный капитал цель управление оборотный капитал левосторонний правосторонний риск формирование оптимальный структура оборотный капитал управление структура затрата регулирование масса динамика прибыль политика управление текущий актив текущий пассив матрица выбор тип политика управление текущий актив текущий пассив прогнозирование денежный поток расчет потребность краткосрочный финансирование разработка бюджет денежный средство классический способ преодоление локальный денежный дефицит учет вексель факторинг форфейтинг опосредовать финансирование определение оптимальный уровень денежный средство модель баумоль миллера-орра управление денежный средство главный парадокс дилемма финансовый менеджмент оптимизация источник финансирование предприятие источник структура средство предприятие система противоречие интерес руководитель кредитор акционер определение способ внешний финансирование самофинансирование развитие предприятие структура капитал предприятие рационализация оценка стоимость использование разный источник финансирование рыночный цена предприятие цена капитал выбор инвестиционный проект основа определение цена капитал предельный цена капитал оптимальный структура капитал тема финансовый политика предприятие содержание финансовый политика предприятие дивидендный политика фирма теория дивидендный политика основной цель дивидендный политика предприятие тип политика дивидендный политика политика развитие предприятие метод выплата дивиденд преимущество недостаток метод выплата дивиденд политика развитие предприятие устойчивый темп рост концепция повысить занизить темп рост модель поведение ассортиментный политик предприятие финансовый цель разный фаза жизненный цикл товар тема лабораторный практикум учебный план курс финансовый менеджмент практический занятие программа курс предполагать проведение компьютерный практикум проведение практикум использоваться компьютерный имитационный модель отра¬жать ограничить количество структурный элемент внешний связь виртуальный предприятие позволять не менее достаточно полно воспро¬извести основной процесс управление предприятие также внешний условие предприятие осуществлять деятельность методический рекомендация принятие решение деловой игра изложить методический пособие стратегия тактика управление бизнес условие конкуренция пособие разместить сайт научный библиотека ни тгу также иметься раздаточный материал</t>
+  </si>
+  <si>
+    <t>понятие финансовый бухгалтерский учет цель финансовый учет пользователь финансовый информация гармонизация российский учет международный стандарт международный стандарт учет финансовый отчетность реформирование система бухгалтерский учет российский федерация основной принцип допущение учетный политика российский федерация допущение временной определенность факт хозяйственный деятельность допущение последовательность применение учетный политика требование учетный политика финансовый бухгалтерский отчетность основной элемент учетный политика инвентаризация актив обязательство порядок отражение результат учет порядок утверждение учетный политика организация критерий отнесение актив основный средство соответствие российский учетный практика состав единица учет основный средство отражение учет операция поступление основный средство оценка основный средство первоначальный признание переоценка восстановление основный средство порядок отражение учет амортизация основный средство метод начисление амортизация порядок отражение учет модернизация реконструкция ремонт основный средство бухгалтерский запись выбытие основный средство документальный оформление операция основный средство понятие доходный вложение материальный ценность аренда основный средство особенность отражение учет операционный финансовый аренда понятие вид нематериальный актив нма критерий отнесение актив нематериальный актив единица учет нематериальный актив порядок отражение учет операция поступление нма оценка нематериальный актив первоначальный признание переоценка нематериальный актив порядок отражение учет амортизация нематериальный актив порядок отражение учет деловой репутация организация порядок отражение учет учет расход научно-исследовательский опытно-конструкторский технологический работа документальный оформление операция нма состав материально-производственный запас порядок способ учет материал формирование себестоимость материал порядок учет затрата производство порядок способ учет готовый продукция метод калькулирование себестоимость метод учет товар метод оценка материально-производственный запас выбытие порядок формирование резерв обесценение материально-производственный запас учет продажа материально-производственный запас материал товар готовый продукция документирование хозяйственный операция материально-производственный запас порядок ведение учет кассовый операция порядок ведение учет безналичный расчет денежный средство валютный счет организация порядок учет денежный средство специальный счет банк порядок отражение учет перевод путь документирование операция денежный средство порядок оформление платежный поручение очередность платеж состав критерий признание единица учет финансовый вложение оценка финансовый вложение финансовый инструмент порядок отражение учет операция ценный бумага акция облигация вексель производный финансовый инструмент метод оценка ценный бумага выбытие доход расход финансовый вложение документальный оформление операция финансовый вложение понятие дебиторский задолженность состав резерв сомнительный долг списание безнадежный долг учет обязательство организация операционный обязательство организация финансовый обязательство списание просрочить кредиторский задолженность особенность учет отдельный вид финансовый обязательство особенность учет арендный обязательство финансовый аренда лизинг учет вознаграждение работник документальный оформление дебиторский кредиторский задолженность понятие классификация доход расход организация порядок отражение доход обычный вид деятельность соответствие российский международный стандарт пбу доход организация пбу расход организация формирование конечный финансовый результат реформирование баланс бухгалтерский прибыль порядок формирование особенность формирование налогооблагаемый прибыль постоянный временной разница бухгалтерский налогооблагаемый прибыль постоянный налоговый обязательство отложить налоговый обязательство отложить налоговый актив условный расход доход налог прибыль текущий налог прибыль порядок отражение финансовый отчетность понятие собственный капитал организация элемент собственный капитал эмиссия акция обыкновенный акция привилегированный акция учет уставный капитал учет добавочный капитал учет резервный капитал отражение собственный капитал финансовый отчетность понятие финансовый отчетность цель создание назначение концептуальный основа финансовый отчетность пользователь финансовый информация качественный характеристика полезный финансовый информация основополагающий допущение элемент финансовый отчетность актив обязательство капитал доход расход критерий признание отчетность элемент капитал концепция поддержание капитал представление финансовый отчетность соответствие российский международный стандарт финансовый отчетность бухгалтерский баланс порядок формирование отчет финансовый результат порядок формирование отчет изменение капитал отчет движение денежный средство пояснение финансовый отчетность промежуточный финансовый отчетность понятие консолидированный финансовый отчетность правило формирование показатель составление консолидированный финансовый отчетность раскрытие финансовый отчетность информация прекратить деятельность событие отчетный дата порядок раскрытие информация учет отчетность раскрытие информация пояснение операционный сегмент справедливый раскрытие информация связать сторона использование метод финансовый анализ цель дополнительный раскрытие информация финансовый отчетность</t>
+  </si>
+  <si>
+    <t>тема общий теория ценообразование экономический сущность цена функция цена задача цена основной участник ценообразование тема методология ценообразование основный принцип ценообразование методика ценообразование метод ценообразование тема структура цена элемент цена взаимосвязь себестоимость продукция переменный постоянный издержка прибыль компания косвенный налог цена влияние налоговый режим цена продукция услуга нпд усн осн тема система цена общий характеристика система цена классификация цена соотношение цена динамика цена фактор ценообразование тема цена компания ценовый политика компания ценовый стратегия компания алгоритм формирование ценовый стратегия компания тема государственный регулирование цена общий характеристика государственный регулирование цена инструмент государственный регулирование цена государственный регулирование цена рубеж тема мировой цена основной вид мировой цена влияние мировой цена национальный система ценообразование</t>
+  </si>
+  <si>
+    <t>понятие математический модель математический моделирование математический моделирование экономика классификация математический модель метод экономика предмет эконометрика возможность применение количественный анализ социально-экономический процесс пример эконометрический модель эконометрические метод эффективный средство количественный описание анализ моделирование прогноз социально-экономический процесс явление поддержка принятие решение бизнес управление проблема связать построение эконометрический модель обзор современный эконометрический метод важность качественный информационный обеспечение понятие регрессионный зависимость вид зависимость предмет регрессионный анализ линейный регрессия класс задача решать помощь модель линейный регрессия пример линейный регрессионный зависимость экономический переменный понятие экзогенный эндогенный переменный основной формально-математический проблема возникать построение регрессионный модель роль информационный обеспечение модель модель парный линейный регрессия пример парный линейный зависимость экономический интерпретация параметр модель оценка параметр модель метод малый квадрат метод максимальный правдоподобие сравнительный содержательный анализ мнк мп метод статистический проверка предпосылка лежать основа метод малый квадрат теоретический предпосылка основа строиться мнк-оценка роль правдоподобность выполнение реальный практический задача гомоскедастичность статистический свойство мнк-оценка несмещенность состоятельность оптимальность эффективность теорема гаусс-марков проверка статистический гипотеза коэффициент регрессия построение доверительный интервал коэффициент регрессия остаточный ошибка модель свойство статистический критерий проверка адекватность модель коэффициент детерминация модель множественный линейный регрессия пример социально-экономический процесс описание можно использовать модель многомерный линейный регрессия содержательный интерпретация коэффициент стохастический составлять проблема оценка параметр модель многомерный метод малый квадрат вывод нормальный уравнение теоретический предпосылка основа строиться оценка параметр модель многомерный мнк статистический свойство оценка параметр линейный модель множественный регрессия теорема гаусс-марков спецификация модель множественный линейный регрессия проверка адекватность модель множественный линейный регрессия остаток модель свойство коэффициент детерминация проверка статистический гипотеза коэффициент неоднородность дисперсия остаток гетероскедастичность автокорреляция коэффициент автокорреляция мультиколлинеарность метод устранение корректировка состав объяснять переменный регрессионный модель пример проблемный ситуация необходимый построение обобщенный модель обобщенный регрессионный модель обобщенный метод малый квадрат обобщенный линейный модель регрессия гетероскедастичный остаточный ошибка регрессионный модель переменный структура использование фиктивный переменный нелинейный модель регрессия метод линеаризация линейный модель стохастический регрессор метод инструментальный переменный пример применение обобщенный модель множественный линейный регрессия обсуждение проблема связать построение понятие временной ряд пример временной ряд экономика вид временной ряд одномерный стационарный нестационарный многомерный пример цель основной проблема связать анализ временной ряд модель стационарный временной ряд авторегрессия скользящий средний авторегрессии-скользящий средний идентификация одномерный стационарный ряд проверка адекватность модель метод прогнозирование математический описание нестационарный ряд метод выделение тренд сезонный регулярный составлять метод последовательный разность модель авторегрессии-проинтегрированного скользящий средний проверка адекватность модель нестационарный временной ряд модель распределенный лаг прогнозирование экономический показатель основа модель временной ряд система линейный одновременный уравнение модель динамический процесс экономика описывать система одновременный уравнение структурный привести форма уравнение идентификация статистический оценивание параметр система линейный одновременный уравнение косвенный метод малый квадрат свойство оценка неидентифицируемость сверхидентифицируемость двухшаговый трехшаговый метод малый квадрат точечный интервальный прогноз эндогенный переменный проблема проверка адекватность модель описывать система одновременный уравнение</t>
+  </si>
+  <si>
+    <t>формирование контур отдельный наука название курс гарвардский парадигма объект анализ отраслевой организация рынок предмет наука подход исследование товарный рынок субъект отраслевой рынок парадигма теория отраслевой рынок развитие классификация отраслевой рынок уровень концентрация отраслевой рынок оценка концентрация отраслевой рынок организационный структура размер эффективность фирма внутренний структура фирма альтернативный цель фирма агент фирма влияние цель фирма рыночный поведение технологический контрактный стратегический концепция поведение фирма отраслевой рынок феномен дифференциация продукт дифференциация продукт условие монополистический конкуренция вертикальный дифференциация продукт бренд проявление дифференциация продукт реклама роль функция рекламный расход российский опыт контекст международный сопоставление понятие барьер вход-выход классификация рынок уровень входной барьер вид нестратегический барьер вход фирма рынок барьер социально-экономический характер разновидность правительственный барьер гражданский барьер барьер выход фирма рынок показатель статистика вход-выход фирма рынок понятие вертикальный интеграция вид побудительный мотив фирма вертикальный интеграция интеграционный процесс отраслевой рынок интеграция аутсоринг вид интеграция вертикальный ограничение тип вертикальный ограничение следствие вертикальный интеграция слияние поглощение дискриминационный ценообразование практика продажа степень ценовый дискриминация воздействие ценовый дискриминация экономический процесс ограниченность информация качество товар возможный путь преодоление ограниченность информация качество товар ограниченность информация цена товар теория сигнал информационный роль реклама регулирование функционирование отраслевой рынок форма регулирование естественный монополия приватизация национализация теоретический основа государственный антимонопольный политика государственный антимонопольный политика отношение слияние поглощение фирма особенность государственный политика соглашение фиксирование цена ценовый дискриминация</t>
+  </si>
+  <si>
+    <t>определение экономический социология сходство различие экономико-теоретический экономико-социологический подход предметный область экономический социология метод экономический социология основной категория экономический социология экономический действие центральный категория экономический социология экономический действие социальный структура модель поведение homo economicus homo sociologicus основной направление проблематика современный экономический социология понятие хозяйственный мотив мотивационный структура регулятор экономический поведение модель экономический социологический человек проблема рациональность интерпретация граница рациональность множественность тип рациональный действие определение рынок конституировать элемент рынок рынок совокупность социальный сеть различный форма сетевой связь формирование социальный капитал основа социальный сеть этнический экономика институциональный подход анализ рынок фундаментальный порядок вовлеченность связь конвенция координация социокультурный подход анализ рынок культура экономика форма способ взаимовлияние аспект рыночный культура когнитивный ценностный символический проблема формирование экономический культура современный россия понятие государство эволюция государственный вмешательство хозяйственный жизнь основный функция современный государство новый парадигма отношение государство рынок тип государственный регулирование модель взаимодействие государство рынок модель социальный политика государство всеобщий благосостояние характеристика коррупционный отношение захват государство государственный регулирование экономика современный россия структурный институциональный подход анализ ненаблюдаемый экономика неформальный экономика сегмент хозяйствование теневой экономика нелегальный криминальный экономика измерение неформальный экономика экономический этнокультурный социальный фактор существование неформальный экономика причина рост теневой экономика влияние государственный регулирование степень формализация экономика формальный неформальный правило формализация деформализация правило ненаблюдаемый экономика современный россия отношение занятость спрос предложение рынок труд работодатель наемный работник трудовой мотивация рынок труд сегментация рынок труд внутренний внешний рынок труд первичный вторичный рынок труд ядро периферия фактор сегментация рынок труд социальный механизм трудовой наем заполнение рабочий место социально-демографический портрет безработный последствие безработица рынок труд рынок образовательный услуга проблема соответствие характеристика российский рынок труд особенность рынок труд российский регион определение предпринимательство предприниматель социально-психологический портрет эволюция предпринимательский функция собственник капитал комбинатор экономический ресурс носитель риск неопределенность инноватор мотивация предпринимательский деятельность способ изучение предпринимательский поведение ресурсный основание деятельность отношение группа предприниматель взаимодействие представитель властный структура крупный бизнес малый средний бизнес роль государство содействие предпринимательство предпринимательский деятельность современный россия домашний хозяйство домашний труд современный семья особенность различный страна распределение использование семейный ресурс внутрисемейный иерархия принцип распределение труд супруг домашний хозяйство бюджет время современный домашний хозяйство экономический социологический подход изучение потребительский поведение модель потребительский поведение понятие габитус система потребительский предпочтение стиль жизнь потребление инновационный процесс структура функция финансовый поведение сберегательный инвестиционный поведение домохозяйство экономико-социологический подход исследование социальный неравенство социальный структура общество стратификация критерий социальный статус общественный группа основной показатель способ измерение социально-экономический стратификация управленческий хозяйственный элита средний класс место роль развитие общество средний класс россия проблема идентификация</t>
+  </si>
+  <si>
+    <t>тема организация статистический деятельность рф тема источник статистический данные тема статистический исследование тема сводка группировка тема анализ получить результат тема индекс цена измерение инфляция тема система национальный счет измерение ввп</t>
+  </si>
+  <si>
+    <t>тема экономический анализ наука практика тема информационный обеспечение экономический анализ тема вид экономический анализ тема метод прием экономический анализ тема аспектный экономический анализ тема рейтинговый скоринговый подход аналитический процедура тема техника составление аналитический заключение</t>
+  </si>
+  <si>
+    <t>обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка общеразвивать упражнение общеразвивать упражнение предмет предмет строевой упражнение поворот место движение перестроение место движение упражнение направить формирование правильный осанка прикладной упражнение ходьба бег прыжок упражнение равновесие подтягивание перекладина сгибание разгибание рука упор лежать упражнение использование отягощение прыжок длина прыжок препятствие челночный бег подвижный игра эстафета плавание обучение умение держаться вода прыжок вода обучение классический стиль плавание атлетический гимнастика упражнение отягощение тренажер развитие сила рука плечевой пояс шея туловище нога волейбол обучение стойка перемещение ходьба бег скачок прыжок старт остановка поворот обучение техника подача сверху снизу прием мяч сверху снизу рука основа тактика волейбол розыгрыш мяч касание игрок зона игровой практика баскетбол техника игра защита защитный стойка перемещение обычный приставной шаг различный направление передвижение спина вперед обучение техника владение мяч ловля мяч место движение ведение мяч правый левый рука движение шаг бег бросок мяч корзина штрафной бросок игровой практика контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка техника выполнение упражнение атлетический гимнастика тренировка отдельный мышечный группа обучение основа техника упражнение жим штанга лежа горизонтальный скамья разводка гантель сторона лежа подъем штанга бицепс стоя жим лежать узкий хват французский жим стоя жим штанга стоить грудь приседание штанга плечо становой тяга тяга штанга наклон пояс шраги пресс наклонный скамья пресс консольный брус развитие отдельный группа мышца тренажер тяга рукоятка блок подбородок стоить тяга рукоятка блок голова широкий хватом сидеть тяга рукоятка блок живот сидя сгибание рука штанга скамья скотт сгибание рука блочный устройство трицепсовый жим блок стоить разгибание рука блок сидеть разгибание нога тренажер сидя сгибание нога тренажер сидя жим нога тренажер сидеть сведение рука грудь тренажер сидя голень тренажер сидя пресс римский стул гиперэкстензия кроссовер отжимание брус блочный устройство упражнение увеличение мышечный масса мышца рука сгибание рука штанга читинг подтягивание обратный хват отягощение пояс жим лежать узкий хват французский жим узкий хват лежать мышца спина сведение плечо назад-вверх штанга рука тяга гантель наклон попеременно тяга спина штанга мышца нога приседание штанга плечо грудь становой тяга выпрямить нога дельтовидный мышца жим штанга стоить широкий хват грудь тяга штанга подбородок узкий хват коррекция отдельный группа мышца бицепс сгибание рука скамья скотт сгибание рука гантель сгибание рука штанга трицепс французский жим стоить лежать лоб отведение рука гантель назад наклон мышца спина вращение плечо гантель рука тяга блок живот сидя гиперэкстензия квадрицепс полуприсед штанга приседание штанга рука спина бицепс бедро половинчатый сгибание нога блок дельтовидный мышца жим сидя широкий хват грудь голова жим сидеть локти сторона мышца грудь разводка лежа жим штанга лежать отрицательный угол упражнение тренажер различный тип тяга рукоятка блок подбородок стоить тяга рукоятка блок голова широкий хватом сидеть тяга рукоятка блок живот сидя сгибание рука штанга скамья скотт сгибание рука блочный устройство трицепсовый жим блок стоить разгибание рука блок сидеть разгибание нога тренажер сидя сгибание нога тренажер сидя жим нога тренажер сидеть сведение рука грудь тренажер сидя голень тренажер сидя пресс римский стул гиперэкстензия кроссовер отжимание брус блочный устройство контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка техника выполнение обязательный элемент шаг аэробика обучение техника обязательный элемент система нон-стоп проведение упражнение поточный метод обучение согласовать движение рука нога комплекс упражнение аэробика этап составление комбинация выбор музыкальный сопровождение подбор упражнение логичный переход движение перемещение смена направление изучение совершенствование техника упражнение аэробика система нон-стоп метод квадрат пирамидальный метод обучение техника соединение упражнение смена нога первый упражнение последний упражнение середина комбинация прикладной вид аэробика аэробика снаряд степ-аэробика слайд-аэробика фитбол- аэробика аква- аэробика прикладной вид аэробика танцевальный аэробика латиноамериканский танец джаз-аэробика фанк-хип-хоп классический танец аэробика йога аэробика общий характеристика специфика основный понятие йога система физический умственный духовный тренировка основный ступень йога построение урок музыкальный сопровождение занятие освоение основный асан гора дерево вытянуть треугольник воин тадасан методика построение комплекс фитнес йога освоение техника релаксация медитация дыхание система йога восточный вид единоборство аэробика исторический аспект появление программа аэробика соединение восточный вид единоборство основной стиль карате аэробика айкидо дзю- дзюца винчунь кикбоксинг таеквондо физиологический биохимический основа движение взаимосвязь принцип построение хореография классический аэробика элемент восточный вид единоборство особенность структура урок методика составление программа основный положение движение основный стойка нейтральный стойка удар рука удар нога практический выполнение различный шаг соединение парный тренировка закрепление техника совершенствование различный композиция достижение высокий уровень спортивный форма психологический подготовка студент особенность работа опорно-двигательный аппарат работа мышца работа сенсорный система организм основной закономерность управление двигательный действие выполнение базовый шаг скачок подскок прыжок особенность опора выполнение равновесие правильный осанка равновесие тело центр тяжесть тело угол устойчивость техника упражнение выполнять место техника беговой упражнение овладение методика аутотренинг метод совершенствование коммуникационный способность настройка дыхание движение настройка интонация настройка внутренний ритм контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка специальный физический подготовка упражнение развитие физический качество необходимый волейболист сила быстрота координация движение гибкость общий скоростной выносливость прыгучесть совершенствование техника игра волейбол стойка перемещение основный стойка перемещение ходьба бег скачок прыжок техника владение мяч подача нижний прямой нижний боковой верхний прямой подача точность различный зона площадка передача мяч передача рука сверху стойка движение место перемещение вперед назад длинный средний короткий передача нападать удар нападать удар прямой перевод перевод поворот туловище блок обход блок прием мяч прием мяч сверху рука снизу рука рука блокирование блокирование одиночный групповой неподвижный подвижный тактика нападение индивидуальный тактический действие пасовать нападающий групповой командный тактический действие пасовать зона тактика защита индивидуальный групповой командный тактический действие система защита угол вперед страховка нападающий страховка блокировать контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка специальный физический подготовка упражнение развитие физический качество необходимый баскетболист сила быстрота координация движение гибкость общий скоростной выносливость прыгучесть совершенствование техника игра баскетбол техника перемещение бег обычный приставной шаг изменение скорость направление прыжок остановка поворот рывок техника владение мяч ловля передача мяч правый левый рука место движение шаг бег ведение мяч правый левый рука место движение шаг бег бросок мяч корзина штрафной бросок техника овладение мяч противодействие овладение мяч отскок щит корзина вырывание выбивание перехват мяч способ противодействие бросок корзина элемент тактика игра нападение индивидуальный действие игрок мяч мяч взаимодействие игрок противник противник элемент тактика игра защита действие защитник игрок мяч мяч взаимодействие более игрок защита командный действие вариант тактический система защита контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка специальный физический подготовка упражнение развитие физический качество необходимый футболист сила быстрота координация движение гибкость общий специальный выносливость техника полевой игрок передвижение бег прыжок остановка поворот техника удар нога голова техника остановка мяч техника ведение мяч техника финт упражнение обучение техника остановка мяч внутренний сторона стопа подошва середина подъем упражнение удар мяч нога различный способ различный положение движение техника отбор мяч владение мяч техника вбрасывание мяч техника вратарь упражнение ловля отбивание перевод бросок мяч упражнение техника вбрасывание мяч упражнение ловля мяч лететь уровень колено бедро пояс грудь катиться земля тактика нападение индивидуальный действие игрок мяч мяч взаимодействие игрок противник противник тактика защита действие защитник игрок мяч мяч взаимодействие более игрок защита командный действие вариант тактический система защита контрольный тестирование уровень спортивно-технический подготовленность обучение техника попеременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника одновременный лыжный ход развитие быстрота сила выносливость скоростно-силовой качество координационный способность обучение техника спуск подъем развитие ловкость сила скоростно-силовой качество контрольный тестирование лыжный подготовка развитие совершенствование сердечно-сосудистый дыхательный система организм упражнение развитие совершенствование сердечно-сосудистый дыхательный система организм развитие физический качество выносливость гибкость координация скоростно-силовой подготовка упражнение координация подвижность сустав имитационный дыхательный упражнение подготовительный упражнение освоение вода специальный имитационный упражнение суша учебный прыжок вода игра развлечение вода упражнение изучение техника спортивный способ плавание обучение техника плавание кроль грудь кроль спина обучение совершенствование техника плавание брасс обучение совершенствование техника плавание способ баттерфляй контрольный тестирование уровень спортивно-технический подготовленность специальный физический подготовка комплекс общеразвивать упражнение направить раз¬витие гибкость координационный способность силовой выносли¬вость спортивный подвижный игра направить развитие ловкость быстрота выносливость эстафета прыжковый упраж¬нение направить развитие скоростно-силовой способность быстрота циклический упражнение направить развитие выносливость имитационный упражнение кроссовый подготовка ходьба преимущественно направить увеличение аэробный произ¬водительность организм развитие волевой качество специфи¬ческий лыжник-гонщик комплекс специальный упражне¬ние лыжа лыжероллер развитие силовой выносливо¬сть мышца нога плечевой пояс обучение совершенствование техника лыжный ход ступать шаг скользящий шаг обучение ступать шаг скольжение лыжа стойка лыжник поворот отталкивание нога рука перед¬вижения попеременный двухшажный ход последовательность обучение фазовый состав структура движение попеременный двухшажный одновременный лыжный ход изучение совершенствова¬ний элемент классический ход обучение подседаний отталки¬вание мах рука нога активный постановка палка формирование целесообразный ритм двигательный действие передвижение классический ход классификация коньковый лыжный ход последовательность обучение фазовый состав структура движение изучение совершенствова¬ний элемент конь¬ковый ход обучение маховый вынос нога постановка опора подседания опорный нога отталкивание боковой сколь¬зящий упор ударный постановка палка финальный усилие отталкивание рука формирование целесообразный ритм двигательный действие передвижение коньковый ход обучение совершенствование техника подъем спуск елочка полуелочка лесенка ступать шаг торможение плуг полуплуг специфичный двигательный действие прохождение подъем лыжный ход движение контролировать обучение высокий средний низкий стойка спуск своевременный выпрямление траектория движение обучение техника преодоление неровность характерный двигательный действие вид торможение лыжа особенность обучение торможение палка управляемый падение обучение поворот движение переступание плуг упор параллельный лыжа характерный двигательный действие выполнение различный поворот движение место тренировка дистанция применение изучить лыжный ход прохождение дистанция различный темп равнинный пересечь местность силовой тренировка подъем короткий ускорение дистанция равномерный интервальный контрольный круговой тренировка лыжа игра игровой упражнение лыжа контрольный тестирование уровень спортивно-технический подготовленность тема активация вестибулярный функциональный система ор ходьба место поворот вращение голова туловище бег вращаясь ор узкий ограничить опора ходьба бег прыжок гимнастический скамейка низкий высокий гимнастический бревно ходьба поворот градус тема общеразвивающие дыхательный релаксировать упражнение ходьба бег сочетание ходьба бег плавание упражнение место движение ходьба бег упражнение координация равновесие тема упражнение предмет фитбол гимнастический палка малый мяч тема упражнение место лежать коврик движение ходьба упражнение координация равновесие упражнение сидеть лежать коврик укрепление различный мышечный группа общеразвивать упражнение сочетание дыхательный упражнение тренажер укрепление локальный мышечный группа развитие мышечный корсет тема комплекс лечебный физический культура заболевание тема контрольный тестирование</t>
   </si>
 </sst>
 </file>
@@ -659,535 +1388,1928 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>126</v>
+      </c>
+      <c r="D15" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>127</v>
+      </c>
+      <c r="D16" t="s">
+        <v>225</v>
+      </c>
+      <c r="E16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>128</v>
+      </c>
+      <c r="D17" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>134</v>
+      </c>
+      <c r="D23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>135</v>
+      </c>
+      <c r="D24" t="s">
+        <v>225</v>
+      </c>
+      <c r="E24" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>137</v>
+      </c>
+      <c r="D26" t="s">
+        <v>225</v>
+      </c>
+      <c r="E26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>138</v>
+      </c>
+      <c r="D27" t="s">
+        <v>225</v>
+      </c>
+      <c r="E27" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>139</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>140</v>
+      </c>
+      <c r="D29" t="s">
+        <v>225</v>
+      </c>
+      <c r="E29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>141</v>
+      </c>
+      <c r="D30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>142</v>
+      </c>
+      <c r="D31" t="s">
+        <v>225</v>
+      </c>
+      <c r="E31" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
+        <v>225</v>
+      </c>
+      <c r="E32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>144</v>
+      </c>
+      <c r="D33" t="s">
+        <v>225</v>
+      </c>
+      <c r="E33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>145</v>
+      </c>
+      <c r="D34" t="s">
+        <v>225</v>
+      </c>
+      <c r="E34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>146</v>
+      </c>
+      <c r="D35" t="s">
+        <v>225</v>
+      </c>
+      <c r="E35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>147</v>
+      </c>
+      <c r="D36" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>148</v>
+      </c>
+      <c r="D37" t="s">
+        <v>225</v>
+      </c>
+      <c r="E37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>151</v>
+      </c>
+      <c r="D40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>152</v>
+      </c>
+      <c r="D41" t="s">
+        <v>225</v>
+      </c>
+      <c r="E41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>153</v>
+      </c>
+      <c r="D42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>154</v>
+      </c>
+      <c r="D43" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="D44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>156</v>
+      </c>
+      <c r="D45" t="s">
+        <v>225</v>
+      </c>
+      <c r="E45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>157</v>
+      </c>
+      <c r="D46" t="s">
+        <v>225</v>
+      </c>
+      <c r="E46" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>158</v>
+      </c>
+      <c r="D47" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" t="s">
+        <v>225</v>
+      </c>
+      <c r="E48" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" t="s">
+        <v>226</v>
+      </c>
+      <c r="E50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" t="s">
+        <v>226</v>
+      </c>
+      <c r="E51" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" t="s">
+        <v>226</v>
+      </c>
+      <c r="E52" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" t="s">
+        <v>226</v>
+      </c>
+      <c r="E53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" t="s">
+        <v>226</v>
+      </c>
+      <c r="E54" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" t="s">
+        <v>226</v>
+      </c>
+      <c r="E55" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" t="s">
+        <v>226</v>
+      </c>
+      <c r="E56" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" t="s">
+        <v>169</v>
+      </c>
+      <c r="D58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" t="s">
+        <v>226</v>
+      </c>
+      <c r="E59" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" t="s">
+        <v>226</v>
+      </c>
+      <c r="E60" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>226</v>
+      </c>
+      <c r="E61" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>226</v>
+      </c>
+      <c r="E62" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E63" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" t="s">
+        <v>175</v>
+      </c>
+      <c r="D64" t="s">
+        <v>226</v>
+      </c>
+      <c r="E64" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" t="s">
+        <v>176</v>
+      </c>
+      <c r="D65" t="s">
+        <v>226</v>
+      </c>
+      <c r="E65" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" t="s">
+        <v>178</v>
+      </c>
+      <c r="D67" t="s">
+        <v>226</v>
+      </c>
+      <c r="E67" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" t="s">
+        <v>226</v>
+      </c>
+      <c r="E68" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>180</v>
+      </c>
+      <c r="D69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E69" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" t="s">
+        <v>226</v>
+      </c>
+      <c r="E70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" t="s">
+        <v>182</v>
+      </c>
+      <c r="D71" t="s">
+        <v>226</v>
+      </c>
+      <c r="E71" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" t="s">
+        <v>226</v>
+      </c>
+      <c r="E72" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D73" t="s">
+        <v>226</v>
+      </c>
+      <c r="E73" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E74" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" t="s">
+        <v>226</v>
+      </c>
+      <c r="E75" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" t="s">
+        <v>187</v>
+      </c>
+      <c r="D76" t="s">
+        <v>226</v>
+      </c>
+      <c r="E76" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77" t="s">
+        <v>226</v>
+      </c>
+      <c r="E77" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" t="s">
+        <v>226</v>
+      </c>
+      <c r="E78" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" t="s">
+        <v>226</v>
+      </c>
+      <c r="E79" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" t="s">
+        <v>191</v>
+      </c>
+      <c r="D80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
+        <v>192</v>
+      </c>
+      <c r="D81" t="s">
+        <v>226</v>
+      </c>
+      <c r="E81" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" t="s">
+        <v>193</v>
+      </c>
+      <c r="D82" t="s">
+        <v>226</v>
+      </c>
+      <c r="E82" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83" t="s">
+        <v>194</v>
+      </c>
+      <c r="D83" t="s">
+        <v>226</v>
+      </c>
+      <c r="E83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C84" t="s">
+        <v>195</v>
+      </c>
+      <c r="D84" t="s">
+        <v>226</v>
+      </c>
+      <c r="E84" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" t="s">
+        <v>226</v>
+      </c>
+      <c r="E85" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" t="s">
+        <v>197</v>
+      </c>
+      <c r="D86" t="s">
+        <v>226</v>
+      </c>
+      <c r="E86" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" t="s">
+        <v>226</v>
+      </c>
+      <c r="E87" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" t="s">
+        <v>226</v>
+      </c>
+      <c r="E88" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89" t="s">
+        <v>200</v>
+      </c>
+      <c r="D89" t="s">
+        <v>226</v>
+      </c>
+      <c r="E89" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" t="s">
+        <v>201</v>
+      </c>
+      <c r="D90" t="s">
+        <v>226</v>
+      </c>
+      <c r="E90" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" t="s">
+        <v>202</v>
+      </c>
+      <c r="D91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E91" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92" t="s">
+        <v>203</v>
+      </c>
+      <c r="D92" t="s">
+        <v>226</v>
+      </c>
+      <c r="E92" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>94</v>
+      </c>
+      <c r="C93" t="s">
+        <v>204</v>
+      </c>
+      <c r="D93" t="s">
+        <v>226</v>
+      </c>
+      <c r="E93" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
         <v>95</v>
+      </c>
+      <c r="C94" t="s">
+        <v>205</v>
+      </c>
+      <c r="D94" t="s">
+        <v>226</v>
+      </c>
+      <c r="E94" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95" t="s">
+        <v>206</v>
+      </c>
+      <c r="D95" t="s">
+        <v>226</v>
+      </c>
+      <c r="E95" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+      <c r="C96" t="s">
+        <v>207</v>
+      </c>
+      <c r="D96" t="s">
+        <v>226</v>
+      </c>
+      <c r="E96" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>98</v>
+      </c>
+      <c r="C97" t="s">
+        <v>208</v>
+      </c>
+      <c r="D97" t="s">
+        <v>226</v>
+      </c>
+      <c r="E97" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98" t="s">
+        <v>209</v>
+      </c>
+      <c r="D98" t="s">
+        <v>226</v>
+      </c>
+      <c r="E98" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" t="s">
+        <v>210</v>
+      </c>
+      <c r="D99" t="s">
+        <v>226</v>
+      </c>
+      <c r="E99" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" t="s">
+        <v>211</v>
+      </c>
+      <c r="D100" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>45</v>
+      </c>
+      <c r="C101" t="s">
+        <v>212</v>
+      </c>
+      <c r="D101" t="s">
+        <v>226</v>
+      </c>
+      <c r="E101" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" t="s">
+        <v>213</v>
+      </c>
+      <c r="D102" t="s">
+        <v>226</v>
+      </c>
+      <c r="E102" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>102</v>
+      </c>
+      <c r="C103" t="s">
+        <v>214</v>
+      </c>
+      <c r="D103" t="s">
+        <v>226</v>
+      </c>
+      <c r="E103" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>103</v>
+      </c>
+      <c r="C104" t="s">
+        <v>215</v>
+      </c>
+      <c r="D104" t="s">
+        <v>226</v>
+      </c>
+      <c r="E104" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>104</v>
+      </c>
+      <c r="C105" t="s">
+        <v>216</v>
+      </c>
+      <c r="D105" t="s">
+        <v>226</v>
+      </c>
+      <c r="E105" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>105</v>
+      </c>
+      <c r="C106" t="s">
+        <v>217</v>
+      </c>
+      <c r="D106" t="s">
+        <v>226</v>
+      </c>
+      <c r="E106" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>106</v>
+      </c>
+      <c r="C107" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" t="s">
+        <v>226</v>
+      </c>
+      <c r="E107" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" t="s">
+        <v>219</v>
+      </c>
+      <c r="D108" t="s">
+        <v>226</v>
+      </c>
+      <c r="E108" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" t="s">
+        <v>220</v>
+      </c>
+      <c r="D109" t="s">
+        <v>226</v>
+      </c>
+      <c r="E109" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>221</v>
+      </c>
+      <c r="D110" t="s">
+        <v>226</v>
+      </c>
+      <c r="E110" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>222</v>
+      </c>
+      <c r="D111" t="s">
+        <v>226</v>
+      </c>
+      <c r="E111" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" t="s">
+        <v>223</v>
+      </c>
+      <c r="D112" t="s">
+        <v>226</v>
+      </c>
+      <c r="E112" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" t="s">
+        <v>224</v>
+      </c>
+      <c r="D113" t="s">
+        <v>226</v>
+      </c>
+      <c r="E113" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>